<commit_message>
correct name of ${plw_name} in wom anth
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/RapidSMART/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="137" documentId="8_{8B91821C-8A1F-41C6-BC52-3B553F88EB8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1EC4CF29-F95E-4814-A47D-3E27AF840B16}"/>
+  <xr:revisionPtr revIDLastSave="142" documentId="8_{8B91821C-8A1F-41C6-BC52-3B553F88EB8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4456EB33-AB7A-4CB3-8E69-6EEEEB054CD0}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1886,9 +1886,6 @@
     <t>wom_muac</t>
   </si>
   <si>
-    <t>Woman's MUAC in MM of (${woman_1})</t>
-  </si>
-  <si>
     <t xml:space="preserve">(. &gt;= 90 and . &lt;650) </t>
   </si>
   <si>
@@ -1901,15 +1898,9 @@
     <t>wom_wgt</t>
   </si>
   <si>
-    <t>Woman's WEIGHT in KG of (${woman_1})</t>
-  </si>
-  <si>
     <t xml:space="preserve">(. &gt;= 110 and . &lt;210) </t>
   </si>
   <si>
-    <t>Woman's HEIGHT in CM of (${woman_1})</t>
-  </si>
-  <si>
     <t>Please remeasure woman's HEIGHT</t>
   </si>
   <si>
@@ -1950,6 +1941,15 @@
   </si>
   <si>
     <t>indexed-repeat(${age_years}, ${hh_roster}, ${plw_hh_position})</t>
+  </si>
+  <si>
+    <t>Woman's MUAC in MM of (${plw_name})</t>
+  </si>
+  <si>
+    <t>Woman's HEIGHT in CM of (${plw_name})</t>
+  </si>
+  <si>
+    <t>Woman's WEIGHT in KG of (${plw_name})</t>
   </si>
 </sst>
 </file>
@@ -1997,7 +1997,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2006,6 +2006,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2347,8 +2350,8 @@
   <dimension ref="A1:N187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E183" sqref="E183"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C164" sqref="C164:C166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4791,7 +4794,7 @@
         <v>550</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="159" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4799,7 +4802,7 @@
         <v>17</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="C159" s="4"/>
       <c r="G159" t="s">
@@ -4811,11 +4814,11 @@
         <v>17</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C160" s="4"/>
       <c r="G160" s="3" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="161" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4823,11 +4826,11 @@
         <v>17</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="C161" s="4"/>
       <c r="G161" s="3" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="162" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4835,11 +4838,11 @@
         <v>17</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C162" s="4"/>
       <c r="G162" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="163" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4847,16 +4850,16 @@
         <v>64</v>
       </c>
       <c r="B163" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>136</v>
       </c>
       <c r="M163" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="164" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4866,17 +4869,17 @@
       <c r="B164" t="s">
         <v>552</v>
       </c>
-      <c r="C164" s="4" t="s">
+      <c r="C164" s="6" t="s">
+        <v>572</v>
+      </c>
+      <c r="J164" t="s">
         <v>553</v>
       </c>
-      <c r="J164" t="s">
+      <c r="K164" t="s">
         <v>554</v>
       </c>
-      <c r="K164" t="s">
-        <v>555</v>
-      </c>
       <c r="M164" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="165" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4884,19 +4887,19 @@
         <v>551</v>
       </c>
       <c r="B165" t="s">
-        <v>556</v>
-      </c>
-      <c r="C165" s="4" t="s">
-        <v>560</v>
+        <v>555</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>573</v>
       </c>
       <c r="J165" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="K165" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="M165" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="166" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4904,19 +4907,19 @@
         <v>551</v>
       </c>
       <c r="B166" t="s">
-        <v>557</v>
-      </c>
-      <c r="C166" s="4" t="s">
-        <v>558</v>
+        <v>556</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>574</v>
       </c>
       <c r="J166" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="K166" t="s">
+        <v>559</v>
+      </c>
+      <c r="M166" s="3" t="s">
         <v>562</v>
-      </c>
-      <c r="M166" s="3" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="167" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5671,21 +5674,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6124,7 +6112,81 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
@@ -6188,82 +6250,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6286,16 +6273,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6309,9 +6306,15 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
removed 2nd 'or' from if plw line
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rojohnston\OneDrive - UNICEF\1 UNICEF Work\1 Afghanistan\Surveys\UrbanSMART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{8B91821C-8A1F-41C6-BC52-3B553F88EB8F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4456EB33-AB7A-4CB3-8E69-6EEEEB054CD0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C61D27C-EDF1-4C0C-9784-8C74395617FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1862,9 +1862,6 @@
     <t>is_plw</t>
   </si>
   <si>
-    <t>if(${curr_pregnant}='1' or ${curr_breastfeed}='1' or ,true(),false())</t>
-  </si>
-  <si>
     <t>plw</t>
   </si>
   <si>
@@ -1950,6 +1947,9 @@
   </si>
   <si>
     <t>Woman's WEIGHT in KG of (${plw_name})</t>
+  </si>
+  <si>
+    <t>if(${curr_pregnant}='1' or ${curr_breastfeed}='1',true(),false())</t>
   </si>
 </sst>
 </file>
@@ -2350,8 +2350,8 @@
   <dimension ref="A1:N187"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C164" sqref="C164:C166"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2876,7 +2876,7 @@
         <v>544</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>545</v>
+        <v>574</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2886,6 +2886,7 @@
       <c r="B35" t="s">
         <v>99</v>
       </c>
+      <c r="C35" s="3"/>
       <c r="G35" t="s">
         <v>100</v>
       </c>
@@ -2979,10 +2980,10 @@
         <v>17</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="G43" s="1" t="s">
         <v>546</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2990,10 +2991,10 @@
         <v>17</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4791,10 +4792,10 @@
         <v>75</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="159" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4802,7 +4803,7 @@
         <v>17</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="C159" s="4"/>
       <c r="G159" t="s">
@@ -4814,11 +4815,11 @@
         <v>17</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="C160" s="4"/>
       <c r="G160" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="161" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4826,11 +4827,11 @@
         <v>17</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="C161" s="4"/>
       <c r="G161" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="162" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4838,11 +4839,11 @@
         <v>17</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="C162" s="4"/>
       <c r="G162" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="163" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4850,76 +4851,76 @@
         <v>64</v>
       </c>
       <c r="B163" t="s">
+        <v>566</v>
+      </c>
+      <c r="C163" s="5" t="s">
         <v>567</v>
-      </c>
-      <c r="C163" s="5" t="s">
-        <v>568</v>
       </c>
       <c r="D163" s="3" t="s">
         <v>136</v>
       </c>
       <c r="M163" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="164" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
+        <v>550</v>
+      </c>
+      <c r="B164" t="s">
         <v>551</v>
       </c>
-      <c r="B164" t="s">
+      <c r="C164" s="6" t="s">
+        <v>571</v>
+      </c>
+      <c r="J164" t="s">
         <v>552</v>
       </c>
-      <c r="C164" s="6" t="s">
-        <v>572</v>
-      </c>
-      <c r="J164" t="s">
+      <c r="K164" t="s">
         <v>553</v>
       </c>
-      <c r="K164" t="s">
-        <v>554</v>
-      </c>
       <c r="M164" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="165" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B165" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="J165" t="s">
+        <v>556</v>
+      </c>
+      <c r="K165" t="s">
         <v>557</v>
       </c>
-      <c r="K165" t="s">
-        <v>558</v>
-      </c>
       <c r="M165" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="166" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B166" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="J166" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="K166" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="M166" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="167" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4927,7 +4928,7 @@
         <v>101</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5674,6 +5675,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6112,81 +6128,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
@@ -6250,7 +6192,82 @@
 </p:properties>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6273,26 +6290,16 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6306,15 +6313,9 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Removed unnecessary lines of code
Duplicate start date, time, end time, calc of time
Removed note to double check the z-score checks - should not be presented to interviewer
PLW section is not working
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rojohnston\OneDrive - UNICEF\1 UNICEF Work\1 Afghanistan\Surveys\UrbanSMART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C61D27C-EDF1-4C0C-9784-8C74395617FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F28D39D-4BD8-415F-98EE-8E1CB0ED9AC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="575">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="554">
   <si>
     <t>type</t>
   </si>
@@ -117,27 +117,9 @@
     <t>date</t>
   </si>
   <si>
-    <t>SURVDAT</t>
-  </si>
-  <si>
-    <t>Date of interview</t>
-  </si>
-  <si>
-    <t>Date de l'entretien</t>
-  </si>
-  <si>
     <t>no-calendar</t>
   </si>
   <si>
-    <t>.&lt;= today()</t>
-  </si>
-  <si>
-    <t>The interview cannot take place in the future.</t>
-  </si>
-  <si>
-    <t>La date d'entretien ne peut être dans le futur.</t>
-  </si>
-  <si>
     <t>integer</t>
   </si>
   <si>
@@ -184,18 +166,6 @@
   </si>
   <si>
     <t>end_group</t>
-  </si>
-  <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>starttime</t>
-  </si>
-  <si>
-    <t>Interview start time</t>
-  </si>
-  <si>
-    <t>Heure de début de l'entretien</t>
   </si>
   <si>
     <t>selected</t>
@@ -909,33 +879,6 @@
     <t>if (${haz_flag}=1 or ${whz_flag}=1 or ${waz_flag}=1 or ${muac_flag}=1, '1', '0')</t>
   </si>
   <si>
-    <t>show_calculations</t>
-  </si>
-  <si>
-    <t>agemos ${MONTHS}
-hgt ${HEIGHT}
-wgt ${WEIGHT}
-whz_neg3 ${whz_neg3}
-whz_pos3 ${whz_pos3}
-whz_flag ${whz_flag}
-whz_neg2 ${whz_neg2}
-haz_neg35 ${haz_neg35}
-haz_pos35 ${haz_pos35}
-haz_flag	${haz_flag}
-waz_neg3 ${waz_neg3}
-waz_pos3 ${waz_pos3}
-waz_flag ${waz_flag}
-muac mm ${MUAC}
-muac_neg3 ${muac_neg3}
-muac_pos3 ${muac_pos3}
-muac_flag ${muac_flag}
-sam_muac ${sam_muac}
-mam_muac ${mam_muac}
-sam ${sam}
-mam ${mam}
-flag ${flag}</t>
-  </si>
-  <si>
     <t>second_measure</t>
   </si>
   <si>
@@ -1397,9 +1340,6 @@
     <t>sam_ref_note</t>
   </si>
   <si>
-    <t>${child_name}  has conditions indicating SEVERE ACUTE MALNUTRITION (SAM).</t>
-  </si>
-  <si>
     <t>${child_name}  présente des conditions indiquant une MALNUTRITION AIGÜE SÉVÈRE (MAS).</t>
   </si>
   <si>
@@ -1427,9 +1367,6 @@
     <t>mam_ref_note</t>
   </si>
   <si>
-    <t>${child_name}  has conditions indicating MODERATE ACUTE MALNUTRITION (MAM).</t>
-  </si>
-  <si>
     <t>${child_name}  présente des conditions indiquant une MALNUTRITION AIGÜE MODÉRÉE (MAM).</t>
   </si>
   <si>
@@ -1457,9 +1394,6 @@
     <t>no_acutemal</t>
   </si>
   <si>
-    <t>${child_name}  doesn't have conditions indicating acute malnutrition</t>
-  </si>
-  <si>
     <t>${child_name}  ne présente pas de conditions indiquant une malnutrition aigüe</t>
   </si>
   <si>
@@ -1562,39 +1496,6 @@
     <t>Veuillez noter tous commentaires pertinents et relatifs à l'entretien (OPTIONNEL)</t>
   </si>
   <si>
-    <t>endtime</t>
-  </si>
-  <si>
-    <t>Interview end time</t>
-  </si>
-  <si>
-    <t>Heure de fin de l'entretien</t>
-  </si>
-  <si>
-    <t>duration</t>
-  </si>
-  <si>
-    <t>(decimal-time(${endtime}) - decimal-time(${starttime})) * 1440</t>
-  </si>
-  <si>
-    <t>hhrefused</t>
-  </si>
-  <si>
-    <t>${int_resultref} = 3</t>
-  </si>
-  <si>
-    <t>hhabsent</t>
-  </si>
-  <si>
-    <t>${int_resultoth} = 4</t>
-  </si>
-  <si>
-    <t>hhabandoned</t>
-  </si>
-  <si>
-    <t>${int_resultoth} = 5</t>
-  </si>
-  <si>
     <t>total_eligible</t>
   </si>
   <si>
@@ -1950,6 +1851,21 @@
   </si>
   <si>
     <t>if(${curr_pregnant}='1' or ${curr_breastfeed}='1',true(),false())</t>
+  </si>
+  <si>
+    <t>Pregnant &amp; Lactating Woman section</t>
+  </si>
+  <si>
+    <t>${child_name} - has SEVERE ACUTE MALNUTRITION (SAM).</t>
+  </si>
+  <si>
+    <t>${child_name} -  has MODERATE ACUTE MALNUTRITION (MAM).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${child_name} - is NOT acutely malnourished </t>
+  </si>
+  <si>
+    <t>Other (No one present)</t>
   </si>
 </sst>
 </file>
@@ -1965,7 +1881,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1984,6 +1900,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1997,7 +1919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2009,6 +1931,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2349,9 +2272,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E184" sqref="E184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2433,10 +2356,10 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="A5" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G5" t="s">
@@ -2488,111 +2411,82 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" t="s">
-        <v>34</v>
-      </c>
-      <c r="J9" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="H10" t="s">
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="L10" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="H11" t="s">
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="L11" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="H12" t="s">
         <v>24</v>
       </c>
       <c r="J12" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2600,35 +2494,18 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G13" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B14" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
-      <c r="C15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H15" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2636,7 +2513,7 @@
         <v>27</v>
       </c>
       <c r="B16" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2644,21 +2521,21 @@
         <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="H18" t="s">
         <v>24</v>
@@ -2666,70 +2543,70 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B19" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="M19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="M20" t="s">
         <v>59</v>
-      </c>
-      <c r="M20" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F21" t="s">
         <v>64</v>
       </c>
-      <c r="B21" t="s">
-        <v>70</v>
-      </c>
-      <c r="C21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" t="s">
-        <v>73</v>
-      </c>
-      <c r="F21" t="s">
-        <v>74</v>
-      </c>
       <c r="M21" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B22" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="D22" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="M22" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2737,7 +2614,7 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="I23" t="s">
         <v>29</v>
@@ -2751,10 +2628,10 @@
         <v>1</v>
       </c>
       <c r="C24" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
         <v>24</v>
@@ -2762,16 +2639,16 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="C25" t="s">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="H25" t="s">
         <v>24</v>
@@ -2779,82 +2656,82 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B26" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="D26" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="E26" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="F26" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="H26" t="s">
         <v>24</v>
       </c>
       <c r="J26" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="K26" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="L26" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B29" t="s">
-        <v>542</v>
+        <v>516</v>
       </c>
       <c r="C29" t="s">
-        <v>540</v>
+        <v>514</v>
       </c>
       <c r="D29" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="H29" t="s">
         <v>24</v>
       </c>
       <c r="M29" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B30" t="s">
-        <v>543</v>
+        <v>517</v>
       </c>
       <c r="C30" t="s">
-        <v>541</v>
+        <v>515</v>
       </c>
       <c r="D30" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="H30" t="s">
         <v>24</v>
       </c>
       <c r="M30" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B32" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2862,10 +2739,10 @@
         <v>17</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2873,10 +2750,10 @@
         <v>17</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>544</v>
+        <v>518</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>574</v>
+        <v>548</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2884,19 +2761,19 @@
         <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C35" s="3"/>
       <c r="G35" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2904,53 +2781,53 @@
         <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="G37" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" t="s">
         <v>94</v>
       </c>
-      <c r="B38" t="s">
-        <v>104</v>
-      </c>
       <c r="C38" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="H38" t="s">
         <v>24</v>
       </c>
       <c r="M38" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="E39" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="F39" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="M39" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2958,10 +2835,10 @@
         <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2969,10 +2846,10 @@
         <v>17</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2980,10 +2857,10 @@
         <v>17</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>545</v>
+        <v>519</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>546</v>
+        <v>520</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2991,27 +2868,27 @@
         <v>17</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>548</v>
+        <v>522</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>547</v>
+        <v>521</v>
       </c>
     </row>
     <row r="45" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3019,10 +2896,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="G46" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3030,10 +2907,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="G47" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3041,10 +2918,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="G48" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3052,10 +2929,10 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="G49" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3063,27 +2940,27 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="G50" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B51" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D51" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="M51" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3091,30 +2968,30 @@
         <v>27</v>
       </c>
       <c r="B52" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M52" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B53" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C53" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="E53" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F53" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="H53" t="s">
         <v>24</v>
@@ -3125,60 +3002,60 @@
         <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="C54" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="D54" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E54" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F54" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="I54" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J54" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="M54" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B55" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C55" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D55" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E55" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F55" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="J55" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="K55" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="L55" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="M55" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3186,13 +3063,13 @@
         <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="G56" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="M56" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3200,64 +3077,64 @@
         <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="G57" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B58" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="C58" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D58" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="M58" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="C59" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D59" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="M59" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B60" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="C60" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="D60" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="H60" t="s">
         <v>24</v>
       </c>
       <c r="M60" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3265,212 +3142,212 @@
         <v>27</v>
       </c>
       <c r="B61" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="M61" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B62" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C62" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="D62" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="E62" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F62" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="J62" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="K62" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="L62" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B63" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="C63" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="D63" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="M63" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B64" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="D64" t="s">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="E64" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="F64" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="J64" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="K64" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="L64" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B65" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="C65" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="D65" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="M65" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B66" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="C66" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D66" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="M66" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B67" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C67" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D67" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="M67" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B68" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C68" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D68" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="J68" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="K68" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="L68" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="M68" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B69" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="C69" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="D69" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B70" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="C70" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D70" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="H70" t="s">
         <v>24</v>
       </c>
       <c r="M70" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B71" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B72" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3478,10 +3355,10 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="G73" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3489,10 +3366,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="G74" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3500,10 +3377,10 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="G75" t="s">
-        <v>539</v>
+        <v>513</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3511,10 +3388,10 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="G76" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3522,13 +3399,13 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="G77" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="M77" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3536,13 +3413,13 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="G78" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="M78" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3550,10 +3427,10 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="G79" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3561,13 +3438,13 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="G80" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="M80" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3575,13 +3452,13 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="G81" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="M81" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3589,10 +3466,10 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="G82" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3600,13 +3477,13 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="G83" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="M83" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3614,13 +3491,13 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="G84" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="M84" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3628,10 +3505,10 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="G85" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3639,10 +3516,10 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="G86" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3650,13 +3527,13 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="G87" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="M87" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3664,13 +3541,13 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="G88" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="M88" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3678,10 +3555,10 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="G89" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3689,10 +3566,10 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="G90" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3700,13 +3577,13 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="G91" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="M91" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3714,13 +3591,13 @@
         <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="G92" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="M92" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3728,69 +3605,59 @@
         <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="G93" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="M93" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" t="s">
-        <v>64</v>
-      </c>
-      <c r="B94" t="s">
-        <v>269</v>
-      </c>
-      <c r="C94" t="s">
-        <v>270</v>
-      </c>
-    </row>
+        <v>167</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>27</v>
       </c>
       <c r="B95" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
       <c r="M95" t="s">
-        <v>272</v>
+        <v>260</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B96" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C96" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D96" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B97" t="s">
-        <v>276</v>
+        <v>264</v>
       </c>
       <c r="C97" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="D97" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E97" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F97" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3798,60 +3665,60 @@
         <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>279</v>
+        <v>267</v>
       </c>
       <c r="C98" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="D98" t="s">
-        <v>281</v>
+        <v>269</v>
       </c>
       <c r="E98" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F98" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="I98" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J98" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="M98" t="s">
-        <v>282</v>
+        <v>270</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B99" t="s">
-        <v>283</v>
+        <v>271</v>
       </c>
       <c r="C99" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="D99" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="E99" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F99" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="J99" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="K99" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="L99" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="M99" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3859,13 +3726,13 @@
         <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="G100" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
       <c r="M100" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3873,170 +3740,170 @@
         <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>290</v>
+        <v>278</v>
       </c>
       <c r="G101" t="s">
-        <v>291</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B102" t="s">
-        <v>292</v>
+        <v>280</v>
       </c>
       <c r="C102" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="D102" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="M102" t="s">
-        <v>295</v>
+        <v>283</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B103" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="C103" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="D103" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="M103" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B104" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="C104" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="D104" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="E104" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F104" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="J104" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="K104" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="L104" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
-        <v>303</v>
+        <v>291</v>
       </c>
       <c r="C105" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="D105" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="M105" t="s">
-        <v>306</v>
+        <v>294</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B106" t="s">
-        <v>307</v>
+        <v>295</v>
       </c>
       <c r="C106" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="D106" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="E106" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="F106" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="J106" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="K106" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="L106" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B107" t="s">
-        <v>310</v>
+        <v>298</v>
       </c>
       <c r="C107" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="D107" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="M107" t="s">
-        <v>313</v>
+        <v>301</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B108" t="s">
-        <v>314</v>
+        <v>302</v>
       </c>
       <c r="C108" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D108" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="M108" t="s">
-        <v>315</v>
+        <v>303</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B109" t="s">
-        <v>316</v>
+        <v>304</v>
       </c>
       <c r="C109" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D109" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="M109" t="s">
-        <v>317</v>
+        <v>305</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4044,10 +3911,10 @@
         <v>17</v>
       </c>
       <c r="B110" t="s">
-        <v>318</v>
+        <v>306</v>
       </c>
       <c r="G110" t="s">
-        <v>319</v>
+        <v>307</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4055,36 +3922,36 @@
         <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>320</v>
+        <v>308</v>
       </c>
       <c r="G111" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B112" t="s">
-        <v>322</v>
+        <v>310</v>
       </c>
       <c r="C112" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D112" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="J112" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="K112" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="L112" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="M112" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4092,13 +3959,13 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>326</v>
+        <v>314</v>
       </c>
       <c r="G113" t="s">
-        <v>327</v>
+        <v>315</v>
       </c>
       <c r="M113" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4106,13 +3973,13 @@
         <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
       <c r="G114" t="s">
-        <v>329</v>
+        <v>317</v>
       </c>
       <c r="M114" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4120,10 +3987,10 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
       <c r="G115" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4131,10 +3998,10 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
       <c r="G116" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4142,13 +4009,13 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
       <c r="G117" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
       <c r="M117" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4156,21 +4023,21 @@
         <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
       <c r="G118" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="M118" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B119" t="s">
-        <v>271</v>
+        <v>259</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4178,44 +4045,44 @@
         <v>27</v>
       </c>
       <c r="B120" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
       <c r="M120" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B121" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
       <c r="C121" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="D121" t="s">
-        <v>275</v>
+        <v>263</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B122" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
       <c r="C122" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="D122" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="E122" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="F122" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4223,60 +4090,60 @@
         <v>30</v>
       </c>
       <c r="B123" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C123" t="s">
-        <v>280</v>
+        <v>268</v>
       </c>
       <c r="D123" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
       <c r="E123" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="F123" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="I123" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J123" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="M123" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B124" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="C124" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="D124" t="s">
-        <v>285</v>
+        <v>273</v>
       </c>
       <c r="E124" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="F124" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="J124" t="s">
-        <v>286</v>
+        <v>274</v>
       </c>
       <c r="K124" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="L124" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="M124" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4284,13 +4151,13 @@
         <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
       <c r="G125" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
       <c r="M125" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4298,170 +4165,170 @@
         <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>349</v>
+        <v>337</v>
       </c>
       <c r="G126" t="s">
-        <v>350</v>
+        <v>338</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B127" t="s">
-        <v>351</v>
+        <v>339</v>
       </c>
       <c r="C127" t="s">
-        <v>293</v>
+        <v>281</v>
       </c>
       <c r="D127" t="s">
-        <v>294</v>
+        <v>282</v>
       </c>
       <c r="M127" t="s">
-        <v>352</v>
+        <v>340</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B128" t="s">
-        <v>353</v>
+        <v>341</v>
       </c>
       <c r="C128" t="s">
-        <v>354</v>
+        <v>342</v>
       </c>
       <c r="D128" t="s">
-        <v>355</v>
+        <v>343</v>
       </c>
       <c r="M128" t="s">
-        <v>356</v>
+        <v>344</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B129" t="s">
-        <v>357</v>
+        <v>345</v>
       </c>
       <c r="C129" t="s">
-        <v>301</v>
+        <v>289</v>
       </c>
       <c r="D129" t="s">
-        <v>302</v>
+        <v>290</v>
       </c>
       <c r="E129" t="s">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="F129" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="J129" t="s">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="K129" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="L129" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B130" t="s">
-        <v>358</v>
+        <v>346</v>
       </c>
       <c r="C130" t="s">
-        <v>304</v>
+        <v>292</v>
       </c>
       <c r="D130" t="s">
-        <v>305</v>
+        <v>293</v>
       </c>
       <c r="M130" t="s">
-        <v>359</v>
+        <v>347</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B131" t="s">
-        <v>360</v>
+        <v>348</v>
       </c>
       <c r="C131" t="s">
-        <v>308</v>
+        <v>296</v>
       </c>
       <c r="D131" t="s">
-        <v>309</v>
+        <v>297</v>
       </c>
       <c r="E131" t="s">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="F131" t="s">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="J131" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="K131" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="L131" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B132" t="s">
-        <v>361</v>
+        <v>349</v>
       </c>
       <c r="C132" t="s">
-        <v>311</v>
+        <v>299</v>
       </c>
       <c r="D132" t="s">
-        <v>312</v>
+        <v>300</v>
       </c>
       <c r="M132" t="s">
-        <v>362</v>
+        <v>350</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B133" t="s">
-        <v>363</v>
+        <v>351</v>
       </c>
       <c r="C133" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="D133" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="M133" t="s">
-        <v>364</v>
+        <v>352</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B134" t="s">
-        <v>365</v>
+        <v>353</v>
       </c>
       <c r="C134" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D134" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="M134" t="s">
-        <v>366</v>
+        <v>354</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4469,10 +4336,10 @@
         <v>17</v>
       </c>
       <c r="B135" t="s">
-        <v>367</v>
+        <v>355</v>
       </c>
       <c r="G135" t="s">
-        <v>368</v>
+        <v>356</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4480,36 +4347,36 @@
         <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>369</v>
+        <v>357</v>
       </c>
       <c r="G136" t="s">
-        <v>370</v>
+        <v>358</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B137" t="s">
-        <v>371</v>
+        <v>359</v>
       </c>
       <c r="C137" t="s">
-        <v>323</v>
+        <v>311</v>
       </c>
       <c r="D137" t="s">
-        <v>324</v>
+        <v>312</v>
       </c>
       <c r="J137" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="K137" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="L137" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="M137" t="s">
-        <v>372</v>
+        <v>360</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4517,13 +4384,13 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>373</v>
+        <v>361</v>
       </c>
       <c r="G138" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="M138" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4531,13 +4398,13 @@
         <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="G139" t="s">
-        <v>376</v>
+        <v>364</v>
       </c>
       <c r="M139" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4545,10 +4412,10 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>377</v>
+        <v>365</v>
       </c>
       <c r="G140" t="s">
-        <v>378</v>
+        <v>366</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4556,10 +4423,10 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
       <c r="G141" t="s">
-        <v>380</v>
+        <v>368</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4567,13 +4434,13 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>381</v>
+        <v>369</v>
       </c>
       <c r="G142" t="s">
-        <v>382</v>
+        <v>370</v>
       </c>
       <c r="M142" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4581,21 +4448,21 @@
         <v>17</v>
       </c>
       <c r="B143" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="G143" t="s">
-        <v>384</v>
+        <v>372</v>
       </c>
       <c r="M143" t="s">
-        <v>177</v>
+        <v>167</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B144" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4603,13 +4470,13 @@
         <v>17</v>
       </c>
       <c r="B145" t="s">
-        <v>385</v>
+        <v>373</v>
       </c>
       <c r="G145" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M145" t="s">
-        <v>386</v>
+        <v>374</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4617,110 +4484,110 @@
         <v>17</v>
       </c>
       <c r="B146" t="s">
-        <v>387</v>
+        <v>375</v>
       </c>
       <c r="G146" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M146" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B147" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="C147" t="s">
-        <v>390</v>
+        <v>550</v>
       </c>
       <c r="D147" t="s">
-        <v>391</v>
+        <v>378</v>
       </c>
       <c r="E147" t="s">
-        <v>392</v>
+        <v>379</v>
       </c>
       <c r="F147" t="s">
-        <v>393</v>
+        <v>380</v>
       </c>
       <c r="M147" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
-        <v>395</v>
+        <v>382</v>
       </c>
       <c r="B148" t="s">
-        <v>396</v>
+        <v>383</v>
       </c>
       <c r="C148" t="s">
-        <v>397</v>
+        <v>384</v>
       </c>
       <c r="D148" t="s">
-        <v>398</v>
+        <v>385</v>
       </c>
       <c r="M148" t="s">
-        <v>394</v>
+        <v>381</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B149" t="s">
-        <v>399</v>
+        <v>386</v>
       </c>
       <c r="C149" t="s">
-        <v>400</v>
+        <v>551</v>
       </c>
       <c r="D149" t="s">
-        <v>401</v>
+        <v>387</v>
       </c>
       <c r="E149" t="s">
-        <v>402</v>
+        <v>388</v>
       </c>
       <c r="F149" t="s">
-        <v>403</v>
+        <v>389</v>
       </c>
       <c r="M149" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
-        <v>405</v>
+        <v>391</v>
       </c>
       <c r="B150" t="s">
-        <v>406</v>
+        <v>392</v>
       </c>
       <c r="C150" t="s">
-        <v>407</v>
+        <v>393</v>
       </c>
       <c r="D150" t="s">
-        <v>408</v>
+        <v>394</v>
       </c>
       <c r="M150" t="s">
-        <v>404</v>
+        <v>390</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B151" t="s">
-        <v>409</v>
+        <v>395</v>
       </c>
       <c r="C151" t="s">
-        <v>410</v>
+        <v>552</v>
       </c>
       <c r="D151" t="s">
-        <v>411</v>
+        <v>396</v>
       </c>
       <c r="M151" t="s">
-        <v>412</v>
+        <v>397</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4728,13 +4595,13 @@
         <v>17</v>
       </c>
       <c r="B152" t="s">
-        <v>413</v>
+        <v>398</v>
       </c>
       <c r="G152" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M152" t="s">
-        <v>414</v>
+        <v>399</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4742,13 +4609,13 @@
         <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>415</v>
+        <v>400</v>
       </c>
       <c r="G153" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M153" t="s">
-        <v>416</v>
+        <v>401</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4756,13 +4623,13 @@
         <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="G154" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M154" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
     </row>
     <row r="155" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4770,32 +4637,35 @@
         <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>419</v>
+        <v>404</v>
       </c>
       <c r="G155" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="M155" t="s">
-        <v>420</v>
+        <v>405</v>
       </c>
     </row>
     <row r="156" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" s="2" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
     </row>
     <row r="158" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B158" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>549</v>
       </c>
       <c r="N158" s="1" t="s">
-        <v>560</v>
+        <v>534</v>
       </c>
     </row>
     <row r="159" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4803,11 +4673,11 @@
         <v>17</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>562</v>
+        <v>536</v>
       </c>
       <c r="C159" s="4"/>
       <c r="G159" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
     </row>
     <row r="160" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4815,11 +4685,11 @@
         <v>17</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>563</v>
+        <v>537</v>
       </c>
       <c r="C160" s="4"/>
       <c r="G160" s="3" t="s">
-        <v>568</v>
+        <v>542</v>
       </c>
     </row>
     <row r="161" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4827,11 +4697,11 @@
         <v>17</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>564</v>
+        <v>538</v>
       </c>
       <c r="C161" s="4"/>
       <c r="G161" s="3" t="s">
-        <v>569</v>
+        <v>543</v>
       </c>
     </row>
     <row r="162" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4839,202 +4709,202 @@
         <v>17</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>565</v>
+        <v>539</v>
       </c>
       <c r="C162" s="4"/>
       <c r="G162" s="3" t="s">
-        <v>570</v>
+        <v>544</v>
       </c>
     </row>
     <row r="163" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B163" t="s">
-        <v>566</v>
+        <v>540</v>
       </c>
       <c r="C163" s="5" t="s">
-        <v>567</v>
+        <v>541</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="M163" s="3" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
     </row>
     <row r="164" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
-        <v>550</v>
+        <v>524</v>
       </c>
       <c r="B164" t="s">
-        <v>551</v>
+        <v>525</v>
       </c>
       <c r="C164" s="6" t="s">
-        <v>571</v>
+        <v>545</v>
       </c>
       <c r="J164" t="s">
-        <v>552</v>
+        <v>526</v>
       </c>
       <c r="K164" t="s">
-        <v>553</v>
+        <v>527</v>
       </c>
       <c r="M164" s="3" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
     </row>
     <row r="165" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
-        <v>550</v>
+        <v>524</v>
       </c>
       <c r="B165" t="s">
-        <v>554</v>
+        <v>528</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>572</v>
+        <v>546</v>
       </c>
       <c r="J165" t="s">
-        <v>556</v>
+        <v>530</v>
       </c>
       <c r="K165" t="s">
-        <v>557</v>
+        <v>531</v>
       </c>
       <c r="M165" s="3" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
     </row>
     <row r="166" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
-        <v>550</v>
+        <v>524</v>
       </c>
       <c r="B166" t="s">
-        <v>555</v>
+        <v>529</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>573</v>
+        <v>547</v>
       </c>
       <c r="J166" t="s">
-        <v>559</v>
+        <v>533</v>
       </c>
       <c r="K166" t="s">
-        <v>558</v>
+        <v>532</v>
       </c>
       <c r="M166" s="3" t="s">
-        <v>561</v>
+        <v>535</v>
       </c>
     </row>
     <row r="167" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="1" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>549</v>
+        <v>523</v>
       </c>
     </row>
     <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B169" t="s">
-        <v>421</v>
+        <v>406</v>
       </c>
       <c r="C169" t="s">
-        <v>422</v>
+        <v>407</v>
       </c>
       <c r="D169" t="s">
-        <v>423</v>
+        <v>408</v>
       </c>
       <c r="E169" t="s">
-        <v>424</v>
+        <v>409</v>
       </c>
       <c r="F169" t="s">
-        <v>425</v>
+        <v>410</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="B170" t="s">
-        <v>427</v>
+        <v>412</v>
       </c>
       <c r="C170" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="D170" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="E170" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="F170" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="H170" t="s">
         <v>24</v>
       </c>
       <c r="M170" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
-        <v>433</v>
+        <v>418</v>
       </c>
       <c r="B171" t="s">
-        <v>434</v>
+        <v>419</v>
       </c>
       <c r="C171" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="D171" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="E171" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="F171" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="M171" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
-        <v>435</v>
+        <v>420</v>
       </c>
       <c r="B172" t="s">
-        <v>436</v>
+        <v>421</v>
       </c>
       <c r="C172" t="s">
-        <v>428</v>
+        <v>413</v>
       </c>
       <c r="D172" t="s">
-        <v>429</v>
+        <v>414</v>
       </c>
       <c r="H172" t="s">
         <v>24</v>
       </c>
       <c r="M172" t="s">
-        <v>437</v>
+        <v>422</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B173" t="s">
-        <v>438</v>
+        <v>423</v>
       </c>
       <c r="C173" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="D173" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="M173" t="s">
-        <v>441</v>
+        <v>426</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5042,157 +4912,87 @@
         <v>20</v>
       </c>
       <c r="B174" t="s">
-        <v>442</v>
+        <v>427</v>
       </c>
       <c r="C174" t="s">
-        <v>443</v>
+        <v>428</v>
       </c>
       <c r="D174" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B175" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="177" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A177" t="s">
-        <v>54</v>
-      </c>
-      <c r="B177" t="s">
-        <v>445</v>
-      </c>
-      <c r="C177" t="s">
-        <v>446</v>
-      </c>
-      <c r="D177" t="s">
-        <v>447</v>
-      </c>
-      <c r="H177" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="178" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A178" t="s">
-        <v>17</v>
-      </c>
-      <c r="B178" t="s">
-        <v>448</v>
-      </c>
-      <c r="G178" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A179" t="s">
-        <v>17</v>
-      </c>
-      <c r="B179" t="s">
-        <v>450</v>
-      </c>
-      <c r="G179" t="s">
-        <v>113</v>
-      </c>
-      <c r="M179" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A180" t="s">
-        <v>17</v>
-      </c>
-      <c r="B180" t="s">
-        <v>452</v>
-      </c>
-      <c r="G180" t="s">
-        <v>113</v>
-      </c>
-      <c r="M180" t="s">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" t="s">
-        <v>17</v>
-      </c>
-      <c r="B181" t="s">
-        <v>454</v>
-      </c>
-      <c r="G181" t="s">
-        <v>113</v>
-      </c>
-      <c r="M181" t="s">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
         <v>17</v>
       </c>
       <c r="B182" t="s">
-        <v>456</v>
+        <v>430</v>
       </c>
       <c r="G182" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
         <v>17</v>
       </c>
       <c r="B183" t="s">
-        <v>458</v>
+        <v>432</v>
       </c>
       <c r="G183" t="s">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
         <v>17</v>
       </c>
       <c r="B184" t="s">
-        <v>460</v>
+        <v>434</v>
       </c>
       <c r="G184" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
         <v>17</v>
       </c>
       <c r="B185" t="s">
-        <v>462</v>
+        <v>436</v>
       </c>
       <c r="G185" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="186" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
         <v>17</v>
       </c>
       <c r="B186" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
       <c r="G186" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
         <v>17</v>
       </c>
       <c r="B187" t="s">
-        <v>466</v>
+        <v>440</v>
       </c>
       <c r="G187" t="s">
-        <v>467</v>
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -5204,7 +5004,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -5213,7 +5015,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>468</v>
+        <v>442</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5227,405 +5029,405 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C2" t="s">
-        <v>469</v>
+        <v>443</v>
       </c>
       <c r="D2" t="s">
-        <v>470</v>
+        <v>444</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="C3" t="s">
-        <v>472</v>
+        <v>446</v>
       </c>
       <c r="D3" t="s">
-        <v>473</v>
+        <v>447</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>474</v>
+        <v>448</v>
       </c>
       <c r="B4" t="s">
-        <v>474</v>
+        <v>448</v>
       </c>
       <c r="C4" t="s">
-        <v>474</v>
+        <v>448</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="D5" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="C6" t="s">
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="D6" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="C7" t="s">
-        <v>480</v>
+        <v>553</v>
       </c>
       <c r="D7" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="B8" t="s">
-        <v>483</v>
+        <v>457</v>
       </c>
       <c r="C8" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="D8" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="B9" t="s">
-        <v>484</v>
+        <v>458</v>
       </c>
       <c r="C9" t="s">
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="D9" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="B10" t="s">
-        <v>486</v>
+        <v>460</v>
       </c>
       <c r="C10" t="s">
-        <v>487</v>
+        <v>461</v>
       </c>
       <c r="D10" t="s">
-        <v>488</v>
+        <v>462</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>485</v>
+        <v>459</v>
       </c>
       <c r="B11" t="s">
-        <v>489</v>
+        <v>463</v>
       </c>
       <c r="C11" t="s">
-        <v>490</v>
+        <v>464</v>
       </c>
       <c r="D11" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="B12" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
       <c r="C12" t="s">
-        <v>494</v>
+        <v>468</v>
       </c>
       <c r="D12" t="s">
-        <v>495</v>
+        <v>469</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="B13" t="s">
-        <v>496</v>
+        <v>470</v>
       </c>
       <c r="C13" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
       <c r="D13" t="s">
-        <v>498</v>
+        <v>472</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B14" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C14" t="s">
-        <v>499</v>
+        <v>473</v>
       </c>
       <c r="D14" t="s">
-        <v>500</v>
+        <v>474</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B15" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="C15" t="s">
-        <v>501</v>
+        <v>475</v>
       </c>
       <c r="D15" t="s">
-        <v>502</v>
+        <v>476</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B16" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="C16" t="s">
-        <v>503</v>
+        <v>477</v>
       </c>
       <c r="D16" t="s">
-        <v>504</v>
+        <v>478</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B17" t="s">
-        <v>505</v>
+        <v>479</v>
       </c>
       <c r="C17" t="s">
-        <v>480</v>
+        <v>454</v>
       </c>
       <c r="D17" t="s">
-        <v>481</v>
+        <v>455</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C18" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="D18" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="B19" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="C19" t="s">
-        <v>507</v>
+        <v>481</v>
       </c>
       <c r="D19" t="s">
-        <v>508</v>
+        <v>482</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>506</v>
+        <v>480</v>
       </c>
       <c r="B20" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="C20" t="s">
-        <v>509</v>
+        <v>483</v>
       </c>
       <c r="D20" t="s">
-        <v>510</v>
+        <v>484</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>511</v>
+        <v>485</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C21" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="D21" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>511</v>
+        <v>485</v>
       </c>
       <c r="B22" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="C22" t="s">
-        <v>512</v>
+        <v>486</v>
       </c>
       <c r="D22" t="s">
-        <v>513</v>
+        <v>487</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>511</v>
+        <v>485</v>
       </c>
       <c r="B23" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="C23" t="s">
-        <v>514</v>
+        <v>488</v>
       </c>
       <c r="D23" t="s">
-        <v>515</v>
+        <v>489</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>516</v>
+        <v>490</v>
       </c>
       <c r="B24" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C24" t="s">
-        <v>517</v>
+        <v>491</v>
       </c>
       <c r="D24" t="s">
-        <v>518</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>516</v>
+        <v>490</v>
       </c>
       <c r="B25" t="s">
-        <v>471</v>
+        <v>445</v>
       </c>
       <c r="C25" t="s">
-        <v>519</v>
+        <v>493</v>
       </c>
       <c r="D25" t="s">
-        <v>520</v>
+        <v>494</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>521</v>
+        <v>495</v>
       </c>
       <c r="B26" t="s">
-        <v>505</v>
+        <v>479</v>
       </c>
       <c r="C26" t="s">
-        <v>522</v>
+        <v>496</v>
       </c>
       <c r="D26" t="s">
-        <v>522</v>
+        <v>496</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>521</v>
+        <v>495</v>
       </c>
       <c r="B27" t="s">
-        <v>523</v>
+        <v>497</v>
       </c>
       <c r="C27" t="s">
-        <v>524</v>
+        <v>498</v>
       </c>
       <c r="D27" t="s">
-        <v>525</v>
+        <v>499</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>526</v>
+        <v>500</v>
       </c>
       <c r="B28" t="s">
-        <v>479</v>
+        <v>453</v>
       </c>
       <c r="C28" t="s">
-        <v>527</v>
+        <v>501</v>
       </c>
       <c r="D28" t="s">
-        <v>528</v>
+        <v>502</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>529</v>
+        <v>503</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C29" t="s">
-        <v>475</v>
+        <v>449</v>
       </c>
       <c r="D29" t="s">
-        <v>476</v>
+        <v>450</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>529</v>
+        <v>503</v>
       </c>
       <c r="B30" t="s">
-        <v>530</v>
+        <v>504</v>
       </c>
       <c r="C30" t="s">
-        <v>477</v>
+        <v>451</v>
       </c>
       <c r="D30" t="s">
-        <v>478</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -5643,30 +5445,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>531</v>
+        <v>505</v>
       </c>
       <c r="B1" t="s">
-        <v>532</v>
+        <v>506</v>
       </c>
       <c r="C1" t="s">
-        <v>533</v>
+        <v>507</v>
       </c>
       <c r="D1" t="s">
-        <v>534</v>
+        <v>508</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>535</v>
+        <v>509</v>
       </c>
       <c r="B2" t="s">
-        <v>536</v>
+        <v>510</v>
       </c>
       <c r="C2" t="s">
-        <v>537</v>
+        <v>511</v>
       </c>
       <c r="D2" t="s">
-        <v>538</v>
+        <v>512</v>
       </c>
     </row>
   </sheetData>
@@ -5675,21 +5477,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6128,7 +5915,81 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
+</file>
+
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
@@ -6192,82 +6053,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6290,16 +6076,26 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6313,9 +6109,15 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added show to debug PLW
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rojohnston\OneDrive - UNICEF\1 UNICEF Work\1 Afghanistan\Surveys\UrbanSMART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE2F851A-EDBA-43D1-8034-789FE3404A1F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0232D5E-F71B-4B02-BA89-06F54BF02B33}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="555">
   <si>
     <t>type</t>
   </si>
@@ -1805,9 +1805,6 @@
     <t>${numplw}</t>
   </si>
   <si>
-    <t>${consent}='1' and ${is_plw}='1'</t>
-  </si>
-  <si>
     <t>plw_selected_position</t>
   </si>
   <si>
@@ -1844,9 +1841,6 @@
     <t>Woman's WEIGHT in KG of (${plw_name})</t>
   </si>
   <si>
-    <t>if(${curr_pregnant}='1' or ${curr_breastfeed}='1',true(),false())</t>
-  </si>
-  <si>
     <t>Pregnant &amp; Lactating Woman section</t>
   </si>
   <si>
@@ -1860,6 +1854,21 @@
   </si>
   <si>
     <t>Other (No one present)</t>
+  </si>
+  <si>
+    <t>show PLW</t>
+  </si>
+  <si>
+    <t>if(${curr_pregnant}=1 or ${curr_breastfeed}=1,true(),false())</t>
+  </si>
+  <si>
+    <t>PLW ${plw} numPLW ${numplw}</t>
+  </si>
+  <si>
+    <t>IS PLW ${is_plw} PReg ${curr_pregnant} Breastfeed ${curr_breastfeed}</t>
+  </si>
+  <si>
+    <t>${consent}='1' and ${is_plw}=1</t>
   </si>
 </sst>
 </file>
@@ -1875,7 +1884,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1894,6 +1903,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1907,7 +1922,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1919,6 +1934,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2257,11 +2273,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N186"/>
+  <dimension ref="A1:N188"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="A5:B5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N162" sqref="N162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2729,92 +2745,92 @@
         <v>516</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" t="s">
-        <v>17</v>
-      </c>
-      <c r="B34" t="s">
-        <v>87</v>
-      </c>
-      <c r="C34" s="3"/>
-      <c r="G34" t="s">
-        <v>88</v>
+        <v>551</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>89</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>64</v>
+        <v>87</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="G35" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>17</v>
+        <v>89</v>
       </c>
       <c r="B36" t="s">
-        <v>90</v>
-      </c>
-      <c r="G36" t="s">
-        <v>91</v>
+        <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="B37" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" t="s">
-        <v>93</v>
-      </c>
-      <c r="D37" t="s">
-        <v>94</v>
-      </c>
-      <c r="H37" t="s">
-        <v>24</v>
-      </c>
-      <c r="M37" t="s">
-        <v>57</v>
+        <v>90</v>
+      </c>
+      <c r="G37" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" t="s">
+        <v>92</v>
+      </c>
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" t="s">
+        <v>94</v>
+      </c>
+      <c r="H38" t="s">
+        <v>24</v>
+      </c>
+      <c r="M38" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
         <v>32</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>95</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>96</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D39" t="s">
         <v>97</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E39" t="s">
         <v>98</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F39" t="s">
         <v>99</v>
       </c>
-      <c r="M38" t="s">
+      <c r="M39" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2822,21 +2838,21 @@
         <v>17</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G41" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>518</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2844,49 +2860,49 @@
         <v>17</v>
       </c>
       <c r="B43" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>520</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G44" s="1" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="2" t="s">
+    <row r="45" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>550</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="N46" s="2" t="s">
         <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" t="s">
-        <v>112</v>
-      </c>
-      <c r="G45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" t="s">
-        <v>17</v>
-      </c>
-      <c r="B46" t="s">
-        <v>114</v>
-      </c>
-      <c r="G46" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2894,10 +2910,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G47" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2905,10 +2921,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="G48" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2916,258 +2932,234 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="G49" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>122</v>
-      </c>
-      <c r="C50" t="s">
-        <v>123</v>
-      </c>
-      <c r="D50" t="s">
-        <v>124</v>
-      </c>
-      <c r="M50" t="s">
-        <v>125</v>
+        <v>118</v>
+      </c>
+      <c r="G50" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B51" t="s">
-        <v>126</v>
-      </c>
-      <c r="M51" t="s">
-        <v>125</v>
+        <v>120</v>
+      </c>
+      <c r="G51" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
-      </c>
-      <c r="E52" t="s">
-        <v>130</v>
-      </c>
-      <c r="F52" t="s">
-        <v>131</v>
-      </c>
-      <c r="H52" t="s">
-        <v>24</v>
+        <v>124</v>
+      </c>
+      <c r="M52" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B53" t="s">
-        <v>132</v>
-      </c>
-      <c r="C53" t="s">
-        <v>133</v>
-      </c>
-      <c r="D53" t="s">
-        <v>134</v>
-      </c>
-      <c r="E53" t="s">
-        <v>135</v>
-      </c>
-      <c r="F53" t="s">
-        <v>136</v>
-      </c>
-      <c r="I53" t="s">
-        <v>31</v>
-      </c>
-      <c r="J53" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
       <c r="M53" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B54" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C54" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="E54" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
-      </c>
-      <c r="J54" t="s">
-        <v>144</v>
-      </c>
-      <c r="K54" t="s">
-        <v>145</v>
-      </c>
-      <c r="L54" t="s">
-        <v>146</v>
-      </c>
-      <c r="M54" t="s">
-        <v>147</v>
+        <v>131</v>
+      </c>
+      <c r="H54" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
-      </c>
-      <c r="G55" t="s">
-        <v>149</v>
+        <v>132</v>
+      </c>
+      <c r="C55" t="s">
+        <v>133</v>
+      </c>
+      <c r="D55" t="s">
+        <v>134</v>
+      </c>
+      <c r="E55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" t="s">
+        <v>136</v>
+      </c>
+      <c r="I55" t="s">
+        <v>31</v>
+      </c>
+      <c r="J55" t="s">
+        <v>137</v>
       </c>
       <c r="M55" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B56" t="s">
-        <v>150</v>
-      </c>
-      <c r="G56" t="s">
-        <v>151</v>
+        <v>139</v>
+      </c>
+      <c r="C56" t="s">
+        <v>140</v>
+      </c>
+      <c r="D56" t="s">
+        <v>141</v>
+      </c>
+      <c r="E56" t="s">
+        <v>142</v>
+      </c>
+      <c r="F56" t="s">
+        <v>143</v>
+      </c>
+      <c r="J56" t="s">
+        <v>144</v>
+      </c>
+      <c r="K56" t="s">
+        <v>145</v>
+      </c>
+      <c r="L56" t="s">
+        <v>146</v>
+      </c>
+      <c r="M56" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>152</v>
-      </c>
-      <c r="C57" t="s">
-        <v>153</v>
-      </c>
-      <c r="D57" t="s">
-        <v>154</v>
+        <v>148</v>
+      </c>
+      <c r="G57" t="s">
+        <v>149</v>
       </c>
       <c r="M57" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>156</v>
-      </c>
-      <c r="C58" t="s">
-        <v>157</v>
-      </c>
-      <c r="D58" t="s">
-        <v>158</v>
-      </c>
-      <c r="M58" t="s">
-        <v>159</v>
+        <v>150</v>
+      </c>
+      <c r="G58" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B59" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C59" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D59" t="s">
-        <v>162</v>
-      </c>
-      <c r="H59" t="s">
-        <v>24</v>
+        <v>154</v>
       </c>
       <c r="M59" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>27</v>
+        <v>52</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
+        <v>156</v>
+      </c>
+      <c r="C60" t="s">
+        <v>157</v>
+      </c>
+      <c r="D60" t="s">
+        <v>158</v>
       </c>
       <c r="M60" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>82</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C61" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="D61" t="s">
-        <v>169</v>
-      </c>
-      <c r="E61" t="s">
-        <v>170</v>
-      </c>
-      <c r="F61" t="s">
-        <v>171</v>
-      </c>
-      <c r="J61" t="s">
-        <v>172</v>
-      </c>
-      <c r="K61" t="s">
-        <v>173</v>
-      </c>
-      <c r="L61" t="s">
-        <v>174</v>
+        <v>162</v>
+      </c>
+      <c r="H61" t="s">
+        <v>24</v>
+      </c>
+      <c r="M61" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>27</v>
       </c>
       <c r="B62" t="s">
-        <v>176</v>
-      </c>
-      <c r="C62" t="s">
-        <v>177</v>
-      </c>
-      <c r="D62" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="M62" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3175,177 +3167,201 @@
         <v>166</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>167</v>
       </c>
       <c r="C63" t="s">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="D63" t="s">
-        <v>182</v>
+        <v>169</v>
       </c>
       <c r="E63" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F63" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J63" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="K63" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="L63" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B64" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C64" t="s">
-        <v>190</v>
+        <v>177</v>
       </c>
       <c r="D64" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
       <c r="M64" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="B65" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="C65" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="D65" t="s">
-        <v>195</v>
-      </c>
-      <c r="M65" t="s">
-        <v>196</v>
+        <v>182</v>
+      </c>
+      <c r="E65" t="s">
+        <v>183</v>
+      </c>
+      <c r="F65" t="s">
+        <v>184</v>
+      </c>
+      <c r="J65" t="s">
+        <v>185</v>
+      </c>
+      <c r="K65" t="s">
+        <v>186</v>
+      </c>
+      <c r="L65" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="B66" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C66" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D66" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="M66" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B67" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C67" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="D67" t="s">
-        <v>203</v>
-      </c>
-      <c r="J67" t="s">
-        <v>204</v>
-      </c>
-      <c r="K67" t="s">
-        <v>205</v>
-      </c>
-      <c r="L67" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="M67" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B68" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C68" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D68" t="s">
-        <v>210</v>
+        <v>199</v>
+      </c>
+      <c r="M68" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="B69" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="C69" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D69" t="s">
-        <v>213</v>
-      </c>
-      <c r="H69" t="s">
-        <v>24</v>
+        <v>203</v>
+      </c>
+      <c r="J69" t="s">
+        <v>204</v>
+      </c>
+      <c r="K69" t="s">
+        <v>205</v>
+      </c>
+      <c r="L69" t="s">
+        <v>206</v>
       </c>
       <c r="M69" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>45</v>
+        <v>175</v>
       </c>
       <c r="B70" t="s">
-        <v>164</v>
+        <v>208</v>
+      </c>
+      <c r="C70" t="s">
+        <v>209</v>
+      </c>
+      <c r="D70" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B71" t="s">
-        <v>126</v>
+        <v>211</v>
+      </c>
+      <c r="C71" t="s">
+        <v>212</v>
+      </c>
+      <c r="D71" t="s">
+        <v>213</v>
+      </c>
+      <c r="H71" t="s">
+        <v>24</v>
+      </c>
+      <c r="M71" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B72" t="s">
-        <v>215</v>
-      </c>
-      <c r="G72" t="s">
-        <v>216</v>
+        <v>164</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B73" t="s">
-        <v>217</v>
-      </c>
-      <c r="G73" t="s">
-        <v>218</v>
+        <v>126</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3353,10 +3369,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G74" t="s">
-        <v>511</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3364,10 +3380,10 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="G75" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3375,13 +3391,10 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="G76" t="s">
-        <v>223</v>
-      </c>
-      <c r="M76" t="s">
-        <v>224</v>
+        <v>511</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3389,13 +3402,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="G77" t="s">
-        <v>226</v>
-      </c>
-      <c r="M77" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3403,10 +3413,13 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="G78" t="s">
-        <v>228</v>
+        <v>223</v>
+      </c>
+      <c r="M78" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3414,10 +3427,10 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G79" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="M79" t="s">
         <v>224</v>
@@ -3428,13 +3441,10 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="G80" t="s">
-        <v>232</v>
-      </c>
-      <c r="M80" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3442,10 +3452,13 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="G81" t="s">
-        <v>234</v>
+        <v>230</v>
+      </c>
+      <c r="M81" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3453,10 +3466,10 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="G82" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="M82" t="s">
         <v>224</v>
@@ -3467,13 +3480,10 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G83" t="s">
-        <v>238</v>
-      </c>
-      <c r="M83" t="s">
-        <v>224</v>
+        <v>234</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3481,10 +3491,13 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G84" t="s">
-        <v>240</v>
+        <v>236</v>
+      </c>
+      <c r="M84" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3492,10 +3505,13 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="G85" t="s">
-        <v>242</v>
+        <v>238</v>
+      </c>
+      <c r="M85" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3503,13 +3519,10 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="G86" t="s">
-        <v>244</v>
-      </c>
-      <c r="M86" t="s">
-        <v>165</v>
+        <v>240</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3517,13 +3530,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="G87" t="s">
-        <v>246</v>
-      </c>
-      <c r="M87" t="s">
-        <v>165</v>
+        <v>242</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3531,10 +3541,13 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="G88" t="s">
-        <v>248</v>
+        <v>244</v>
+      </c>
+      <c r="M88" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3542,10 +3555,13 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G89" t="s">
-        <v>250</v>
+        <v>246</v>
+      </c>
+      <c r="M89" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3553,13 +3569,10 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G90" t="s">
-        <v>252</v>
-      </c>
-      <c r="M90" t="s">
-        <v>165</v>
+        <v>248</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3567,13 +3580,10 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="G91" t="s">
-        <v>254</v>
-      </c>
-      <c r="M91" t="s">
-        <v>165</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3581,225 +3591,207 @@
         <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="G92" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="M92" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" t="s">
+        <v>253</v>
+      </c>
+      <c r="G93" t="s">
+        <v>254</v>
+      </c>
+      <c r="M93" t="s">
+        <v>165</v>
+      </c>
+    </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>257</v>
+        <v>255</v>
+      </c>
+      <c r="G94" t="s">
+        <v>256</v>
       </c>
       <c r="M94" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A95" t="s">
-        <v>52</v>
-      </c>
-      <c r="B95" t="s">
-        <v>259</v>
-      </c>
-      <c r="C95" t="s">
-        <v>260</v>
-      </c>
-      <c r="D95" t="s">
-        <v>261</v>
-      </c>
-    </row>
+        <v>165</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="B96" t="s">
-        <v>262</v>
-      </c>
-      <c r="C96" t="s">
-        <v>263</v>
-      </c>
-      <c r="D96" t="s">
-        <v>264</v>
-      </c>
-      <c r="E96" t="s">
-        <v>130</v>
-      </c>
-      <c r="F96" t="s">
-        <v>131</v>
+        <v>257</v>
+      </c>
+      <c r="M96" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B97" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="C97" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D97" t="s">
-        <v>267</v>
-      </c>
-      <c r="E97" t="s">
-        <v>135</v>
-      </c>
-      <c r="F97" t="s">
-        <v>136</v>
-      </c>
-      <c r="I97" t="s">
-        <v>31</v>
-      </c>
-      <c r="J97" t="s">
-        <v>137</v>
-      </c>
-      <c r="M97" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B98" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C98" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D98" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E98" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="F98" t="s">
-        <v>143</v>
-      </c>
-      <c r="J98" t="s">
-        <v>272</v>
-      </c>
-      <c r="K98" t="s">
-        <v>145</v>
-      </c>
-      <c r="L98" t="s">
-        <v>146</v>
-      </c>
-      <c r="M98" t="s">
-        <v>273</v>
+        <v>131</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B99" t="s">
-        <v>274</v>
-      </c>
-      <c r="G99" t="s">
-        <v>275</v>
+        <v>265</v>
+      </c>
+      <c r="C99" t="s">
+        <v>266</v>
+      </c>
+      <c r="D99" t="s">
+        <v>267</v>
+      </c>
+      <c r="E99" t="s">
+        <v>135</v>
+      </c>
+      <c r="F99" t="s">
+        <v>136</v>
+      </c>
+      <c r="I99" t="s">
+        <v>31</v>
+      </c>
+      <c r="J99" t="s">
+        <v>137</v>
       </c>
       <c r="M99" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B100" t="s">
-        <v>276</v>
-      </c>
-      <c r="G100" t="s">
-        <v>277</v>
+        <v>269</v>
+      </c>
+      <c r="C100" t="s">
+        <v>270</v>
+      </c>
+      <c r="D100" t="s">
+        <v>271</v>
+      </c>
+      <c r="E100" t="s">
+        <v>142</v>
+      </c>
+      <c r="F100" t="s">
+        <v>143</v>
+      </c>
+      <c r="J100" t="s">
+        <v>272</v>
+      </c>
+      <c r="K100" t="s">
+        <v>145</v>
+      </c>
+      <c r="L100" t="s">
+        <v>146</v>
+      </c>
+      <c r="M100" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>278</v>
-      </c>
-      <c r="C101" t="s">
-        <v>279</v>
-      </c>
-      <c r="D101" t="s">
-        <v>280</v>
+        <v>274</v>
+      </c>
+      <c r="G101" t="s">
+        <v>275</v>
       </c>
       <c r="M101" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>282</v>
-      </c>
-      <c r="C102" t="s">
-        <v>283</v>
-      </c>
-      <c r="D102" t="s">
-        <v>284</v>
-      </c>
-      <c r="M102" t="s">
-        <v>285</v>
+        <v>276</v>
+      </c>
+      <c r="G102" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>166</v>
+        <v>52</v>
       </c>
       <c r="B103" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C103" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D103" t="s">
-        <v>288</v>
-      </c>
-      <c r="E103" t="s">
-        <v>170</v>
-      </c>
-      <c r="F103" t="s">
-        <v>171</v>
-      </c>
-      <c r="J103" t="s">
-        <v>172</v>
-      </c>
-      <c r="K103" t="s">
-        <v>173</v>
-      </c>
-      <c r="L103" t="s">
-        <v>174</v>
+        <v>280</v>
+      </c>
+      <c r="M103" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B104" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C104" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="D104" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="M104" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3807,127 +3799,136 @@
         <v>166</v>
       </c>
       <c r="B105" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C105" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D105" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E105" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F105" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J105" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="K105" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="L105" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B106" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C106" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D106" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="M106" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="B107" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C107" t="s">
-        <v>194</v>
+        <v>294</v>
       </c>
       <c r="D107" t="s">
-        <v>195</v>
-      </c>
-      <c r="M107" t="s">
-        <v>301</v>
+        <v>295</v>
+      </c>
+      <c r="E107" t="s">
+        <v>183</v>
+      </c>
+      <c r="F107" t="s">
+        <v>184</v>
+      </c>
+      <c r="J107" t="s">
+        <v>185</v>
+      </c>
+      <c r="K107" t="s">
+        <v>186</v>
+      </c>
+      <c r="L107" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="B108" t="s">
-        <v>302</v>
+        <v>296</v>
       </c>
       <c r="C108" t="s">
-        <v>198</v>
+        <v>297</v>
       </c>
       <c r="D108" t="s">
-        <v>199</v>
+        <v>298</v>
       </c>
       <c r="M108" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B109" t="s">
-        <v>304</v>
-      </c>
-      <c r="G109" t="s">
-        <v>305</v>
+        <v>300</v>
+      </c>
+      <c r="C109" t="s">
+        <v>194</v>
+      </c>
+      <c r="D109" t="s">
+        <v>195</v>
+      </c>
+      <c r="M109" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B110" t="s">
-        <v>306</v>
-      </c>
-      <c r="G110" t="s">
-        <v>307</v>
+        <v>302</v>
+      </c>
+      <c r="C110" t="s">
+        <v>198</v>
+      </c>
+      <c r="D110" t="s">
+        <v>199</v>
+      </c>
+      <c r="M110" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>308</v>
-      </c>
-      <c r="C111" t="s">
-        <v>309</v>
-      </c>
-      <c r="D111" t="s">
-        <v>310</v>
-      </c>
-      <c r="J111" t="s">
-        <v>204</v>
-      </c>
-      <c r="K111" t="s">
-        <v>205</v>
-      </c>
-      <c r="L111" t="s">
-        <v>206</v>
-      </c>
-      <c r="M111" t="s">
-        <v>311</v>
+        <v>304</v>
+      </c>
+      <c r="G111" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3935,27 +3936,36 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="G112" t="s">
-        <v>313</v>
-      </c>
-      <c r="M112" t="s">
-        <v>165</v>
+        <v>307</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B113" t="s">
-        <v>314</v>
-      </c>
-      <c r="G113" t="s">
-        <v>315</v>
+        <v>308</v>
+      </c>
+      <c r="C113" t="s">
+        <v>309</v>
+      </c>
+      <c r="D113" t="s">
+        <v>310</v>
+      </c>
+      <c r="J113" t="s">
+        <v>204</v>
+      </c>
+      <c r="K113" t="s">
+        <v>205</v>
+      </c>
+      <c r="L113" t="s">
+        <v>206</v>
       </c>
       <c r="M113" t="s">
-        <v>165</v>
+        <v>311</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3963,10 +3973,13 @@
         <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="G114" t="s">
-        <v>317</v>
+        <v>313</v>
+      </c>
+      <c r="M114" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3974,10 +3987,13 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="G115" t="s">
-        <v>319</v>
+        <v>315</v>
+      </c>
+      <c r="M115" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3985,13 +4001,10 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="G116" t="s">
-        <v>321</v>
-      </c>
-      <c r="M116" t="s">
-        <v>165</v>
+        <v>317</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3999,232 +4012,211 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="G117" t="s">
-        <v>323</v>
-      </c>
-      <c r="M117" t="s">
-        <v>165</v>
+        <v>319</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>257</v>
+        <v>320</v>
+      </c>
+      <c r="G118" t="s">
+        <v>321</v>
+      </c>
+      <c r="M118" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="B119" t="s">
-        <v>324</v>
+        <v>322</v>
+      </c>
+      <c r="G119" t="s">
+        <v>323</v>
       </c>
       <c r="M119" t="s">
-        <v>325</v>
+        <v>165</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B120" t="s">
-        <v>326</v>
-      </c>
-      <c r="C120" t="s">
-        <v>260</v>
-      </c>
-      <c r="D120" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>82</v>
+        <v>27</v>
       </c>
       <c r="B121" t="s">
-        <v>327</v>
-      </c>
-      <c r="C121" t="s">
-        <v>263</v>
-      </c>
-      <c r="D121" t="s">
-        <v>264</v>
-      </c>
-      <c r="E121" t="s">
-        <v>130</v>
-      </c>
-      <c r="F121" t="s">
-        <v>131</v>
+        <v>324</v>
+      </c>
+      <c r="M121" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B122" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C122" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="D122" t="s">
-        <v>329</v>
-      </c>
-      <c r="E122" t="s">
-        <v>135</v>
-      </c>
-      <c r="F122" t="s">
-        <v>136</v>
-      </c>
-      <c r="I122" t="s">
-        <v>31</v>
-      </c>
-      <c r="J122" t="s">
-        <v>137</v>
-      </c>
-      <c r="M122" t="s">
-        <v>330</v>
+        <v>261</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>32</v>
+        <v>82</v>
       </c>
       <c r="B123" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C123" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="D123" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="E123" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="F123" t="s">
-        <v>143</v>
-      </c>
-      <c r="J123" t="s">
-        <v>272</v>
-      </c>
-      <c r="K123" t="s">
-        <v>145</v>
-      </c>
-      <c r="L123" t="s">
-        <v>146</v>
-      </c>
-      <c r="M123" t="s">
-        <v>332</v>
+        <v>131</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B124" t="s">
-        <v>333</v>
-      </c>
-      <c r="G124" t="s">
-        <v>334</v>
+        <v>328</v>
+      </c>
+      <c r="C124" t="s">
+        <v>266</v>
+      </c>
+      <c r="D124" t="s">
+        <v>329</v>
+      </c>
+      <c r="E124" t="s">
+        <v>135</v>
+      </c>
+      <c r="F124" t="s">
+        <v>136</v>
+      </c>
+      <c r="I124" t="s">
+        <v>31</v>
+      </c>
+      <c r="J124" t="s">
+        <v>137</v>
       </c>
       <c r="M124" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B125" t="s">
-        <v>335</v>
-      </c>
-      <c r="G125" t="s">
-        <v>336</v>
+        <v>331</v>
+      </c>
+      <c r="C125" t="s">
+        <v>270</v>
+      </c>
+      <c r="D125" t="s">
+        <v>271</v>
+      </c>
+      <c r="E125" t="s">
+        <v>142</v>
+      </c>
+      <c r="F125" t="s">
+        <v>143</v>
+      </c>
+      <c r="J125" t="s">
+        <v>272</v>
+      </c>
+      <c r="K125" t="s">
+        <v>145</v>
+      </c>
+      <c r="L125" t="s">
+        <v>146</v>
+      </c>
+      <c r="M125" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>337</v>
-      </c>
-      <c r="C126" t="s">
-        <v>279</v>
-      </c>
-      <c r="D126" t="s">
-        <v>280</v>
+        <v>333</v>
+      </c>
+      <c r="G126" t="s">
+        <v>334</v>
       </c>
       <c r="M126" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>339</v>
-      </c>
-      <c r="C127" t="s">
-        <v>340</v>
-      </c>
-      <c r="D127" t="s">
-        <v>341</v>
-      </c>
-      <c r="M127" t="s">
-        <v>342</v>
+        <v>335</v>
+      </c>
+      <c r="G127" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>166</v>
+        <v>52</v>
       </c>
       <c r="B128" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C128" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D128" t="s">
-        <v>288</v>
-      </c>
-      <c r="E128" t="s">
-        <v>170</v>
-      </c>
-      <c r="F128" t="s">
-        <v>171</v>
-      </c>
-      <c r="J128" t="s">
-        <v>172</v>
-      </c>
-      <c r="K128" t="s">
-        <v>173</v>
-      </c>
-      <c r="L128" t="s">
-        <v>174</v>
+        <v>280</v>
+      </c>
+      <c r="M128" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B129" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C129" t="s">
-        <v>290</v>
+        <v>340</v>
       </c>
       <c r="D129" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
       <c r="M129" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4232,127 +4224,136 @@
         <v>166</v>
       </c>
       <c r="B130" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C130" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="D130" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="E130" t="s">
-        <v>183</v>
+        <v>170</v>
       </c>
       <c r="F130" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="J130" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="K130" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="L130" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>175</v>
       </c>
       <c r="B131" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C131" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="D131" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="M131" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>52</v>
+        <v>166</v>
       </c>
       <c r="B132" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C132" t="s">
-        <v>194</v>
+        <v>294</v>
       </c>
       <c r="D132" t="s">
-        <v>195</v>
-      </c>
-      <c r="M132" t="s">
-        <v>350</v>
+        <v>295</v>
+      </c>
+      <c r="E132" t="s">
+        <v>183</v>
+      </c>
+      <c r="F132" t="s">
+        <v>184</v>
+      </c>
+      <c r="J132" t="s">
+        <v>185</v>
+      </c>
+      <c r="K132" t="s">
+        <v>186</v>
+      </c>
+      <c r="L132" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>52</v>
+        <v>188</v>
       </c>
       <c r="B133" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="C133" t="s">
-        <v>198</v>
+        <v>297</v>
       </c>
       <c r="D133" t="s">
-        <v>199</v>
+        <v>298</v>
       </c>
       <c r="M133" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B134" t="s">
-        <v>353</v>
-      </c>
-      <c r="G134" t="s">
-        <v>354</v>
+        <v>349</v>
+      </c>
+      <c r="C134" t="s">
+        <v>194</v>
+      </c>
+      <c r="D134" t="s">
+        <v>195</v>
+      </c>
+      <c r="M134" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B135" t="s">
-        <v>355</v>
-      </c>
-      <c r="G135" t="s">
-        <v>356</v>
+        <v>351</v>
+      </c>
+      <c r="C135" t="s">
+        <v>198</v>
+      </c>
+      <c r="D135" t="s">
+        <v>199</v>
+      </c>
+      <c r="M135" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>357</v>
-      </c>
-      <c r="C136" t="s">
-        <v>309</v>
-      </c>
-      <c r="D136" t="s">
-        <v>310</v>
-      </c>
-      <c r="J136" t="s">
-        <v>204</v>
-      </c>
-      <c r="K136" t="s">
-        <v>205</v>
-      </c>
-      <c r="L136" t="s">
-        <v>206</v>
-      </c>
-      <c r="M136" t="s">
-        <v>358</v>
+        <v>353</v>
+      </c>
+      <c r="G136" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4360,27 +4361,36 @@
         <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="G137" t="s">
-        <v>360</v>
-      </c>
-      <c r="M137" t="s">
-        <v>165</v>
+        <v>356</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="B138" t="s">
-        <v>361</v>
-      </c>
-      <c r="G138" t="s">
-        <v>362</v>
+        <v>357</v>
+      </c>
+      <c r="C138" t="s">
+        <v>309</v>
+      </c>
+      <c r="D138" t="s">
+        <v>310</v>
+      </c>
+      <c r="J138" t="s">
+        <v>204</v>
+      </c>
+      <c r="K138" t="s">
+        <v>205</v>
+      </c>
+      <c r="L138" t="s">
+        <v>206</v>
       </c>
       <c r="M138" t="s">
-        <v>165</v>
+        <v>358</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4388,10 +4398,13 @@
         <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="G139" t="s">
-        <v>364</v>
+        <v>360</v>
+      </c>
+      <c r="M139" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4399,10 +4412,13 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="G140" t="s">
-        <v>366</v>
+        <v>362</v>
+      </c>
+      <c r="M140" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4410,13 +4426,10 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="G141" t="s">
-        <v>368</v>
-      </c>
-      <c r="M141" t="s">
-        <v>165</v>
+        <v>364</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4424,21 +4437,24 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="G142" t="s">
-        <v>370</v>
-      </c>
-      <c r="M142" t="s">
-        <v>165</v>
+        <v>366</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B143" t="s">
-        <v>324</v>
+        <v>367</v>
+      </c>
+      <c r="G143" t="s">
+        <v>368</v>
+      </c>
+      <c r="M143" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4446,67 +4462,49 @@
         <v>17</v>
       </c>
       <c r="B144" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G144" t="s">
-        <v>101</v>
+        <v>370</v>
       </c>
       <c r="M144" t="s">
-        <v>372</v>
+        <v>165</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B145" t="s">
-        <v>373</v>
-      </c>
-      <c r="G145" t="s">
-        <v>101</v>
-      </c>
-      <c r="M145" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B146" t="s">
-        <v>375</v>
-      </c>
-      <c r="C146" t="s">
-        <v>548</v>
-      </c>
-      <c r="D146" t="s">
-        <v>376</v>
-      </c>
-      <c r="E146" t="s">
-        <v>377</v>
-      </c>
-      <c r="F146" t="s">
-        <v>378</v>
+        <v>371</v>
+      </c>
+      <c r="G146" t="s">
+        <v>101</v>
       </c>
       <c r="M146" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
-        <v>380</v>
+        <v>17</v>
       </c>
       <c r="B147" t="s">
-        <v>381</v>
-      </c>
-      <c r="C147" t="s">
-        <v>382</v>
-      </c>
-      <c r="D147" t="s">
-        <v>383</v>
+        <v>373</v>
+      </c>
+      <c r="G147" t="s">
+        <v>101</v>
       </c>
       <c r="M147" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4514,39 +4512,39 @@
         <v>52</v>
       </c>
       <c r="B148" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
       <c r="C148" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="D148" t="s">
-        <v>385</v>
+        <v>376</v>
       </c>
       <c r="E148" t="s">
-        <v>386</v>
+        <v>377</v>
       </c>
       <c r="F148" t="s">
-        <v>387</v>
+        <v>378</v>
       </c>
       <c r="M148" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
-        <v>389</v>
+        <v>380</v>
       </c>
       <c r="B149" t="s">
-        <v>390</v>
+        <v>381</v>
       </c>
       <c r="C149" t="s">
-        <v>391</v>
+        <v>382</v>
       </c>
       <c r="D149" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="M149" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4554,44 +4552,56 @@
         <v>52</v>
       </c>
       <c r="B150" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="C150" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="D150" t="s">
-        <v>394</v>
+        <v>385</v>
+      </c>
+      <c r="E150" t="s">
+        <v>386</v>
+      </c>
+      <c r="F150" t="s">
+        <v>387</v>
       </c>
       <c r="M150" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
-        <v>17</v>
+        <v>389</v>
       </c>
       <c r="B151" t="s">
-        <v>396</v>
-      </c>
-      <c r="G151" t="s">
-        <v>101</v>
+        <v>390</v>
+      </c>
+      <c r="C151" t="s">
+        <v>391</v>
+      </c>
+      <c r="D151" t="s">
+        <v>392</v>
       </c>
       <c r="M151" t="s">
-        <v>397</v>
+        <v>388</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B152" t="s">
-        <v>398</v>
-      </c>
-      <c r="G152" t="s">
-        <v>101</v>
+        <v>393</v>
+      </c>
+      <c r="C152" t="s">
+        <v>548</v>
+      </c>
+      <c r="D152" t="s">
+        <v>394</v>
       </c>
       <c r="M152" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4599,13 +4609,13 @@
         <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="G153" t="s">
         <v>101</v>
       </c>
       <c r="M153" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="154" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4613,59 +4623,63 @@
         <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="G154" t="s">
         <v>101</v>
       </c>
       <c r="M154" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A155" t="s">
+        <v>17</v>
+      </c>
+      <c r="B155" t="s">
+        <v>400</v>
+      </c>
+      <c r="G155" t="s">
+        <v>101</v>
+      </c>
+      <c r="M155" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" t="s">
+        <v>17</v>
+      </c>
+      <c r="B156" t="s">
+        <v>402</v>
+      </c>
+      <c r="G156" t="s">
+        <v>101</v>
+      </c>
+      <c r="M156" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="155" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A155" s="2" t="s">
+    <row r="157" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B157" s="2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="157" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A157" s="1" t="s">
+    <row r="159" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B157" s="1" t="s">
+      <c r="B159" s="1" t="s">
         <v>521</v>
       </c>
-      <c r="C157" s="1" t="s">
-        <v>547</v>
-      </c>
-      <c r="N157" s="1" t="s">
+      <c r="C159" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="N159" s="1" t="s">
         <v>532</v>
-      </c>
-    </row>
-    <row r="158" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A158" t="s">
-        <v>17</v>
-      </c>
-      <c r="B158" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="C158" s="4"/>
-      <c r="G158" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="159" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A159" t="s">
-        <v>17</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="C159" s="4"/>
-      <c r="G159" s="3" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="160" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4673,11 +4687,11 @@
         <v>17</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C160" s="4"/>
-      <c r="G160" s="3" t="s">
-        <v>541</v>
+      <c r="G160" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="161" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4685,68 +4699,52 @@
         <v>17</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="C161" s="4"/>
       <c r="G161" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
     </row>
     <row r="162" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" t="s">
-        <v>52</v>
-      </c>
-      <c r="B162" t="s">
-        <v>538</v>
-      </c>
-      <c r="C162" s="5" t="s">
-        <v>539</v>
-      </c>
-      <c r="D162" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="M162" s="3" t="s">
-        <v>533</v>
+        <v>17</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="C162" s="4"/>
+      <c r="G162" s="3" t="s">
+        <v>540</v>
       </c>
     </row>
     <row r="163" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
-        <v>522</v>
-      </c>
-      <c r="B163" t="s">
-        <v>523</v>
-      </c>
-      <c r="C163" s="6" t="s">
-        <v>543</v>
-      </c>
-      <c r="J163" t="s">
-        <v>524</v>
-      </c>
-      <c r="K163" t="s">
-        <v>525</v>
-      </c>
-      <c r="M163" s="3" t="s">
-        <v>533</v>
+        <v>17</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>536</v>
+      </c>
+      <c r="C163" s="4"/>
+      <c r="G163" s="3" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="164" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
-        <v>522</v>
+        <v>52</v>
       </c>
       <c r="B164" t="s">
-        <v>526</v>
-      </c>
-      <c r="C164" s="6" t="s">
-        <v>544</v>
-      </c>
-      <c r="J164" t="s">
-        <v>528</v>
-      </c>
-      <c r="K164" t="s">
-        <v>529</v>
+        <v>537</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>538</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="M164" s="3" t="s">
-        <v>533</v>
+        <v>554</v>
       </c>
     </row>
     <row r="165" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4754,104 +4752,95 @@
         <v>522</v>
       </c>
       <c r="B165" t="s">
+        <v>523</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="J165" t="s">
+        <v>524</v>
+      </c>
+      <c r="K165" t="s">
+        <v>525</v>
+      </c>
+      <c r="M165" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" t="s">
+        <v>522</v>
+      </c>
+      <c r="B166" t="s">
+        <v>526</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="J166" t="s">
+        <v>528</v>
+      </c>
+      <c r="K166" t="s">
+        <v>529</v>
+      </c>
+      <c r="M166" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" t="s">
+        <v>522</v>
+      </c>
+      <c r="B167" t="s">
         <v>527</v>
       </c>
-      <c r="C165" s="6" t="s">
-        <v>545</v>
-      </c>
-      <c r="J165" t="s">
+      <c r="C167" s="6" t="s">
+        <v>544</v>
+      </c>
+      <c r="J167" t="s">
         <v>531</v>
       </c>
-      <c r="K165" t="s">
+      <c r="K167" t="s">
         <v>530</v>
       </c>
-      <c r="M165" s="3" t="s">
-        <v>533</v>
-      </c>
-    </row>
-    <row r="166" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" s="1" t="s">
+      <c r="M167" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="B166" s="1" t="s">
+      <c r="B168" s="1" t="s">
         <v>521</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" t="s">
-        <v>103</v>
-      </c>
-      <c r="B168" t="s">
-        <v>404</v>
-      </c>
-      <c r="C168" t="s">
-        <v>405</v>
-      </c>
-      <c r="D168" t="s">
-        <v>406</v>
-      </c>
-      <c r="E168" t="s">
-        <v>407</v>
-      </c>
-      <c r="F168" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="169" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A169" t="s">
-        <v>409</v>
-      </c>
-      <c r="B169" t="s">
-        <v>410</v>
-      </c>
-      <c r="C169" t="s">
-        <v>411</v>
-      </c>
-      <c r="D169" t="s">
-        <v>412</v>
-      </c>
-      <c r="E169" t="s">
-        <v>413</v>
-      </c>
-      <c r="F169" t="s">
-        <v>414</v>
-      </c>
-      <c r="H169" t="s">
-        <v>24</v>
-      </c>
-      <c r="M169" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
-        <v>416</v>
+        <v>103</v>
       </c>
       <c r="B170" t="s">
-        <v>417</v>
+        <v>404</v>
       </c>
       <c r="C170" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
       <c r="D170" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="E170" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
       <c r="F170" t="s">
-        <v>414</v>
-      </c>
-      <c r="M170" t="s">
-        <v>56</v>
+        <v>408</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="B171" t="s">
-        <v>419</v>
+        <v>410</v>
       </c>
       <c r="C171" t="s">
         <v>411</v>
@@ -4859,72 +4848,99 @@
       <c r="D171" t="s">
         <v>412</v>
       </c>
+      <c r="E171" t="s">
+        <v>413</v>
+      </c>
+      <c r="F171" t="s">
+        <v>414</v>
+      </c>
       <c r="H171" t="s">
         <v>24</v>
       </c>
       <c r="M171" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
-        <v>52</v>
+        <v>416</v>
       </c>
       <c r="B172" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="C172" t="s">
-        <v>422</v>
+        <v>411</v>
       </c>
       <c r="D172" t="s">
-        <v>423</v>
+        <v>412</v>
+      </c>
+      <c r="E172" t="s">
+        <v>413</v>
+      </c>
+      <c r="F172" t="s">
+        <v>414</v>
       </c>
       <c r="M172" t="s">
-        <v>424</v>
+        <v>56</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
-        <v>20</v>
+        <v>418</v>
       </c>
       <c r="B173" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="C173" t="s">
-        <v>426</v>
+        <v>411</v>
       </c>
       <c r="D173" t="s">
-        <v>427</v>
+        <v>412</v>
+      </c>
+      <c r="H173" t="s">
+        <v>24</v>
+      </c>
+      <c r="M173" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
+        <v>52</v>
+      </c>
+      <c r="B174" t="s">
+        <v>421</v>
+      </c>
+      <c r="C174" t="s">
+        <v>422</v>
+      </c>
+      <c r="D174" t="s">
+        <v>423</v>
+      </c>
+      <c r="M174" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" t="s">
+        <v>20</v>
+      </c>
+      <c r="B175" t="s">
+        <v>425</v>
+      </c>
+      <c r="C175" t="s">
+        <v>426</v>
+      </c>
+      <c r="D175" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" t="s">
         <v>45</v>
       </c>
-      <c r="B174" t="s">
+      <c r="B176" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" t="s">
-        <v>17</v>
-      </c>
-      <c r="B181" t="s">
-        <v>428</v>
-      </c>
-      <c r="G181" t="s">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A182" t="s">
-        <v>17</v>
-      </c>
-      <c r="B182" t="s">
-        <v>430</v>
-      </c>
-      <c r="G182" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4932,10 +4948,10 @@
         <v>17</v>
       </c>
       <c r="B183" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="G183" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4943,10 +4959,10 @@
         <v>17</v>
       </c>
       <c r="B184" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="G184" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4954,10 +4970,10 @@
         <v>17</v>
       </c>
       <c r="B185" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="G185" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4965,9 +4981,31 @@
         <v>17</v>
       </c>
       <c r="B186" t="s">
+        <v>434</v>
+      </c>
+      <c r="G186" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" t="s">
+        <v>17</v>
+      </c>
+      <c r="B187" t="s">
+        <v>436</v>
+      </c>
+      <c r="G187" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" t="s">
+        <v>17</v>
+      </c>
+      <c r="B188" t="s">
         <v>438</v>
       </c>
-      <c r="G186" t="s">
+      <c r="G188" t="s">
         <v>439</v>
       </c>
     </row>
@@ -5078,7 +5116,7 @@
         <v>451</v>
       </c>
       <c r="C7" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D7" t="s">
         <v>453</v>
@@ -5453,21 +5491,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5906,7 +5929,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
@@ -5970,7 +5993,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -5979,7 +6002,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6029,23 +6052,22 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6068,7 +6090,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6082,7 +6104,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6090,10 +6112,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
moved preg lact questions to women's sect
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rojohnston\OneDrive - UNICEF\1 UNICEF Work\1 Afghanistan\Surveys\UrbanSMART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F8D3ADF-7F6E-47E9-8BE3-D739C546EE58}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A840712-88ED-4A15-9988-5F68AA980E7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="556">
   <si>
     <t>type</t>
   </si>
@@ -274,9 +274,6 @@
   </si>
   <si>
     <t>Est-ce que le membre du ménage ${name} était enceinte au début de la période de rappel ?</t>
-  </si>
-  <si>
-    <t>${age_years} &gt;=15 and ${age_years} &lt;=49 and ${sex}= 'f'</t>
   </si>
   <si>
     <t>is_child</t>
@@ -1754,21 +1751,6 @@
     <t>curr_breastfeed</t>
   </si>
   <si>
-    <t>is_plw</t>
-  </si>
-  <si>
-    <t>plw</t>
-  </si>
-  <si>
-    <t>join(' ',${hh_roster}[is_plw = true()]/hh_position)</t>
-  </si>
-  <si>
-    <t>count-selected(${plw})</t>
-  </si>
-  <si>
-    <t>numplw</t>
-  </si>
-  <si>
     <t>preg_lact_wom</t>
   </si>
   <si>
@@ -1802,36 +1784,6 @@
     <t xml:space="preserve">(. &gt;= 25 and . &lt;200) </t>
   </si>
   <si>
-    <t>${numplw}</t>
-  </si>
-  <si>
-    <t>plw_selected_position</t>
-  </si>
-  <si>
-    <t>plw_hh_position</t>
-  </si>
-  <si>
-    <t>plw_name</t>
-  </si>
-  <si>
-    <t>plw_age_years</t>
-  </si>
-  <si>
-    <t>plw_name_note</t>
-  </si>
-  <si>
-    <t>Now entering data for woman: ${plw_name} aged  ${plw_age_years} years</t>
-  </si>
-  <si>
-    <t>number(selected-at(${plw}, ${plw_selected_position}))</t>
-  </si>
-  <si>
-    <t>indexed-repeat(${name}, ${hh_roster}, ${plw_hh_position})</t>
-  </si>
-  <si>
-    <t>indexed-repeat(${age_years}, ${hh_roster}, ${plw_hh_position})</t>
-  </si>
-  <si>
     <t>Woman's MUAC in MM of (${plw_name})</t>
   </si>
   <si>
@@ -1859,16 +1811,67 @@
     <t>show PLW</t>
   </si>
   <si>
-    <t>if(${curr_pregnant}=1 or ${curr_breastfeed}=1,true(),false())</t>
-  </si>
-  <si>
-    <t>PLW ${plw} numPLW ${numplw}</t>
-  </si>
-  <si>
-    <t>IS PLW ${is_plw} PReg ${curr_pregnant} Breastfeed ${curr_breastfeed}</t>
-  </si>
-  <si>
-    <t>${consent}=1 and ${is_plw}='true'</t>
+    <t>is_woman</t>
+  </si>
+  <si>
+    <t>if(${age_years} &gt;=15 and ${age_years} &lt;=49 and ${sex}= 'f',true(),false())</t>
+  </si>
+  <si>
+    <t>women</t>
+  </si>
+  <si>
+    <t>numwomen</t>
+  </si>
+  <si>
+    <t>join(' ',${hh_roster}[is_woman = true()]/hh_position)</t>
+  </si>
+  <si>
+    <t>count-selected(${women})</t>
+  </si>
+  <si>
+    <t>${numwomen}</t>
+  </si>
+  <si>
+    <t>wom_selected_position</t>
+  </si>
+  <si>
+    <t>wom_hh_position</t>
+  </si>
+  <si>
+    <t>wom_name</t>
+  </si>
+  <si>
+    <t>wom_age_years</t>
+  </si>
+  <si>
+    <t>wom_name_note</t>
+  </si>
+  <si>
+    <t>Now entering data for woman: ${wom_name} aged  ${wom_age_years} years</t>
+  </si>
+  <si>
+    <t>indexed-repeat(${name}, ${hh_roster}, ${wom_hh_position})</t>
+  </si>
+  <si>
+    <t>indexed-repeat(${age_years}, ${hh_roster}, ${wom_hh_position})</t>
+  </si>
+  <si>
+    <t>${consent}=1 and ${is_woman}='true'</t>
+  </si>
+  <si>
+    <t>${curr_pregnant}=1 or ${curr_breastfeed}=1</t>
+  </si>
+  <si>
+    <t>${curr_pregnant}=1 or ${curr_breastfeed}=2</t>
+  </si>
+  <si>
+    <t>${curr_pregnant}=1 or ${curr_breastfeed}=3</t>
+  </si>
+  <si>
+    <t>number(selected-at(${women}, ${wom_selected_position}))</t>
+  </si>
+  <si>
+    <t>woman-${wom_selected_position} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
   </si>
 </sst>
 </file>
@@ -2279,11 +2282,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N188"/>
+  <dimension ref="A1:N189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M164" sqref="M164:M167"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A162" sqref="A162:XFD162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2684,231 +2687,203 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" t="s">
-        <v>514</v>
-      </c>
-      <c r="C28" t="s">
-        <v>512</v>
-      </c>
-      <c r="D28" t="s">
-        <v>83</v>
-      </c>
-      <c r="H28" t="s">
-        <v>24</v>
-      </c>
-      <c r="M28" t="s">
-        <v>84</v>
-      </c>
-    </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>515</v>
-      </c>
-      <c r="C29" t="s">
-        <v>513</v>
-      </c>
-      <c r="D29" t="s">
-        <v>83</v>
-      </c>
-      <c r="H29" t="s">
-        <v>24</v>
-      </c>
-      <c r="M29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" s="2" t="s">
+      <c r="G30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G32" s="2" t="s">
+    </row>
+    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>535</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A34" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>553</v>
+      <c r="C32" s="3"/>
+      <c r="G32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" t="s">
+        <v>89</v>
+      </c>
+      <c r="G34" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="3"/>
-      <c r="G35" t="s">
-        <v>88</v>
+        <v>91</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>93</v>
+      </c>
+      <c r="H35" t="s">
+        <v>24</v>
+      </c>
+      <c r="M35" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
       <c r="B36" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" t="s">
-        <v>90</v>
-      </c>
-      <c r="G37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" t="s">
-        <v>82</v>
-      </c>
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-      <c r="C38" t="s">
-        <v>93</v>
-      </c>
-      <c r="D38" t="s">
         <v>94</v>
       </c>
-      <c r="H38" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A39" t="s">
-        <v>32</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="C36" t="s">
         <v>95</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D36" t="s">
         <v>96</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E36" t="s">
         <v>97</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F36" t="s">
         <v>98</v>
       </c>
-      <c r="F39" t="s">
+      <c r="M36" t="s">
         <v>99</v>
       </c>
-      <c r="M39" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A41" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B41" s="2" t="s">
+    </row>
+    <row r="38" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="G41" s="2" t="s">
+    </row>
+    <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="42" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A42" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B42" s="2" t="s">
+      <c r="G39" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G42" s="2" t="s">
+    </row>
+    <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>537</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="43" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B43" s="2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="G43" s="1" t="s">
-        <v>518</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="G44" s="1" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>550</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A46" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="N46" s="2" t="s">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>17</v>
+      </c>
+      <c r="B44" t="s">
         <v>111</v>
+      </c>
+      <c r="G44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46" t="s">
+        <v>115</v>
+      </c>
+      <c r="G46" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2916,10 +2891,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="G47" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2927,447 +2902,447 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="G48" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B49" t="s">
-        <v>116</v>
-      </c>
-      <c r="G49" t="s">
-        <v>117</v>
+        <v>121</v>
+      </c>
+      <c r="C49" t="s">
+        <v>122</v>
+      </c>
+      <c r="D49" t="s">
+        <v>123</v>
+      </c>
+      <c r="M49" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B50" t="s">
-        <v>118</v>
-      </c>
-      <c r="G50" t="s">
-        <v>119</v>
+        <v>125</v>
+      </c>
+      <c r="M50" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
-      </c>
-      <c r="G51" t="s">
-        <v>121</v>
+        <v>126</v>
+      </c>
+      <c r="C51" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" t="s">
+        <v>128</v>
+      </c>
+      <c r="E51" t="s">
+        <v>129</v>
+      </c>
+      <c r="F51" t="s">
+        <v>130</v>
+      </c>
+      <c r="H51" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C52" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D52" t="s">
-        <v>124</v>
+        <v>133</v>
+      </c>
+      <c r="E52" t="s">
+        <v>134</v>
+      </c>
+      <c r="F52" t="s">
+        <v>135</v>
+      </c>
+      <c r="I52" t="s">
+        <v>31</v>
+      </c>
+      <c r="J52" t="s">
+        <v>136</v>
       </c>
       <c r="M52" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>138</v>
+      </c>
+      <c r="C53" t="s">
+        <v>139</v>
+      </c>
+      <c r="D53" t="s">
+        <v>140</v>
+      </c>
+      <c r="E53" t="s">
+        <v>141</v>
+      </c>
+      <c r="F53" t="s">
+        <v>142</v>
+      </c>
+      <c r="J53" t="s">
+        <v>143</v>
+      </c>
+      <c r="K53" t="s">
+        <v>144</v>
+      </c>
+      <c r="L53" t="s">
+        <v>145</v>
       </c>
       <c r="M53" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>127</v>
-      </c>
-      <c r="C54" t="s">
-        <v>128</v>
-      </c>
-      <c r="D54" t="s">
-        <v>129</v>
-      </c>
-      <c r="E54" t="s">
-        <v>130</v>
-      </c>
-      <c r="F54" t="s">
-        <v>131</v>
-      </c>
-      <c r="H54" t="s">
-        <v>24</v>
+        <v>147</v>
+      </c>
+      <c r="G54" t="s">
+        <v>148</v>
+      </c>
+      <c r="M54" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
-      </c>
-      <c r="C55" t="s">
-        <v>133</v>
-      </c>
-      <c r="D55" t="s">
-        <v>134</v>
-      </c>
-      <c r="E55" t="s">
-        <v>135</v>
-      </c>
-      <c r="F55" t="s">
-        <v>136</v>
-      </c>
-      <c r="I55" t="s">
-        <v>31</v>
-      </c>
-      <c r="J55" t="s">
-        <v>137</v>
-      </c>
-      <c r="M55" t="s">
-        <v>138</v>
+        <v>149</v>
+      </c>
+      <c r="G55" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B56" t="s">
-        <v>139</v>
+        <v>151</v>
       </c>
       <c r="C56" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="D56" t="s">
-        <v>141</v>
-      </c>
-      <c r="E56" t="s">
-        <v>142</v>
-      </c>
-      <c r="F56" t="s">
-        <v>143</v>
-      </c>
-      <c r="J56" t="s">
-        <v>144</v>
-      </c>
-      <c r="K56" t="s">
-        <v>145</v>
-      </c>
-      <c r="L56" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="M56" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
-      </c>
-      <c r="G57" t="s">
-        <v>149</v>
+        <v>155</v>
+      </c>
+      <c r="C57" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57" t="s">
+        <v>157</v>
       </c>
       <c r="M57" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>17</v>
+        <v>82</v>
       </c>
       <c r="B58" t="s">
-        <v>150</v>
-      </c>
-      <c r="G58" t="s">
-        <v>151</v>
+        <v>159</v>
+      </c>
+      <c r="C58" t="s">
+        <v>160</v>
+      </c>
+      <c r="D58" t="s">
+        <v>161</v>
+      </c>
+      <c r="H58" t="s">
+        <v>24</v>
+      </c>
+      <c r="M58" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
-      </c>
-      <c r="C59" t="s">
-        <v>153</v>
-      </c>
-      <c r="D59" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="M59" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="B60" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="C60" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="D60" t="s">
-        <v>158</v>
-      </c>
-      <c r="M60" t="s">
-        <v>159</v>
+        <v>168</v>
+      </c>
+      <c r="E60" t="s">
+        <v>169</v>
+      </c>
+      <c r="F60" t="s">
+        <v>170</v>
+      </c>
+      <c r="J60" t="s">
+        <v>171</v>
+      </c>
+      <c r="K60" t="s">
+        <v>172</v>
+      </c>
+      <c r="L60" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>82</v>
+        <v>174</v>
       </c>
       <c r="B61" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="C61" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>162</v>
-      </c>
-      <c r="H61" t="s">
-        <v>24</v>
+        <v>177</v>
       </c>
       <c r="M61" t="s">
-        <v>163</v>
+        <v>178</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>27</v>
+        <v>165</v>
       </c>
       <c r="B62" t="s">
-        <v>164</v>
-      </c>
-      <c r="M62" t="s">
-        <v>165</v>
+        <v>179</v>
+      </c>
+      <c r="C62" t="s">
+        <v>180</v>
+      </c>
+      <c r="D62" t="s">
+        <v>181</v>
+      </c>
+      <c r="E62" t="s">
+        <v>182</v>
+      </c>
+      <c r="F62" t="s">
+        <v>183</v>
+      </c>
+      <c r="J62" t="s">
+        <v>184</v>
+      </c>
+      <c r="K62" t="s">
+        <v>185</v>
+      </c>
+      <c r="L62" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B63" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="C63" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="D63" t="s">
-        <v>169</v>
-      </c>
-      <c r="E63" t="s">
-        <v>170</v>
-      </c>
-      <c r="F63" t="s">
-        <v>171</v>
-      </c>
-      <c r="J63" t="s">
-        <v>172</v>
-      </c>
-      <c r="K63" t="s">
-        <v>173</v>
-      </c>
-      <c r="L63" t="s">
-        <v>174</v>
+        <v>190</v>
+      </c>
+      <c r="M63" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>176</v>
+        <v>192</v>
       </c>
       <c r="C64" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="D64" t="s">
-        <v>178</v>
+        <v>194</v>
       </c>
       <c r="M64" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>166</v>
+        <v>52</v>
       </c>
       <c r="B65" t="s">
-        <v>180</v>
+        <v>196</v>
       </c>
       <c r="C65" t="s">
-        <v>181</v>
+        <v>197</v>
       </c>
       <c r="D65" t="s">
-        <v>182</v>
-      </c>
-      <c r="E65" t="s">
-        <v>183</v>
-      </c>
-      <c r="F65" t="s">
-        <v>184</v>
-      </c>
-      <c r="J65" t="s">
-        <v>185</v>
-      </c>
-      <c r="K65" t="s">
-        <v>186</v>
-      </c>
-      <c r="L65" t="s">
-        <v>187</v>
+        <v>198</v>
+      </c>
+      <c r="M65" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>188</v>
+        <v>32</v>
       </c>
       <c r="B66" t="s">
-        <v>189</v>
+        <v>200</v>
       </c>
       <c r="C66" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="D66" t="s">
-        <v>191</v>
+        <v>202</v>
+      </c>
+      <c r="J66" t="s">
+        <v>203</v>
+      </c>
+      <c r="K66" t="s">
+        <v>204</v>
+      </c>
+      <c r="L66" t="s">
+        <v>205</v>
       </c>
       <c r="M66" t="s">
-        <v>192</v>
+        <v>206</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="B67" t="s">
-        <v>193</v>
+        <v>207</v>
       </c>
       <c r="C67" t="s">
-        <v>194</v>
+        <v>208</v>
       </c>
       <c r="D67" t="s">
-        <v>195</v>
-      </c>
-      <c r="M67" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B68" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="C68" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="D68" t="s">
-        <v>199</v>
+        <v>212</v>
+      </c>
+      <c r="H68" t="s">
+        <v>24</v>
       </c>
       <c r="M68" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="B69" t="s">
-        <v>201</v>
-      </c>
-      <c r="C69" t="s">
-        <v>202</v>
-      </c>
-      <c r="D69" t="s">
-        <v>203</v>
-      </c>
-      <c r="J69" t="s">
-        <v>204</v>
-      </c>
-      <c r="K69" t="s">
-        <v>205</v>
-      </c>
-      <c r="L69" t="s">
-        <v>206</v>
-      </c>
-      <c r="M69" t="s">
-        <v>207</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>45</v>
       </c>
       <c r="B70" t="s">
-        <v>208</v>
-      </c>
-      <c r="C70" t="s">
-        <v>209</v>
-      </c>
-      <c r="D70" t="s">
-        <v>210</v>
+        <v>125</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>211</v>
-      </c>
-      <c r="C71" t="s">
-        <v>212</v>
-      </c>
-      <c r="D71" t="s">
-        <v>213</v>
-      </c>
-      <c r="H71" t="s">
-        <v>24</v>
-      </c>
-      <c r="M71" t="s">
         <v>214</v>
+      </c>
+      <c r="G71" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>164</v>
+        <v>216</v>
+      </c>
+      <c r="G72" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>126</v>
+        <v>218</v>
+      </c>
+      <c r="G73" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3375,10 +3350,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="G74" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3386,10 +3361,13 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="G75" t="s">
-        <v>218</v>
+        <v>222</v>
+      </c>
+      <c r="M75" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3397,10 +3375,13 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>219</v>
+        <v>224</v>
       </c>
       <c r="G76" t="s">
-        <v>511</v>
+        <v>225</v>
+      </c>
+      <c r="M76" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3408,10 +3389,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="G77" t="s">
-        <v>221</v>
+        <v>227</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3419,13 +3400,13 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>222</v>
+        <v>228</v>
       </c>
       <c r="G78" t="s">
+        <v>229</v>
+      </c>
+      <c r="M78" t="s">
         <v>223</v>
-      </c>
-      <c r="M78" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3433,13 +3414,13 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>230</v>
       </c>
       <c r="G79" t="s">
-        <v>226</v>
+        <v>231</v>
       </c>
       <c r="M79" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3447,10 +3428,10 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>227</v>
+        <v>232</v>
       </c>
       <c r="G80" t="s">
-        <v>228</v>
+        <v>233</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3458,13 +3439,13 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>229</v>
+        <v>234</v>
       </c>
       <c r="G81" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="M81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3472,13 +3453,13 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="G82" t="s">
-        <v>232</v>
+        <v>237</v>
       </c>
       <c r="M82" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3486,10 +3467,10 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="G83" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3497,13 +3478,10 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="G84" t="s">
-        <v>236</v>
-      </c>
-      <c r="M84" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3511,13 +3489,13 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="G85" t="s">
-        <v>238</v>
+        <v>243</v>
       </c>
       <c r="M85" t="s">
-        <v>224</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3525,10 +3503,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="G86" t="s">
-        <v>240</v>
+        <v>245</v>
+      </c>
+      <c r="M86" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3536,10 +3517,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>241</v>
+        <v>246</v>
       </c>
       <c r="G87" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3547,13 +3528,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>243</v>
+        <v>248</v>
       </c>
       <c r="G88" t="s">
-        <v>244</v>
-      </c>
-      <c r="M88" t="s">
-        <v>165</v>
+        <v>249</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3561,13 +3539,13 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>245</v>
+        <v>250</v>
       </c>
       <c r="G89" t="s">
-        <v>246</v>
+        <v>251</v>
       </c>
       <c r="M89" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3575,10 +3553,13 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>247</v>
+        <v>252</v>
       </c>
       <c r="G90" t="s">
-        <v>248</v>
+        <v>253</v>
+      </c>
+      <c r="M90" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3586,344 +3567,353 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="G91" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A92" t="s">
-        <v>17</v>
-      </c>
-      <c r="B92" t="s">
-        <v>251</v>
-      </c>
-      <c r="G92" t="s">
-        <v>252</v>
-      </c>
-      <c r="M92" t="s">
-        <v>165</v>
-      </c>
-    </row>
+        <v>255</v>
+      </c>
+      <c r="M91" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B93" t="s">
-        <v>253</v>
-      </c>
-      <c r="G93" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="M93" t="s">
-        <v>165</v>
+        <v>257</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B94" t="s">
-        <v>255</v>
-      </c>
-      <c r="G94" t="s">
-        <v>256</v>
-      </c>
-      <c r="M94" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+        <v>258</v>
+      </c>
+      <c r="C94" t="s">
+        <v>259</v>
+      </c>
+      <c r="D94" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" t="s">
+        <v>82</v>
+      </c>
+      <c r="B95" t="s">
+        <v>261</v>
+      </c>
+      <c r="C95" t="s">
+        <v>262</v>
+      </c>
+      <c r="D95" t="s">
+        <v>263</v>
+      </c>
+      <c r="E95" t="s">
+        <v>129</v>
+      </c>
+      <c r="F95" t="s">
+        <v>130</v>
+      </c>
+    </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B96" t="s">
-        <v>257</v>
+        <v>264</v>
+      </c>
+      <c r="C96" t="s">
+        <v>265</v>
+      </c>
+      <c r="D96" t="s">
+        <v>266</v>
+      </c>
+      <c r="E96" t="s">
+        <v>134</v>
+      </c>
+      <c r="F96" t="s">
+        <v>135</v>
+      </c>
+      <c r="I96" t="s">
+        <v>31</v>
+      </c>
+      <c r="J96" t="s">
+        <v>136</v>
       </c>
       <c r="M96" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B97" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C97" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D97" t="s">
-        <v>261</v>
+        <v>270</v>
+      </c>
+      <c r="E97" t="s">
+        <v>141</v>
+      </c>
+      <c r="F97" t="s">
+        <v>142</v>
+      </c>
+      <c r="J97" t="s">
+        <v>271</v>
+      </c>
+      <c r="K97" t="s">
+        <v>144</v>
+      </c>
+      <c r="L97" t="s">
+        <v>145</v>
+      </c>
+      <c r="M97" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>262</v>
-      </c>
-      <c r="C98" t="s">
-        <v>263</v>
-      </c>
-      <c r="D98" t="s">
-        <v>264</v>
-      </c>
-      <c r="E98" t="s">
-        <v>130</v>
-      </c>
-      <c r="F98" t="s">
-        <v>131</v>
+        <v>273</v>
+      </c>
+      <c r="G98" t="s">
+        <v>274</v>
+      </c>
+      <c r="M98" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B99" t="s">
-        <v>265</v>
-      </c>
-      <c r="C99" t="s">
-        <v>266</v>
-      </c>
-      <c r="D99" t="s">
-        <v>267</v>
-      </c>
-      <c r="E99" t="s">
-        <v>135</v>
-      </c>
-      <c r="F99" t="s">
-        <v>136</v>
-      </c>
-      <c r="I99" t="s">
-        <v>31</v>
-      </c>
-      <c r="J99" t="s">
-        <v>137</v>
-      </c>
-      <c r="M99" t="s">
-        <v>268</v>
+        <v>275</v>
+      </c>
+      <c r="G99" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B100" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
       <c r="C100" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D100" t="s">
-        <v>271</v>
-      </c>
-      <c r="E100" t="s">
-        <v>142</v>
-      </c>
-      <c r="F100" t="s">
-        <v>143</v>
-      </c>
-      <c r="J100" t="s">
-        <v>272</v>
-      </c>
-      <c r="K100" t="s">
-        <v>145</v>
-      </c>
-      <c r="L100" t="s">
-        <v>146</v>
+        <v>279</v>
       </c>
       <c r="M100" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B101" t="s">
-        <v>274</v>
-      </c>
-      <c r="G101" t="s">
-        <v>275</v>
+        <v>281</v>
+      </c>
+      <c r="C101" t="s">
+        <v>282</v>
+      </c>
+      <c r="D101" t="s">
+        <v>283</v>
       </c>
       <c r="M101" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
       <c r="B102" t="s">
-        <v>276</v>
-      </c>
-      <c r="G102" t="s">
-        <v>277</v>
+        <v>285</v>
+      </c>
+      <c r="C102" t="s">
+        <v>286</v>
+      </c>
+      <c r="D102" t="s">
+        <v>287</v>
+      </c>
+      <c r="E102" t="s">
+        <v>169</v>
+      </c>
+      <c r="F102" t="s">
+        <v>170</v>
+      </c>
+      <c r="J102" t="s">
+        <v>171</v>
+      </c>
+      <c r="K102" t="s">
+        <v>172</v>
+      </c>
+      <c r="L102" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="B103" t="s">
-        <v>278</v>
+        <v>288</v>
       </c>
       <c r="C103" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="D103" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="M103" t="s">
-        <v>281</v>
+        <v>291</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="B104" t="s">
-        <v>282</v>
+        <v>292</v>
       </c>
       <c r="C104" t="s">
-        <v>283</v>
+        <v>293</v>
       </c>
       <c r="D104" t="s">
-        <v>284</v>
-      </c>
-      <c r="M104" t="s">
-        <v>285</v>
+        <v>294</v>
+      </c>
+      <c r="E104" t="s">
+        <v>182</v>
+      </c>
+      <c r="F104" t="s">
+        <v>183</v>
+      </c>
+      <c r="J104" t="s">
+        <v>184</v>
+      </c>
+      <c r="K104" t="s">
+        <v>185</v>
+      </c>
+      <c r="L104" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B105" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="C105" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="D105" t="s">
-        <v>288</v>
-      </c>
-      <c r="E105" t="s">
-        <v>170</v>
-      </c>
-      <c r="F105" t="s">
-        <v>171</v>
-      </c>
-      <c r="J105" t="s">
-        <v>172</v>
-      </c>
-      <c r="K105" t="s">
-        <v>173</v>
-      </c>
-      <c r="L105" t="s">
-        <v>174</v>
+        <v>297</v>
+      </c>
+      <c r="M105" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B106" t="s">
-        <v>289</v>
+        <v>299</v>
       </c>
       <c r="C106" t="s">
-        <v>290</v>
+        <v>193</v>
       </c>
       <c r="D106" t="s">
-        <v>291</v>
+        <v>194</v>
       </c>
       <c r="M106" t="s">
-        <v>292</v>
+        <v>300</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>166</v>
+        <v>52</v>
       </c>
       <c r="B107" t="s">
-        <v>293</v>
+        <v>301</v>
       </c>
       <c r="C107" t="s">
-        <v>294</v>
+        <v>197</v>
       </c>
       <c r="D107" t="s">
-        <v>295</v>
-      </c>
-      <c r="E107" t="s">
-        <v>183</v>
-      </c>
-      <c r="F107" t="s">
-        <v>184</v>
-      </c>
-      <c r="J107" t="s">
-        <v>185</v>
-      </c>
-      <c r="K107" t="s">
-        <v>186</v>
-      </c>
-      <c r="L107" t="s">
-        <v>187</v>
+        <v>198</v>
+      </c>
+      <c r="M107" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>296</v>
-      </c>
-      <c r="C108" t="s">
-        <v>297</v>
-      </c>
-      <c r="D108" t="s">
-        <v>298</v>
-      </c>
-      <c r="M108" t="s">
-        <v>299</v>
+        <v>303</v>
+      </c>
+      <c r="G108" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>300</v>
-      </c>
-      <c r="C109" t="s">
-        <v>194</v>
-      </c>
-      <c r="D109" t="s">
-        <v>195</v>
-      </c>
-      <c r="M109" t="s">
-        <v>301</v>
+        <v>305</v>
+      </c>
+      <c r="G109" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B110" t="s">
-        <v>302</v>
+        <v>307</v>
       </c>
       <c r="C110" t="s">
-        <v>198</v>
+        <v>308</v>
       </c>
       <c r="D110" t="s">
-        <v>199</v>
+        <v>309</v>
+      </c>
+      <c r="J110" t="s">
+        <v>203</v>
+      </c>
+      <c r="K110" t="s">
+        <v>204</v>
+      </c>
+      <c r="L110" t="s">
+        <v>205</v>
       </c>
       <c r="M110" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3931,10 +3921,13 @@
         <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="G111" t="s">
-        <v>305</v>
+        <v>312</v>
+      </c>
+      <c r="M111" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3942,36 +3935,24 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="G112" t="s">
-        <v>307</v>
+        <v>314</v>
+      </c>
+      <c r="M112" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>308</v>
-      </c>
-      <c r="C113" t="s">
-        <v>309</v>
-      </c>
-      <c r="D113" t="s">
-        <v>310</v>
-      </c>
-      <c r="J113" t="s">
-        <v>204</v>
-      </c>
-      <c r="K113" t="s">
-        <v>205</v>
-      </c>
-      <c r="L113" t="s">
-        <v>206</v>
-      </c>
-      <c r="M113" t="s">
-        <v>311</v>
+        <v>315</v>
+      </c>
+      <c r="G113" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3979,13 +3960,10 @@
         <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>312</v>
+        <v>317</v>
       </c>
       <c r="G114" t="s">
-        <v>313</v>
-      </c>
-      <c r="M114" t="s">
-        <v>165</v>
+        <v>318</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3993,13 +3971,13 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="G115" t="s">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="M115" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4007,348 +3985,360 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>316</v>
+        <v>321</v>
       </c>
       <c r="G116" t="s">
-        <v>317</v>
+        <v>322</v>
+      </c>
+      <c r="M116" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B117" t="s">
-        <v>318</v>
-      </c>
-      <c r="G117" t="s">
-        <v>319</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B118" t="s">
-        <v>320</v>
-      </c>
-      <c r="G118" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="M118" t="s">
-        <v>165</v>
+        <v>324</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B119" t="s">
-        <v>322</v>
-      </c>
-      <c r="G119" t="s">
-        <v>323</v>
-      </c>
-      <c r="M119" t="s">
-        <v>165</v>
+        <v>325</v>
+      </c>
+      <c r="C119" t="s">
+        <v>259</v>
+      </c>
+      <c r="D119" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>45</v>
+        <v>82</v>
       </c>
       <c r="B120" t="s">
-        <v>257</v>
+        <v>326</v>
+      </c>
+      <c r="C120" t="s">
+        <v>262</v>
+      </c>
+      <c r="D120" t="s">
+        <v>263</v>
+      </c>
+      <c r="E120" t="s">
+        <v>129</v>
+      </c>
+      <c r="F120" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B121" t="s">
-        <v>324</v>
+        <v>327</v>
+      </c>
+      <c r="C121" t="s">
+        <v>265</v>
+      </c>
+      <c r="D121" t="s">
+        <v>328</v>
+      </c>
+      <c r="E121" t="s">
+        <v>134</v>
+      </c>
+      <c r="F121" t="s">
+        <v>135</v>
+      </c>
+      <c r="I121" t="s">
+        <v>31</v>
+      </c>
+      <c r="J121" t="s">
+        <v>136</v>
       </c>
       <c r="M121" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B122" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="C122" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D122" t="s">
-        <v>261</v>
+        <v>270</v>
+      </c>
+      <c r="E122" t="s">
+        <v>141</v>
+      </c>
+      <c r="F122" t="s">
+        <v>142</v>
+      </c>
+      <c r="J122" t="s">
+        <v>271</v>
+      </c>
+      <c r="K122" t="s">
+        <v>144</v>
+      </c>
+      <c r="L122" t="s">
+        <v>145</v>
+      </c>
+      <c r="M122" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>327</v>
-      </c>
-      <c r="C123" t="s">
-        <v>263</v>
-      </c>
-      <c r="D123" t="s">
-        <v>264</v>
-      </c>
-      <c r="E123" t="s">
-        <v>130</v>
-      </c>
-      <c r="F123" t="s">
-        <v>131</v>
+        <v>332</v>
+      </c>
+      <c r="G123" t="s">
+        <v>333</v>
+      </c>
+      <c r="M123" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>328</v>
-      </c>
-      <c r="C124" t="s">
-        <v>266</v>
-      </c>
-      <c r="D124" t="s">
-        <v>329</v>
-      </c>
-      <c r="E124" t="s">
-        <v>135</v>
-      </c>
-      <c r="F124" t="s">
-        <v>136</v>
-      </c>
-      <c r="I124" t="s">
-        <v>31</v>
-      </c>
-      <c r="J124" t="s">
-        <v>137</v>
-      </c>
-      <c r="M124" t="s">
-        <v>330</v>
+        <v>334</v>
+      </c>
+      <c r="G124" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="B125" t="s">
-        <v>331</v>
+        <v>336</v>
       </c>
       <c r="C125" t="s">
-        <v>270</v>
+        <v>278</v>
       </c>
       <c r="D125" t="s">
-        <v>271</v>
-      </c>
-      <c r="E125" t="s">
-        <v>142</v>
-      </c>
-      <c r="F125" t="s">
-        <v>143</v>
-      </c>
-      <c r="J125" t="s">
-        <v>272</v>
-      </c>
-      <c r="K125" t="s">
-        <v>145</v>
-      </c>
-      <c r="L125" t="s">
-        <v>146</v>
+        <v>279</v>
       </c>
       <c r="M125" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B126" t="s">
-        <v>333</v>
-      </c>
-      <c r="G126" t="s">
-        <v>334</v>
+        <v>338</v>
+      </c>
+      <c r="C126" t="s">
+        <v>339</v>
+      </c>
+      <c r="D126" t="s">
+        <v>340</v>
       </c>
       <c r="M126" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>165</v>
       </c>
       <c r="B127" t="s">
-        <v>335</v>
-      </c>
-      <c r="G127" t="s">
-        <v>336</v>
+        <v>342</v>
+      </c>
+      <c r="C127" t="s">
+        <v>286</v>
+      </c>
+      <c r="D127" t="s">
+        <v>287</v>
+      </c>
+      <c r="E127" t="s">
+        <v>169</v>
+      </c>
+      <c r="F127" t="s">
+        <v>170</v>
+      </c>
+      <c r="J127" t="s">
+        <v>171</v>
+      </c>
+      <c r="K127" t="s">
+        <v>172</v>
+      </c>
+      <c r="L127" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>52</v>
+        <v>174</v>
       </c>
       <c r="B128" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C128" t="s">
-        <v>279</v>
+        <v>289</v>
       </c>
       <c r="D128" t="s">
-        <v>280</v>
+        <v>290</v>
       </c>
       <c r="M128" t="s">
-        <v>338</v>
+        <v>344</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="B129" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="C129" t="s">
-        <v>340</v>
+        <v>293</v>
       </c>
       <c r="D129" t="s">
-        <v>341</v>
-      </c>
-      <c r="M129" t="s">
-        <v>342</v>
+        <v>294</v>
+      </c>
+      <c r="E129" t="s">
+        <v>182</v>
+      </c>
+      <c r="F129" t="s">
+        <v>183</v>
+      </c>
+      <c r="J129" t="s">
+        <v>184</v>
+      </c>
+      <c r="K129" t="s">
+        <v>185</v>
+      </c>
+      <c r="L129" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="B130" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="C130" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="D130" t="s">
-        <v>288</v>
-      </c>
-      <c r="E130" t="s">
-        <v>170</v>
-      </c>
-      <c r="F130" t="s">
-        <v>171</v>
-      </c>
-      <c r="J130" t="s">
-        <v>172</v>
-      </c>
-      <c r="K130" t="s">
-        <v>173</v>
-      </c>
-      <c r="L130" t="s">
-        <v>174</v>
+        <v>297</v>
+      </c>
+      <c r="M130" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>175</v>
+        <v>52</v>
       </c>
       <c r="B131" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="C131" t="s">
-        <v>290</v>
+        <v>193</v>
       </c>
       <c r="D131" t="s">
-        <v>291</v>
+        <v>194</v>
       </c>
       <c r="M131" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>166</v>
+        <v>52</v>
       </c>
       <c r="B132" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="C132" t="s">
-        <v>294</v>
+        <v>197</v>
       </c>
       <c r="D132" t="s">
-        <v>295</v>
-      </c>
-      <c r="E132" t="s">
-        <v>183</v>
-      </c>
-      <c r="F132" t="s">
-        <v>184</v>
-      </c>
-      <c r="J132" t="s">
-        <v>185</v>
-      </c>
-      <c r="K132" t="s">
-        <v>186</v>
-      </c>
-      <c r="L132" t="s">
-        <v>187</v>
+        <v>198</v>
+      </c>
+      <c r="M132" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>188</v>
+        <v>17</v>
       </c>
       <c r="B133" t="s">
-        <v>347</v>
-      </c>
-      <c r="C133" t="s">
-        <v>297</v>
-      </c>
-      <c r="D133" t="s">
-        <v>298</v>
-      </c>
-      <c r="M133" t="s">
-        <v>348</v>
+        <v>352</v>
+      </c>
+      <c r="G133" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B134" t="s">
-        <v>349</v>
-      </c>
-      <c r="C134" t="s">
-        <v>194</v>
-      </c>
-      <c r="D134" t="s">
-        <v>195</v>
-      </c>
-      <c r="M134" t="s">
-        <v>350</v>
+        <v>354</v>
+      </c>
+      <c r="G134" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B135" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
       <c r="C135" t="s">
-        <v>198</v>
+        <v>308</v>
       </c>
       <c r="D135" t="s">
-        <v>199</v>
+        <v>309</v>
+      </c>
+      <c r="J135" t="s">
+        <v>203</v>
+      </c>
+      <c r="K135" t="s">
+        <v>204</v>
+      </c>
+      <c r="L135" t="s">
+        <v>205</v>
       </c>
       <c r="M135" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4356,10 +4346,13 @@
         <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
       <c r="G136" t="s">
-        <v>354</v>
+        <v>359</v>
+      </c>
+      <c r="M136" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4367,36 +4360,24 @@
         <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
       <c r="G137" t="s">
-        <v>356</v>
+        <v>361</v>
+      </c>
+      <c r="M137" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A138" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>357</v>
-      </c>
-      <c r="C138" t="s">
-        <v>309</v>
-      </c>
-      <c r="D138" t="s">
-        <v>310</v>
-      </c>
-      <c r="J138" t="s">
-        <v>204</v>
-      </c>
-      <c r="K138" t="s">
-        <v>205</v>
-      </c>
-      <c r="L138" t="s">
-        <v>206</v>
-      </c>
-      <c r="M138" t="s">
-        <v>358</v>
+        <v>362</v>
+      </c>
+      <c r="G138" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4404,13 +4385,10 @@
         <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
       <c r="G139" t="s">
-        <v>360</v>
-      </c>
-      <c r="M139" t="s">
-        <v>165</v>
+        <v>365</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4418,13 +4396,13 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
       <c r="G140" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="M140" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4432,21 +4410,21 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="G141" t="s">
-        <v>364</v>
+        <v>369</v>
+      </c>
+      <c r="M141" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="B142" t="s">
-        <v>365</v>
-      </c>
-      <c r="G142" t="s">
-        <v>366</v>
+        <v>323</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4454,13 +4432,13 @@
         <v>17</v>
       </c>
       <c r="B143" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="G143" t="s">
-        <v>368</v>
+        <v>100</v>
       </c>
       <c r="M143" t="s">
-        <v>165</v>
+        <v>371</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4468,146 +4446,152 @@
         <v>17</v>
       </c>
       <c r="B144" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="G144" t="s">
-        <v>370</v>
+        <v>100</v>
       </c>
       <c r="M144" t="s">
-        <v>165</v>
+        <v>373</v>
       </c>
     </row>
     <row r="145" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B145" t="s">
-        <v>324</v>
+        <v>374</v>
+      </c>
+      <c r="C145" t="s">
+        <v>530</v>
+      </c>
+      <c r="D145" t="s">
+        <v>375</v>
+      </c>
+      <c r="E145" t="s">
+        <v>376</v>
+      </c>
+      <c r="F145" t="s">
+        <v>377</v>
+      </c>
+      <c r="M145" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
-        <v>17</v>
+        <v>379</v>
       </c>
       <c r="B146" t="s">
-        <v>371</v>
-      </c>
-      <c r="G146" t="s">
-        <v>101</v>
+        <v>380</v>
+      </c>
+      <c r="C146" t="s">
+        <v>381</v>
+      </c>
+      <c r="D146" t="s">
+        <v>382</v>
       </c>
       <c r="M146" t="s">
-        <v>372</v>
+        <v>378</v>
       </c>
     </row>
     <row r="147" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
-        <v>17</v>
+        <v>52</v>
       </c>
       <c r="B147" t="s">
-        <v>373</v>
-      </c>
-      <c r="G147" t="s">
-        <v>101</v>
+        <v>383</v>
+      </c>
+      <c r="C147" t="s">
+        <v>531</v>
+      </c>
+      <c r="D147" t="s">
+        <v>384</v>
+      </c>
+      <c r="E147" t="s">
+        <v>385</v>
+      </c>
+      <c r="F147" t="s">
+        <v>386</v>
       </c>
       <c r="M147" t="s">
-        <v>374</v>
+        <v>387</v>
       </c>
     </row>
     <row r="148" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
-        <v>52</v>
+        <v>388</v>
       </c>
       <c r="B148" t="s">
-        <v>375</v>
+        <v>389</v>
       </c>
       <c r="C148" t="s">
-        <v>546</v>
+        <v>390</v>
       </c>
       <c r="D148" t="s">
-        <v>376</v>
-      </c>
-      <c r="E148" t="s">
-        <v>377</v>
-      </c>
-      <c r="F148" t="s">
-        <v>378</v>
+        <v>391</v>
       </c>
       <c r="M148" t="s">
-        <v>379</v>
+        <v>387</v>
       </c>
     </row>
     <row r="149" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
-        <v>380</v>
+        <v>52</v>
       </c>
       <c r="B149" t="s">
-        <v>381</v>
+        <v>392</v>
       </c>
       <c r="C149" t="s">
-        <v>382</v>
+        <v>532</v>
       </c>
       <c r="D149" t="s">
-        <v>383</v>
+        <v>393</v>
       </c>
       <c r="M149" t="s">
-        <v>379</v>
+        <v>394</v>
       </c>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B150" t="s">
-        <v>384</v>
-      </c>
-      <c r="C150" t="s">
-        <v>547</v>
-      </c>
-      <c r="D150" t="s">
-        <v>385</v>
-      </c>
-      <c r="E150" t="s">
-        <v>386</v>
-      </c>
-      <c r="F150" t="s">
-        <v>387</v>
+        <v>395</v>
+      </c>
+      <c r="G150" t="s">
+        <v>100</v>
       </c>
       <c r="M150" t="s">
-        <v>388</v>
+        <v>396</v>
       </c>
     </row>
     <row r="151" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
-        <v>389</v>
+        <v>17</v>
       </c>
       <c r="B151" t="s">
-        <v>390</v>
-      </c>
-      <c r="C151" t="s">
-        <v>391</v>
-      </c>
-      <c r="D151" t="s">
-        <v>392</v>
+        <v>397</v>
+      </c>
+      <c r="G151" t="s">
+        <v>100</v>
       </c>
       <c r="M151" t="s">
-        <v>388</v>
+        <v>398</v>
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
-        <v>52</v>
+        <v>17</v>
       </c>
       <c r="B152" t="s">
-        <v>393</v>
-      </c>
-      <c r="C152" t="s">
-        <v>548</v>
-      </c>
-      <c r="D152" t="s">
-        <v>394</v>
+        <v>399</v>
+      </c>
+      <c r="G152" t="s">
+        <v>100</v>
       </c>
       <c r="M152" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4615,77 +4599,71 @@
         <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="G153" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="M153" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A154" t="s">
-        <v>17</v>
-      </c>
-      <c r="B154" t="s">
-        <v>398</v>
-      </c>
-      <c r="G154" t="s">
-        <v>101</v>
-      </c>
-      <c r="M154" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A155" t="s">
-        <v>17</v>
-      </c>
-      <c r="B155" t="s">
-        <v>400</v>
-      </c>
-      <c r="G155" t="s">
-        <v>101</v>
-      </c>
-      <c r="M155" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A156" t="s">
-        <v>17</v>
-      </c>
-      <c r="B156" t="s">
         <v>402</v>
       </c>
-      <c r="G156" t="s">
-        <v>101</v>
-      </c>
-      <c r="M156" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="157" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A157" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B157" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="159" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A159" s="1" t="s">
+    </row>
+    <row r="154" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="156" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A156" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>545</v>
-      </c>
-      <c r="N159" s="1" t="s">
-        <v>532</v>
+      <c r="B156" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="C156" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="N156" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="157" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A157" t="s">
+        <v>17</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="C157" s="4"/>
+      <c r="G157" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="158" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A158" t="s">
+        <v>17</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C158" s="4"/>
+      <c r="G158" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="159" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" t="s">
+        <v>17</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="C159" s="4"/>
+      <c r="G159" s="3" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="160" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4693,271 +4671,275 @@
         <v>17</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>533</v>
+        <v>545</v>
       </c>
       <c r="C160" s="4"/>
-      <c r="G160" t="s">
-        <v>113</v>
+      <c r="G160" s="3" t="s">
+        <v>549</v>
       </c>
     </row>
     <row r="161" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
-        <v>17</v>
-      </c>
-      <c r="B161" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B161" t="s">
+        <v>546</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M161" s="3" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B162" s="7" t="s">
         <v>534</v>
       </c>
-      <c r="C161" s="4"/>
-      <c r="G161" s="3" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="162" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A162" t="s">
-        <v>17</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="C162" s="4"/>
-      <c r="G162" s="3" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="163" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C162" s="7" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A163" t="s">
-        <v>17</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="C163" s="4"/>
-      <c r="G163" s="3" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="164" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>82</v>
+      </c>
+      <c r="B163" t="s">
+        <v>513</v>
+      </c>
+      <c r="C163" t="s">
+        <v>511</v>
+      </c>
+      <c r="D163" t="s">
+        <v>83</v>
+      </c>
+      <c r="H163" t="s">
+        <v>24</v>
+      </c>
+      <c r="M163" s="3" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B164" t="s">
-        <v>537</v>
-      </c>
-      <c r="C164" s="5" t="s">
-        <v>538</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>124</v>
+        <v>514</v>
+      </c>
+      <c r="C164" t="s">
+        <v>512</v>
+      </c>
+      <c r="D164" t="s">
+        <v>83</v>
+      </c>
+      <c r="H164" t="s">
+        <v>24</v>
       </c>
       <c r="M164" s="3" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
     </row>
     <row r="165" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A165" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B165" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
       <c r="J165" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="K165" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="M165" s="3" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
     </row>
     <row r="166" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A166" t="s">
+        <v>516</v>
+      </c>
+      <c r="B166" t="s">
+        <v>520</v>
+      </c>
+      <c r="C166" s="6" t="s">
+        <v>527</v>
+      </c>
+      <c r="J166" t="s">
         <v>522</v>
       </c>
-      <c r="B166" t="s">
-        <v>526</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>543</v>
-      </c>
-      <c r="J166" t="s">
-        <v>528</v>
-      </c>
       <c r="K166" t="s">
-        <v>529</v>
+        <v>523</v>
       </c>
       <c r="M166" s="3" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="167" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="B167" t="s">
-        <v>527</v>
+        <v>521</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>544</v>
+        <v>528</v>
       </c>
       <c r="J167" t="s">
-        <v>531</v>
+        <v>525</v>
       </c>
       <c r="K167" t="s">
-        <v>530</v>
+        <v>524</v>
       </c>
       <c r="M167" s="3" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="168" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B168" s="1" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="170" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A170" t="s">
-        <v>103</v>
-      </c>
-      <c r="B170" t="s">
-        <v>404</v>
-      </c>
-      <c r="C170" t="s">
-        <v>405</v>
-      </c>
-      <c r="D170" t="s">
-        <v>406</v>
-      </c>
-      <c r="E170" t="s">
-        <v>407</v>
-      </c>
-      <c r="F170" t="s">
-        <v>408</v>
+        <v>553</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="171" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
-        <v>409</v>
+        <v>102</v>
       </c>
       <c r="B171" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C171" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="D171" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="E171" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="F171" t="s">
-        <v>414</v>
-      </c>
-      <c r="H171" t="s">
-        <v>24</v>
-      </c>
-      <c r="M171" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
     </row>
     <row r="172" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="B172" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="C172" t="s">
+        <v>410</v>
+      </c>
+      <c r="D172" t="s">
         <v>411</v>
       </c>
-      <c r="D172" t="s">
+      <c r="E172" t="s">
         <v>412</v>
       </c>
-      <c r="E172" t="s">
+      <c r="F172" t="s">
         <v>413</v>
       </c>
-      <c r="F172" t="s">
+      <c r="H172" t="s">
+        <v>24</v>
+      </c>
+      <c r="M172" t="s">
         <v>414</v>
-      </c>
-      <c r="M172" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="173" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B173" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C173" t="s">
+        <v>410</v>
+      </c>
+      <c r="D173" t="s">
         <v>411</v>
       </c>
-      <c r="D173" t="s">
+      <c r="E173" t="s">
         <v>412</v>
       </c>
-      <c r="H173" t="s">
-        <v>24</v>
+      <c r="F173" t="s">
+        <v>413</v>
       </c>
       <c r="M173" t="s">
-        <v>420</v>
+        <v>56</v>
       </c>
     </row>
     <row r="174" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>52</v>
+        <v>417</v>
       </c>
       <c r="B174" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C174" t="s">
-        <v>422</v>
+        <v>410</v>
       </c>
       <c r="D174" t="s">
-        <v>423</v>
+        <v>411</v>
+      </c>
+      <c r="H174" t="s">
+        <v>24</v>
       </c>
       <c r="M174" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
     </row>
     <row r="175" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B175" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="C175" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D175" t="s">
-        <v>427</v>
+        <v>422</v>
+      </c>
+      <c r="M175" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="176" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
+        <v>20</v>
+      </c>
+      <c r="B176" t="s">
+        <v>424</v>
+      </c>
+      <c r="C176" t="s">
+        <v>425</v>
+      </c>
+      <c r="D176" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="177" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" t="s">
         <v>45</v>
       </c>
-      <c r="B176" t="s">
+      <c r="B177" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A183" t="s">
-        <v>17</v>
-      </c>
-      <c r="B183" t="s">
-        <v>428</v>
-      </c>
-      <c r="G183" t="s">
-        <v>429</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4965,10 +4947,10 @@
         <v>17</v>
       </c>
       <c r="B184" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="G184" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4976,10 +4958,10 @@
         <v>17</v>
       </c>
       <c r="B185" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="G185" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4987,10 +4969,10 @@
         <v>17</v>
       </c>
       <c r="B186" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="G186" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -4998,10 +4980,10 @@
         <v>17</v>
       </c>
       <c r="B187" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="G187" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5009,10 +4991,21 @@
         <v>17</v>
       </c>
       <c r="B188" t="s">
+        <v>435</v>
+      </c>
+      <c r="G188" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A189" t="s">
+        <v>17</v>
+      </c>
+      <c r="B189" t="s">
+        <v>437</v>
+      </c>
+      <c r="G189" t="s">
         <v>438</v>
-      </c>
-      <c r="G188" t="s">
-        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -5036,7 +5029,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5050,41 +5043,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C2" t="s">
+        <v>440</v>
+      </c>
+      <c r="D2" t="s">
         <v>441</v>
-      </c>
-      <c r="D2" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
+        <v>442</v>
+      </c>
+      <c r="C3" t="s">
         <v>443</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>444</v>
-      </c>
-      <c r="D3" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C4" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5092,13 +5085,13 @@
         <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C5" t="s">
+        <v>446</v>
+      </c>
+      <c r="D5" t="s">
         <v>447</v>
-      </c>
-      <c r="D5" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5106,13 +5099,13 @@
         <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C6" t="s">
+        <v>448</v>
+      </c>
+      <c r="D6" t="s">
         <v>449</v>
-      </c>
-      <c r="D6" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5120,335 +5113,335 @@
         <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C7" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="D7" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
+        <v>453</v>
+      </c>
+      <c r="B8" t="s">
         <v>454</v>
       </c>
-      <c r="B8" t="s">
-        <v>455</v>
-      </c>
       <c r="C8" t="s">
+        <v>446</v>
+      </c>
+      <c r="D8" t="s">
         <v>447</v>
-      </c>
-      <c r="D8" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B9" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C9" t="s">
+        <v>448</v>
+      </c>
+      <c r="D9" t="s">
         <v>449</v>
-      </c>
-      <c r="D9" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
+        <v>456</v>
+      </c>
+      <c r="B10" t="s">
         <v>457</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>458</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>459</v>
-      </c>
-      <c r="D10" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B11" t="s">
+        <v>460</v>
+      </c>
+      <c r="C11" t="s">
         <v>461</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>462</v>
-      </c>
-      <c r="D11" t="s">
-        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
+        <v>463</v>
+      </c>
+      <c r="B12" t="s">
         <v>464</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>465</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>466</v>
-      </c>
-      <c r="D12" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B13" t="s">
+        <v>467</v>
+      </c>
+      <c r="C13" t="s">
         <v>468</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>469</v>
-      </c>
-      <c r="D13" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C14" t="s">
+        <v>470</v>
+      </c>
+      <c r="D14" t="s">
         <v>471</v>
-      </c>
-      <c r="D14" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C15" t="s">
+        <v>472</v>
+      </c>
+      <c r="D15" t="s">
         <v>473</v>
-      </c>
-      <c r="D15" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C16" t="s">
+        <v>474</v>
+      </c>
+      <c r="D16" t="s">
         <v>475</v>
-      </c>
-      <c r="D16" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C17" t="s">
+        <v>451</v>
+      </c>
+      <c r="D17" t="s">
         <v>452</v>
-      </c>
-      <c r="D17" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C18" t="s">
+        <v>446</v>
+      </c>
+      <c r="D18" t="s">
         <v>447</v>
-      </c>
-      <c r="D18" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
+        <v>477</v>
+      </c>
+      <c r="B19" t="s">
+        <v>442</v>
+      </c>
+      <c r="C19" t="s">
         <v>478</v>
       </c>
-      <c r="B19" t="s">
-        <v>443</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>479</v>
-      </c>
-      <c r="D19" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B20" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C20" t="s">
+        <v>480</v>
+      </c>
+      <c r="D20" t="s">
         <v>481</v>
-      </c>
-      <c r="D20" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C21" t="s">
+        <v>446</v>
+      </c>
+      <c r="D21" t="s">
         <v>447</v>
-      </c>
-      <c r="D21" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
+        <v>482</v>
+      </c>
+      <c r="B22" t="s">
+        <v>442</v>
+      </c>
+      <c r="C22" t="s">
         <v>483</v>
       </c>
-      <c r="B22" t="s">
-        <v>443</v>
-      </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>484</v>
-      </c>
-      <c r="D22" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B23" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C23" t="s">
+        <v>485</v>
+      </c>
+      <c r="D23" t="s">
         <v>486</v>
-      </c>
-      <c r="D23" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>487</v>
+      </c>
+      <c r="B24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C24" t="s">
         <v>488</v>
       </c>
-      <c r="B24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>489</v>
-      </c>
-      <c r="D24" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B25" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C25" t="s">
+        <v>490</v>
+      </c>
+      <c r="D25" t="s">
         <v>491</v>
-      </c>
-      <c r="D25" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
+        <v>492</v>
+      </c>
+      <c r="B26" t="s">
+        <v>476</v>
+      </c>
+      <c r="C26" t="s">
         <v>493</v>
       </c>
-      <c r="B26" t="s">
-        <v>477</v>
-      </c>
-      <c r="C26" t="s">
-        <v>494</v>
-      </c>
       <c r="D26" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B27" t="s">
+        <v>494</v>
+      </c>
+      <c r="C27" t="s">
         <v>495</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>496</v>
-      </c>
-      <c r="D27" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
+        <v>497</v>
+      </c>
+      <c r="B28" t="s">
+        <v>450</v>
+      </c>
+      <c r="C28" t="s">
         <v>498</v>
       </c>
-      <c r="B28" t="s">
-        <v>451</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>499</v>
-      </c>
-      <c r="D28" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
+        <v>446</v>
+      </c>
+      <c r="D29" t="s">
         <v>447</v>
-      </c>
-      <c r="D29" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
+        <v>500</v>
+      </c>
+      <c r="B30" t="s">
         <v>501</v>
       </c>
-      <c r="B30" t="s">
-        <v>502</v>
-      </c>
       <c r="C30" t="s">
+        <v>448</v>
+      </c>
+      <c r="D30" t="s">
         <v>449</v>
-      </c>
-      <c r="D30" t="s">
-        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -5466,30 +5459,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>502</v>
+      </c>
+      <c r="B1" t="s">
         <v>503</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>504</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>505</v>
-      </c>
-      <c r="D1" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>506</v>
+      </c>
+      <c r="B2" t="s">
         <v>507</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>508</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>509</v>
-      </c>
-      <c r="D2" t="s">
-        <v>510</v>
       </c>
     </row>
   </sheetData>
@@ -5498,144 +5491,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6074,53 +5929,145 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6141,4 +6088,50 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
corrected age range of is_woman and HGT WGT contraint
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rojohnston\OneDrive - UNICEF\1 UNICEF Work\1 Afghanistan\Surveys\UrbanSMART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A840712-88ED-4A15-9988-5F68AA980E7B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1AB3C9-F10B-4512-9AF0-40E042238A02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="913" uniqueCount="554">
   <si>
     <t>type</t>
   </si>
@@ -1784,15 +1784,6 @@
     <t xml:space="preserve">(. &gt;= 25 and . &lt;200) </t>
   </si>
   <si>
-    <t>Woman's MUAC in MM of (${plw_name})</t>
-  </si>
-  <si>
-    <t>Woman's HEIGHT in CM of (${plw_name})</t>
-  </si>
-  <si>
-    <t>Woman's WEIGHT in KG of (${plw_name})</t>
-  </si>
-  <si>
     <t>Pregnant &amp; Lactating Woman section</t>
   </si>
   <si>
@@ -1814,9 +1805,6 @@
     <t>is_woman</t>
   </si>
   <si>
-    <t>if(${age_years} &gt;=15 and ${age_years} &lt;=49 and ${sex}= 'f',true(),false())</t>
-  </si>
-  <si>
     <t>women</t>
   </si>
   <si>
@@ -1862,16 +1850,22 @@
     <t>${curr_pregnant}=1 or ${curr_breastfeed}=1</t>
   </si>
   <si>
-    <t>${curr_pregnant}=1 or ${curr_breastfeed}=2</t>
-  </si>
-  <si>
-    <t>${curr_pregnant}=1 or ${curr_breastfeed}=3</t>
-  </si>
-  <si>
     <t>number(selected-at(${women}, ${wom_selected_position}))</t>
   </si>
   <si>
     <t>woman-${wom_selected_position} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
+  </si>
+  <si>
+    <t>Woman's HEIGHT in CM of (${wom_name})</t>
+  </si>
+  <si>
+    <t>Woman's MUAC in MM of (${wom_name})</t>
+  </si>
+  <si>
+    <t>Woman's WEIGHT in KG of (${wom_name})</t>
+  </si>
+  <si>
+    <t>if(${age_years} &gt;14 and ${age_years} &lt;50 and ${sex}= 'f',true(),false())</t>
   </si>
 </sst>
 </file>
@@ -2282,11 +2276,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N189"/>
+  <dimension ref="A1:N184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A162" sqref="A162:XFD162"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B191" sqref="B191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2711,10 +2705,10 @@
         <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>536</v>
+        <v>553</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2818,10 +2812,10 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2829,10 +2823,10 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -4463,7 +4457,7 @@
         <v>374</v>
       </c>
       <c r="C145" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="D145" t="s">
         <v>375</v>
@@ -4503,7 +4497,7 @@
         <v>383</v>
       </c>
       <c r="C147" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="D147" t="s">
         <v>384</v>
@@ -4543,7 +4537,7 @@
         <v>392</v>
       </c>
       <c r="C149" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="D149" t="s">
         <v>393</v>
@@ -4624,10 +4618,10 @@
         <v>515</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="N156" s="1" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="157" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4635,7 +4629,7 @@
         <v>17</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="C157" s="4"/>
       <c r="G157" t="s">
@@ -4647,11 +4641,11 @@
         <v>17</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C158" s="4"/>
       <c r="G158" s="3" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
     </row>
     <row r="159" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4659,11 +4653,11 @@
         <v>17</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C159" s="4"/>
       <c r="G159" s="3" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
     </row>
     <row r="160" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4671,11 +4665,11 @@
         <v>17</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C160" s="4"/>
       <c r="G160" s="3" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="161" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4683,16 +4677,16 @@
         <v>52</v>
       </c>
       <c r="B161" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C161" s="5" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="D161" s="3" t="s">
         <v>123</v>
       </c>
       <c r="M161" s="3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="162" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4700,10 +4694,10 @@
         <v>52</v>
       </c>
       <c r="B162" s="7" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C162" s="7" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
     </row>
     <row r="163" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4723,7 +4717,7 @@
         <v>24</v>
       </c>
       <c r="M163" s="3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="164" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4743,7 +4737,7 @@
         <v>24</v>
       </c>
       <c r="M164" s="3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="165" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4754,7 +4748,7 @@
         <v>517</v>
       </c>
       <c r="C165" s="6" t="s">
-        <v>526</v>
+        <v>551</v>
       </c>
       <c r="J165" t="s">
         <v>518</v>
@@ -4763,7 +4757,7 @@
         <v>519</v>
       </c>
       <c r="M165" s="3" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
     </row>
     <row r="166" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4774,7 +4768,7 @@
         <v>520</v>
       </c>
       <c r="C166" s="6" t="s">
-        <v>527</v>
+        <v>550</v>
       </c>
       <c r="J166" t="s">
         <v>522</v>
@@ -4783,7 +4777,7 @@
         <v>523</v>
       </c>
       <c r="M166" s="3" t="s">
-        <v>552</v>
+        <v>547</v>
       </c>
     </row>
     <row r="167" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4794,7 +4788,7 @@
         <v>521</v>
       </c>
       <c r="C167" s="6" t="s">
-        <v>528</v>
+        <v>552</v>
       </c>
       <c r="J167" t="s">
         <v>525</v>
@@ -4803,7 +4797,7 @@
         <v>524</v>
       </c>
       <c r="M167" s="3" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
     </row>
     <row r="169" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4942,69 +4936,69 @@
         <v>46</v>
       </c>
     </row>
+    <row r="179" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" t="s">
+        <v>17</v>
+      </c>
+      <c r="B179" t="s">
+        <v>427</v>
+      </c>
+      <c r="G179" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" t="s">
+        <v>17</v>
+      </c>
+      <c r="B180" t="s">
+        <v>429</v>
+      </c>
+      <c r="G180" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="181" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" t="s">
+        <v>17</v>
+      </c>
+      <c r="B181" t="s">
+        <v>431</v>
+      </c>
+      <c r="G181" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" t="s">
+        <v>17</v>
+      </c>
+      <c r="B182" t="s">
+        <v>433</v>
+      </c>
+      <c r="G182" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A183" t="s">
+        <v>17</v>
+      </c>
+      <c r="B183" t="s">
+        <v>435</v>
+      </c>
+      <c r="G183" t="s">
+        <v>436</v>
+      </c>
+    </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
         <v>17</v>
       </c>
       <c r="B184" t="s">
-        <v>427</v>
+        <v>437</v>
       </c>
       <c r="G184" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="185" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A185" t="s">
-        <v>17</v>
-      </c>
-      <c r="B185" t="s">
-        <v>429</v>
-      </c>
-      <c r="G185" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A186" t="s">
-        <v>17</v>
-      </c>
-      <c r="B186" t="s">
-        <v>431</v>
-      </c>
-      <c r="G186" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A187" t="s">
-        <v>17</v>
-      </c>
-      <c r="B187" t="s">
-        <v>433</v>
-      </c>
-      <c r="G187" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="188" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A188" t="s">
-        <v>17</v>
-      </c>
-      <c r="B188" t="s">
-        <v>435</v>
-      </c>
-      <c r="G188" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="189" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A189" t="s">
-        <v>17</v>
-      </c>
-      <c r="B189" t="s">
-        <v>437</v>
-      </c>
-      <c r="G189" t="s">
         <v>438</v>
       </c>
     </row>
@@ -5116,7 +5110,7 @@
         <v>450</v>
       </c>
       <c r="C7" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="D7" t="s">
         <v>452</v>
@@ -5491,6 +5485,70 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -5929,7 +5987,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
   <xsnLocation/>
@@ -5939,12 +5997,12 @@
 </customXsn>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -5994,7 +6052,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6003,71 +6061,21 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6090,7 +6098,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
@@ -6098,7 +6106,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -6106,7 +6114,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -6114,24 +6122,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
error in french province
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rojohnston\OneDrive - UNICEF\1 UNICEF Work\1 Afghanistan\Surveys\UrbanSMART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3C225A-320A-4D14-9158-DDFC3E9321CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD4C0B15-AA6A-4989-B1C9-9420D380D2E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -166,12 +166,6 @@
   </si>
   <si>
     <t>consent</t>
-  </si>
-  <si>
-    <t>Hello my name is ________.   I am with ________ [organization/governmental agency]. Please let me introduce you to the other team members: _________ and _______.   We are here today to gather household information related to nutrition and ________.  If there are any children under 5 in the household we would like to take some measurements (weight, height, MUAC, oedema / explain) to help determine the overall under 5 nutrition status in ${region} region, district of ${district}.  Please note that it is not currently known what actions (if any) will be taken after the results of the survey are finalized. All information will be kept completely confidential.  Do you have any questions? May I begin?</t>
-  </si>
-  <si>
-    <t>Bonjour, mon nom est ________. Je travaille pour ________ [organisation / agence gouvernementale]. Permettez-moi de vous présenter les autres membres de l'équipe: _________ et _______. Nous sommes ici aujourd'hui pour recueillir des informations liées à la nutrition et à ________ des ménages. Si vous avez des enfants de moins de 5 ans dans le ménage, nous aimerions prendre quelques mesures (poids, taille, PB, œdème /expliquer). Cela nous aidera à déterminer l'état nutritionnel global des enfants de moins de 5 ans dans la région de ${region} et le district de ${district}. Nous ne savons pas actuellement si d'éventuelles mesures seront prises une fois les résultats de l'enquête finalisés. Toutes les informations collectées resteront confidentielles. Avez-vous des questions? Puis-je commencer?</t>
   </si>
   <si>
     <t>note</t>
@@ -2019,6 +2013,12 @@
   </si>
   <si>
     <t>34</t>
+  </si>
+  <si>
+    <t>Hello my name is ________.   I am with ________ [organization/governmental agency]. Please let me introduce you to the other team members: _________ and _______.   We are here today to gather household information related to nutrition and ________.  If there are any children under 5 in the household we would like to take some measurements (weight, height, MUAC, oedema / explain) to help determine the overall under 5 nutrition status in ${province} province, district of ${district}.  Please note that it is not currently known what actions (if any) will be taken after the results of the survey are finalized. All information will be kept completely confidential.  Do you have any questions? May I begin?</t>
+  </si>
+  <si>
+    <t>Bonjour, mon nom est ________. Je travaille pour ________ [organisation / agence gouvernementale]. Permettez-moi de vous présenter les autres membres de l'équipe: _________ et _______. Nous sommes ici aujourd'hui pour recueillir des informations liées à la nutrition et à ________ des ménages. Si vous avez des enfants de moins de 5 ans dans le ménage, nous aimerions prendre quelques mesures (poids, taille, PB, œdème /expliquer). Cela nous aidera à déterminer l'état nutritionnel global des enfants de moins de 5 ans dans la province de ${province} et le district de ${district}. Nous ne savons pas actuellement si d'éventuelles mesures seront prises une fois les résultats de l'enquête finalisés. Toutes les informations collectées resteront confidentielles. Avez-vous des questions? Puis-je commencer?</t>
   </si>
 </sst>
 </file>
@@ -2431,9 +2431,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N192"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2527,13 +2527,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>566</v>
+      </c>
+      <c r="B6" t="s">
+        <v>567</v>
+      </c>
+      <c r="C6" t="s">
         <v>568</v>
-      </c>
-      <c r="B6" t="s">
-        <v>569</v>
-      </c>
-      <c r="C6" t="s">
-        <v>570</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
@@ -2680,10 +2680,10 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>603</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>604</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2691,19 +2691,19 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
         <v>50</v>
       </c>
-      <c r="B18" t="s">
+      <c r="D18" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
+      <c r="M18" t="s">
         <v>52</v>
-      </c>
-      <c r="D18" t="s">
-        <v>53</v>
-      </c>
-      <c r="M18" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2714,47 +2714,47 @@
         <v>45</v>
       </c>
       <c r="M19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>57</v>
       </c>
-      <c r="D20" t="s">
+      <c r="F20" t="s">
         <v>58</v>
       </c>
-      <c r="E20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" t="s">
-        <v>60</v>
-      </c>
       <c r="M20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" t="s">
+      <c r="D21" t="s">
         <v>62</v>
       </c>
-      <c r="C21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
       <c r="M21" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2762,7 +2762,7 @@
         <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I22" t="s">
         <v>27</v>
@@ -2776,10 +2776,10 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H23" t="s">
         <v>22</v>
@@ -2787,16 +2787,16 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
         <v>69</v>
-      </c>
-      <c r="C24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" t="s">
-        <v>71</v>
       </c>
       <c r="H24" t="s">
         <v>22</v>
@@ -2807,31 +2807,31 @@
         <v>30</v>
       </c>
       <c r="B25" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" t="s">
         <v>72</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>73</v>
       </c>
-      <c r="D25" t="s">
+      <c r="F25" t="s">
         <v>74</v>
-      </c>
-      <c r="E25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F25" t="s">
-        <v>76</v>
       </c>
       <c r="H25" t="s">
         <v>22</v>
       </c>
       <c r="J25" t="s">
+        <v>75</v>
+      </c>
+      <c r="K25" t="s">
+        <v>76</v>
+      </c>
+      <c r="L25" t="s">
         <v>77</v>
-      </c>
-      <c r="K25" t="s">
-        <v>78</v>
-      </c>
-      <c r="L25" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2839,7 +2839,7 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2847,10 +2847,10 @@
         <v>17</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2858,10 +2858,10 @@
         <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2869,19 +2869,19 @@
         <v>17</v>
       </c>
       <c r="B32" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C32" s="3"/>
       <c r="G32" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B33" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2889,30 +2889,30 @@
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G34" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B35" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" t="s">
         <v>89</v>
-      </c>
-      <c r="C35" t="s">
-        <v>90</v>
-      </c>
-      <c r="D35" t="s">
-        <v>91</v>
       </c>
       <c r="H35" t="s">
         <v>22</v>
       </c>
       <c r="M35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -2920,22 +2920,22 @@
         <v>30</v>
       </c>
       <c r="B36" t="s">
+        <v>90</v>
+      </c>
+      <c r="C36" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" t="s">
         <v>92</v>
       </c>
-      <c r="C36" t="s">
+      <c r="E36" t="s">
         <v>93</v>
       </c>
-      <c r="D36" t="s">
+      <c r="F36" t="s">
         <v>94</v>
       </c>
-      <c r="E36" t="s">
+      <c r="M36" t="s">
         <v>95</v>
-      </c>
-      <c r="F36" t="s">
-        <v>96</v>
-      </c>
-      <c r="M36" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="38" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2943,10 +2943,10 @@
         <v>17</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2954,10 +2954,10 @@
         <v>17</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2965,10 +2965,10 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>529</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2976,28 +2976,28 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>530</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="43" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="N43" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="N43" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3005,10 +3005,10 @@
         <v>17</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G44" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3016,10 +3016,10 @@
         <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G45" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3027,10 +3027,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G46" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3038,10 +3038,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G47" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3049,27 +3049,27 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G48" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" t="s">
+        <v>118</v>
+      </c>
+      <c r="D49" t="s">
         <v>119</v>
       </c>
-      <c r="C49" t="s">
+      <c r="M49" t="s">
         <v>120</v>
-      </c>
-      <c r="D49" t="s">
-        <v>121</v>
-      </c>
-      <c r="M49" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3077,30 +3077,30 @@
         <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M50" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B51" t="s">
+        <v>122</v>
+      </c>
+      <c r="C51" t="s">
+        <v>123</v>
+      </c>
+      <c r="D51" t="s">
         <v>124</v>
       </c>
-      <c r="C51" t="s">
+      <c r="E51" t="s">
         <v>125</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
         <v>126</v>
-      </c>
-      <c r="E51" t="s">
-        <v>127</v>
-      </c>
-      <c r="F51" t="s">
-        <v>128</v>
       </c>
       <c r="H51" t="s">
         <v>22</v>
@@ -3111,28 +3111,28 @@
         <v>28</v>
       </c>
       <c r="B52" t="s">
+        <v>127</v>
+      </c>
+      <c r="C52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D52" t="s">
         <v>129</v>
       </c>
-      <c r="C52" t="s">
+      <c r="E52" t="s">
         <v>130</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
         <v>131</v>
-      </c>
-      <c r="E52" t="s">
-        <v>132</v>
-      </c>
-      <c r="F52" t="s">
-        <v>133</v>
       </c>
       <c r="I52" t="s">
         <v>29</v>
       </c>
       <c r="J52" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M52" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3140,31 +3140,31 @@
         <v>30</v>
       </c>
       <c r="B53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" t="s">
         <v>136</v>
       </c>
-      <c r="C53" t="s">
+      <c r="E53" t="s">
         <v>137</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
         <v>138</v>
       </c>
-      <c r="E53" t="s">
+      <c r="J53" t="s">
         <v>139</v>
       </c>
-      <c r="F53" t="s">
+      <c r="K53" t="s">
         <v>140</v>
       </c>
-      <c r="J53" t="s">
+      <c r="L53" t="s">
         <v>141</v>
       </c>
-      <c r="K53" t="s">
+      <c r="M53" t="s">
         <v>142</v>
-      </c>
-      <c r="L53" t="s">
-        <v>143</v>
-      </c>
-      <c r="M53" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3172,13 +3172,13 @@
         <v>17</v>
       </c>
       <c r="B54" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G54" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="M54" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3186,64 +3186,64 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G55" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B56" t="s">
+        <v>147</v>
+      </c>
+      <c r="C56" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" t="s">
         <v>149</v>
       </c>
-      <c r="C56" t="s">
+      <c r="M56" t="s">
         <v>150</v>
-      </c>
-      <c r="D56" t="s">
-        <v>151</v>
-      </c>
-      <c r="M56" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B57" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" t="s">
         <v>153</v>
       </c>
-      <c r="C57" t="s">
+      <c r="M57" t="s">
         <v>154</v>
-      </c>
-      <c r="D57" t="s">
-        <v>155</v>
-      </c>
-      <c r="M57" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C58" t="s">
+        <v>156</v>
+      </c>
+      <c r="D58" t="s">
         <v>157</v>
-      </c>
-      <c r="C58" t="s">
-        <v>158</v>
-      </c>
-      <c r="D58" t="s">
-        <v>159</v>
       </c>
       <c r="H58" t="s">
         <v>22</v>
       </c>
       <c r="M58" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3251,136 +3251,136 @@
         <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="M59" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" t="s">
+        <v>162</v>
+      </c>
+      <c r="C60" t="s">
         <v>163</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
         <v>164</v>
       </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>165</v>
       </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
         <v>166</v>
       </c>
-      <c r="E60" t="s">
+      <c r="J60" t="s">
         <v>167</v>
       </c>
-      <c r="F60" t="s">
+      <c r="K60" t="s">
         <v>168</v>
       </c>
-      <c r="J60" t="s">
+      <c r="L60" t="s">
         <v>169</v>
-      </c>
-      <c r="K60" t="s">
-        <v>170</v>
-      </c>
-      <c r="L60" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>170</v>
+      </c>
+      <c r="B61" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" t="s">
         <v>172</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
         <v>173</v>
       </c>
-      <c r="C61" t="s">
+      <c r="M61" t="s">
         <v>174</v>
-      </c>
-      <c r="D61" t="s">
-        <v>175</v>
-      </c>
-      <c r="M61" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B62" t="s">
+        <v>175</v>
+      </c>
+      <c r="C62" t="s">
+        <v>176</v>
+      </c>
+      <c r="D62" t="s">
         <v>177</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E62" t="s">
         <v>178</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
         <v>179</v>
       </c>
-      <c r="E62" t="s">
+      <c r="J62" t="s">
         <v>180</v>
       </c>
-      <c r="F62" t="s">
+      <c r="K62" t="s">
         <v>181</v>
       </c>
-      <c r="J62" t="s">
+      <c r="L62" t="s">
         <v>182</v>
-      </c>
-      <c r="K62" t="s">
-        <v>183</v>
-      </c>
-      <c r="L62" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" t="s">
+        <v>184</v>
+      </c>
+      <c r="C63" t="s">
         <v>185</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>186</v>
       </c>
-      <c r="C63" t="s">
+      <c r="M63" t="s">
         <v>187</v>
-      </c>
-      <c r="D63" t="s">
-        <v>188</v>
-      </c>
-      <c r="M63" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B64" t="s">
+        <v>188</v>
+      </c>
+      <c r="C64" t="s">
+        <v>189</v>
+      </c>
+      <c r="D64" t="s">
         <v>190</v>
       </c>
-      <c r="C64" t="s">
+      <c r="M64" t="s">
         <v>191</v>
-      </c>
-      <c r="D64" t="s">
-        <v>192</v>
-      </c>
-      <c r="M64" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B65" t="s">
+        <v>192</v>
+      </c>
+      <c r="C65" t="s">
+        <v>193</v>
+      </c>
+      <c r="D65" t="s">
         <v>194</v>
       </c>
-      <c r="C65" t="s">
+      <c r="M65" t="s">
         <v>195</v>
-      </c>
-      <c r="D65" t="s">
-        <v>196</v>
-      </c>
-      <c r="M65" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3388,59 +3388,59 @@
         <v>30</v>
       </c>
       <c r="B66" t="s">
+        <v>196</v>
+      </c>
+      <c r="C66" t="s">
+        <v>197</v>
+      </c>
+      <c r="D66" t="s">
         <v>198</v>
       </c>
-      <c r="C66" t="s">
+      <c r="J66" t="s">
         <v>199</v>
       </c>
-      <c r="D66" t="s">
+      <c r="K66" t="s">
         <v>200</v>
       </c>
-      <c r="J66" t="s">
+      <c r="L66" t="s">
         <v>201</v>
       </c>
-      <c r="K66" t="s">
+      <c r="M66" t="s">
         <v>202</v>
-      </c>
-      <c r="L66" t="s">
-        <v>203</v>
-      </c>
-      <c r="M66" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B67" t="s">
+        <v>203</v>
+      </c>
+      <c r="C67" t="s">
+        <v>204</v>
+      </c>
+      <c r="D67" t="s">
         <v>205</v>
-      </c>
-      <c r="C67" t="s">
-        <v>206</v>
-      </c>
-      <c r="D67" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B68" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68" t="s">
+        <v>207</v>
+      </c>
+      <c r="D68" t="s">
         <v>208</v>
-      </c>
-      <c r="C68" t="s">
-        <v>209</v>
-      </c>
-      <c r="D68" t="s">
-        <v>210</v>
       </c>
       <c r="H68" t="s">
         <v>22</v>
       </c>
       <c r="M68" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3448,7 +3448,7 @@
         <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3456,7 +3456,7 @@
         <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3464,10 +3464,10 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G71" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3475,10 +3475,10 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G72" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3486,10 +3486,10 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G73" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3497,10 +3497,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G74" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3508,13 +3508,13 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
+        <v>217</v>
+      </c>
+      <c r="G75" t="s">
+        <v>218</v>
+      </c>
+      <c r="M75" t="s">
         <v>219</v>
-      </c>
-      <c r="G75" t="s">
-        <v>220</v>
-      </c>
-      <c r="M75" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3522,13 +3522,13 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G76" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M76" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3536,10 +3536,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G77" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3547,13 +3547,13 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G78" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M78" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3561,13 +3561,13 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G79" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M79" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3575,10 +3575,10 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G80" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3586,13 +3586,13 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G81" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M81" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3600,13 +3600,13 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G82" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M82" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3614,10 +3614,10 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G83" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3625,10 +3625,10 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G84" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3636,13 +3636,13 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G85" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="M85" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3650,13 +3650,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G86" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M86" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3664,10 +3664,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G87" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3675,10 +3675,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G88" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3686,13 +3686,13 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G89" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="M89" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3700,13 +3700,13 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G90" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M90" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3714,13 +3714,13 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G91" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M91" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="92" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3729,44 +3729,44 @@
         <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="M93" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B94" t="s">
+        <v>254</v>
+      </c>
+      <c r="C94" t="s">
+        <v>255</v>
+      </c>
+      <c r="D94" t="s">
         <v>256</v>
-      </c>
-      <c r="C94" t="s">
-        <v>257</v>
-      </c>
-      <c r="D94" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B95" t="s">
+        <v>257</v>
+      </c>
+      <c r="C95" t="s">
+        <v>258</v>
+      </c>
+      <c r="D95" t="s">
         <v>259</v>
       </c>
-      <c r="C95" t="s">
-        <v>260</v>
-      </c>
-      <c r="D95" t="s">
-        <v>261</v>
-      </c>
       <c r="E95" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F95" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3774,28 +3774,28 @@
         <v>28</v>
       </c>
       <c r="B96" t="s">
+        <v>260</v>
+      </c>
+      <c r="C96" t="s">
+        <v>261</v>
+      </c>
+      <c r="D96" t="s">
         <v>262</v>
       </c>
-      <c r="C96" t="s">
-        <v>263</v>
-      </c>
-      <c r="D96" t="s">
-        <v>264</v>
-      </c>
       <c r="E96" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F96" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I96" t="s">
         <v>29</v>
       </c>
       <c r="J96" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M96" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3803,31 +3803,31 @@
         <v>30</v>
       </c>
       <c r="B97" t="s">
+        <v>264</v>
+      </c>
+      <c r="C97" t="s">
+        <v>265</v>
+      </c>
+      <c r="D97" t="s">
         <v>266</v>
       </c>
-      <c r="C97" t="s">
+      <c r="E97" t="s">
+        <v>137</v>
+      </c>
+      <c r="F97" t="s">
+        <v>138</v>
+      </c>
+      <c r="J97" t="s">
         <v>267</v>
       </c>
-      <c r="D97" t="s">
+      <c r="K97" t="s">
+        <v>140</v>
+      </c>
+      <c r="L97" t="s">
+        <v>141</v>
+      </c>
+      <c r="M97" t="s">
         <v>268</v>
-      </c>
-      <c r="E97" t="s">
-        <v>139</v>
-      </c>
-      <c r="F97" t="s">
-        <v>140</v>
-      </c>
-      <c r="J97" t="s">
-        <v>269</v>
-      </c>
-      <c r="K97" t="s">
-        <v>142</v>
-      </c>
-      <c r="L97" t="s">
-        <v>143</v>
-      </c>
-      <c r="M97" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3835,13 +3835,13 @@
         <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="G98" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="M98" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3849,170 +3849,170 @@
         <v>17</v>
       </c>
       <c r="B99" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G99" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B100" t="s">
+        <v>273</v>
+      </c>
+      <c r="C100" t="s">
+        <v>274</v>
+      </c>
+      <c r="D100" t="s">
         <v>275</v>
       </c>
-      <c r="C100" t="s">
+      <c r="M100" t="s">
         <v>276</v>
-      </c>
-      <c r="D100" t="s">
-        <v>277</v>
-      </c>
-      <c r="M100" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B101" t="s">
+        <v>277</v>
+      </c>
+      <c r="C101" t="s">
+        <v>278</v>
+      </c>
+      <c r="D101" t="s">
         <v>279</v>
       </c>
-      <c r="C101" t="s">
+      <c r="M101" t="s">
         <v>280</v>
-      </c>
-      <c r="D101" t="s">
-        <v>281</v>
-      </c>
-      <c r="M101" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B102" t="s">
+        <v>281</v>
+      </c>
+      <c r="C102" t="s">
+        <v>282</v>
+      </c>
+      <c r="D102" t="s">
         <v>283</v>
       </c>
-      <c r="C102" t="s">
-        <v>284</v>
-      </c>
-      <c r="D102" t="s">
-        <v>285</v>
-      </c>
       <c r="E102" t="s">
+        <v>165</v>
+      </c>
+      <c r="F102" t="s">
+        <v>166</v>
+      </c>
+      <c r="J102" t="s">
         <v>167</v>
       </c>
-      <c r="F102" t="s">
+      <c r="K102" t="s">
         <v>168</v>
       </c>
-      <c r="J102" t="s">
+      <c r="L102" t="s">
         <v>169</v>
-      </c>
-      <c r="K102" t="s">
-        <v>170</v>
-      </c>
-      <c r="L102" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B103" t="s">
+        <v>284</v>
+      </c>
+      <c r="C103" t="s">
+        <v>285</v>
+      </c>
+      <c r="D103" t="s">
         <v>286</v>
       </c>
-      <c r="C103" t="s">
+      <c r="M103" t="s">
         <v>287</v>
-      </c>
-      <c r="D103" t="s">
-        <v>288</v>
-      </c>
-      <c r="M103" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B104" t="s">
+        <v>288</v>
+      </c>
+      <c r="C104" t="s">
+        <v>289</v>
+      </c>
+      <c r="D104" t="s">
         <v>290</v>
       </c>
-      <c r="C104" t="s">
-        <v>291</v>
-      </c>
-      <c r="D104" t="s">
-        <v>292</v>
-      </c>
       <c r="E104" t="s">
+        <v>178</v>
+      </c>
+      <c r="F104" t="s">
+        <v>179</v>
+      </c>
+      <c r="J104" t="s">
         <v>180</v>
       </c>
-      <c r="F104" t="s">
+      <c r="K104" t="s">
         <v>181</v>
       </c>
-      <c r="J104" t="s">
+      <c r="L104" t="s">
         <v>182</v>
-      </c>
-      <c r="K104" t="s">
-        <v>183</v>
-      </c>
-      <c r="L104" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B105" t="s">
+        <v>291</v>
+      </c>
+      <c r="C105" t="s">
+        <v>292</v>
+      </c>
+      <c r="D105" t="s">
         <v>293</v>
       </c>
-      <c r="C105" t="s">
+      <c r="M105" t="s">
         <v>294</v>
-      </c>
-      <c r="D105" t="s">
-        <v>295</v>
-      </c>
-      <c r="M105" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B106" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C106" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D106" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M106" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B107" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C107" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D107" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M107" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4020,10 +4020,10 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G108" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4031,10 +4031,10 @@
         <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G109" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4042,25 +4042,25 @@
         <v>30</v>
       </c>
       <c r="B110" t="s">
+        <v>303</v>
+      </c>
+      <c r="C110" t="s">
+        <v>304</v>
+      </c>
+      <c r="D110" t="s">
         <v>305</v>
       </c>
-      <c r="C110" t="s">
+      <c r="J110" t="s">
+        <v>199</v>
+      </c>
+      <c r="K110" t="s">
+        <v>200</v>
+      </c>
+      <c r="L110" t="s">
+        <v>201</v>
+      </c>
+      <c r="M110" t="s">
         <v>306</v>
-      </c>
-      <c r="D110" t="s">
-        <v>307</v>
-      </c>
-      <c r="J110" t="s">
-        <v>201</v>
-      </c>
-      <c r="K110" t="s">
-        <v>202</v>
-      </c>
-      <c r="L110" t="s">
-        <v>203</v>
-      </c>
-      <c r="M110" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4068,13 +4068,13 @@
         <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G111" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="M111" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4082,13 +4082,13 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G112" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M112" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4096,10 +4096,10 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G113" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4107,10 +4107,10 @@
         <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="G114" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4118,13 +4118,13 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G115" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="M115" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4132,13 +4132,13 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G116" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="M116" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4146,7 +4146,7 @@
         <v>43</v>
       </c>
       <c r="B117" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4154,44 +4154,44 @@
         <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="M118" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B119" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C119" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D119" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B120" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C120" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D120" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E120" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F120" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4199,28 +4199,28 @@
         <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C121" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D121" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="E121" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F121" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="I121" t="s">
         <v>29</v>
       </c>
       <c r="J121" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M121" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4228,31 +4228,31 @@
         <v>30</v>
       </c>
       <c r="B122" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C122" t="s">
+        <v>265</v>
+      </c>
+      <c r="D122" t="s">
+        <v>266</v>
+      </c>
+      <c r="E122" t="s">
+        <v>137</v>
+      </c>
+      <c r="F122" t="s">
+        <v>138</v>
+      </c>
+      <c r="J122" t="s">
         <v>267</v>
       </c>
-      <c r="D122" t="s">
-        <v>268</v>
-      </c>
-      <c r="E122" t="s">
-        <v>139</v>
-      </c>
-      <c r="F122" t="s">
+      <c r="K122" t="s">
         <v>140</v>
       </c>
-      <c r="J122" t="s">
-        <v>269</v>
-      </c>
-      <c r="K122" t="s">
-        <v>142</v>
-      </c>
       <c r="L122" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M122" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4260,13 +4260,13 @@
         <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="G123" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="M123" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4274,170 +4274,170 @@
         <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G124" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B125" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C125" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D125" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="M125" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B126" t="s">
+        <v>334</v>
+      </c>
+      <c r="C126" t="s">
+        <v>335</v>
+      </c>
+      <c r="D126" t="s">
         <v>336</v>
       </c>
-      <c r="C126" t="s">
+      <c r="M126" t="s">
         <v>337</v>
-      </c>
-      <c r="D126" t="s">
-        <v>338</v>
-      </c>
-      <c r="M126" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B127" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C127" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D127" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E127" t="s">
+        <v>165</v>
+      </c>
+      <c r="F127" t="s">
+        <v>166</v>
+      </c>
+      <c r="J127" t="s">
         <v>167</v>
       </c>
-      <c r="F127" t="s">
+      <c r="K127" t="s">
         <v>168</v>
       </c>
-      <c r="J127" t="s">
+      <c r="L127" t="s">
         <v>169</v>
-      </c>
-      <c r="K127" t="s">
-        <v>170</v>
-      </c>
-      <c r="L127" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B128" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C128" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D128" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M128" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B129" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="C129" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D129" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E129" t="s">
+        <v>178</v>
+      </c>
+      <c r="F129" t="s">
+        <v>179</v>
+      </c>
+      <c r="J129" t="s">
         <v>180</v>
       </c>
-      <c r="F129" t="s">
+      <c r="K129" t="s">
         <v>181</v>
       </c>
-      <c r="J129" t="s">
+      <c r="L129" t="s">
         <v>182</v>
-      </c>
-      <c r="K129" t="s">
-        <v>183</v>
-      </c>
-      <c r="L129" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B130" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="C130" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D130" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="M130" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B131" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="C131" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D131" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M131" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B132" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C132" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D132" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="M132" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4445,10 +4445,10 @@
         <v>17</v>
       </c>
       <c r="B133" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G133" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4456,10 +4456,10 @@
         <v>17</v>
       </c>
       <c r="B134" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G134" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4467,25 +4467,25 @@
         <v>30</v>
       </c>
       <c r="B135" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="C135" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D135" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="J135" t="s">
+        <v>199</v>
+      </c>
+      <c r="K135" t="s">
+        <v>200</v>
+      </c>
+      <c r="L135" t="s">
         <v>201</v>
       </c>
-      <c r="K135" t="s">
-        <v>202</v>
-      </c>
-      <c r="L135" t="s">
-        <v>203</v>
-      </c>
       <c r="M135" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4493,13 +4493,13 @@
         <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G136" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="M136" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4507,13 +4507,13 @@
         <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G137" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="M137" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4521,10 +4521,10 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G138" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4532,10 +4532,10 @@
         <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G139" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4543,13 +4543,13 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G140" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="M140" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4557,13 +4557,13 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G141" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="M141" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4571,88 +4571,88 @@
         <v>43</v>
       </c>
       <c r="B142" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B144" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C144" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="M144" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A145" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B145" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C145" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="E145" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="M145" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B146" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C146" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="E146" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="M146" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A147" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B147" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C147" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A148" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B148" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C148" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B149" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C149" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4660,13 +4660,13 @@
         <v>17</v>
       </c>
       <c r="B151" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G151" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M151" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4674,110 +4674,110 @@
         <v>17</v>
       </c>
       <c r="B152" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="G152" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M152" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B153" t="s">
+        <v>370</v>
+      </c>
+      <c r="C153" t="s">
+        <v>521</v>
+      </c>
+      <c r="D153" t="s">
+        <v>371</v>
+      </c>
+      <c r="E153" t="s">
         <v>372</v>
       </c>
-      <c r="C153" t="s">
-        <v>523</v>
-      </c>
-      <c r="D153" t="s">
+      <c r="F153" t="s">
         <v>373</v>
       </c>
-      <c r="E153" t="s">
+      <c r="M153" t="s">
         <v>374</v>
-      </c>
-      <c r="F153" t="s">
-        <v>375</v>
-      </c>
-      <c r="M153" t="s">
-        <v>376</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
+        <v>375</v>
+      </c>
+      <c r="B154" t="s">
+        <v>376</v>
+      </c>
+      <c r="C154" t="s">
         <v>377</v>
       </c>
-      <c r="B154" t="s">
+      <c r="D154" t="s">
         <v>378</v>
       </c>
-      <c r="C154" t="s">
-        <v>379</v>
-      </c>
-      <c r="D154" t="s">
-        <v>380</v>
-      </c>
       <c r="M154" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B155" t="s">
+        <v>379</v>
+      </c>
+      <c r="C155" t="s">
+        <v>522</v>
+      </c>
+      <c r="D155" t="s">
+        <v>380</v>
+      </c>
+      <c r="E155" t="s">
         <v>381</v>
       </c>
-      <c r="C155" t="s">
-        <v>524</v>
-      </c>
-      <c r="D155" t="s">
+      <c r="F155" t="s">
         <v>382</v>
       </c>
-      <c r="E155" t="s">
+      <c r="M155" t="s">
         <v>383</v>
-      </c>
-      <c r="F155" t="s">
-        <v>384</v>
-      </c>
-      <c r="M155" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
+        <v>384</v>
+      </c>
+      <c r="B156" t="s">
+        <v>385</v>
+      </c>
+      <c r="C156" t="s">
         <v>386</v>
       </c>
-      <c r="B156" t="s">
+      <c r="D156" t="s">
         <v>387</v>
       </c>
-      <c r="C156" t="s">
-        <v>388</v>
-      </c>
-      <c r="D156" t="s">
-        <v>389</v>
-      </c>
       <c r="M156" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B157" t="s">
+        <v>388</v>
+      </c>
+      <c r="C157" t="s">
+        <v>523</v>
+      </c>
+      <c r="D157" t="s">
+        <v>389</v>
+      </c>
+      <c r="M157" t="s">
         <v>390</v>
-      </c>
-      <c r="C157" t="s">
-        <v>525</v>
-      </c>
-      <c r="D157" t="s">
-        <v>391</v>
-      </c>
-      <c r="M157" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4785,13 +4785,13 @@
         <v>17</v>
       </c>
       <c r="B158" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G158" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M158" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4799,13 +4799,13 @@
         <v>17</v>
       </c>
       <c r="B159" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="G159" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M159" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4813,13 +4813,13 @@
         <v>17</v>
       </c>
       <c r="B160" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="G160" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M160" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4827,35 +4827,35 @@
         <v>17</v>
       </c>
       <c r="B161" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="G161" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="M161" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="162" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A162" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="164" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A164" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
     </row>
     <row r="165" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4863,11 +4863,11 @@
         <v>17</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C165" s="4"/>
       <c r="G165" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="166" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4875,11 +4875,11 @@
         <v>17</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="C166" s="4"/>
       <c r="G166" s="3" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
     </row>
     <row r="167" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4887,11 +4887,11 @@
         <v>17</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C167" s="4"/>
       <c r="G167" s="3" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
     </row>
     <row r="168" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4899,253 +4899,253 @@
         <v>17</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="C168" s="4"/>
       <c r="G168" s="3" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="169" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B169" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M169" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="170" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B171" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="C171" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D171" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H171" t="s">
         <v>22</v>
       </c>
       <c r="M171" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A172" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B172" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C172" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D172" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H172" t="s">
         <v>22</v>
       </c>
       <c r="M172" s="3" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="173" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
+        <v>510</v>
+      </c>
+      <c r="B173" t="s">
+        <v>511</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>543</v>
+      </c>
+      <c r="J173" t="s">
         <v>512</v>
       </c>
-      <c r="B173" t="s">
+      <c r="K173" t="s">
         <v>513</v>
       </c>
-      <c r="C173" s="6" t="s">
-        <v>545</v>
-      </c>
-      <c r="J173" t="s">
-        <v>514</v>
-      </c>
-      <c r="K173" t="s">
-        <v>515</v>
-      </c>
       <c r="M173" s="3" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="174" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B174" t="s">
+        <v>514</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>542</v>
+      </c>
+      <c r="J174" t="s">
         <v>516</v>
       </c>
-      <c r="C174" s="6" t="s">
-        <v>544</v>
-      </c>
-      <c r="J174" t="s">
-        <v>518</v>
-      </c>
       <c r="K174" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="175" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="B175" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="J175" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="K175" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="M175" s="3" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
     </row>
     <row r="177" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B179" t="s">
+        <v>399</v>
+      </c>
+      <c r="C179" t="s">
+        <v>400</v>
+      </c>
+      <c r="D179" t="s">
         <v>401</v>
       </c>
-      <c r="C179" t="s">
+      <c r="E179" t="s">
         <v>402</v>
       </c>
-      <c r="D179" t="s">
+      <c r="F179" t="s">
         <v>403</v>
-      </c>
-      <c r="E179" t="s">
-        <v>404</v>
-      </c>
-      <c r="F179" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
+        <v>404</v>
+      </c>
+      <c r="B180" t="s">
+        <v>405</v>
+      </c>
+      <c r="C180" t="s">
         <v>406</v>
       </c>
-      <c r="B180" t="s">
+      <c r="D180" t="s">
         <v>407</v>
       </c>
-      <c r="C180" t="s">
+      <c r="E180" t="s">
         <v>408</v>
       </c>
-      <c r="D180" t="s">
+      <c r="F180" t="s">
         <v>409</v>
-      </c>
-      <c r="E180" t="s">
-        <v>410</v>
-      </c>
-      <c r="F180" t="s">
-        <v>411</v>
       </c>
       <c r="H180" t="s">
         <v>22</v>
       </c>
       <c r="M180" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B181" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C181" t="s">
+        <v>406</v>
+      </c>
+      <c r="D181" t="s">
+        <v>407</v>
+      </c>
+      <c r="E181" t="s">
         <v>408</v>
       </c>
-      <c r="D181" t="s">
+      <c r="F181" t="s">
         <v>409</v>
       </c>
-      <c r="E181" t="s">
-        <v>410</v>
-      </c>
-      <c r="F181" t="s">
-        <v>411</v>
-      </c>
       <c r="M181" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B182" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C182" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="D182" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H182" t="s">
         <v>22</v>
       </c>
       <c r="M182" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B183" t="s">
+        <v>416</v>
+      </c>
+      <c r="C183" t="s">
+        <v>417</v>
+      </c>
+      <c r="D183" t="s">
         <v>418</v>
       </c>
-      <c r="C183" t="s">
+      <c r="M183" t="s">
         <v>419</v>
-      </c>
-      <c r="D183" t="s">
-        <v>420</v>
-      </c>
-      <c r="M183" t="s">
-        <v>421</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5153,13 +5153,13 @@
         <v>20</v>
       </c>
       <c r="B184" t="s">
+        <v>420</v>
+      </c>
+      <c r="C184" t="s">
+        <v>421</v>
+      </c>
+      <c r="D184" t="s">
         <v>422</v>
-      </c>
-      <c r="C184" t="s">
-        <v>423</v>
-      </c>
-      <c r="D184" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5175,10 +5175,10 @@
         <v>17</v>
       </c>
       <c r="B187" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G187" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5186,10 +5186,10 @@
         <v>17</v>
       </c>
       <c r="B188" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G188" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5197,10 +5197,10 @@
         <v>17</v>
       </c>
       <c r="B189" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G189" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5208,10 +5208,10 @@
         <v>17</v>
       </c>
       <c r="B190" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G190" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5219,10 +5219,10 @@
         <v>17</v>
       </c>
       <c r="B191" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="G191" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5230,10 +5230,10 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G192" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
   </sheetData>
@@ -5246,7 +5246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E41" sqref="A8:E41"/>
     </sheetView>
   </sheetViews>
@@ -5257,7 +5257,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5271,41 +5271,41 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D2" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
+        <v>438</v>
+      </c>
+      <c r="C3" t="s">
+        <v>439</v>
+      </c>
+      <c r="D3" t="s">
         <v>440</v>
-      </c>
-      <c r="C3" t="s">
-        <v>441</v>
-      </c>
-      <c r="D3" t="s">
-        <v>442</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="B4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C4" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5313,13 +5313,13 @@
         <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D5" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5327,13 +5327,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5341,709 +5341,709 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
+        <v>446</v>
+      </c>
+      <c r="C7" t="s">
+        <v>524</v>
+      </c>
+      <c r="D7" t="s">
         <v>448</v>
-      </c>
-      <c r="C7" t="s">
-        <v>526</v>
-      </c>
-      <c r="D7" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>569</v>
+      </c>
+      <c r="B9" t="s">
+        <v>438</v>
+      </c>
+      <c r="C9" t="s">
         <v>571</v>
-      </c>
-      <c r="B9" t="s">
-        <v>440</v>
-      </c>
-      <c r="C9" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B10" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C10" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B11" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C11" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B12" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="C12" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
+        <v>569</v>
+      </c>
+      <c r="B13" t="s">
+        <v>574</v>
+      </c>
+      <c r="C13" t="s">
         <v>571</v>
-      </c>
-      <c r="B13" t="s">
-        <v>576</v>
-      </c>
-      <c r="C13" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B14" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C14" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B15" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C15" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B16" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C16" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
+        <v>569</v>
+      </c>
+      <c r="B17" t="s">
+        <v>578</v>
+      </c>
+      <c r="C17" t="s">
         <v>571</v>
-      </c>
-      <c r="B17" t="s">
-        <v>580</v>
-      </c>
-      <c r="C17" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B18" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C18" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B19" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C19" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B20" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C20" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>569</v>
+      </c>
+      <c r="B21" t="s">
+        <v>582</v>
+      </c>
+      <c r="C21" t="s">
         <v>571</v>
-      </c>
-      <c r="B21" t="s">
-        <v>584</v>
-      </c>
-      <c r="C21" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B22" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C22" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B23" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C23" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B24" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C24" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>569</v>
+      </c>
+      <c r="B25" t="s">
+        <v>586</v>
+      </c>
+      <c r="C25" t="s">
         <v>571</v>
-      </c>
-      <c r="B25" t="s">
-        <v>588</v>
-      </c>
-      <c r="C25" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B26" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C26" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B27" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C27" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B28" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C28" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
+        <v>569</v>
+      </c>
+      <c r="B29" t="s">
+        <v>590</v>
+      </c>
+      <c r="C29" t="s">
         <v>571</v>
-      </c>
-      <c r="B29" t="s">
-        <v>592</v>
-      </c>
-      <c r="C29" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B30" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C30" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B31" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C31" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B32" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C32" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
+        <v>569</v>
+      </c>
+      <c r="B33" t="s">
+        <v>594</v>
+      </c>
+      <c r="C33" t="s">
         <v>571</v>
-      </c>
-      <c r="B33" t="s">
-        <v>596</v>
-      </c>
-      <c r="C33" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B34" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C34" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B35" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C35" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B36" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C36" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
+        <v>569</v>
+      </c>
+      <c r="B37" t="s">
+        <v>598</v>
+      </c>
+      <c r="C37" t="s">
         <v>571</v>
-      </c>
-      <c r="B37" t="s">
-        <v>600</v>
-      </c>
-      <c r="C37" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B38" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C38" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B39" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C39" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="B40" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C40" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
+        <v>569</v>
+      </c>
+      <c r="B41" t="s">
+        <v>602</v>
+      </c>
+      <c r="C41" t="s">
         <v>571</v>
-      </c>
-      <c r="B41" t="s">
-        <v>604</v>
-      </c>
-      <c r="C41" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="B42" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C42" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D42" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
+        <v>449</v>
+      </c>
+      <c r="B43" t="s">
         <v>451</v>
       </c>
-      <c r="B43" t="s">
-        <v>453</v>
-      </c>
       <c r="C43" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D43" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
+        <v>452</v>
+      </c>
+      <c r="B44" t="s">
+        <v>453</v>
+      </c>
+      <c r="C44" t="s">
         <v>454</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>455</v>
-      </c>
-      <c r="C44" t="s">
-        <v>456</v>
-      </c>
-      <c r="D44" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="B45" t="s">
+        <v>456</v>
+      </c>
+      <c r="C45" t="s">
+        <v>457</v>
+      </c>
+      <c r="D45" t="s">
         <v>458</v>
-      </c>
-      <c r="C45" t="s">
-        <v>459</v>
-      </c>
-      <c r="D45" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>459</v>
+      </c>
+      <c r="B46" t="s">
+        <v>460</v>
+      </c>
+      <c r="C46" t="s">
         <v>461</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>462</v>
-      </c>
-      <c r="C46" t="s">
-        <v>463</v>
-      </c>
-      <c r="D46" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="B47" t="s">
+        <v>463</v>
+      </c>
+      <c r="C47" t="s">
+        <v>464</v>
+      </c>
+      <c r="D47" t="s">
         <v>465</v>
-      </c>
-      <c r="C47" t="s">
-        <v>466</v>
-      </c>
-      <c r="D47" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D48" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C49" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="D49" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C50" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D50" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C51" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D51" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B52" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D52" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
+        <v>473</v>
+      </c>
+      <c r="B53" t="s">
+        <v>438</v>
+      </c>
+      <c r="C53" t="s">
+        <v>474</v>
+      </c>
+      <c r="D53" t="s">
         <v>475</v>
-      </c>
-      <c r="B53" t="s">
-        <v>440</v>
-      </c>
-      <c r="C53" t="s">
-        <v>476</v>
-      </c>
-      <c r="D53" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B54" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C54" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="D54" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B55" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D55" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
+        <v>478</v>
+      </c>
+      <c r="B56" t="s">
+        <v>438</v>
+      </c>
+      <c r="C56" t="s">
+        <v>479</v>
+      </c>
+      <c r="D56" t="s">
         <v>480</v>
-      </c>
-      <c r="B56" t="s">
-        <v>440</v>
-      </c>
-      <c r="C56" t="s">
-        <v>481</v>
-      </c>
-      <c r="D56" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B57" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C57" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="D57" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
+        <v>483</v>
+      </c>
+      <c r="B58" t="s">
+        <v>96</v>
+      </c>
+      <c r="C58" t="s">
+        <v>484</v>
+      </c>
+      <c r="D58" t="s">
         <v>485</v>
-      </c>
-      <c r="B58" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" t="s">
-        <v>486</v>
-      </c>
-      <c r="D58" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="B59" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C59" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="D59" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B60" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="C60" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D60" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>488</v>
+      </c>
+      <c r="B61" t="s">
         <v>490</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
+        <v>491</v>
+      </c>
+      <c r="D61" t="s">
         <v>492</v>
-      </c>
-      <c r="C61" t="s">
-        <v>493</v>
-      </c>
-      <c r="D61" t="s">
-        <v>494</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
+        <v>493</v>
+      </c>
+      <c r="B62" t="s">
+        <v>446</v>
+      </c>
+      <c r="C62" t="s">
+        <v>494</v>
+      </c>
+      <c r="D62" t="s">
         <v>495</v>
-      </c>
-      <c r="B62" t="s">
-        <v>448</v>
-      </c>
-      <c r="C62" t="s">
-        <v>496</v>
-      </c>
-      <c r="D62" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B63" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="D63" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B64" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="C64" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D64" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -6061,30 +6061,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>498</v>
+      </c>
+      <c r="B1" t="s">
+        <v>499</v>
+      </c>
+      <c r="C1" t="s">
         <v>500</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>501</v>
-      </c>
-      <c r="C1" t="s">
-        <v>502</v>
-      </c>
-      <c r="D1" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>502</v>
+      </c>
+      <c r="B2" t="s">
+        <v>503</v>
+      </c>
+      <c r="C2" t="s">
         <v>504</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>505</v>
-      </c>
-      <c r="C2" t="s">
-        <v>506</v>
-      </c>
-      <c r="D2" t="s">
-        <v>507</v>
       </c>
     </row>
   </sheetData>
@@ -6093,21 +6093,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6157,80 +6142,22 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6669,10 +6596,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6686,36 +6686,14 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6736,4 +6714,26 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added constraints to morbidity questions
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DA8702D8-EFA6-4D80-ADD1-0AEEFC804C66}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1041" uniqueCount="636">
   <si>
     <t>type</t>
   </si>
@@ -1874,18 +1874,12 @@
     <t>fever</t>
   </si>
   <si>
-    <t>${MONTHS}&lt;24</t>
-  </si>
-  <si>
     <t xml:space="preserve">Is the child  ${child_name}  currently breastfeeding? </t>
   </si>
   <si>
     <t xml:space="preserve">Has the child  ${child_name}  received vitamin A in the past 6 months ? </t>
   </si>
   <si>
-    <t>${MONTHS}&gt;5</t>
-  </si>
-  <si>
     <t xml:space="preserve">Has the child  ${child_name}  received a measles vaccination? </t>
   </si>
   <si>
@@ -2109,6 +2103,15 @@
   </si>
   <si>
     <t>Zabul</t>
+  </si>
+  <si>
+    <t>${MONTHS} &lt;60 or ${MONTHS}=98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">${MONTHS}&lt;24  or (${MONTHS}=98 and ${HEIGHT}&lt;=87) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">${MONTHS}&gt;5 or (${MONTHS}=98 and ${HEIGHT}&gt;67) </t>
   </si>
 </sst>
 </file>
@@ -2521,9 +2524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N192"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A137" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E196" sqref="E196"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2617,13 +2620,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>564</v>
+      </c>
+      <c r="B6" t="s">
+        <v>565</v>
+      </c>
+      <c r="C6" t="s">
         <v>566</v>
-      </c>
-      <c r="B6" t="s">
-        <v>567</v>
-      </c>
-      <c r="C6" t="s">
-        <v>568</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2770,10 +2773,10 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="E17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -4672,10 +4675,10 @@
         <v>550</v>
       </c>
       <c r="C144" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="M144" t="s">
-        <v>556</v>
+        <v>634</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4686,13 +4689,13 @@
         <v>551</v>
       </c>
       <c r="C145" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D145" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="M145" t="s">
-        <v>559</v>
+        <v>635</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4703,13 +4706,13 @@
         <v>552</v>
       </c>
       <c r="C146" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="D146" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="M146" t="s">
-        <v>559</v>
+        <v>635</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4720,7 +4723,10 @@
         <v>553</v>
       </c>
       <c r="C147" t="s">
-        <v>561</v>
+        <v>559</v>
+      </c>
+      <c r="M147" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4731,7 +4737,10 @@
         <v>554</v>
       </c>
       <c r="C148" t="s">
-        <v>562</v>
+        <v>560</v>
+      </c>
+      <c r="M148" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4742,7 +4751,10 @@
         <v>555</v>
       </c>
       <c r="C149" t="s">
-        <v>563</v>
+        <v>561</v>
+      </c>
+      <c r="M149" t="s">
+        <v>633</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5336,7 +5348,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
@@ -5442,376 +5454,376 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B8" t="s">
         <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B9" t="s">
         <v>438</v>
       </c>
       <c r="C9" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B10" t="s">
         <v>446</v>
       </c>
       <c r="C10" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B11" t="s">
         <v>472</v>
       </c>
       <c r="C11" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B12" t="s">
         <v>490</v>
       </c>
       <c r="C12" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B13" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C13" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B14" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C14" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B15" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C15" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B16" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C16" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B17" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C17" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B18" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C18" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B19" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C19" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B20" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C20" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B21" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C21" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B22" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C22" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B23" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C23" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B24" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C24" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B25" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C25" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B26" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C26" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B27" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C27" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B28" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C28" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B29" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C29" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B30" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C30" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B31" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C31" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B32" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C32" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B33" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C33" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B34" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C34" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B35" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C35" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B36" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C36" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B37" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C37" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B38" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="C38" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B39" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C39" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B40" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C40" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B41" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C41" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -6183,21 +6195,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6247,80 +6244,22 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6759,10 +6698,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6776,36 +6788,14 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6826,4 +6816,26 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added upper to child name
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0A0EC0EE-9F77-4AA4-946E-576A5AF19B48}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{73604562-AEA9-4D69-B304-AEA80BD84D13}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,9 +378,6 @@
     <t>child_name_note</t>
   </si>
   <si>
-    <t>Now entering data for child: ${child_name} (${CHSEX}) with age in years: ${child_age_years}</t>
-  </si>
-  <si>
     <t>Saisie des données pour l'enfant : ${child_name} (${CHSEX}) âgé(e) de ${child_age_years} an(s)</t>
   </si>
   <si>
@@ -478,9 +475,6 @@
   </si>
   <si>
     <t>age_confirm</t>
-  </si>
-  <si>
-    <t>${child_name}   is ${MONTHS} months old.</t>
   </si>
   <si>
     <t>${child_name}   est âgé(e) de ${MONTHS} mois.</t>
@@ -2100,6 +2094,12 @@
   </si>
   <si>
     <t xml:space="preserve">${MONTHS}&gt;5 or (${MONTHS}=98 and ${HEIGHT}&gt;67) </t>
+  </si>
+  <si>
+    <t>(${child_name}) is ${MONTHS} months old.</t>
+  </si>
+  <si>
+    <t>Now entering data for child: upper(${child_name}) (${CHSEX}) with age in years: ${child_age_years}</t>
   </si>
 </sst>
 </file>
@@ -2513,8 +2513,8 @@
   <dimension ref="A1:N192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58:XFD58"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2608,13 +2608,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>558</v>
+      </c>
+      <c r="B6" t="s">
+        <v>559</v>
+      </c>
+      <c r="C6" t="s">
         <v>560</v>
-      </c>
-      <c r="B6" t="s">
-        <v>561</v>
-      </c>
-      <c r="C6" t="s">
-        <v>562</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2761,10 +2761,10 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="E17" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2939,10 +2939,10 @@
         <v>17</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3046,10 +3046,10 @@
         <v>17</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>521</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>523</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3057,10 +3057,10 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="G41" s="1" t="s">
         <v>524</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3144,13 +3144,13 @@
         <v>117</v>
       </c>
       <c r="C49" t="s">
+        <v>631</v>
+      </c>
+      <c r="E49" t="s">
         <v>118</v>
       </c>
-      <c r="E49" t="s">
+      <c r="M49" t="s">
         <v>119</v>
-      </c>
-      <c r="M49" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3158,10 +3158,10 @@
         <v>25</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="M50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3169,19 +3169,19 @@
         <v>78</v>
       </c>
       <c r="B51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" t="s">
         <v>122</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
+        <v>124</v>
+      </c>
+      <c r="E51" t="s">
         <v>123</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
         <v>125</v>
-      </c>
-      <c r="E51" t="s">
-        <v>124</v>
-      </c>
-      <c r="F51" t="s">
-        <v>126</v>
       </c>
       <c r="H51" t="s">
         <v>22</v>
@@ -3192,28 +3192,28 @@
         <v>28</v>
       </c>
       <c r="B52" t="s">
+        <v>126</v>
+      </c>
+      <c r="C52" t="s">
         <v>127</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
+        <v>129</v>
+      </c>
+      <c r="E52" t="s">
         <v>128</v>
       </c>
-      <c r="D52" t="s">
+      <c r="F52" t="s">
         <v>130</v>
-      </c>
-      <c r="E52" t="s">
-        <v>129</v>
-      </c>
-      <c r="F52" t="s">
-        <v>131</v>
       </c>
       <c r="I52" t="s">
         <v>29</v>
       </c>
       <c r="J52" t="s">
+        <v>131</v>
+      </c>
+      <c r="M52" t="s">
         <v>132</v>
-      </c>
-      <c r="M52" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3221,31 +3221,31 @@
         <v>30</v>
       </c>
       <c r="B53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C53" t="s">
         <v>134</v>
       </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
+        <v>136</v>
+      </c>
+      <c r="E53" t="s">
         <v>135</v>
       </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
         <v>137</v>
       </c>
-      <c r="E53" t="s">
-        <v>136</v>
-      </c>
-      <c r="F53" t="s">
+      <c r="J53" t="s">
         <v>138</v>
       </c>
-      <c r="J53" t="s">
+      <c r="K53" t="s">
         <v>139</v>
       </c>
-      <c r="K53" t="s">
+      <c r="L53" t="s">
         <v>140</v>
       </c>
-      <c r="L53" t="s">
+      <c r="M53" t="s">
         <v>141</v>
-      </c>
-      <c r="M53" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3253,13 +3253,13 @@
         <v>17</v>
       </c>
       <c r="B54" t="s">
+        <v>142</v>
+      </c>
+      <c r="G54" t="s">
         <v>143</v>
       </c>
-      <c r="G54" t="s">
-        <v>144</v>
-      </c>
       <c r="M54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3267,10 +3267,10 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
+        <v>144</v>
+      </c>
+      <c r="G55" t="s">
         <v>145</v>
-      </c>
-      <c r="G55" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3278,16 +3278,16 @@
         <v>48</v>
       </c>
       <c r="B56" t="s">
+        <v>146</v>
+      </c>
+      <c r="C56" t="s">
         <v>147</v>
       </c>
-      <c r="C56" t="s">
+      <c r="E56" t="s">
         <v>148</v>
       </c>
-      <c r="E56" t="s">
+      <c r="M56" t="s">
         <v>149</v>
-      </c>
-      <c r="M56" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3295,16 +3295,16 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
+        <v>150</v>
+      </c>
+      <c r="C57" t="s">
+        <v>630</v>
+      </c>
+      <c r="E57" t="s">
         <v>151</v>
       </c>
-      <c r="C57" t="s">
+      <c r="M57" t="s">
         <v>152</v>
-      </c>
-      <c r="E57" t="s">
-        <v>153</v>
-      </c>
-      <c r="M57" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3312,102 +3312,102 @@
         <v>25</v>
       </c>
       <c r="B59" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M59" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" t="s">
+        <v>156</v>
+      </c>
+      <c r="C60" t="s">
         <v>157</v>
       </c>
-      <c r="B60" t="s">
+      <c r="D60" t="s">
+        <v>159</v>
+      </c>
+      <c r="E60" t="s">
         <v>158</v>
       </c>
-      <c r="C60" t="s">
-        <v>159</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
+        <v>160</v>
+      </c>
+      <c r="J60" t="s">
         <v>161</v>
       </c>
-      <c r="E60" t="s">
-        <v>160</v>
-      </c>
-      <c r="F60" t="s">
+      <c r="K60" t="s">
         <v>162</v>
       </c>
-      <c r="J60" t="s">
+      <c r="L60" t="s">
         <v>163</v>
-      </c>
-      <c r="K60" t="s">
-        <v>164</v>
-      </c>
-      <c r="L60" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>164</v>
+      </c>
+      <c r="B61" t="s">
+        <v>165</v>
+      </c>
+      <c r="C61" t="s">
         <v>166</v>
       </c>
-      <c r="B61" t="s">
+      <c r="E61" t="s">
         <v>167</v>
       </c>
-      <c r="C61" t="s">
+      <c r="M61" t="s">
         <v>168</v>
-      </c>
-      <c r="E61" t="s">
-        <v>169</v>
-      </c>
-      <c r="M61" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
+        <v>169</v>
+      </c>
+      <c r="C62" t="s">
+        <v>170</v>
+      </c>
+      <c r="D62" t="s">
+        <v>172</v>
+      </c>
+      <c r="E62" t="s">
         <v>171</v>
       </c>
-      <c r="C62" t="s">
-        <v>172</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
+        <v>173</v>
+      </c>
+      <c r="J62" t="s">
         <v>174</v>
       </c>
-      <c r="E62" t="s">
-        <v>173</v>
-      </c>
-      <c r="F62" t="s">
+      <c r="K62" t="s">
         <v>175</v>
       </c>
-      <c r="J62" t="s">
+      <c r="L62" t="s">
         <v>176</v>
-      </c>
-      <c r="K62" t="s">
-        <v>177</v>
-      </c>
-      <c r="L62" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
+        <v>177</v>
+      </c>
+      <c r="B63" t="s">
+        <v>178</v>
+      </c>
+      <c r="C63" t="s">
         <v>179</v>
       </c>
-      <c r="B63" t="s">
+      <c r="E63" t="s">
         <v>180</v>
       </c>
-      <c r="C63" t="s">
+      <c r="M63" t="s">
         <v>181</v>
-      </c>
-      <c r="E63" t="s">
-        <v>182</v>
-      </c>
-      <c r="M63" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3415,16 +3415,16 @@
         <v>48</v>
       </c>
       <c r="B64" t="s">
+        <v>182</v>
+      </c>
+      <c r="C64" t="s">
+        <v>183</v>
+      </c>
+      <c r="E64" t="s">
         <v>184</v>
       </c>
-      <c r="C64" t="s">
+      <c r="M64" t="s">
         <v>185</v>
-      </c>
-      <c r="E64" t="s">
-        <v>186</v>
-      </c>
-      <c r="M64" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3432,16 +3432,16 @@
         <v>48</v>
       </c>
       <c r="B65" t="s">
+        <v>186</v>
+      </c>
+      <c r="C65" t="s">
+        <v>187</v>
+      </c>
+      <c r="E65" t="s">
         <v>188</v>
       </c>
-      <c r="C65" t="s">
+      <c r="M65" t="s">
         <v>189</v>
-      </c>
-      <c r="E65" t="s">
-        <v>190</v>
-      </c>
-      <c r="M65" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3449,39 +3449,39 @@
         <v>30</v>
       </c>
       <c r="B66" t="s">
+        <v>190</v>
+      </c>
+      <c r="C66" t="s">
+        <v>191</v>
+      </c>
+      <c r="E66" t="s">
         <v>192</v>
       </c>
-      <c r="C66" t="s">
+      <c r="J66" t="s">
         <v>193</v>
       </c>
-      <c r="E66" t="s">
+      <c r="K66" t="s">
         <v>194</v>
       </c>
-      <c r="J66" t="s">
+      <c r="L66" t="s">
         <v>195</v>
       </c>
-      <c r="K66" t="s">
+      <c r="M66" t="s">
         <v>196</v>
-      </c>
-      <c r="L66" t="s">
-        <v>197</v>
-      </c>
-      <c r="M66" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B67" t="s">
+        <v>197</v>
+      </c>
+      <c r="C67" t="s">
+        <v>198</v>
+      </c>
+      <c r="E67" t="s">
         <v>199</v>
-      </c>
-      <c r="C67" t="s">
-        <v>200</v>
-      </c>
-      <c r="E67" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3489,19 +3489,19 @@
         <v>78</v>
       </c>
       <c r="B68" t="s">
+        <v>200</v>
+      </c>
+      <c r="C68" t="s">
+        <v>201</v>
+      </c>
+      <c r="E68" t="s">
         <v>202</v>
-      </c>
-      <c r="C68" t="s">
-        <v>203</v>
-      </c>
-      <c r="E68" t="s">
-        <v>204</v>
       </c>
       <c r="H68" t="s">
         <v>22</v>
       </c>
       <c r="M68" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3509,7 +3509,7 @@
         <v>43</v>
       </c>
       <c r="B69" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3517,7 +3517,7 @@
         <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3525,10 +3525,10 @@
         <v>17</v>
       </c>
       <c r="B71" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="G71" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3536,10 +3536,10 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G72" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3547,10 +3547,10 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G73" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3558,10 +3558,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G74" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3569,13 +3569,13 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
+        <v>211</v>
+      </c>
+      <c r="G75" t="s">
+        <v>212</v>
+      </c>
+      <c r="M75" t="s">
         <v>213</v>
-      </c>
-      <c r="G75" t="s">
-        <v>214</v>
-      </c>
-      <c r="M75" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3583,13 +3583,13 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G76" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="M76" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3597,10 +3597,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G77" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3608,13 +3608,13 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G78" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M78" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3622,13 +3622,13 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G79" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M79" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3636,10 +3636,10 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G80" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3647,13 +3647,13 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G81" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M81" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3661,13 +3661,13 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G82" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M82" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3675,10 +3675,10 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G83" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3686,10 +3686,10 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G84" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3697,13 +3697,13 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G85" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="M85" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3711,13 +3711,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G86" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M86" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3725,10 +3725,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="G87" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3736,10 +3736,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="G88" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3747,13 +3747,13 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G89" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="M89" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3761,13 +3761,13 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="G90" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M90" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3775,13 +3775,13 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G91" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M91" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="92" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3790,10 +3790,10 @@
         <v>25</v>
       </c>
       <c r="B93" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="M93" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3801,13 +3801,13 @@
         <v>48</v>
       </c>
       <c r="B94" t="s">
+        <v>248</v>
+      </c>
+      <c r="C94" t="s">
+        <v>249</v>
+      </c>
+      <c r="E94" t="s">
         <v>250</v>
-      </c>
-      <c r="C94" t="s">
-        <v>251</v>
-      </c>
-      <c r="E94" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3815,19 +3815,19 @@
         <v>78</v>
       </c>
       <c r="B95" t="s">
+        <v>251</v>
+      </c>
+      <c r="C95" t="s">
+        <v>252</v>
+      </c>
+      <c r="D95" t="s">
+        <v>124</v>
+      </c>
+      <c r="E95" t="s">
         <v>253</v>
       </c>
-      <c r="C95" t="s">
-        <v>254</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="F95" t="s">
         <v>125</v>
-      </c>
-      <c r="E95" t="s">
-        <v>255</v>
-      </c>
-      <c r="F95" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3835,28 +3835,28 @@
         <v>28</v>
       </c>
       <c r="B96" t="s">
+        <v>254</v>
+      </c>
+      <c r="C96" t="s">
+        <v>255</v>
+      </c>
+      <c r="D96" t="s">
+        <v>129</v>
+      </c>
+      <c r="E96" t="s">
         <v>256</v>
       </c>
-      <c r="C96" t="s">
-        <v>257</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="F96" t="s">
         <v>130</v>
-      </c>
-      <c r="E96" t="s">
-        <v>258</v>
-      </c>
-      <c r="F96" t="s">
-        <v>131</v>
       </c>
       <c r="I96" t="s">
         <v>29</v>
       </c>
       <c r="J96" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M96" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3864,31 +3864,31 @@
         <v>30</v>
       </c>
       <c r="B97" t="s">
+        <v>258</v>
+      </c>
+      <c r="C97" t="s">
+        <v>259</v>
+      </c>
+      <c r="D97" t="s">
+        <v>136</v>
+      </c>
+      <c r="E97" t="s">
         <v>260</v>
       </c>
-      <c r="C97" t="s">
+      <c r="F97" t="s">
+        <v>137</v>
+      </c>
+      <c r="J97" t="s">
         <v>261</v>
       </c>
-      <c r="D97" t="s">
-        <v>137</v>
-      </c>
-      <c r="E97" t="s">
+      <c r="K97" t="s">
+        <v>139</v>
+      </c>
+      <c r="L97" t="s">
+        <v>140</v>
+      </c>
+      <c r="M97" t="s">
         <v>262</v>
-      </c>
-      <c r="F97" t="s">
-        <v>138</v>
-      </c>
-      <c r="J97" t="s">
-        <v>263</v>
-      </c>
-      <c r="K97" t="s">
-        <v>140</v>
-      </c>
-      <c r="L97" t="s">
-        <v>141</v>
-      </c>
-      <c r="M97" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3896,13 +3896,13 @@
         <v>17</v>
       </c>
       <c r="B98" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G98" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M98" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3910,10 +3910,10 @@
         <v>17</v>
       </c>
       <c r="B99" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="G99" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3921,16 +3921,16 @@
         <v>48</v>
       </c>
       <c r="B100" t="s">
+        <v>267</v>
+      </c>
+      <c r="C100" t="s">
+        <v>268</v>
+      </c>
+      <c r="E100" t="s">
         <v>269</v>
       </c>
-      <c r="C100" t="s">
+      <c r="M100" t="s">
         <v>270</v>
-      </c>
-      <c r="E100" t="s">
-        <v>271</v>
-      </c>
-      <c r="M100" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3938,108 +3938,108 @@
         <v>48</v>
       </c>
       <c r="B101" t="s">
+        <v>271</v>
+      </c>
+      <c r="C101" t="s">
+        <v>272</v>
+      </c>
+      <c r="E101" t="s">
         <v>273</v>
       </c>
-      <c r="C101" t="s">
+      <c r="M101" t="s">
         <v>274</v>
-      </c>
-      <c r="E101" t="s">
-        <v>275</v>
-      </c>
-      <c r="M101" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B102" t="s">
+        <v>275</v>
+      </c>
+      <c r="C102" t="s">
+        <v>276</v>
+      </c>
+      <c r="D102" t="s">
+        <v>159</v>
+      </c>
+      <c r="E102" t="s">
         <v>277</v>
       </c>
-      <c r="C102" t="s">
-        <v>278</v>
-      </c>
-      <c r="D102" t="s">
+      <c r="F102" t="s">
+        <v>160</v>
+      </c>
+      <c r="J102" t="s">
         <v>161</v>
       </c>
-      <c r="E102" t="s">
-        <v>279</v>
-      </c>
-      <c r="F102" t="s">
+      <c r="K102" t="s">
         <v>162</v>
       </c>
-      <c r="J102" t="s">
+      <c r="L102" t="s">
         <v>163</v>
-      </c>
-      <c r="K102" t="s">
-        <v>164</v>
-      </c>
-      <c r="L102" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B103" t="s">
+        <v>278</v>
+      </c>
+      <c r="C103" t="s">
+        <v>279</v>
+      </c>
+      <c r="E103" t="s">
         <v>280</v>
       </c>
-      <c r="C103" t="s">
+      <c r="M103" t="s">
         <v>281</v>
-      </c>
-      <c r="E103" t="s">
-        <v>282</v>
-      </c>
-      <c r="M103" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B104" t="s">
+        <v>282</v>
+      </c>
+      <c r="C104" t="s">
+        <v>283</v>
+      </c>
+      <c r="D104" t="s">
+        <v>172</v>
+      </c>
+      <c r="E104" t="s">
         <v>284</v>
       </c>
-      <c r="C104" t="s">
-        <v>285</v>
-      </c>
-      <c r="D104" t="s">
+      <c r="F104" t="s">
+        <v>173</v>
+      </c>
+      <c r="J104" t="s">
         <v>174</v>
       </c>
-      <c r="E104" t="s">
-        <v>286</v>
-      </c>
-      <c r="F104" t="s">
+      <c r="K104" t="s">
         <v>175</v>
       </c>
-      <c r="J104" t="s">
+      <c r="L104" t="s">
         <v>176</v>
-      </c>
-      <c r="K104" t="s">
-        <v>177</v>
-      </c>
-      <c r="L104" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
+        <v>285</v>
+      </c>
+      <c r="C105" t="s">
+        <v>286</v>
+      </c>
+      <c r="E105" t="s">
         <v>287</v>
       </c>
-      <c r="C105" t="s">
+      <c r="M105" t="s">
         <v>288</v>
-      </c>
-      <c r="E105" t="s">
-        <v>289</v>
-      </c>
-      <c r="M105" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4047,16 +4047,16 @@
         <v>48</v>
       </c>
       <c r="B106" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C106" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E106" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M106" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4064,16 +4064,16 @@
         <v>48</v>
       </c>
       <c r="B107" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C107" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E107" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M107" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4081,10 +4081,10 @@
         <v>17</v>
       </c>
       <c r="B108" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G108" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4092,10 +4092,10 @@
         <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G109" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4103,25 +4103,25 @@
         <v>30</v>
       </c>
       <c r="B110" t="s">
+        <v>297</v>
+      </c>
+      <c r="C110" t="s">
+        <v>298</v>
+      </c>
+      <c r="E110" t="s">
         <v>299</v>
       </c>
-      <c r="C110" t="s">
+      <c r="J110" t="s">
+        <v>193</v>
+      </c>
+      <c r="K110" t="s">
+        <v>194</v>
+      </c>
+      <c r="L110" t="s">
+        <v>195</v>
+      </c>
+      <c r="M110" t="s">
         <v>300</v>
-      </c>
-      <c r="E110" t="s">
-        <v>301</v>
-      </c>
-      <c r="J110" t="s">
-        <v>195</v>
-      </c>
-      <c r="K110" t="s">
-        <v>196</v>
-      </c>
-      <c r="L110" t="s">
-        <v>197</v>
-      </c>
-      <c r="M110" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4129,13 +4129,13 @@
         <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G111" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M111" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4143,13 +4143,13 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G112" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M112" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4157,10 +4157,10 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="G113" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4168,10 +4168,10 @@
         <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="G114" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4179,13 +4179,13 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="G115" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="M115" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4193,13 +4193,13 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="G116" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="M116" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4207,7 +4207,7 @@
         <v>43</v>
       </c>
       <c r="B117" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4215,10 +4215,10 @@
         <v>25</v>
       </c>
       <c r="B118" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M118" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4226,13 +4226,13 @@
         <v>48</v>
       </c>
       <c r="B119" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C119" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E119" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4240,19 +4240,19 @@
         <v>78</v>
       </c>
       <c r="B120" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C120" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D120" t="s">
+        <v>124</v>
+      </c>
+      <c r="E120" t="s">
+        <v>253</v>
+      </c>
+      <c r="F120" t="s">
         <v>125</v>
-      </c>
-      <c r="E120" t="s">
-        <v>255</v>
-      </c>
-      <c r="F120" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4260,28 +4260,28 @@
         <v>28</v>
       </c>
       <c r="B121" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C121" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D121" t="s">
+        <v>129</v>
+      </c>
+      <c r="E121" t="s">
+        <v>318</v>
+      </c>
+      <c r="F121" t="s">
         <v>130</v>
-      </c>
-      <c r="E121" t="s">
-        <v>320</v>
-      </c>
-      <c r="F121" t="s">
-        <v>131</v>
       </c>
       <c r="I121" t="s">
         <v>29</v>
       </c>
       <c r="J121" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="M121" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4289,31 +4289,31 @@
         <v>30</v>
       </c>
       <c r="B122" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C122" t="s">
+        <v>259</v>
+      </c>
+      <c r="D122" t="s">
+        <v>136</v>
+      </c>
+      <c r="E122" t="s">
+        <v>260</v>
+      </c>
+      <c r="F122" t="s">
+        <v>137</v>
+      </c>
+      <c r="J122" t="s">
         <v>261</v>
       </c>
-      <c r="D122" t="s">
-        <v>137</v>
-      </c>
-      <c r="E122" t="s">
-        <v>262</v>
-      </c>
-      <c r="F122" t="s">
-        <v>138</v>
-      </c>
-      <c r="J122" t="s">
-        <v>263</v>
-      </c>
       <c r="K122" t="s">
+        <v>139</v>
+      </c>
+      <c r="L122" t="s">
         <v>140</v>
       </c>
-      <c r="L122" t="s">
-        <v>141</v>
-      </c>
       <c r="M122" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4321,13 +4321,13 @@
         <v>17</v>
       </c>
       <c r="B123" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="G123" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="M123" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4335,10 +4335,10 @@
         <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G124" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4346,16 +4346,16 @@
         <v>48</v>
       </c>
       <c r="B125" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="C125" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E125" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="M125" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4363,108 +4363,108 @@
         <v>48</v>
       </c>
       <c r="B126" t="s">
+        <v>328</v>
+      </c>
+      <c r="C126" t="s">
+        <v>329</v>
+      </c>
+      <c r="E126" t="s">
         <v>330</v>
       </c>
-      <c r="C126" t="s">
+      <c r="M126" t="s">
         <v>331</v>
-      </c>
-      <c r="E126" t="s">
-        <v>332</v>
-      </c>
-      <c r="M126" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B127" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C127" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D127" t="s">
+        <v>159</v>
+      </c>
+      <c r="E127" t="s">
+        <v>277</v>
+      </c>
+      <c r="F127" t="s">
+        <v>160</v>
+      </c>
+      <c r="J127" t="s">
         <v>161</v>
       </c>
-      <c r="E127" t="s">
-        <v>279</v>
-      </c>
-      <c r="F127" t="s">
+      <c r="K127" t="s">
         <v>162</v>
       </c>
-      <c r="J127" t="s">
+      <c r="L127" t="s">
         <v>163</v>
-      </c>
-      <c r="K127" t="s">
-        <v>164</v>
-      </c>
-      <c r="L127" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B128" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C128" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E128" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="M128" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B129" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C129" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D129" t="s">
+        <v>172</v>
+      </c>
+      <c r="E129" t="s">
+        <v>284</v>
+      </c>
+      <c r="F129" t="s">
+        <v>173</v>
+      </c>
+      <c r="J129" t="s">
         <v>174</v>
       </c>
-      <c r="E129" t="s">
-        <v>286</v>
-      </c>
-      <c r="F129" t="s">
+      <c r="K129" t="s">
         <v>175</v>
       </c>
-      <c r="J129" t="s">
+      <c r="L129" t="s">
         <v>176</v>
-      </c>
-      <c r="K129" t="s">
-        <v>177</v>
-      </c>
-      <c r="L129" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B130" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C130" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E130" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="M130" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4472,16 +4472,16 @@
         <v>48</v>
       </c>
       <c r="B131" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C131" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E131" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M131" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4489,16 +4489,16 @@
         <v>48</v>
       </c>
       <c r="B132" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C132" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E132" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M132" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4506,10 +4506,10 @@
         <v>17</v>
       </c>
       <c r="B133" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G133" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4517,10 +4517,10 @@
         <v>17</v>
       </c>
       <c r="B134" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G134" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4528,25 +4528,25 @@
         <v>30</v>
       </c>
       <c r="B135" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="C135" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E135" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="J135" t="s">
+        <v>193</v>
+      </c>
+      <c r="K135" t="s">
+        <v>194</v>
+      </c>
+      <c r="L135" t="s">
         <v>195</v>
       </c>
-      <c r="K135" t="s">
-        <v>196</v>
-      </c>
-      <c r="L135" t="s">
-        <v>197</v>
-      </c>
       <c r="M135" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4554,13 +4554,13 @@
         <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G136" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="M136" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4568,13 +4568,13 @@
         <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G137" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="M137" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4582,10 +4582,10 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G138" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4593,10 +4593,10 @@
         <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G139" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4604,13 +4604,13 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="G140" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="M140" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4618,13 +4618,13 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G141" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M141" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4632,7 +4632,7 @@
         <v>43</v>
       </c>
       <c r="B142" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4640,13 +4640,13 @@
         <v>78</v>
       </c>
       <c r="B144" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C144" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="M144" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4654,16 +4654,16 @@
         <v>78</v>
       </c>
       <c r="B145" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C145" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D145" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="M145" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4671,16 +4671,16 @@
         <v>78</v>
       </c>
       <c r="B146" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C146" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D146" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="M146" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4688,13 +4688,13 @@
         <v>78</v>
       </c>
       <c r="B147" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C147" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="M147" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4702,13 +4702,13 @@
         <v>78</v>
       </c>
       <c r="B148" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C148" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="M148" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4716,13 +4716,13 @@
         <v>78</v>
       </c>
       <c r="B149" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C149" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="M149" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4730,13 +4730,13 @@
         <v>17</v>
       </c>
       <c r="B151" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G151" t="s">
         <v>96</v>
       </c>
       <c r="M151" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4744,13 +4744,13 @@
         <v>17</v>
       </c>
       <c r="B152" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G152" t="s">
         <v>96</v>
       </c>
       <c r="M152" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4758,39 +4758,39 @@
         <v>48</v>
       </c>
       <c r="B153" t="s">
+        <v>364</v>
+      </c>
+      <c r="C153" t="s">
+        <v>515</v>
+      </c>
+      <c r="D153" t="s">
         <v>366</v>
       </c>
-      <c r="C153" t="s">
-        <v>517</v>
-      </c>
-      <c r="D153" t="s">
+      <c r="E153" t="s">
+        <v>365</v>
+      </c>
+      <c r="F153" t="s">
+        <v>367</v>
+      </c>
+      <c r="M153" t="s">
         <v>368</v>
-      </c>
-      <c r="E153" t="s">
-        <v>367</v>
-      </c>
-      <c r="F153" t="s">
-        <v>369</v>
-      </c>
-      <c r="M153" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
+        <v>369</v>
+      </c>
+      <c r="B154" t="s">
+        <v>370</v>
+      </c>
+      <c r="C154" t="s">
         <v>371</v>
       </c>
-      <c r="B154" t="s">
+      <c r="E154" t="s">
         <v>372</v>
       </c>
-      <c r="C154" t="s">
-        <v>373</v>
-      </c>
-      <c r="E154" t="s">
-        <v>374</v>
-      </c>
       <c r="M154" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4798,39 +4798,39 @@
         <v>48</v>
       </c>
       <c r="B155" t="s">
+        <v>373</v>
+      </c>
+      <c r="C155" t="s">
+        <v>516</v>
+      </c>
+      <c r="D155" t="s">
         <v>375</v>
       </c>
-      <c r="C155" t="s">
-        <v>518</v>
-      </c>
-      <c r="D155" t="s">
+      <c r="E155" t="s">
+        <v>374</v>
+      </c>
+      <c r="F155" t="s">
+        <v>376</v>
+      </c>
+      <c r="M155" t="s">
         <v>377</v>
-      </c>
-      <c r="E155" t="s">
-        <v>376</v>
-      </c>
-      <c r="F155" t="s">
-        <v>378</v>
-      </c>
-      <c r="M155" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
+        <v>378</v>
+      </c>
+      <c r="B156" t="s">
+        <v>379</v>
+      </c>
+      <c r="C156" t="s">
         <v>380</v>
       </c>
-      <c r="B156" t="s">
+      <c r="E156" t="s">
         <v>381</v>
       </c>
-      <c r="C156" t="s">
-        <v>382</v>
-      </c>
-      <c r="E156" t="s">
-        <v>383</v>
-      </c>
       <c r="M156" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4838,16 +4838,16 @@
         <v>48</v>
       </c>
       <c r="B157" t="s">
+        <v>382</v>
+      </c>
+      <c r="C157" t="s">
+        <v>517</v>
+      </c>
+      <c r="E157" t="s">
+        <v>383</v>
+      </c>
+      <c r="M157" t="s">
         <v>384</v>
-      </c>
-      <c r="C157" t="s">
-        <v>519</v>
-      </c>
-      <c r="E157" t="s">
-        <v>385</v>
-      </c>
-      <c r="M157" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4855,13 +4855,13 @@
         <v>17</v>
       </c>
       <c r="B158" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G158" t="s">
         <v>96</v>
       </c>
       <c r="M158" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4869,13 +4869,13 @@
         <v>17</v>
       </c>
       <c r="B159" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G159" t="s">
         <v>96</v>
       </c>
       <c r="M159" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4883,13 +4883,13 @@
         <v>17</v>
       </c>
       <c r="B160" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G160" t="s">
         <v>96</v>
       </c>
       <c r="M160" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4897,13 +4897,13 @@
         <v>17</v>
       </c>
       <c r="B161" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="G161" t="s">
         <v>96</v>
       </c>
       <c r="M161" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="162" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4919,13 +4919,13 @@
         <v>59</v>
       </c>
       <c r="B164" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="N164" s="1" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="165" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4933,7 +4933,7 @@
         <v>17</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="C165" s="4"/>
       <c r="G165" t="s">
@@ -4945,11 +4945,11 @@
         <v>17</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="C166" s="4"/>
       <c r="G166" s="3" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="167" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4957,11 +4957,11 @@
         <v>17</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="C167" s="4"/>
       <c r="G167" s="3" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="168" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4969,11 +4969,11 @@
         <v>17</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C168" s="4"/>
       <c r="G168" s="3" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="169" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4981,16 +4981,16 @@
         <v>48</v>
       </c>
       <c r="B169" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C169" s="5" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E169" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="M169" s="3" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="170" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4998,10 +4998,10 @@
         <v>48</v>
       </c>
       <c r="B170" s="7" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C170" s="7" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
     </row>
     <row r="171" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5009,10 +5009,10 @@
         <v>78</v>
       </c>
       <c r="B171" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="C171" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E171" t="s">
         <v>79</v>
@@ -5021,7 +5021,7 @@
         <v>22</v>
       </c>
       <c r="M171" s="3" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5029,10 +5029,10 @@
         <v>78</v>
       </c>
       <c r="B172" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C172" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E172" t="s">
         <v>79</v>
@@ -5041,67 +5041,67 @@
         <v>22</v>
       </c>
       <c r="M172" s="3" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
     </row>
     <row r="173" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
+        <v>504</v>
+      </c>
+      <c r="B173" t="s">
+        <v>505</v>
+      </c>
+      <c r="C173" s="6" t="s">
+        <v>537</v>
+      </c>
+      <c r="J173" t="s">
         <v>506</v>
       </c>
-      <c r="B173" t="s">
+      <c r="K173" t="s">
         <v>507</v>
       </c>
-      <c r="C173" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="J173" t="s">
-        <v>508</v>
-      </c>
-      <c r="K173" t="s">
-        <v>509</v>
-      </c>
       <c r="M173" s="3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="174" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B174" t="s">
+        <v>508</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>536</v>
+      </c>
+      <c r="J174" t="s">
         <v>510</v>
       </c>
-      <c r="C174" s="6" t="s">
-        <v>538</v>
-      </c>
-      <c r="J174" t="s">
-        <v>512</v>
-      </c>
       <c r="K174" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="175" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="B175" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="J175" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="K175" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="M175" s="3" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="177" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5109,7 +5109,7 @@
         <v>84</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
     </row>
     <row r="179" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5117,65 +5117,65 @@
         <v>98</v>
       </c>
       <c r="B179" t="s">
+        <v>393</v>
+      </c>
+      <c r="C179" t="s">
+        <v>394</v>
+      </c>
+      <c r="D179" t="s">
+        <v>396</v>
+      </c>
+      <c r="E179" t="s">
         <v>395</v>
       </c>
-      <c r="C179" t="s">
-        <v>396</v>
-      </c>
-      <c r="D179" t="s">
-        <v>398</v>
-      </c>
-      <c r="E179" t="s">
+      <c r="F179" t="s">
         <v>397</v>
-      </c>
-      <c r="F179" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
+        <v>398</v>
+      </c>
+      <c r="B180" t="s">
+        <v>399</v>
+      </c>
+      <c r="C180" t="s">
         <v>400</v>
       </c>
-      <c r="B180" t="s">
+      <c r="D180" t="s">
+        <v>402</v>
+      </c>
+      <c r="E180" t="s">
         <v>401</v>
       </c>
-      <c r="C180" t="s">
-        <v>402</v>
-      </c>
-      <c r="D180" t="s">
-        <v>404</v>
-      </c>
-      <c r="E180" t="s">
+      <c r="F180" t="s">
         <v>403</v>
-      </c>
-      <c r="F180" t="s">
-        <v>405</v>
       </c>
       <c r="H180" t="s">
         <v>22</v>
       </c>
       <c r="M180" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B181" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C181" t="s">
+        <v>400</v>
+      </c>
+      <c r="D181" t="s">
         <v>402</v>
       </c>
-      <c r="D181" t="s">
-        <v>404</v>
-      </c>
       <c r="E181" t="s">
+        <v>401</v>
+      </c>
+      <c r="F181" t="s">
         <v>403</v>
-      </c>
-      <c r="F181" t="s">
-        <v>405</v>
       </c>
       <c r="M181" t="s">
         <v>52</v>
@@ -5183,22 +5183,22 @@
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B182" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C182" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E182" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H182" t="s">
         <v>22</v>
       </c>
       <c r="M182" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5206,16 +5206,16 @@
         <v>48</v>
       </c>
       <c r="B183" t="s">
+        <v>410</v>
+      </c>
+      <c r="C183" t="s">
+        <v>411</v>
+      </c>
+      <c r="E183" t="s">
         <v>412</v>
       </c>
-      <c r="C183" t="s">
+      <c r="M183" t="s">
         <v>413</v>
-      </c>
-      <c r="E183" t="s">
-        <v>414</v>
-      </c>
-      <c r="M183" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5223,13 +5223,13 @@
         <v>20</v>
       </c>
       <c r="B184" t="s">
+        <v>414</v>
+      </c>
+      <c r="C184" t="s">
+        <v>415</v>
+      </c>
+      <c r="E184" t="s">
         <v>416</v>
-      </c>
-      <c r="C184" t="s">
-        <v>417</v>
-      </c>
-      <c r="E184" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5245,10 +5245,10 @@
         <v>17</v>
       </c>
       <c r="B187" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="G187" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5256,10 +5256,10 @@
         <v>17</v>
       </c>
       <c r="B188" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="G188" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5267,10 +5267,10 @@
         <v>17</v>
       </c>
       <c r="B189" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="G189" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5278,10 +5278,10 @@
         <v>17</v>
       </c>
       <c r="B190" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="G190" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5289,10 +5289,10 @@
         <v>17</v>
       </c>
       <c r="B191" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="G191" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5300,10 +5300,10 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G192" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -5327,7 +5327,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5347,10 +5347,10 @@
         <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D2" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5358,24 +5358,24 @@
         <v>97</v>
       </c>
       <c r="B3" t="s">
+        <v>432</v>
+      </c>
+      <c r="C3" t="s">
+        <v>433</v>
+      </c>
+      <c r="D3" t="s">
         <v>434</v>
-      </c>
-      <c r="C3" t="s">
-        <v>435</v>
-      </c>
-      <c r="D3" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="C4" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5386,10 +5386,10 @@
         <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5397,13 +5397,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5411,471 +5411,471 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
+        <v>440</v>
+      </c>
+      <c r="C7" t="s">
+        <v>518</v>
+      </c>
+      <c r="D7" t="s">
         <v>442</v>
-      </c>
-      <c r="C7" t="s">
-        <v>520</v>
-      </c>
-      <c r="D7" t="s">
-        <v>444</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B8" t="s">
         <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>561</v>
+      </c>
+      <c r="B9" t="s">
+        <v>432</v>
+      </c>
+      <c r="C9" t="s">
         <v>563</v>
-      </c>
-      <c r="B9" t="s">
-        <v>434</v>
-      </c>
-      <c r="C9" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B10" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C10" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B11" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B12" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C12" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B13" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C13" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B14" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="C14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B15" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C15" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B16" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C16" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B17" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C17" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B18" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C18" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B19" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C19" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B20" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="C20" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B21" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C21" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B22" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C22" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B23" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C23" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B24" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C24" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B25" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C25" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B26" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C26" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B27" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C27" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B28" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C28" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B29" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C29" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B30" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C30" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B31" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C31" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B32" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C32" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B33" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C33" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B34" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C34" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B35" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C35" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B36" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C36" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B37" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C37" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B38" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C38" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B39" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C39" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B40" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C40" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B41" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C41" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="B42" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C42" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D42" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
+        <v>443</v>
+      </c>
+      <c r="B43" t="s">
         <v>445</v>
       </c>
-      <c r="B43" t="s">
-        <v>447</v>
-      </c>
       <c r="C43" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D43" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
+        <v>446</v>
+      </c>
+      <c r="B44" t="s">
+        <v>447</v>
+      </c>
+      <c r="C44" t="s">
         <v>448</v>
       </c>
-      <c r="B44" t="s">
+      <c r="D44" t="s">
         <v>449</v>
-      </c>
-      <c r="C44" t="s">
-        <v>450</v>
-      </c>
-      <c r="D44" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="B45" t="s">
+        <v>450</v>
+      </c>
+      <c r="C45" t="s">
+        <v>451</v>
+      </c>
+      <c r="D45" t="s">
         <v>452</v>
-      </c>
-      <c r="C45" t="s">
-        <v>453</v>
-      </c>
-      <c r="D45" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>453</v>
+      </c>
+      <c r="B46" t="s">
+        <v>454</v>
+      </c>
+      <c r="C46" t="s">
         <v>455</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>456</v>
-      </c>
-      <c r="C46" t="s">
-        <v>457</v>
-      </c>
-      <c r="D46" t="s">
-        <v>458</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="B47" t="s">
+        <v>457</v>
+      </c>
+      <c r="C47" t="s">
+        <v>458</v>
+      </c>
+      <c r="D47" t="s">
         <v>459</v>
-      </c>
-      <c r="C47" t="s">
-        <v>460</v>
-      </c>
-      <c r="D47" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5886,10 +5886,10 @@
         <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D48" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5897,13 +5897,13 @@
         <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C49" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D49" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5911,13 +5911,13 @@
         <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C50" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D50" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5925,195 +5925,195 @@
         <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C51" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D51" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B52" t="s">
         <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D52" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
+        <v>467</v>
+      </c>
+      <c r="B53" t="s">
+        <v>432</v>
+      </c>
+      <c r="C53" t="s">
+        <v>468</v>
+      </c>
+      <c r="D53" t="s">
         <v>469</v>
-      </c>
-      <c r="B53" t="s">
-        <v>434</v>
-      </c>
-      <c r="C53" t="s">
-        <v>470</v>
-      </c>
-      <c r="D53" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="B54" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C54" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D54" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B55" t="s">
         <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D55" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
+        <v>472</v>
+      </c>
+      <c r="B56" t="s">
+        <v>432</v>
+      </c>
+      <c r="C56" t="s">
+        <v>473</v>
+      </c>
+      <c r="D56" t="s">
         <v>474</v>
-      </c>
-      <c r="B56" t="s">
-        <v>434</v>
-      </c>
-      <c r="C56" t="s">
-        <v>475</v>
-      </c>
-      <c r="D56" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B57" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C57" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="D57" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B58" t="s">
         <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="D58" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B59" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C59" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="D59" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B60" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="C60" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D60" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>482</v>
+      </c>
+      <c r="B61" t="s">
         <v>484</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
+        <v>485</v>
+      </c>
+      <c r="D61" t="s">
         <v>486</v>
-      </c>
-      <c r="C61" t="s">
-        <v>487</v>
-      </c>
-      <c r="D61" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
+        <v>487</v>
+      </c>
+      <c r="B62" t="s">
+        <v>440</v>
+      </c>
+      <c r="C62" t="s">
+        <v>488</v>
+      </c>
+      <c r="D62" t="s">
         <v>489</v>
-      </c>
-      <c r="B62" t="s">
-        <v>442</v>
-      </c>
-      <c r="C62" t="s">
-        <v>490</v>
-      </c>
-      <c r="D62" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B63" t="s">
         <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="D63" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B64" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C64" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="D64" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -6131,30 +6131,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B1" t="s">
+        <v>493</v>
+      </c>
+      <c r="C1" t="s">
         <v>494</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>495</v>
-      </c>
-      <c r="C1" t="s">
-        <v>496</v>
-      </c>
-      <c r="D1" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
+        <v>496</v>
+      </c>
+      <c r="B2" t="s">
+        <v>497</v>
+      </c>
+      <c r="C2" t="s">
         <v>498</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>499</v>
-      </c>
-      <c r="C2" t="s">
-        <v>500</v>
-      </c>
-      <c r="D2" t="s">
-        <v>501</v>
       </c>
     </row>
   </sheetData>
@@ -6163,21 +6163,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6227,80 +6212,22 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6739,10 +6666,83 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6756,36 +6756,14 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6806,4 +6784,26 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
removed upper from name
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{0A0EC0EE-9F77-4AA4-946E-576A5AF19B48}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C9DDF55E-0FA5-454C-99F0-6557C1245B8D}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1035" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="634">
   <si>
     <t>type</t>
   </si>
@@ -378,9 +378,6 @@
     <t>child_name_note</t>
   </si>
   <si>
-    <t>Now entering data for child: ${child_name} (${CHSEX}) with age in years: ${child_age_years}</t>
-  </si>
-  <si>
     <t>Saisie des données pour l'enfant : ${child_name} (${CHSEX}) âgé(e) de ${child_age_years} an(s)</t>
   </si>
   <si>
@@ -480,9 +477,6 @@
     <t>age_confirm</t>
   </si>
   <si>
-    <t>${child_name}   is ${MONTHS} months old.</t>
-  </si>
-  <si>
     <t>${child_name}   est âgé(e) de ${MONTHS} mois.</t>
   </si>
   <si>
@@ -490,9 +484,6 @@
   </si>
   <si>
     <t>child_under_five</t>
-  </si>
-  <si>
-    <t>${child_present} = 1</t>
   </si>
   <si>
     <t>decimal</t>
@@ -1364,9 +1355,6 @@
     <t>${child_name}  ne présente pas de conditions indiquant une malnutrition aigüe</t>
   </si>
   <si>
-    <t>${child_present} = 1 and ${mam_case} !=1 and ${sam_case} !=1</t>
-  </si>
-  <si>
     <t>child_eligible</t>
   </si>
   <si>
@@ -1376,9 +1364,6 @@
     <t>child_measured</t>
   </si>
   <si>
-    <t>${child_present} = 1 and (${WEIGHT}&gt;0 or ${HEIGHT}&gt;0 or ${MUAC}&gt;0 or ${EDEMA} = 'y' or ${EDEMA} = 'n')</t>
-  </si>
-  <si>
     <t>child_malnourished</t>
   </si>
   <si>
@@ -1700,15 +1685,9 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>SMART_Survey_GPS_059_EN_FR_10</t>
-  </si>
-  <si>
     <t>1 (2021-05-28 13:32:32)</t>
   </si>
   <si>
-    <t>concat('SMART_Survey_GPS_059','_HH',${HH})</t>
-  </si>
-  <si>
     <t>English</t>
   </si>
   <si>
@@ -2100,6 +2079,33 @@
   </si>
   <si>
     <t xml:space="preserve">${MONTHS}&gt;5 or (${MONTHS}=98 and ${HEIGHT}&gt;67) </t>
+  </si>
+  <si>
+    <t>(${child_name}) is ${MONTHS} months old.</t>
+  </si>
+  <si>
+    <t>ACO_SMART_Survey_2021</t>
+  </si>
+  <si>
+    <t>concat('ACO_SMART_Survey_2021','_HH',${HH})</t>
+  </si>
+  <si>
+    <t>${mam_case} !=1 and ${sam_case} !=1</t>
+  </si>
+  <si>
+    <t>(${WEIGHT}&gt;0 or ${HEIGHT}&gt;0 or ${MUAC}&gt;0 or ${EDEMA} = 'y' or ${EDEMA} = 'n')</t>
+  </si>
+  <si>
+    <t>name_lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name </t>
+  </si>
+  <si>
+    <t>translate(${name_lower}, "abcdefghijklmnopqrstuvwxyz", "ABCDEFGHIJKLMNOPQRSTUVWXYZ")</t>
+  </si>
+  <si>
+    <t>Now entering data for child: ${child_name} (${CHSEX}) with age in years: ${child_age_years}</t>
   </si>
 </sst>
 </file>
@@ -2159,7 +2165,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -2172,6 +2178,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2510,11 +2520,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N192"/>
+  <dimension ref="A1:N193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58:XFD58"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2608,13 +2618,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>560</v>
+        <v>553</v>
       </c>
       <c r="B6" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="C6" t="s">
-        <v>562</v>
+        <v>555</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2761,10 +2771,10 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>597</v>
+        <v>590</v>
       </c>
       <c r="E17" t="s">
-        <v>598</v>
+        <v>591</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2854,7 +2864,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>1</v>
+        <v>630</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
@@ -2867,167 +2877,169 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" t="s">
-        <v>68</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" t="s">
-        <v>22</v>
+      <c r="A24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="G24" s="8" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="H25" t="s">
         <v>22</v>
       </c>
-      <c r="J25" t="s">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H26" t="s">
+        <v>22</v>
+      </c>
+      <c r="J26" t="s">
         <v>75</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K26" t="s">
         <v>76</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L26" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A29" t="s">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
         <v>43</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="2" t="s">
+    <row r="31" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G31" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A31" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>522</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A32" t="s">
-        <v>17</v>
-      </c>
-      <c r="B32" t="s">
-        <v>82</v>
-      </c>
-      <c r="C32" s="3"/>
-      <c r="G32" t="s">
-        <v>83</v>
+    <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>534</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="B33" t="s">
-        <v>60</v>
+        <v>82</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="G33" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>85</v>
-      </c>
-      <c r="G34" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="B35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" t="s">
-        <v>88</v>
-      </c>
-      <c r="E35" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" t="s">
-        <v>22</v>
-      </c>
-      <c r="M35" t="s">
-        <v>53</v>
+        <v>85</v>
+      </c>
+      <c r="G35" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" t="s">
+        <v>89</v>
+      </c>
+      <c r="H36" t="s">
+        <v>22</v>
+      </c>
+      <c r="M36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
         <v>30</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>90</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C37" t="s">
         <v>91</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D37" t="s">
         <v>93</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E37" t="s">
         <v>92</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F37" t="s">
         <v>94</v>
       </c>
-      <c r="M36" t="s">
+      <c r="M37" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="39" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3035,21 +3047,21 @@
         <v>17</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="G40" s="2" t="s">
         <v>102</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A40" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>523</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>525</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3057,39 +3069,39 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="G41" s="1" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="43" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A43" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="44" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N43" s="2" t="s">
+      <c r="N44" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" t="s">
-        <v>17</v>
-      </c>
-      <c r="B44" t="s">
-        <v>107</v>
-      </c>
-      <c r="G44" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3097,10 +3109,10 @@
         <v>17</v>
       </c>
       <c r="B45" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G45" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3108,10 +3120,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G46" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3119,10 +3131,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G47" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3130,136 +3142,133 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G48" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>117</v>
-      </c>
-      <c r="C49" t="s">
-        <v>118</v>
-      </c>
-      <c r="E49" t="s">
-        <v>119</v>
-      </c>
-      <c r="M49" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="G49" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>121</v>
+        <v>117</v>
+      </c>
+      <c r="C50" t="s">
+        <v>633</v>
+      </c>
+      <c r="E50" t="s">
+        <v>118</v>
       </c>
       <c r="M50" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B51" t="s">
-        <v>122</v>
-      </c>
-      <c r="C51" t="s">
-        <v>123</v>
-      </c>
-      <c r="D51" t="s">
-        <v>125</v>
-      </c>
-      <c r="E51" t="s">
-        <v>124</v>
-      </c>
-      <c r="F51" t="s">
-        <v>126</v>
-      </c>
-      <c r="H51" t="s">
-        <v>22</v>
+        <v>120</v>
+      </c>
+      <c r="M51" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B52" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C52" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D52" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E52" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="F52" t="s">
-        <v>131</v>
-      </c>
-      <c r="I52" t="s">
-        <v>29</v>
-      </c>
-      <c r="J52" t="s">
-        <v>132</v>
-      </c>
-      <c r="M52" t="s">
-        <v>133</v>
+        <v>125</v>
+      </c>
+      <c r="H52" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B53" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="D53" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E53" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F53" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="I53" t="s">
+        <v>29</v>
       </c>
       <c r="J53" t="s">
-        <v>139</v>
-      </c>
-      <c r="K53" t="s">
-        <v>140</v>
-      </c>
-      <c r="L53" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="M53" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>143</v>
-      </c>
-      <c r="G54" t="s">
-        <v>144</v>
+        <v>133</v>
+      </c>
+      <c r="C54" t="s">
+        <v>134</v>
+      </c>
+      <c r="D54" t="s">
+        <v>136</v>
+      </c>
+      <c r="E54" t="s">
+        <v>135</v>
+      </c>
+      <c r="F54" t="s">
+        <v>137</v>
+      </c>
+      <c r="J54" t="s">
+        <v>138</v>
+      </c>
+      <c r="K54" t="s">
+        <v>139</v>
+      </c>
+      <c r="L54" t="s">
+        <v>140</v>
       </c>
       <c r="M54" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3267,27 +3276,24 @@
         <v>17</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G55" t="s">
-        <v>146</v>
+        <v>143</v>
+      </c>
+      <c r="M55" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
-      </c>
-      <c r="C56" t="s">
-        <v>148</v>
-      </c>
-      <c r="E56" t="s">
-        <v>149</v>
-      </c>
-      <c r="M56" t="s">
-        <v>150</v>
+        <v>144</v>
+      </c>
+      <c r="G56" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3295,136 +3301,133 @@
         <v>48</v>
       </c>
       <c r="B57" t="s">
+        <v>146</v>
+      </c>
+      <c r="C57" t="s">
+        <v>147</v>
+      </c>
+      <c r="E57" t="s">
+        <v>148</v>
+      </c>
+      <c r="M57" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>48</v>
+      </c>
+      <c r="B58" t="s">
+        <v>150</v>
+      </c>
+      <c r="C58" t="s">
+        <v>625</v>
+      </c>
+      <c r="E58" t="s">
         <v>151</v>
       </c>
-      <c r="C57" t="s">
+      <c r="M58" t="s">
         <v>152</v>
-      </c>
-      <c r="E57" t="s">
-        <v>153</v>
-      </c>
-      <c r="M57" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A59" t="s">
-        <v>25</v>
-      </c>
-      <c r="B59" t="s">
-        <v>155</v>
-      </c>
-      <c r="M59" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>157</v>
+        <v>25</v>
       </c>
       <c r="B60" t="s">
-        <v>158</v>
-      </c>
-      <c r="C60" t="s">
-        <v>159</v>
-      </c>
-      <c r="D60" t="s">
-        <v>161</v>
-      </c>
-      <c r="E60" t="s">
-        <v>160</v>
-      </c>
-      <c r="F60" t="s">
-        <v>162</v>
-      </c>
-      <c r="J60" t="s">
-        <v>163</v>
-      </c>
-      <c r="K60" t="s">
-        <v>164</v>
-      </c>
-      <c r="L60" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C61" t="s">
-        <v>168</v>
+        <v>156</v>
+      </c>
+      <c r="D61" t="s">
+        <v>158</v>
       </c>
       <c r="E61" t="s">
-        <v>169</v>
-      </c>
-      <c r="M61" t="s">
-        <v>170</v>
+        <v>157</v>
+      </c>
+      <c r="F61" t="s">
+        <v>159</v>
+      </c>
+      <c r="J61" t="s">
+        <v>160</v>
+      </c>
+      <c r="K61" t="s">
+        <v>161</v>
+      </c>
+      <c r="L61" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B62" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="C62" t="s">
-        <v>172</v>
-      </c>
-      <c r="D62" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="E62" t="s">
-        <v>173</v>
-      </c>
-      <c r="F62" t="s">
-        <v>175</v>
-      </c>
-      <c r="J62" t="s">
-        <v>176</v>
-      </c>
-      <c r="K62" t="s">
-        <v>177</v>
-      </c>
-      <c r="L62" t="s">
-        <v>178</v>
+        <v>166</v>
+      </c>
+      <c r="M62" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="C63" t="s">
-        <v>181</v>
+        <v>169</v>
+      </c>
+      <c r="D63" t="s">
+        <v>171</v>
       </c>
       <c r="E63" t="s">
-        <v>182</v>
-      </c>
-      <c r="M63" t="s">
-        <v>183</v>
+        <v>170</v>
+      </c>
+      <c r="F63" t="s">
+        <v>172</v>
+      </c>
+      <c r="J63" t="s">
+        <v>173</v>
+      </c>
+      <c r="K63" t="s">
+        <v>174</v>
+      </c>
+      <c r="L63" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B64" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C64" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="E64" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="M64" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3432,84 +3435,93 @@
         <v>48</v>
       </c>
       <c r="B65" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C65" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E65" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="M65" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C66" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E66" t="s">
-        <v>194</v>
-      </c>
-      <c r="J66" t="s">
-        <v>195</v>
-      </c>
-      <c r="K66" t="s">
-        <v>196</v>
-      </c>
-      <c r="L66" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="M66" t="s">
-        <v>198</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>166</v>
+        <v>30</v>
       </c>
       <c r="B67" t="s">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="E67" t="s">
-        <v>201</v>
+        <v>191</v>
+      </c>
+      <c r="J67" t="s">
+        <v>192</v>
+      </c>
+      <c r="K67" t="s">
+        <v>193</v>
+      </c>
+      <c r="L67" t="s">
+        <v>194</v>
+      </c>
+      <c r="M67" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
       <c r="B68" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="C68" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E68" t="s">
-        <v>204</v>
-      </c>
-      <c r="H68" t="s">
-        <v>22</v>
-      </c>
-      <c r="M68" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B69" t="s">
-        <v>155</v>
+        <v>199</v>
+      </c>
+      <c r="C69" t="s">
+        <v>200</v>
+      </c>
+      <c r="E69" t="s">
+        <v>201</v>
+      </c>
+      <c r="H69" t="s">
+        <v>22</v>
+      </c>
+      <c r="M69" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3517,18 +3529,15 @@
         <v>43</v>
       </c>
       <c r="B70" t="s">
-        <v>121</v>
+        <v>153</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>206</v>
-      </c>
-      <c r="G71" t="s">
-        <v>207</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3536,10 +3545,10 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="G72" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3547,10 +3556,10 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="G73" t="s">
-        <v>502</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3558,10 +3567,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="G74" t="s">
-        <v>212</v>
+        <v>495</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3569,13 +3578,10 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="G75" t="s">
-        <v>214</v>
-      </c>
-      <c r="M75" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3583,13 +3589,13 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G76" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="M76" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3597,10 +3603,13 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="G77" t="s">
-        <v>219</v>
+        <v>214</v>
+      </c>
+      <c r="M77" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3608,13 +3617,10 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="G78" t="s">
-        <v>221</v>
-      </c>
-      <c r="M78" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3622,13 +3628,13 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G79" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="M79" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3636,10 +3642,13 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="G80" t="s">
-        <v>225</v>
+        <v>220</v>
+      </c>
+      <c r="M80" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3647,13 +3656,10 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="G81" t="s">
-        <v>227</v>
-      </c>
-      <c r="M81" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3661,13 +3667,13 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="G82" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="M82" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3675,10 +3681,13 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="G83" t="s">
-        <v>231</v>
+        <v>226</v>
+      </c>
+      <c r="M83" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3686,10 +3695,10 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="G84" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3697,13 +3706,10 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="G85" t="s">
-        <v>235</v>
-      </c>
-      <c r="M85" t="s">
-        <v>156</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3711,13 +3717,10 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="G86" t="s">
-        <v>237</v>
-      </c>
-      <c r="M86" t="s">
-        <v>156</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3725,10 +3728,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="G87" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3736,10 +3739,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="G88" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3747,13 +3750,10 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="G89" t="s">
-        <v>243</v>
-      </c>
-      <c r="M89" t="s">
-        <v>156</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3761,13 +3761,10 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="G90" t="s">
-        <v>245</v>
-      </c>
-      <c r="M90" t="s">
-        <v>156</v>
+        <v>240</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3775,134 +3772,128 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G91" t="s">
-        <v>247</v>
-      </c>
-      <c r="M91" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A93" t="s">
-        <v>25</v>
-      </c>
-      <c r="B93" t="s">
-        <v>248</v>
-      </c>
-      <c r="M93" t="s">
-        <v>249</v>
-      </c>
-    </row>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>243</v>
+      </c>
+      <c r="G92" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B94" t="s">
-        <v>250</v>
-      </c>
-      <c r="C94" t="s">
-        <v>251</v>
-      </c>
-      <c r="E94" t="s">
-        <v>252</v>
+        <v>245</v>
+      </c>
+      <c r="M94" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B95" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="C95" t="s">
-        <v>254</v>
-      </c>
-      <c r="D95" t="s">
-        <v>125</v>
+        <v>248</v>
       </c>
       <c r="E95" t="s">
-        <v>255</v>
-      </c>
-      <c r="F95" t="s">
-        <v>126</v>
+        <v>249</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B96" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="C96" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D96" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E96" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="F96" t="s">
-        <v>131</v>
-      </c>
-      <c r="I96" t="s">
-        <v>29</v>
-      </c>
-      <c r="J96" t="s">
-        <v>132</v>
-      </c>
-      <c r="M96" t="s">
-        <v>259</v>
+        <v>125</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B97" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C97" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D97" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E97" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F97" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="I97" t="s">
+        <v>29</v>
       </c>
       <c r="J97" t="s">
-        <v>263</v>
-      </c>
-      <c r="K97" t="s">
-        <v>140</v>
-      </c>
-      <c r="L97" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="M97" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B98" t="s">
-        <v>265</v>
-      </c>
-      <c r="G98" t="s">
-        <v>266</v>
+        <v>257</v>
+      </c>
+      <c r="C98" t="s">
+        <v>258</v>
+      </c>
+      <c r="D98" t="s">
+        <v>136</v>
+      </c>
+      <c r="E98" t="s">
+        <v>259</v>
+      </c>
+      <c r="F98" t="s">
+        <v>137</v>
+      </c>
+      <c r="J98" t="s">
+        <v>260</v>
+      </c>
+      <c r="K98" t="s">
+        <v>139</v>
+      </c>
+      <c r="L98" t="s">
+        <v>140</v>
       </c>
       <c r="M98" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3910,27 +3901,24 @@
         <v>17</v>
       </c>
       <c r="B99" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G99" t="s">
-        <v>268</v>
+        <v>263</v>
+      </c>
+      <c r="M99" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>269</v>
-      </c>
-      <c r="C100" t="s">
-        <v>270</v>
-      </c>
-      <c r="E100" t="s">
-        <v>271</v>
-      </c>
-      <c r="M100" t="s">
-        <v>272</v>
+        <v>264</v>
+      </c>
+      <c r="G100" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3938,125 +3926,125 @@
         <v>48</v>
       </c>
       <c r="B101" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C101" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E101" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="M101" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
       <c r="B102" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C102" t="s">
-        <v>278</v>
-      </c>
-      <c r="D102" t="s">
-        <v>161</v>
+        <v>271</v>
       </c>
       <c r="E102" t="s">
-        <v>279</v>
-      </c>
-      <c r="F102" t="s">
-        <v>162</v>
-      </c>
-      <c r="J102" t="s">
-        <v>163</v>
-      </c>
-      <c r="K102" t="s">
-        <v>164</v>
-      </c>
-      <c r="L102" t="s">
-        <v>165</v>
+        <v>272</v>
+      </c>
+      <c r="M102" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B103" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="C103" t="s">
-        <v>281</v>
+        <v>275</v>
+      </c>
+      <c r="D103" t="s">
+        <v>158</v>
       </c>
       <c r="E103" t="s">
-        <v>282</v>
-      </c>
-      <c r="M103" t="s">
-        <v>283</v>
+        <v>276</v>
+      </c>
+      <c r="F103" t="s">
+        <v>159</v>
+      </c>
+      <c r="J103" t="s">
+        <v>160</v>
+      </c>
+      <c r="K103" t="s">
+        <v>161</v>
+      </c>
+      <c r="L103" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B104" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C104" t="s">
-        <v>285</v>
-      </c>
-      <c r="D104" t="s">
-        <v>174</v>
+        <v>278</v>
       </c>
       <c r="E104" t="s">
-        <v>286</v>
-      </c>
-      <c r="F104" t="s">
-        <v>175</v>
-      </c>
-      <c r="J104" t="s">
-        <v>176</v>
-      </c>
-      <c r="K104" t="s">
-        <v>177</v>
-      </c>
-      <c r="L104" t="s">
-        <v>178</v>
+        <v>279</v>
+      </c>
+      <c r="M104" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="B105" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C105" t="s">
-        <v>288</v>
+        <v>282</v>
+      </c>
+      <c r="D105" t="s">
+        <v>171</v>
       </c>
       <c r="E105" t="s">
-        <v>289</v>
-      </c>
-      <c r="M105" t="s">
-        <v>290</v>
+        <v>283</v>
+      </c>
+      <c r="F105" t="s">
+        <v>172</v>
+      </c>
+      <c r="J105" t="s">
+        <v>173</v>
+      </c>
+      <c r="K105" t="s">
+        <v>174</v>
+      </c>
+      <c r="L105" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B106" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C106" t="s">
-        <v>185</v>
+        <v>285</v>
       </c>
       <c r="E106" t="s">
-        <v>186</v>
+        <v>286</v>
       </c>
       <c r="M106" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4064,27 +4052,33 @@
         <v>48</v>
       </c>
       <c r="B107" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C107" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E107" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="M107" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B108" t="s">
-        <v>295</v>
-      </c>
-      <c r="G108" t="s">
-        <v>296</v>
+        <v>290</v>
+      </c>
+      <c r="C108" t="s">
+        <v>186</v>
+      </c>
+      <c r="E108" t="s">
+        <v>187</v>
+      </c>
+      <c r="M108" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4092,50 +4086,47 @@
         <v>17</v>
       </c>
       <c r="B109" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="G109" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B110" t="s">
-        <v>299</v>
-      </c>
-      <c r="C110" t="s">
-        <v>300</v>
-      </c>
-      <c r="E110" t="s">
-        <v>301</v>
-      </c>
-      <c r="J110" t="s">
-        <v>195</v>
-      </c>
-      <c r="K110" t="s">
-        <v>196</v>
-      </c>
-      <c r="L110" t="s">
-        <v>197</v>
-      </c>
-      <c r="M110" t="s">
-        <v>302</v>
+        <v>294</v>
+      </c>
+      <c r="G110" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B111" t="s">
-        <v>303</v>
-      </c>
-      <c r="G111" t="s">
-        <v>304</v>
+        <v>296</v>
+      </c>
+      <c r="C111" t="s">
+        <v>297</v>
+      </c>
+      <c r="E111" t="s">
+        <v>298</v>
+      </c>
+      <c r="J111" t="s">
+        <v>192</v>
+      </c>
+      <c r="K111" t="s">
+        <v>193</v>
+      </c>
+      <c r="L111" t="s">
+        <v>194</v>
       </c>
       <c r="M111" t="s">
-        <v>156</v>
+        <v>299</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4143,13 +4134,10 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="G112" t="s">
-        <v>306</v>
-      </c>
-      <c r="M112" t="s">
-        <v>156</v>
+        <v>301</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4157,10 +4145,10 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="G113" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4168,10 +4156,10 @@
         <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="G114" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4179,13 +4167,10 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="G115" t="s">
-        <v>312</v>
-      </c>
-      <c r="M115" t="s">
-        <v>156</v>
+        <v>307</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4193,141 +4178,135 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="G116" t="s">
-        <v>314</v>
-      </c>
-      <c r="M116" t="s">
-        <v>156</v>
+        <v>309</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A117" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>248</v>
+        <v>310</v>
+      </c>
+      <c r="G117" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B118" t="s">
-        <v>315</v>
-      </c>
-      <c r="M118" t="s">
-        <v>316</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B119" t="s">
-        <v>317</v>
-      </c>
-      <c r="C119" t="s">
-        <v>251</v>
-      </c>
-      <c r="E119" t="s">
-        <v>252</v>
+        <v>312</v>
+      </c>
+      <c r="M119" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B120" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C120" t="s">
-        <v>254</v>
-      </c>
-      <c r="D120" t="s">
-        <v>125</v>
+        <v>248</v>
       </c>
       <c r="E120" t="s">
-        <v>255</v>
-      </c>
-      <c r="F120" t="s">
-        <v>126</v>
+        <v>249</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B121" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C121" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D121" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E121" t="s">
-        <v>320</v>
+        <v>252</v>
       </c>
       <c r="F121" t="s">
-        <v>131</v>
-      </c>
-      <c r="I121" t="s">
-        <v>29</v>
-      </c>
-      <c r="J121" t="s">
-        <v>132</v>
-      </c>
-      <c r="M121" t="s">
-        <v>321</v>
+        <v>125</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B122" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="C122" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="D122" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E122" t="s">
-        <v>262</v>
+        <v>317</v>
       </c>
       <c r="F122" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="I122" t="s">
+        <v>29</v>
       </c>
       <c r="J122" t="s">
-        <v>263</v>
-      </c>
-      <c r="K122" t="s">
-        <v>140</v>
-      </c>
-      <c r="L122" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="M122" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B123" t="s">
-        <v>324</v>
-      </c>
-      <c r="G123" t="s">
-        <v>325</v>
+        <v>319</v>
+      </c>
+      <c r="C123" t="s">
+        <v>258</v>
+      </c>
+      <c r="D123" t="s">
+        <v>136</v>
+      </c>
+      <c r="E123" t="s">
+        <v>259</v>
+      </c>
+      <c r="F123" t="s">
+        <v>137</v>
+      </c>
+      <c r="J123" t="s">
+        <v>260</v>
+      </c>
+      <c r="K123" t="s">
+        <v>139</v>
+      </c>
+      <c r="L123" t="s">
+        <v>140</v>
       </c>
       <c r="M123" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4335,27 +4314,24 @@
         <v>17</v>
       </c>
       <c r="B124" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="G124" t="s">
-        <v>327</v>
+        <v>322</v>
+      </c>
+      <c r="M124" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>328</v>
-      </c>
-      <c r="C125" t="s">
-        <v>270</v>
-      </c>
-      <c r="E125" t="s">
-        <v>271</v>
-      </c>
-      <c r="M125" t="s">
-        <v>329</v>
+        <v>323</v>
+      </c>
+      <c r="G125" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4363,125 +4339,125 @@
         <v>48</v>
       </c>
       <c r="B126" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C126" t="s">
-        <v>331</v>
+        <v>267</v>
       </c>
       <c r="E126" t="s">
-        <v>332</v>
+        <v>268</v>
       </c>
       <c r="M126" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>157</v>
+        <v>48</v>
       </c>
       <c r="B127" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C127" t="s">
-        <v>278</v>
-      </c>
-      <c r="D127" t="s">
-        <v>161</v>
+        <v>328</v>
       </c>
       <c r="E127" t="s">
-        <v>279</v>
-      </c>
-      <c r="F127" t="s">
-        <v>162</v>
-      </c>
-      <c r="J127" t="s">
-        <v>163</v>
-      </c>
-      <c r="K127" t="s">
-        <v>164</v>
-      </c>
-      <c r="L127" t="s">
-        <v>165</v>
+        <v>329</v>
+      </c>
+      <c r="M127" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>166</v>
+        <v>154</v>
       </c>
       <c r="B128" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="C128" t="s">
-        <v>281</v>
+        <v>275</v>
+      </c>
+      <c r="D128" t="s">
+        <v>158</v>
       </c>
       <c r="E128" t="s">
-        <v>282</v>
-      </c>
-      <c r="M128" t="s">
-        <v>336</v>
+        <v>276</v>
+      </c>
+      <c r="F128" t="s">
+        <v>159</v>
+      </c>
+      <c r="J128" t="s">
+        <v>160</v>
+      </c>
+      <c r="K128" t="s">
+        <v>161</v>
+      </c>
+      <c r="L128" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="B129" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="C129" t="s">
-        <v>285</v>
-      </c>
-      <c r="D129" t="s">
-        <v>174</v>
+        <v>278</v>
       </c>
       <c r="E129" t="s">
-        <v>286</v>
-      </c>
-      <c r="F129" t="s">
-        <v>175</v>
-      </c>
-      <c r="J129" t="s">
-        <v>176</v>
-      </c>
-      <c r="K129" t="s">
-        <v>177</v>
-      </c>
-      <c r="L129" t="s">
-        <v>178</v>
+        <v>279</v>
+      </c>
+      <c r="M129" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="B130" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C130" t="s">
-        <v>288</v>
+        <v>282</v>
+      </c>
+      <c r="D130" t="s">
+        <v>171</v>
       </c>
       <c r="E130" t="s">
-        <v>289</v>
-      </c>
-      <c r="M130" t="s">
-        <v>339</v>
+        <v>283</v>
+      </c>
+      <c r="F130" t="s">
+        <v>172</v>
+      </c>
+      <c r="J130" t="s">
+        <v>173</v>
+      </c>
+      <c r="K130" t="s">
+        <v>174</v>
+      </c>
+      <c r="L130" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B131" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C131" t="s">
-        <v>185</v>
+        <v>285</v>
       </c>
       <c r="E131" t="s">
-        <v>186</v>
+        <v>286</v>
       </c>
       <c r="M131" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4489,27 +4465,33 @@
         <v>48</v>
       </c>
       <c r="B132" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C132" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E132" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="M132" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B133" t="s">
-        <v>344</v>
-      </c>
-      <c r="G133" t="s">
-        <v>345</v>
+        <v>339</v>
+      </c>
+      <c r="C133" t="s">
+        <v>186</v>
+      </c>
+      <c r="E133" t="s">
+        <v>187</v>
+      </c>
+      <c r="M133" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4517,50 +4499,47 @@
         <v>17</v>
       </c>
       <c r="B134" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="G134" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B135" t="s">
-        <v>348</v>
-      </c>
-      <c r="C135" t="s">
-        <v>300</v>
-      </c>
-      <c r="E135" t="s">
-        <v>301</v>
-      </c>
-      <c r="J135" t="s">
-        <v>195</v>
-      </c>
-      <c r="K135" t="s">
-        <v>196</v>
-      </c>
-      <c r="L135" t="s">
-        <v>197</v>
-      </c>
-      <c r="M135" t="s">
-        <v>349</v>
+        <v>343</v>
+      </c>
+      <c r="G135" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B136" t="s">
-        <v>350</v>
-      </c>
-      <c r="G136" t="s">
-        <v>351</v>
+        <v>345</v>
+      </c>
+      <c r="C136" t="s">
+        <v>297</v>
+      </c>
+      <c r="E136" t="s">
+        <v>298</v>
+      </c>
+      <c r="J136" t="s">
+        <v>192</v>
+      </c>
+      <c r="K136" t="s">
+        <v>193</v>
+      </c>
+      <c r="L136" t="s">
+        <v>194</v>
       </c>
       <c r="M136" t="s">
-        <v>156</v>
+        <v>346</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4568,13 +4547,10 @@
         <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>352</v>
+        <v>347</v>
       </c>
       <c r="G137" t="s">
-        <v>353</v>
-      </c>
-      <c r="M137" t="s">
-        <v>156</v>
+        <v>348</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4582,10 +4558,10 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
       <c r="G138" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4593,10 +4569,10 @@
         <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="G139" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4604,13 +4580,10 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="G140" t="s">
-        <v>359</v>
-      </c>
-      <c r="M140" t="s">
-        <v>156</v>
+        <v>354</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4618,35 +4591,29 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
       <c r="G141" t="s">
-        <v>361</v>
-      </c>
-      <c r="M141" t="s">
-        <v>156</v>
+        <v>356</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A142" t="s">
+        <v>17</v>
+      </c>
+      <c r="B142" t="s">
+        <v>357</v>
+      </c>
+      <c r="G142" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A143" t="s">
         <v>43</v>
       </c>
-      <c r="B142" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A144" t="s">
-        <v>78</v>
-      </c>
-      <c r="B144" t="s">
-        <v>546</v>
-      </c>
-      <c r="C144" t="s">
-        <v>552</v>
-      </c>
-      <c r="M144" t="s">
-        <v>630</v>
+      <c r="B143" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4654,16 +4621,13 @@
         <v>78</v>
       </c>
       <c r="B145" t="s">
-        <v>547</v>
+        <v>539</v>
       </c>
       <c r="C145" t="s">
-        <v>553</v>
-      </c>
-      <c r="D145" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="M145" t="s">
-        <v>631</v>
+        <v>623</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4671,16 +4635,16 @@
         <v>78</v>
       </c>
       <c r="B146" t="s">
-        <v>548</v>
+        <v>540</v>
       </c>
       <c r="C146" t="s">
-        <v>554</v>
+        <v>546</v>
       </c>
       <c r="D146" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="M146" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4688,13 +4652,16 @@
         <v>78</v>
       </c>
       <c r="B147" t="s">
-        <v>549</v>
+        <v>541</v>
       </c>
       <c r="C147" t="s">
-        <v>555</v>
+        <v>547</v>
+      </c>
+      <c r="D147" t="s">
+        <v>551</v>
       </c>
       <c r="M147" t="s">
-        <v>629</v>
+        <v>624</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4702,13 +4669,13 @@
         <v>78</v>
       </c>
       <c r="B148" t="s">
-        <v>550</v>
+        <v>542</v>
       </c>
       <c r="C148" t="s">
-        <v>556</v>
+        <v>548</v>
       </c>
       <c r="M148" t="s">
-        <v>629</v>
+        <v>622</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4716,27 +4683,27 @@
         <v>78</v>
       </c>
       <c r="B149" t="s">
-        <v>551</v>
+        <v>543</v>
       </c>
       <c r="C149" t="s">
-        <v>557</v>
+        <v>549</v>
       </c>
       <c r="M149" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A151" t="s">
-        <v>17</v>
-      </c>
-      <c r="B151" t="s">
-        <v>362</v>
-      </c>
-      <c r="G151" t="s">
-        <v>96</v>
-      </c>
-      <c r="M151" t="s">
-        <v>363</v>
+        <v>622</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A150" t="s">
+        <v>78</v>
+      </c>
+      <c r="B150" t="s">
+        <v>544</v>
+      </c>
+      <c r="C150" t="s">
+        <v>550</v>
+      </c>
+      <c r="M150" t="s">
+        <v>622</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4744,124 +4711,124 @@
         <v>17</v>
       </c>
       <c r="B152" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G152" t="s">
         <v>96</v>
       </c>
       <c r="M152" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>366</v>
-      </c>
-      <c r="C153" t="s">
-        <v>517</v>
-      </c>
-      <c r="D153" t="s">
-        <v>368</v>
-      </c>
-      <c r="E153" t="s">
-        <v>367</v>
-      </c>
-      <c r="F153" t="s">
-        <v>369</v>
+        <v>361</v>
+      </c>
+      <c r="G153" t="s">
+        <v>96</v>
       </c>
       <c r="M153" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
-        <v>371</v>
+        <v>48</v>
       </c>
       <c r="B154" t="s">
-        <v>372</v>
+        <v>363</v>
       </c>
       <c r="C154" t="s">
-        <v>373</v>
+        <v>510</v>
+      </c>
+      <c r="D154" t="s">
+        <v>365</v>
       </c>
       <c r="E154" t="s">
-        <v>374</v>
+        <v>364</v>
+      </c>
+      <c r="F154" t="s">
+        <v>366</v>
       </c>
       <c r="M154" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
-        <v>48</v>
+        <v>368</v>
       </c>
       <c r="B155" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="C155" t="s">
-        <v>518</v>
-      </c>
-      <c r="D155" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="E155" t="s">
-        <v>376</v>
-      </c>
-      <c r="F155" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="M155" t="s">
-        <v>379</v>
+        <v>367</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
-        <v>380</v>
+        <v>48</v>
       </c>
       <c r="B156" t="s">
-        <v>381</v>
+        <v>372</v>
       </c>
       <c r="C156" t="s">
-        <v>382</v>
+        <v>511</v>
+      </c>
+      <c r="D156" t="s">
+        <v>374</v>
       </c>
       <c r="E156" t="s">
-        <v>383</v>
+        <v>373</v>
+      </c>
+      <c r="F156" t="s">
+        <v>375</v>
       </c>
       <c r="M156" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
-        <v>48</v>
+        <v>377</v>
       </c>
       <c r="B157" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="C157" t="s">
-        <v>519</v>
+        <v>379</v>
       </c>
       <c r="E157" t="s">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="M157" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B158" t="s">
-        <v>387</v>
-      </c>
-      <c r="G158" t="s">
-        <v>96</v>
+        <v>381</v>
+      </c>
+      <c r="C158" t="s">
+        <v>512</v>
+      </c>
+      <c r="E158" t="s">
+        <v>382</v>
       </c>
       <c r="M158" t="s">
-        <v>388</v>
+        <v>628</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4869,13 +4836,13 @@
         <v>17</v>
       </c>
       <c r="B159" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="G159" t="s">
         <v>96</v>
       </c>
       <c r="M159" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4883,13 +4850,13 @@
         <v>17</v>
       </c>
       <c r="B160" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="G160" t="s">
         <v>96</v>
       </c>
       <c r="M160" t="s">
-        <v>392</v>
+        <v>629</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4897,47 +4864,49 @@
         <v>17</v>
       </c>
       <c r="B161" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="G161" t="s">
         <v>96</v>
       </c>
       <c r="M161" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="162" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A162" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="162" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A162" t="s">
+        <v>17</v>
+      </c>
+      <c r="B162" t="s">
+        <v>388</v>
+      </c>
+      <c r="G162" t="s">
+        <v>96</v>
+      </c>
+      <c r="M162" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B163" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="164" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A164" s="1" t="s">
+    <row r="165" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B164" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="C164" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="N164" s="1" t="s">
-        <v>527</v>
-      </c>
-    </row>
-    <row r="165" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A165" t="s">
-        <v>17</v>
-      </c>
-      <c r="B165" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="C165" s="4"/>
-      <c r="G165" t="s">
-        <v>108</v>
+      <c r="B165" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="C165" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="N165" s="1" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="166" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4945,11 +4914,11 @@
         <v>17</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>529</v>
+        <v>521</v>
       </c>
       <c r="C166" s="4"/>
-      <c r="G166" s="3" t="s">
-        <v>537</v>
+      <c r="G166" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="167" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4957,11 +4926,11 @@
         <v>17</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>530</v>
+        <v>522</v>
       </c>
       <c r="C167" s="4"/>
       <c r="G167" s="3" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
     </row>
     <row r="168" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4969,59 +4938,51 @@
         <v>17</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>531</v>
+        <v>523</v>
       </c>
       <c r="C168" s="4"/>
       <c r="G168" s="3" t="s">
-        <v>535</v>
+        <v>527</v>
       </c>
     </row>
     <row r="169" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" t="s">
+        <v>17</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>524</v>
+      </c>
+      <c r="C169" s="4"/>
+      <c r="G169" s="3" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A170" t="s">
         <v>48</v>
       </c>
-      <c r="B169" t="s">
-        <v>532</v>
-      </c>
-      <c r="C169" s="5" t="s">
-        <v>533</v>
-      </c>
-      <c r="E169" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="M169" s="3" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="170" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A170" s="7" t="s">
+      <c r="B170" t="s">
+        <v>525</v>
+      </c>
+      <c r="C170" s="5" t="s">
+        <v>526</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="M170" s="3" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B170" s="7" t="s">
-        <v>521</v>
-      </c>
-      <c r="C170" s="7" t="s">
-        <v>545</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A171" t="s">
-        <v>78</v>
-      </c>
-      <c r="B171" t="s">
-        <v>503</v>
-      </c>
-      <c r="C171" t="s">
-        <v>542</v>
-      </c>
-      <c r="E171" t="s">
-        <v>79</v>
-      </c>
-      <c r="H171" t="s">
-        <v>22</v>
-      </c>
-      <c r="M171" s="3" t="s">
-        <v>544</v>
+      <c r="B171" s="7" t="s">
+        <v>514</v>
+      </c>
+      <c r="C171" s="7" t="s">
+        <v>538</v>
       </c>
     </row>
     <row r="172" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5029,10 +4990,10 @@
         <v>78</v>
       </c>
       <c r="B172" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="C172" t="s">
-        <v>543</v>
+        <v>535</v>
       </c>
       <c r="E172" t="s">
         <v>79</v>
@@ -5041,214 +5002,223 @@
         <v>22</v>
       </c>
       <c r="M172" s="3" t="s">
-        <v>544</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
-        <v>506</v>
+        <v>78</v>
       </c>
       <c r="B173" t="s">
-        <v>507</v>
-      </c>
-      <c r="C173" s="6" t="s">
-        <v>539</v>
-      </c>
-      <c r="J173" t="s">
-        <v>508</v>
-      </c>
-      <c r="K173" t="s">
-        <v>509</v>
+        <v>497</v>
+      </c>
+      <c r="C173" t="s">
+        <v>536</v>
+      </c>
+      <c r="E173" t="s">
+        <v>79</v>
+      </c>
+      <c r="H173" t="s">
+        <v>22</v>
       </c>
       <c r="M173" s="3" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="174" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>506</v>
+        <v>499</v>
       </c>
       <c r="B174" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="C174" s="6" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="J174" t="s">
-        <v>512</v>
+        <v>501</v>
       </c>
       <c r="K174" t="s">
-        <v>513</v>
+        <v>502</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
     </row>
     <row r="175" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
+        <v>499</v>
+      </c>
+      <c r="B175" t="s">
+        <v>503</v>
+      </c>
+      <c r="C175" s="6" t="s">
+        <v>531</v>
+      </c>
+      <c r="J175" t="s">
+        <v>505</v>
+      </c>
+      <c r="K175" t="s">
         <v>506</v>
       </c>
-      <c r="B175" t="s">
-        <v>511</v>
-      </c>
-      <c r="C175" s="6" t="s">
-        <v>540</v>
-      </c>
-      <c r="J175" t="s">
-        <v>515</v>
-      </c>
-      <c r="K175" t="s">
-        <v>514</v>
-      </c>
       <c r="M175" s="3" t="s">
-        <v>536</v>
-      </c>
-    </row>
-    <row r="177" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A177" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A176" t="s">
+        <v>499</v>
+      </c>
+      <c r="B176" t="s">
+        <v>504</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="J176" t="s">
+        <v>508</v>
+      </c>
+      <c r="K176" t="s">
+        <v>507</v>
+      </c>
+      <c r="M176" s="3" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B177" s="1" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="179" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A179" t="s">
-        <v>98</v>
-      </c>
-      <c r="B179" t="s">
-        <v>395</v>
-      </c>
-      <c r="C179" t="s">
-        <v>396</v>
-      </c>
-      <c r="D179" t="s">
-        <v>398</v>
-      </c>
-      <c r="E179" t="s">
-        <v>397</v>
-      </c>
-      <c r="F179" t="s">
-        <v>399</v>
+      <c r="B178" s="1" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="180" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
-        <v>400</v>
+        <v>98</v>
       </c>
       <c r="B180" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="C180" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="D180" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="E180" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="F180" t="s">
-        <v>405</v>
-      </c>
-      <c r="H180" t="s">
-        <v>22</v>
-      </c>
-      <c r="M180" t="s">
-        <v>406</v>
+        <v>394</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
-        <v>407</v>
+        <v>395</v>
       </c>
       <c r="B181" t="s">
-        <v>408</v>
+        <v>396</v>
       </c>
       <c r="C181" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="D181" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="E181" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="F181" t="s">
-        <v>405</v>
+        <v>400</v>
+      </c>
+      <c r="H181" t="s">
+        <v>22</v>
       </c>
       <c r="M181" t="s">
-        <v>52</v>
+        <v>401</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="B182" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C182" t="s">
-        <v>402</v>
+        <v>397</v>
+      </c>
+      <c r="D182" t="s">
+        <v>399</v>
       </c>
       <c r="E182" t="s">
-        <v>403</v>
-      </c>
-      <c r="H182" t="s">
-        <v>22</v>
+        <v>398</v>
+      </c>
+      <c r="F182" t="s">
+        <v>400</v>
       </c>
       <c r="M182" t="s">
-        <v>411</v>
+        <v>52</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
-        <v>48</v>
+        <v>404</v>
       </c>
       <c r="B183" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C183" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="E183" t="s">
-        <v>414</v>
+        <v>398</v>
+      </c>
+      <c r="H183" t="s">
+        <v>22</v>
       </c>
       <c r="M183" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B184" t="s">
-        <v>416</v>
+        <v>407</v>
       </c>
       <c r="C184" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="E184" t="s">
-        <v>418</v>
+        <v>409</v>
+      </c>
+      <c r="M184" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
+        <v>20</v>
+      </c>
+      <c r="B185" t="s">
+        <v>411</v>
+      </c>
+      <c r="C185" t="s">
+        <v>412</v>
+      </c>
+      <c r="E185" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A186" t="s">
         <v>43</v>
       </c>
-      <c r="B185" t="s">
+      <c r="B186" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A187" t="s">
-        <v>17</v>
-      </c>
-      <c r="B187" t="s">
-        <v>419</v>
-      </c>
-      <c r="G187" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5256,10 +5226,10 @@
         <v>17</v>
       </c>
       <c r="B188" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="G188" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5267,10 +5237,10 @@
         <v>17</v>
       </c>
       <c r="B189" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="G189" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5278,10 +5248,10 @@
         <v>17</v>
       </c>
       <c r="B190" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="G190" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5289,10 +5259,10 @@
         <v>17</v>
       </c>
       <c r="B191" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="G191" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5300,10 +5270,21 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="G192" t="s">
-        <v>430</v>
+        <v>423</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" t="s">
+        <v>17</v>
+      </c>
+      <c r="B193" t="s">
+        <v>424</v>
+      </c>
+      <c r="G193" t="s">
+        <v>425</v>
       </c>
     </row>
   </sheetData>
@@ -5316,7 +5297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
@@ -5327,7 +5308,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5347,10 +5328,10 @@
         <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D2" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5358,24 +5339,24 @@
         <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C3" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="D3" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C4" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5386,10 +5367,10 @@
         <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D5" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5397,13 +5378,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C6" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D6" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5411,471 +5392,471 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C7" t="s">
-        <v>520</v>
+        <v>513</v>
       </c>
       <c r="D7" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B8" t="s">
         <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>564</v>
+        <v>557</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B9" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C9" t="s">
-        <v>565</v>
+        <v>558</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B10" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C10" t="s">
-        <v>566</v>
+        <v>559</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B11" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C11" t="s">
-        <v>567</v>
+        <v>560</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B12" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C12" t="s">
-        <v>599</v>
+        <v>592</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B13" t="s">
-        <v>568</v>
+        <v>561</v>
       </c>
       <c r="C13" t="s">
-        <v>600</v>
+        <v>593</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B14" t="s">
-        <v>569</v>
+        <v>562</v>
       </c>
       <c r="C14" t="s">
-        <v>601</v>
+        <v>594</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
+        <v>556</v>
+      </c>
+      <c r="B15" t="s">
         <v>563</v>
       </c>
-      <c r="B15" t="s">
-        <v>570</v>
-      </c>
       <c r="C15" t="s">
-        <v>602</v>
+        <v>595</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B16" t="s">
-        <v>571</v>
+        <v>564</v>
       </c>
       <c r="C16" t="s">
-        <v>603</v>
+        <v>596</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B17" t="s">
-        <v>572</v>
+        <v>565</v>
       </c>
       <c r="C17" t="s">
-        <v>604</v>
+        <v>597</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B18" t="s">
-        <v>573</v>
+        <v>566</v>
       </c>
       <c r="C18" t="s">
-        <v>605</v>
+        <v>598</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B19" t="s">
-        <v>574</v>
+        <v>567</v>
       </c>
       <c r="C19" t="s">
-        <v>606</v>
+        <v>599</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B20" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
       <c r="C20" t="s">
-        <v>607</v>
+        <v>600</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B21" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
       <c r="C21" t="s">
-        <v>608</v>
+        <v>601</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B22" t="s">
-        <v>577</v>
+        <v>570</v>
       </c>
       <c r="C22" t="s">
-        <v>609</v>
+        <v>602</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B23" t="s">
-        <v>578</v>
+        <v>571</v>
       </c>
       <c r="C23" t="s">
-        <v>610</v>
+        <v>603</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B24" t="s">
-        <v>579</v>
+        <v>572</v>
       </c>
       <c r="C24" t="s">
-        <v>611</v>
+        <v>604</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B25" t="s">
-        <v>580</v>
+        <v>573</v>
       </c>
       <c r="C25" t="s">
-        <v>612</v>
+        <v>605</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B26" t="s">
-        <v>581</v>
+        <v>574</v>
       </c>
       <c r="C26" t="s">
-        <v>613</v>
+        <v>606</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B27" t="s">
-        <v>582</v>
+        <v>575</v>
       </c>
       <c r="C27" t="s">
-        <v>614</v>
+        <v>607</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B28" t="s">
-        <v>583</v>
+        <v>576</v>
       </c>
       <c r="C28" t="s">
-        <v>615</v>
+        <v>608</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B29" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="C29" t="s">
-        <v>616</v>
+        <v>609</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B30" t="s">
-        <v>585</v>
+        <v>578</v>
       </c>
       <c r="C30" t="s">
-        <v>617</v>
+        <v>610</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B31" t="s">
-        <v>586</v>
+        <v>579</v>
       </c>
       <c r="C31" t="s">
-        <v>618</v>
+        <v>611</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B32" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="C32" t="s">
-        <v>619</v>
+        <v>612</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B33" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
       <c r="C33" t="s">
-        <v>620</v>
+        <v>613</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B34" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
       <c r="C34" t="s">
-        <v>621</v>
+        <v>614</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B35" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
       <c r="C35" t="s">
-        <v>622</v>
+        <v>615</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B36" t="s">
-        <v>591</v>
+        <v>584</v>
       </c>
       <c r="C36" t="s">
-        <v>623</v>
+        <v>616</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B37" t="s">
-        <v>592</v>
+        <v>585</v>
       </c>
       <c r="C37" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B38" t="s">
-        <v>593</v>
+        <v>586</v>
       </c>
       <c r="C38" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B39" t="s">
-        <v>594</v>
+        <v>587</v>
       </c>
       <c r="C39" t="s">
-        <v>626</v>
+        <v>619</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B40" t="s">
-        <v>595</v>
+        <v>588</v>
       </c>
       <c r="C40" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>563</v>
+        <v>556</v>
       </c>
       <c r="B41" t="s">
-        <v>596</v>
+        <v>589</v>
       </c>
       <c r="C41" t="s">
-        <v>628</v>
+        <v>621</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B42" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="C42" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D42" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="B43" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="C43" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D43" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="B44" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C44" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="D44" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
+        <v>443</v>
+      </c>
+      <c r="B45" t="s">
+        <v>447</v>
+      </c>
+      <c r="C45" t="s">
         <v>448</v>
       </c>
-      <c r="B45" t="s">
-        <v>452</v>
-      </c>
-      <c r="C45" t="s">
-        <v>453</v>
-      </c>
       <c r="D45" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="B46" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C46" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="D46" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
+        <v>450</v>
+      </c>
+      <c r="B47" t="s">
+        <v>454</v>
+      </c>
+      <c r="C47" t="s">
         <v>455</v>
       </c>
-      <c r="B47" t="s">
-        <v>459</v>
-      </c>
-      <c r="C47" t="s">
-        <v>460</v>
-      </c>
       <c r="D47" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5886,10 +5867,10 @@
         <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="D48" t="s">
-        <v>463</v>
+        <v>458</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5897,13 +5878,13 @@
         <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C49" t="s">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="D49" t="s">
-        <v>465</v>
+        <v>460</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5911,13 +5892,13 @@
         <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C50" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="D50" t="s">
-        <v>467</v>
+        <v>462</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5925,195 +5906,195 @@
         <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C51" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="D51" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B52" t="s">
         <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D52" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B53" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C53" t="s">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="D53" t="s">
-        <v>471</v>
+        <v>466</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="B54" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C54" t="s">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="D54" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B55" t="s">
         <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D55" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B56" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C56" t="s">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="D56" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B57" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C57" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="D57" t="s">
-        <v>478</v>
+        <v>473</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B58" t="s">
         <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="D58" t="s">
-        <v>481</v>
+        <v>476</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="B59" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="C59" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="D59" t="s">
-        <v>483</v>
+        <v>478</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B60" t="s">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="C60" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="D60" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="B61" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="C61" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="D61" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B62" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="C62" t="s">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="D62" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="B63" t="s">
         <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="D63" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="B64" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="C64" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="D64" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
   </sheetData>
@@ -6125,36 +6106,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="B1" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="C1" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="D1" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>498</v>
+        <v>626</v>
       </c>
       <c r="B2" t="s">
-        <v>499</v>
+        <v>493</v>
       </c>
       <c r="C2" t="s">
-        <v>500</v>
+        <v>627</v>
       </c>
       <c r="D2" t="s">
-        <v>501</v>
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -6164,20 +6147,10 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6227,7 +6200,7 @@
 </spe:Receivers>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6236,7 +6209,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
@@ -6300,7 +6273,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6739,15 +6712,17 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -6755,7 +6730,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
@@ -6763,7 +6738,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -6771,7 +6746,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -6785,7 +6760,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6806,4 +6781,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added note to show # HH, wom, child
The count of women and child no longer works
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{C9DDF55E-0FA5-454C-99F0-6557C1245B8D}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{370AB5A9-BA41-4F82-BC14-F23780FBDB5A}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="18192" windowHeight="11592" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1024" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="632">
   <si>
     <t>type</t>
   </si>
@@ -1316,9 +1316,6 @@
     <t>refer_sam</t>
   </si>
   <si>
-    <t>Have you referred the child for management of severe acute malnutrition services?</t>
-  </si>
-  <si>
     <t>Avez-vous referé l'enfant auprès des programmes de prise en charge de la MAS ?</t>
   </si>
   <si>
@@ -1343,18 +1340,9 @@
     <t>refer_mam</t>
   </si>
   <si>
-    <t>Have you referred the child for management of moderate acute malnutrition services?</t>
-  </si>
-  <si>
     <t>Avez-vous referé l'enfant auprès des programmes de prise en charge de la MAM ?</t>
   </si>
   <si>
-    <t>no_acutemal</t>
-  </si>
-  <si>
-    <t>${child_name}  ne présente pas de conditions indiquant une malnutrition aigüe</t>
-  </si>
-  <si>
     <t>child_eligible</t>
   </si>
   <si>
@@ -1601,30 +1589,18 @@
     <t>refermam</t>
   </si>
   <si>
-    <t>No, already enrolled in a nutrition program (TSFP)</t>
-  </si>
-  <si>
     <t>Non, déjà enrôlé dans un programme de nutrition (CRENAM)</t>
   </si>
   <si>
-    <t>No, there is no nutrition program (TSFP) in place</t>
-  </si>
-  <si>
     <t>Non, il n'y a pas de programme de nutrition (CRENAM) mis en place</t>
   </si>
   <si>
     <t>refersam</t>
   </si>
   <si>
-    <t>No, already enrolled in a nutrition program (TFP)</t>
-  </si>
-  <si>
     <t>Non, déjà enrôlé dans un programme de nutrition (CRENAS/CRENI)</t>
   </si>
   <si>
-    <t>No, there is no nutrition program (TFP) in place</t>
-  </si>
-  <si>
     <t>Non, il n'y a pas de programme de nutrition (CRENAS/CRENI) mis en place</t>
   </si>
   <si>
@@ -1733,18 +1709,6 @@
     <t xml:space="preserve">(. &gt;= 25 and . &lt;200) </t>
   </si>
   <si>
-    <t>Pregnant &amp; Lactating Woman section</t>
-  </si>
-  <si>
-    <t>${child_name} - has SEVERE ACUTE MALNUTRITION (SAM).</t>
-  </si>
-  <si>
-    <t>${child_name} -  has MODERATE ACUTE MALNUTRITION (MAM).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${child_name} - is NOT acutely malnourished </t>
-  </si>
-  <si>
     <t>Other (No one present)</t>
   </si>
   <si>
@@ -1799,15 +1763,6 @@
     <t>number(selected-at(${women}, ${wom_selected_position}))</t>
   </si>
   <si>
-    <t>Woman's HEIGHT in CM of (${wom_name})</t>
-  </si>
-  <si>
-    <t>Woman's MUAC in MM of (${wom_name})</t>
-  </si>
-  <si>
-    <t>Woman's WEIGHT in KG of (${wom_name})</t>
-  </si>
-  <si>
     <t>if(${age_years} &gt;14 and ${age_years} &lt;50 and ${sex}= 'f',true(),false())</t>
   </si>
   <si>
@@ -1820,9 +1775,6 @@
     <t>${consent}=1 and ${age_years} &gt;14 and ${age_years} &lt;50 and ${sex}= 'f'</t>
   </si>
   <si>
-    <t>Selposit-${wom_selected_position} HHposit- ${wom_hh_position} Name-${wom_name} Age-${wom_age_years} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
-  </si>
-  <si>
     <t>breastfed</t>
   </si>
   <si>
@@ -2081,18 +2033,12 @@
     <t xml:space="preserve">${MONTHS}&gt;5 or (${MONTHS}=98 and ${HEIGHT}&gt;67) </t>
   </si>
   <si>
-    <t>(${child_name}) is ${MONTHS} months old.</t>
-  </si>
-  <si>
     <t>ACO_SMART_Survey_2021</t>
   </si>
   <si>
     <t>concat('ACO_SMART_Survey_2021','_HH',${HH})</t>
   </si>
   <si>
-    <t>${mam_case} !=1 and ${sam_case} !=1</t>
-  </si>
-  <si>
     <t>(${WEIGHT}&gt;0 or ${HEIGHT}&gt;0 or ${MUAC}&gt;0 or ${EDEMA} = 'y' or ${EDEMA} = 'n')</t>
   </si>
   <si>
@@ -2106,6 +2052,54 @@
   </si>
   <si>
     <t>Now entering data for child: ${child_name} (${CHSEX}) with age in years: ${child_age_years}</t>
+  </si>
+  <si>
+    <t>${child_name} is ${MONTHS} months old.</t>
+  </si>
+  <si>
+    <t>Woman's MUAC in MM of ${wom_name}</t>
+  </si>
+  <si>
+    <t>Woman's HEIGHT in CM of ${wom_name}</t>
+  </si>
+  <si>
+    <t>Woman's WEIGHT in KG of ${wom_name}</t>
+  </si>
+  <si>
+    <t>No, child is already enrolled in a nutrition program for MAM</t>
+  </si>
+  <si>
+    <t>No, there is no nutrition program for children with MAM</t>
+  </si>
+  <si>
+    <t>No, there is no SAM treatment program available</t>
+  </si>
+  <si>
+    <t>No, child is already enrolled in SAM Treatment</t>
+  </si>
+  <si>
+    <t>Woman section</t>
+  </si>
+  <si>
+    <t>Selposit-${wom_selected_position} HHposit- ${wom_hh_position} Name-${wom_name} Sex-${sex} Age-${wom_age_years} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
+  </si>
+  <si>
+    <t>${child_name}  has SEVERE ACUTE MALNUTRITION (SAM).</t>
+  </si>
+  <si>
+    <t>${child_name}  has MODERATE ACUTE MALNUTRITION (MAM).</t>
+  </si>
+  <si>
+    <t>Have you referred ${child_name}  for management of severe acute malnutrition services?</t>
+  </si>
+  <si>
+    <t>Have you referred ${child_name}  for management of moderate acute malnutrition services?</t>
+  </si>
+  <si>
+    <t>show HH data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HH members-${numfamily} # women- ${numwomen} # children-${numchildren} </t>
   </si>
 </sst>
 </file>
@@ -2520,11 +2514,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N193"/>
+  <dimension ref="A1:N194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C36" sqref="C36"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2618,13 +2612,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>553</v>
+        <v>537</v>
       </c>
       <c r="B6" t="s">
-        <v>554</v>
+        <v>538</v>
       </c>
       <c r="C6" t="s">
-        <v>555</v>
+        <v>539</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2771,10 +2765,10 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>590</v>
+        <v>574</v>
       </c>
       <c r="E17" t="s">
-        <v>591</v>
+        <v>575</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2864,7 +2858,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>630</v>
+        <v>612</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
@@ -2881,12 +2875,12 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>631</v>
+        <v>613</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="G24" s="8" t="s">
-        <v>632</v>
+        <v>614</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2962,10 +2956,10 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>515</v>
+        <v>503</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>534</v>
+        <v>519</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3069,10 +3063,10 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>516</v>
+        <v>504</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3080,39 +3074,39 @@
         <v>17</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>517</v>
+        <v>505</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>519</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="44" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A44" s="2" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>630</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="45" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A45" t="s">
-        <v>17</v>
-      </c>
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="G45" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3120,10 +3114,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G46" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3131,10 +3125,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3142,10 +3136,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G48" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3153,35 +3147,35 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G49" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>117</v>
-      </c>
-      <c r="C50" t="s">
-        <v>633</v>
-      </c>
-      <c r="E50" t="s">
-        <v>118</v>
-      </c>
-      <c r="M50" t="s">
-        <v>119</v>
+        <v>115</v>
+      </c>
+      <c r="G50" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>120</v>
+        <v>117</v>
+      </c>
+      <c r="C51" t="s">
+        <v>615</v>
+      </c>
+      <c r="E51" t="s">
+        <v>118</v>
       </c>
       <c r="M51" t="s">
         <v>119</v>
@@ -3189,97 +3183,94 @@
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B52" t="s">
-        <v>121</v>
-      </c>
-      <c r="C52" t="s">
-        <v>122</v>
-      </c>
-      <c r="D52" t="s">
-        <v>124</v>
-      </c>
-      <c r="E52" t="s">
-        <v>123</v>
-      </c>
-      <c r="F52" t="s">
-        <v>125</v>
-      </c>
-      <c r="H52" t="s">
-        <v>22</v>
+        <v>120</v>
+      </c>
+      <c r="M52" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B53" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C53" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D53" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E53" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F53" t="s">
-        <v>130</v>
-      </c>
-      <c r="I53" t="s">
-        <v>29</v>
-      </c>
-      <c r="J53" t="s">
-        <v>131</v>
-      </c>
-      <c r="M53" t="s">
-        <v>132</v>
+        <v>125</v>
+      </c>
+      <c r="H53" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B54" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C54" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D54" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E54" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F54" t="s">
-        <v>137</v>
+        <v>130</v>
+      </c>
+      <c r="I54" t="s">
+        <v>29</v>
       </c>
       <c r="J54" t="s">
-        <v>138</v>
-      </c>
-      <c r="K54" t="s">
-        <v>139</v>
-      </c>
-      <c r="L54" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="M54" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B55" t="s">
-        <v>142</v>
-      </c>
-      <c r="G55" t="s">
-        <v>143</v>
+        <v>133</v>
+      </c>
+      <c r="C55" t="s">
+        <v>134</v>
+      </c>
+      <c r="D55" t="s">
+        <v>136</v>
+      </c>
+      <c r="E55" t="s">
+        <v>135</v>
+      </c>
+      <c r="F55" t="s">
+        <v>137</v>
+      </c>
+      <c r="J55" t="s">
+        <v>138</v>
+      </c>
+      <c r="K55" t="s">
+        <v>139</v>
+      </c>
+      <c r="L55" t="s">
+        <v>140</v>
       </c>
       <c r="M55" t="s">
         <v>141</v>
@@ -3290,27 +3281,24 @@
         <v>17</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G56" t="s">
-        <v>145</v>
+        <v>143</v>
+      </c>
+      <c r="M56" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B57" t="s">
-        <v>146</v>
-      </c>
-      <c r="C57" t="s">
-        <v>147</v>
-      </c>
-      <c r="E57" t="s">
-        <v>148</v>
-      </c>
-      <c r="M57" t="s">
-        <v>149</v>
+        <v>144</v>
+      </c>
+      <c r="G57" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3318,133 +3306,133 @@
         <v>48</v>
       </c>
       <c r="B58" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" t="s">
+        <v>147</v>
+      </c>
+      <c r="E58" t="s">
+        <v>148</v>
+      </c>
+      <c r="M58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>48</v>
+      </c>
+      <c r="B59" t="s">
         <v>150</v>
       </c>
-      <c r="C58" t="s">
-        <v>625</v>
-      </c>
-      <c r="E58" t="s">
+      <c r="C59" t="s">
+        <v>616</v>
+      </c>
+      <c r="E59" t="s">
         <v>151</v>
       </c>
-      <c r="M58" t="s">
+      <c r="M59" t="s">
         <v>152</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A60" t="s">
-        <v>25</v>
-      </c>
-      <c r="B60" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>25</v>
       </c>
       <c r="B61" t="s">
-        <v>155</v>
-      </c>
-      <c r="C61" t="s">
-        <v>156</v>
-      </c>
-      <c r="D61" t="s">
-        <v>158</v>
-      </c>
-      <c r="E61" t="s">
-        <v>157</v>
-      </c>
-      <c r="F61" t="s">
-        <v>159</v>
-      </c>
-      <c r="J61" t="s">
-        <v>160</v>
-      </c>
-      <c r="K61" t="s">
-        <v>161</v>
-      </c>
-      <c r="L61" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B62" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>165</v>
+        <v>156</v>
+      </c>
+      <c r="D62" t="s">
+        <v>158</v>
       </c>
       <c r="E62" t="s">
-        <v>166</v>
-      </c>
-      <c r="M62" t="s">
-        <v>167</v>
+        <v>157</v>
+      </c>
+      <c r="F62" t="s">
+        <v>159</v>
+      </c>
+      <c r="J62" t="s">
+        <v>160</v>
+      </c>
+      <c r="K62" t="s">
+        <v>161</v>
+      </c>
+      <c r="L62" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B63" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C63" t="s">
-        <v>169</v>
-      </c>
-      <c r="D63" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E63" t="s">
-        <v>170</v>
-      </c>
-      <c r="F63" t="s">
-        <v>172</v>
-      </c>
-      <c r="J63" t="s">
-        <v>173</v>
-      </c>
-      <c r="K63" t="s">
-        <v>174</v>
-      </c>
-      <c r="L63" t="s">
-        <v>175</v>
+        <v>166</v>
+      </c>
+      <c r="M63" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="B64" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C64" t="s">
-        <v>178</v>
+        <v>169</v>
+      </c>
+      <c r="D64" t="s">
+        <v>171</v>
       </c>
       <c r="E64" t="s">
-        <v>179</v>
-      </c>
-      <c r="M64" t="s">
-        <v>180</v>
+        <v>170</v>
+      </c>
+      <c r="F64" t="s">
+        <v>172</v>
+      </c>
+      <c r="J64" t="s">
+        <v>173</v>
+      </c>
+      <c r="K64" t="s">
+        <v>174</v>
+      </c>
+      <c r="L64" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B65" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="C65" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="E65" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="M65" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3452,84 +3440,93 @@
         <v>48</v>
       </c>
       <c r="B66" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C66" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E66" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M66" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B67" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C67" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="E67" t="s">
-        <v>191</v>
-      </c>
-      <c r="J67" t="s">
-        <v>192</v>
-      </c>
-      <c r="K67" t="s">
-        <v>193</v>
-      </c>
-      <c r="L67" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="M67" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>163</v>
+        <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C68" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="E68" t="s">
-        <v>198</v>
+        <v>191</v>
+      </c>
+      <c r="J68" t="s">
+        <v>192</v>
+      </c>
+      <c r="K68" t="s">
+        <v>193</v>
+      </c>
+      <c r="L68" t="s">
+        <v>194</v>
+      </c>
+      <c r="M68" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>163</v>
       </c>
       <c r="B69" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C69" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E69" t="s">
-        <v>201</v>
-      </c>
-      <c r="H69" t="s">
-        <v>22</v>
-      </c>
-      <c r="M69" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B70" t="s">
-        <v>153</v>
+        <v>199</v>
+      </c>
+      <c r="C70" t="s">
+        <v>200</v>
+      </c>
+      <c r="E70" t="s">
+        <v>201</v>
+      </c>
+      <c r="H70" t="s">
+        <v>22</v>
+      </c>
+      <c r="M70" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3537,18 +3534,15 @@
         <v>43</v>
       </c>
       <c r="B71" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B72" t="s">
-        <v>203</v>
-      </c>
-      <c r="G72" t="s">
-        <v>204</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3556,10 +3550,10 @@
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G73" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3567,10 +3561,10 @@
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G74" t="s">
-        <v>495</v>
+        <v>206</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3578,10 +3572,10 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G75" t="s">
-        <v>209</v>
+        <v>487</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3589,13 +3583,10 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G76" t="s">
-        <v>211</v>
-      </c>
-      <c r="M76" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3603,10 +3594,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G77" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="M77" t="s">
         <v>212</v>
@@ -3617,10 +3608,13 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G78" t="s">
-        <v>216</v>
+        <v>214</v>
+      </c>
+      <c r="M78" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3628,13 +3622,10 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="G79" t="s">
-        <v>218</v>
-      </c>
-      <c r="M79" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3642,10 +3633,10 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="G80" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="M80" t="s">
         <v>212</v>
@@ -3656,10 +3647,13 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="G81" t="s">
-        <v>222</v>
+        <v>220</v>
+      </c>
+      <c r="M81" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3667,13 +3661,10 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="G82" t="s">
-        <v>224</v>
-      </c>
-      <c r="M82" t="s">
-        <v>212</v>
+        <v>222</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3681,10 +3672,10 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G83" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M83" t="s">
         <v>212</v>
@@ -3695,10 +3686,13 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="G84" t="s">
-        <v>228</v>
+        <v>226</v>
+      </c>
+      <c r="M84" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3706,10 +3700,10 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G85" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3717,10 +3711,10 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G86" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3728,10 +3722,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="G87" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3739,10 +3733,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G88" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3750,10 +3744,10 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="G89" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3761,10 +3755,10 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G90" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3772,10 +3766,10 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="G91" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3783,128 +3777,125 @@
         <v>17</v>
       </c>
       <c r="B92" t="s">
+        <v>241</v>
+      </c>
+      <c r="G92" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" t="s">
+        <v>17</v>
+      </c>
+      <c r="B93" t="s">
         <v>243</v>
       </c>
-      <c r="G92" t="s">
+      <c r="G93" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="93" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A94" t="s">
-        <v>25</v>
-      </c>
-      <c r="B94" t="s">
-        <v>245</v>
-      </c>
-      <c r="M94" t="s">
-        <v>246</v>
-      </c>
-    </row>
+    <row r="94" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B95" t="s">
-        <v>247</v>
-      </c>
-      <c r="C95" t="s">
-        <v>248</v>
-      </c>
-      <c r="E95" t="s">
-        <v>249</v>
+        <v>245</v>
+      </c>
+      <c r="M95" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B96" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="C96" t="s">
-        <v>251</v>
-      </c>
-      <c r="D96" t="s">
-        <v>124</v>
+        <v>248</v>
       </c>
       <c r="E96" t="s">
-        <v>252</v>
-      </c>
-      <c r="F96" t="s">
-        <v>125</v>
+        <v>249</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B97" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C97" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D97" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E97" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="F97" t="s">
-        <v>130</v>
-      </c>
-      <c r="I97" t="s">
-        <v>29</v>
-      </c>
-      <c r="J97" t="s">
-        <v>131</v>
-      </c>
-      <c r="M97" t="s">
-        <v>256</v>
+        <v>125</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B98" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C98" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D98" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E98" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="F98" t="s">
-        <v>137</v>
+        <v>130</v>
+      </c>
+      <c r="I98" t="s">
+        <v>29</v>
       </c>
       <c r="J98" t="s">
-        <v>260</v>
-      </c>
-      <c r="K98" t="s">
-        <v>139</v>
-      </c>
-      <c r="L98" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="M98" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B99" t="s">
-        <v>262</v>
-      </c>
-      <c r="G99" t="s">
-        <v>263</v>
+        <v>257</v>
+      </c>
+      <c r="C99" t="s">
+        <v>258</v>
+      </c>
+      <c r="D99" t="s">
+        <v>136</v>
+      </c>
+      <c r="E99" t="s">
+        <v>259</v>
+      </c>
+      <c r="F99" t="s">
+        <v>137</v>
+      </c>
+      <c r="J99" t="s">
+        <v>260</v>
+      </c>
+      <c r="K99" t="s">
+        <v>139</v>
+      </c>
+      <c r="L99" t="s">
+        <v>140</v>
       </c>
       <c r="M99" t="s">
         <v>261</v>
@@ -3915,27 +3906,24 @@
         <v>17</v>
       </c>
       <c r="B100" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G100" t="s">
-        <v>265</v>
+        <v>263</v>
+      </c>
+      <c r="M100" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B101" t="s">
-        <v>266</v>
-      </c>
-      <c r="C101" t="s">
-        <v>267</v>
-      </c>
-      <c r="E101" t="s">
-        <v>268</v>
-      </c>
-      <c r="M101" t="s">
-        <v>269</v>
+        <v>264</v>
+      </c>
+      <c r="G101" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3943,125 +3931,125 @@
         <v>48</v>
       </c>
       <c r="B102" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C102" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="E102" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="M102" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>154</v>
+        <v>48</v>
       </c>
       <c r="B103" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C103" t="s">
-        <v>275</v>
-      </c>
-      <c r="D103" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
       <c r="E103" t="s">
-        <v>276</v>
-      </c>
-      <c r="F103" t="s">
-        <v>159</v>
-      </c>
-      <c r="J103" t="s">
-        <v>160</v>
-      </c>
-      <c r="K103" t="s">
-        <v>161</v>
-      </c>
-      <c r="L103" t="s">
-        <v>162</v>
+        <v>272</v>
+      </c>
+      <c r="M103" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B104" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C104" t="s">
-        <v>278</v>
+        <v>275</v>
+      </c>
+      <c r="D104" t="s">
+        <v>158</v>
       </c>
       <c r="E104" t="s">
-        <v>279</v>
-      </c>
-      <c r="M104" t="s">
-        <v>280</v>
+        <v>276</v>
+      </c>
+      <c r="F104" t="s">
+        <v>159</v>
+      </c>
+      <c r="J104" t="s">
+        <v>160</v>
+      </c>
+      <c r="K104" t="s">
+        <v>161</v>
+      </c>
+      <c r="L104" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B105" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C105" t="s">
-        <v>282</v>
-      </c>
-      <c r="D105" t="s">
-        <v>171</v>
+        <v>278</v>
       </c>
       <c r="E105" t="s">
-        <v>283</v>
-      </c>
-      <c r="F105" t="s">
-        <v>172</v>
-      </c>
-      <c r="J105" t="s">
-        <v>173</v>
-      </c>
-      <c r="K105" t="s">
-        <v>174</v>
-      </c>
-      <c r="L105" t="s">
-        <v>175</v>
+        <v>279</v>
+      </c>
+      <c r="M105" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="B106" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C106" t="s">
-        <v>285</v>
+        <v>282</v>
+      </c>
+      <c r="D106" t="s">
+        <v>171</v>
       </c>
       <c r="E106" t="s">
-        <v>286</v>
-      </c>
-      <c r="M106" t="s">
-        <v>287</v>
+        <v>283</v>
+      </c>
+      <c r="F106" t="s">
+        <v>172</v>
+      </c>
+      <c r="J106" t="s">
+        <v>173</v>
+      </c>
+      <c r="K106" t="s">
+        <v>174</v>
+      </c>
+      <c r="L106" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B107" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C107" t="s">
-        <v>182</v>
+        <v>285</v>
       </c>
       <c r="E107" t="s">
-        <v>183</v>
+        <v>286</v>
       </c>
       <c r="M107" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4069,27 +4057,33 @@
         <v>48</v>
       </c>
       <c r="B108" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C108" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E108" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M108" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B109" t="s">
-        <v>292</v>
-      </c>
-      <c r="G109" t="s">
-        <v>293</v>
+        <v>290</v>
+      </c>
+      <c r="C109" t="s">
+        <v>186</v>
+      </c>
+      <c r="E109" t="s">
+        <v>187</v>
+      </c>
+      <c r="M109" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4097,47 +4091,47 @@
         <v>17</v>
       </c>
       <c r="B110" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G110" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B111" t="s">
-        <v>296</v>
-      </c>
-      <c r="C111" t="s">
-        <v>297</v>
-      </c>
-      <c r="E111" t="s">
-        <v>298</v>
-      </c>
-      <c r="J111" t="s">
-        <v>192</v>
-      </c>
-      <c r="K111" t="s">
-        <v>193</v>
-      </c>
-      <c r="L111" t="s">
-        <v>194</v>
-      </c>
-      <c r="M111" t="s">
-        <v>299</v>
+        <v>294</v>
+      </c>
+      <c r="G111" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B112" t="s">
-        <v>300</v>
-      </c>
-      <c r="G112" t="s">
-        <v>301</v>
+        <v>296</v>
+      </c>
+      <c r="C112" t="s">
+        <v>297</v>
+      </c>
+      <c r="E112" t="s">
+        <v>298</v>
+      </c>
+      <c r="J112" t="s">
+        <v>192</v>
+      </c>
+      <c r="K112" t="s">
+        <v>193</v>
+      </c>
+      <c r="L112" t="s">
+        <v>194</v>
+      </c>
+      <c r="M112" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4145,10 +4139,10 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="G113" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4156,10 +4150,10 @@
         <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G114" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4167,10 +4161,10 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G115" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4178,10 +4172,10 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G116" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4189,135 +4183,132 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="G117" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A118" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>245</v>
+        <v>310</v>
+      </c>
+      <c r="G118" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B119" t="s">
-        <v>312</v>
-      </c>
-      <c r="M119" t="s">
-        <v>313</v>
+        <v>245</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B120" t="s">
-        <v>314</v>
-      </c>
-      <c r="C120" t="s">
-        <v>248</v>
-      </c>
-      <c r="E120" t="s">
-        <v>249</v>
+        <v>312</v>
+      </c>
+      <c r="M120" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B121" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C121" t="s">
-        <v>251</v>
-      </c>
-      <c r="D121" t="s">
-        <v>124</v>
+        <v>248</v>
       </c>
       <c r="E121" t="s">
-        <v>252</v>
-      </c>
-      <c r="F121" t="s">
-        <v>125</v>
+        <v>249</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B122" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C122" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="D122" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="E122" t="s">
-        <v>317</v>
+        <v>252</v>
       </c>
       <c r="F122" t="s">
-        <v>130</v>
-      </c>
-      <c r="I122" t="s">
-        <v>29</v>
-      </c>
-      <c r="J122" t="s">
-        <v>131</v>
-      </c>
-      <c r="M122" t="s">
-        <v>318</v>
+        <v>125</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B123" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C123" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D123" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E123" t="s">
-        <v>259</v>
+        <v>317</v>
       </c>
       <c r="F123" t="s">
-        <v>137</v>
+        <v>130</v>
+      </c>
+      <c r="I123" t="s">
+        <v>29</v>
       </c>
       <c r="J123" t="s">
-        <v>260</v>
-      </c>
-      <c r="K123" t="s">
-        <v>139</v>
-      </c>
-      <c r="L123" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="M123" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B124" t="s">
-        <v>321</v>
-      </c>
-      <c r="G124" t="s">
-        <v>322</v>
+        <v>319</v>
+      </c>
+      <c r="C124" t="s">
+        <v>258</v>
+      </c>
+      <c r="D124" t="s">
+        <v>136</v>
+      </c>
+      <c r="E124" t="s">
+        <v>259</v>
+      </c>
+      <c r="F124" t="s">
+        <v>137</v>
+      </c>
+      <c r="J124" t="s">
+        <v>260</v>
+      </c>
+      <c r="K124" t="s">
+        <v>139</v>
+      </c>
+      <c r="L124" t="s">
+        <v>140</v>
       </c>
       <c r="M124" t="s">
         <v>320</v>
@@ -4328,27 +4319,24 @@
         <v>17</v>
       </c>
       <c r="B125" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G125" t="s">
-        <v>324</v>
+        <v>322</v>
+      </c>
+      <c r="M125" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B126" t="s">
-        <v>325</v>
-      </c>
-      <c r="C126" t="s">
-        <v>267</v>
-      </c>
-      <c r="E126" t="s">
-        <v>268</v>
-      </c>
-      <c r="M126" t="s">
-        <v>326</v>
+        <v>323</v>
+      </c>
+      <c r="G126" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4356,125 +4344,125 @@
         <v>48</v>
       </c>
       <c r="B127" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C127" t="s">
-        <v>328</v>
+        <v>267</v>
       </c>
       <c r="E127" t="s">
-        <v>329</v>
+        <v>268</v>
       </c>
       <c r="M127" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>154</v>
+        <v>48</v>
       </c>
       <c r="B128" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="C128" t="s">
-        <v>275</v>
-      </c>
-      <c r="D128" t="s">
-        <v>158</v>
+        <v>328</v>
       </c>
       <c r="E128" t="s">
-        <v>276</v>
-      </c>
-      <c r="F128" t="s">
-        <v>159</v>
-      </c>
-      <c r="J128" t="s">
-        <v>160</v>
-      </c>
-      <c r="K128" t="s">
-        <v>161</v>
-      </c>
-      <c r="L128" t="s">
-        <v>162</v>
+        <v>329</v>
+      </c>
+      <c r="M128" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="B129" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C129" t="s">
-        <v>278</v>
+        <v>275</v>
+      </c>
+      <c r="D129" t="s">
+        <v>158</v>
       </c>
       <c r="E129" t="s">
-        <v>279</v>
-      </c>
-      <c r="M129" t="s">
-        <v>333</v>
+        <v>276</v>
+      </c>
+      <c r="F129" t="s">
+        <v>159</v>
+      </c>
+      <c r="J129" t="s">
+        <v>160</v>
+      </c>
+      <c r="K129" t="s">
+        <v>161</v>
+      </c>
+      <c r="L129" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="B130" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C130" t="s">
-        <v>282</v>
-      </c>
-      <c r="D130" t="s">
-        <v>171</v>
+        <v>278</v>
       </c>
       <c r="E130" t="s">
-        <v>283</v>
-      </c>
-      <c r="F130" t="s">
-        <v>172</v>
-      </c>
-      <c r="J130" t="s">
-        <v>173</v>
-      </c>
-      <c r="K130" t="s">
-        <v>174</v>
-      </c>
-      <c r="L130" t="s">
-        <v>175</v>
+        <v>279</v>
+      </c>
+      <c r="M130" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>176</v>
+        <v>154</v>
       </c>
       <c r="B131" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C131" t="s">
-        <v>285</v>
+        <v>282</v>
+      </c>
+      <c r="D131" t="s">
+        <v>171</v>
       </c>
       <c r="E131" t="s">
-        <v>286</v>
-      </c>
-      <c r="M131" t="s">
-        <v>336</v>
+        <v>283</v>
+      </c>
+      <c r="F131" t="s">
+        <v>172</v>
+      </c>
+      <c r="J131" t="s">
+        <v>173</v>
+      </c>
+      <c r="K131" t="s">
+        <v>174</v>
+      </c>
+      <c r="L131" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="B132" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C132" t="s">
-        <v>182</v>
+        <v>285</v>
       </c>
       <c r="E132" t="s">
-        <v>183</v>
+        <v>286</v>
       </c>
       <c r="M132" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4482,27 +4470,33 @@
         <v>48</v>
       </c>
       <c r="B133" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C133" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="E133" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="M133" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B134" t="s">
-        <v>341</v>
-      </c>
-      <c r="G134" t="s">
-        <v>342</v>
+        <v>339</v>
+      </c>
+      <c r="C134" t="s">
+        <v>186</v>
+      </c>
+      <c r="E134" t="s">
+        <v>187</v>
+      </c>
+      <c r="M134" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4510,47 +4504,47 @@
         <v>17</v>
       </c>
       <c r="B135" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G135" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B136" t="s">
-        <v>345</v>
-      </c>
-      <c r="C136" t="s">
-        <v>297</v>
-      </c>
-      <c r="E136" t="s">
-        <v>298</v>
-      </c>
-      <c r="J136" t="s">
-        <v>192</v>
-      </c>
-      <c r="K136" t="s">
-        <v>193</v>
-      </c>
-      <c r="L136" t="s">
-        <v>194</v>
-      </c>
-      <c r="M136" t="s">
-        <v>346</v>
+        <v>343</v>
+      </c>
+      <c r="G136" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B137" t="s">
-        <v>347</v>
-      </c>
-      <c r="G137" t="s">
-        <v>348</v>
+        <v>345</v>
+      </c>
+      <c r="C137" t="s">
+        <v>297</v>
+      </c>
+      <c r="E137" t="s">
+        <v>298</v>
+      </c>
+      <c r="J137" t="s">
+        <v>192</v>
+      </c>
+      <c r="K137" t="s">
+        <v>193</v>
+      </c>
+      <c r="L137" t="s">
+        <v>194</v>
+      </c>
+      <c r="M137" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4558,10 +4552,10 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G138" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4569,10 +4563,10 @@
         <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G139" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4580,10 +4574,10 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G140" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4591,10 +4585,10 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G141" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4602,32 +4596,29 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G142" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A143" t="s">
+        <v>17</v>
+      </c>
+      <c r="B143" t="s">
+        <v>357</v>
+      </c>
+      <c r="G143" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A144" t="s">
         <v>43</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B144" t="s">
         <v>312</v>
-      </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A145" t="s">
-        <v>78</v>
-      </c>
-      <c r="B145" t="s">
-        <v>539</v>
-      </c>
-      <c r="C145" t="s">
-        <v>545</v>
-      </c>
-      <c r="M145" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4635,16 +4626,13 @@
         <v>78</v>
       </c>
       <c r="B146" t="s">
-        <v>540</v>
+        <v>523</v>
       </c>
       <c r="C146" t="s">
-        <v>546</v>
-      </c>
-      <c r="D146" t="s">
-        <v>552</v>
+        <v>529</v>
       </c>
       <c r="M146" t="s">
-        <v>624</v>
+        <v>607</v>
       </c>
     </row>
     <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4652,16 +4640,16 @@
         <v>78</v>
       </c>
       <c r="B147" t="s">
-        <v>541</v>
+        <v>524</v>
       </c>
       <c r="C147" t="s">
-        <v>547</v>
+        <v>530</v>
       </c>
       <c r="D147" t="s">
-        <v>551</v>
+        <v>536</v>
       </c>
       <c r="M147" t="s">
-        <v>624</v>
+        <v>608</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4669,13 +4657,16 @@
         <v>78</v>
       </c>
       <c r="B148" t="s">
-        <v>542</v>
+        <v>525</v>
       </c>
       <c r="C148" t="s">
-        <v>548</v>
+        <v>531</v>
+      </c>
+      <c r="D148" t="s">
+        <v>535</v>
       </c>
       <c r="M148" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4683,13 +4674,13 @@
         <v>78</v>
       </c>
       <c r="B149" t="s">
-        <v>543</v>
+        <v>526</v>
       </c>
       <c r="C149" t="s">
-        <v>549</v>
+        <v>532</v>
       </c>
       <c r="M149" t="s">
-        <v>622</v>
+        <v>606</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4697,27 +4688,27 @@
         <v>78</v>
       </c>
       <c r="B150" t="s">
-        <v>544</v>
+        <v>527</v>
       </c>
       <c r="C150" t="s">
-        <v>550</v>
+        <v>533</v>
       </c>
       <c r="M150" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A152" t="s">
-        <v>17</v>
-      </c>
-      <c r="B152" t="s">
-        <v>359</v>
-      </c>
-      <c r="G152" t="s">
-        <v>96</v>
-      </c>
-      <c r="M152" t="s">
-        <v>360</v>
+        <v>606</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A151" t="s">
+        <v>78</v>
+      </c>
+      <c r="B151" t="s">
+        <v>528</v>
+      </c>
+      <c r="C151" t="s">
+        <v>534</v>
+      </c>
+      <c r="M151" t="s">
+        <v>606</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4725,50 +4716,47 @@
         <v>17</v>
       </c>
       <c r="B153" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G153" t="s">
         <v>96</v>
       </c>
       <c r="M153" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B154" t="s">
-        <v>363</v>
-      </c>
-      <c r="C154" t="s">
-        <v>510</v>
-      </c>
-      <c r="D154" t="s">
-        <v>365</v>
-      </c>
-      <c r="E154" t="s">
-        <v>364</v>
-      </c>
-      <c r="F154" t="s">
-        <v>366</v>
+        <v>361</v>
+      </c>
+      <c r="G154" t="s">
+        <v>96</v>
       </c>
       <c r="M154" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
-        <v>368</v>
+        <v>48</v>
       </c>
       <c r="B155" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="C155" t="s">
-        <v>370</v>
+        <v>626</v>
+      </c>
+      <c r="D155" t="s">
+        <v>365</v>
       </c>
       <c r="E155" t="s">
-        <v>371</v>
+        <v>364</v>
+      </c>
+      <c r="F155" t="s">
+        <v>366</v>
       </c>
       <c r="M155" t="s">
         <v>367</v>
@@ -4776,73 +4764,59 @@
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
-        <v>48</v>
+        <v>368</v>
       </c>
       <c r="B156" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="C156" t="s">
-        <v>511</v>
-      </c>
-      <c r="D156" t="s">
-        <v>374</v>
+        <v>628</v>
       </c>
       <c r="E156" t="s">
-        <v>373</v>
-      </c>
-      <c r="F156" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="M156" t="s">
-        <v>376</v>
+        <v>367</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
-        <v>377</v>
+        <v>48</v>
       </c>
       <c r="B157" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C157" t="s">
-        <v>379</v>
+        <v>627</v>
+      </c>
+      <c r="D157" t="s">
+        <v>373</v>
       </c>
       <c r="E157" t="s">
-        <v>380</v>
+        <v>372</v>
+      </c>
+      <c r="F157" t="s">
+        <v>374</v>
       </c>
       <c r="M157" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
-        <v>48</v>
+        <v>376</v>
       </c>
       <c r="B158" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C158" t="s">
-        <v>512</v>
+        <v>629</v>
       </c>
       <c r="E158" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="M158" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A159" t="s">
-        <v>17</v>
-      </c>
-      <c r="B159" t="s">
-        <v>383</v>
-      </c>
-      <c r="G159" t="s">
-        <v>96</v>
-      </c>
-      <c r="M159" t="s">
-        <v>384</v>
+        <v>375</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4850,13 +4824,13 @@
         <v>17</v>
       </c>
       <c r="B160" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="G160" t="s">
         <v>96</v>
       </c>
       <c r="M160" t="s">
-        <v>629</v>
+        <v>380</v>
       </c>
     </row>
     <row r="161" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4864,13 +4838,13 @@
         <v>17</v>
       </c>
       <c r="B161" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="G161" t="s">
         <v>96</v>
       </c>
       <c r="M161" t="s">
-        <v>387</v>
+        <v>611</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4878,47 +4852,49 @@
         <v>17</v>
       </c>
       <c r="B162" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="G162" t="s">
         <v>96</v>
       </c>
       <c r="M162" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="163" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A163" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="163" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A163" t="s">
+        <v>17</v>
+      </c>
+      <c r="B163" t="s">
+        <v>384</v>
+      </c>
+      <c r="G163" t="s">
+        <v>96</v>
+      </c>
+      <c r="M163" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B164" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="165" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A165" s="1" t="s">
+    <row r="166" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B165" s="1" t="s">
-        <v>498</v>
-      </c>
-      <c r="C165" s="1" t="s">
-        <v>509</v>
-      </c>
-      <c r="N165" s="1" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" t="s">
-        <v>17</v>
-      </c>
-      <c r="B166" s="3" t="s">
-        <v>521</v>
-      </c>
-      <c r="C166" s="4"/>
-      <c r="G166" t="s">
-        <v>108</v>
+      <c r="B166" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="C166" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="N166" s="1" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="167" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4926,11 +4902,11 @@
         <v>17</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>522</v>
+        <v>509</v>
       </c>
       <c r="C167" s="4"/>
-      <c r="G167" s="3" t="s">
-        <v>530</v>
+      <c r="G167" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="168" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4938,11 +4914,11 @@
         <v>17</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="C168" s="4"/>
       <c r="G168" s="3" t="s">
-        <v>527</v>
+        <v>518</v>
       </c>
     </row>
     <row r="169" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4950,59 +4926,51 @@
         <v>17</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>524</v>
+        <v>511</v>
       </c>
       <c r="C169" s="4"/>
       <c r="G169" s="3" t="s">
-        <v>528</v>
+        <v>515</v>
       </c>
     </row>
     <row r="170" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A170" t="s">
+        <v>17</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>512</v>
+      </c>
+      <c r="C170" s="4"/>
+      <c r="G170" s="3" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A171" t="s">
         <v>48</v>
       </c>
-      <c r="B170" t="s">
-        <v>525</v>
-      </c>
-      <c r="C170" s="5" t="s">
-        <v>526</v>
-      </c>
-      <c r="E170" s="3" t="s">
+      <c r="B171" t="s">
+        <v>513</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>514</v>
+      </c>
+      <c r="E171" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="M170" s="3" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="171" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A171" s="7" t="s">
+      <c r="M171" s="3" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B171" s="7" t="s">
-        <v>514</v>
-      </c>
-      <c r="C171" s="7" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A172" t="s">
-        <v>78</v>
-      </c>
-      <c r="B172" t="s">
-        <v>496</v>
-      </c>
-      <c r="C172" t="s">
-        <v>535</v>
-      </c>
-      <c r="E172" t="s">
-        <v>79</v>
-      </c>
-      <c r="H172" t="s">
-        <v>22</v>
-      </c>
-      <c r="M172" s="3" t="s">
-        <v>537</v>
+      <c r="B172" s="7" t="s">
+        <v>502</v>
+      </c>
+      <c r="C172" s="7" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="173" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5010,10 +4978,10 @@
         <v>78</v>
       </c>
       <c r="B173" t="s">
-        <v>497</v>
+        <v>488</v>
       </c>
       <c r="C173" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
       <c r="E173" t="s">
         <v>79</v>
@@ -5022,214 +4990,223 @@
         <v>22</v>
       </c>
       <c r="M173" s="3" t="s">
-        <v>537</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>499</v>
+        <v>78</v>
       </c>
       <c r="B174" t="s">
-        <v>500</v>
-      </c>
-      <c r="C174" s="6" t="s">
-        <v>532</v>
-      </c>
-      <c r="J174" t="s">
-        <v>501</v>
-      </c>
-      <c r="K174" t="s">
-        <v>502</v>
+        <v>489</v>
+      </c>
+      <c r="C174" t="s">
+        <v>521</v>
+      </c>
+      <c r="E174" t="s">
+        <v>79</v>
+      </c>
+      <c r="H174" t="s">
+        <v>22</v>
       </c>
       <c r="M174" s="3" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
     </row>
     <row r="175" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" t="s">
-        <v>499</v>
+        <v>491</v>
       </c>
       <c r="B175" t="s">
-        <v>503</v>
+        <v>492</v>
       </c>
       <c r="C175" s="6" t="s">
-        <v>531</v>
+        <v>617</v>
       </c>
       <c r="J175" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="K175" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="M175" s="3" t="s">
-        <v>529</v>
+        <v>517</v>
       </c>
     </row>
     <row r="176" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
+        <v>491</v>
+      </c>
+      <c r="B176" t="s">
+        <v>495</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>618</v>
+      </c>
+      <c r="J176" t="s">
+        <v>497</v>
+      </c>
+      <c r="K176" t="s">
+        <v>498</v>
+      </c>
+      <c r="M176" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A177" t="s">
+        <v>491</v>
+      </c>
+      <c r="B177" t="s">
+        <v>496</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>619</v>
+      </c>
+      <c r="J177" t="s">
+        <v>500</v>
+      </c>
+      <c r="K177" t="s">
         <v>499</v>
       </c>
-      <c r="B176" t="s">
-        <v>504</v>
-      </c>
-      <c r="C176" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="J176" t="s">
-        <v>508</v>
-      </c>
-      <c r="K176" t="s">
-        <v>507</v>
-      </c>
-      <c r="M176" s="3" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="178" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A178" s="1" t="s">
+      <c r="M177" s="3" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B178" s="1" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A180" t="s">
-        <v>98</v>
-      </c>
-      <c r="B180" t="s">
-        <v>390</v>
-      </c>
-      <c r="C180" t="s">
-        <v>391</v>
-      </c>
-      <c r="D180" t="s">
-        <v>393</v>
-      </c>
-      <c r="E180" t="s">
-        <v>392</v>
-      </c>
-      <c r="F180" t="s">
-        <v>394</v>
+      <c r="B179" s="1" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="181" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A181" t="s">
-        <v>395</v>
+        <v>98</v>
       </c>
       <c r="B181" t="s">
-        <v>396</v>
+        <v>386</v>
       </c>
       <c r="C181" t="s">
-        <v>397</v>
+        <v>387</v>
       </c>
       <c r="D181" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="E181" t="s">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="F181" t="s">
-        <v>400</v>
-      </c>
-      <c r="H181" t="s">
-        <v>22</v>
-      </c>
-      <c r="M181" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
     </row>
     <row r="182" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
       <c r="B182" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C182" t="s">
+        <v>393</v>
+      </c>
+      <c r="D182" t="s">
+        <v>395</v>
+      </c>
+      <c r="E182" t="s">
+        <v>394</v>
+      </c>
+      <c r="F182" t="s">
+        <v>396</v>
+      </c>
+      <c r="H182" t="s">
+        <v>22</v>
+      </c>
+      <c r="M182" t="s">
         <v>397</v>
-      </c>
-      <c r="D182" t="s">
-        <v>399</v>
-      </c>
-      <c r="E182" t="s">
-        <v>398</v>
-      </c>
-      <c r="F182" t="s">
-        <v>400</v>
-      </c>
-      <c r="M182" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="B183" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="C183" t="s">
-        <v>397</v>
+        <v>393</v>
+      </c>
+      <c r="D183" t="s">
+        <v>395</v>
       </c>
       <c r="E183" t="s">
-        <v>398</v>
-      </c>
-      <c r="H183" t="s">
-        <v>22</v>
+        <v>394</v>
+      </c>
+      <c r="F183" t="s">
+        <v>396</v>
       </c>
       <c r="M183" t="s">
-        <v>406</v>
+        <v>52</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
-        <v>48</v>
+        <v>400</v>
       </c>
       <c r="B184" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
       <c r="C184" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="E184" t="s">
-        <v>409</v>
+        <v>394</v>
+      </c>
+      <c r="H184" t="s">
+        <v>22</v>
       </c>
       <c r="M184" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B185" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="C185" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="E185" t="s">
-        <v>413</v>
+        <v>405</v>
+      </c>
+      <c r="M185" t="s">
+        <v>406</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
+        <v>20</v>
+      </c>
+      <c r="B186" t="s">
+        <v>407</v>
+      </c>
+      <c r="C186" t="s">
+        <v>408</v>
+      </c>
+      <c r="E186" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A187" t="s">
         <v>43</v>
       </c>
-      <c r="B186" t="s">
+      <c r="B187" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A188" t="s">
-        <v>17</v>
-      </c>
-      <c r="B188" t="s">
-        <v>414</v>
-      </c>
-      <c r="G188" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5237,10 +5214,10 @@
         <v>17</v>
       </c>
       <c r="B189" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="G189" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="190" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5248,10 +5225,10 @@
         <v>17</v>
       </c>
       <c r="B190" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="G190" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5259,10 +5236,10 @@
         <v>17</v>
       </c>
       <c r="B191" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
       <c r="G191" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5270,10 +5247,10 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="G192" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5281,10 +5258,21 @@
         <v>17</v>
       </c>
       <c r="B193" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="G193" t="s">
-        <v>425</v>
+        <v>419</v>
+      </c>
+    </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A194" t="s">
+        <v>17</v>
+      </c>
+      <c r="B194" t="s">
+        <v>420</v>
+      </c>
+      <c r="G194" t="s">
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -5297,8 +5285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5308,7 +5296,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5328,10 +5316,10 @@
         <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D2" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5339,24 +5327,24 @@
         <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C3" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="D3" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="B4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="C4" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5367,10 +5355,10 @@
         <v>96</v>
       </c>
       <c r="C5" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D5" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5378,13 +5366,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C6" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D6" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5392,471 +5380,471 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C7" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="D7" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B8" t="s">
         <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B9" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C9" t="s">
-        <v>558</v>
+        <v>542</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B10" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C10" t="s">
-        <v>559</v>
+        <v>543</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B11" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C11" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B12" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="C12" t="s">
-        <v>592</v>
+        <v>576</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B13" t="s">
-        <v>561</v>
+        <v>545</v>
       </c>
       <c r="C13" t="s">
-        <v>593</v>
+        <v>577</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B14" t="s">
-        <v>562</v>
+        <v>546</v>
       </c>
       <c r="C14" t="s">
-        <v>594</v>
+        <v>578</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B15" t="s">
-        <v>563</v>
+        <v>547</v>
       </c>
       <c r="C15" t="s">
-        <v>595</v>
+        <v>579</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B16" t="s">
-        <v>564</v>
+        <v>548</v>
       </c>
       <c r="C16" t="s">
-        <v>596</v>
+        <v>580</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B17" t="s">
-        <v>565</v>
+        <v>549</v>
       </c>
       <c r="C17" t="s">
-        <v>597</v>
+        <v>581</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B18" t="s">
-        <v>566</v>
+        <v>550</v>
       </c>
       <c r="C18" t="s">
-        <v>598</v>
+        <v>582</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B19" t="s">
-        <v>567</v>
+        <v>551</v>
       </c>
       <c r="C19" t="s">
-        <v>599</v>
+        <v>583</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B20" t="s">
-        <v>568</v>
+        <v>552</v>
       </c>
       <c r="C20" t="s">
-        <v>600</v>
+        <v>584</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B21" t="s">
-        <v>569</v>
+        <v>553</v>
       </c>
       <c r="C21" t="s">
-        <v>601</v>
+        <v>585</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B22" t="s">
-        <v>570</v>
+        <v>554</v>
       </c>
       <c r="C22" t="s">
-        <v>602</v>
+        <v>586</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B23" t="s">
-        <v>571</v>
+        <v>555</v>
       </c>
       <c r="C23" t="s">
-        <v>603</v>
+        <v>587</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
+        <v>540</v>
+      </c>
+      <c r="B24" t="s">
         <v>556</v>
       </c>
-      <c r="B24" t="s">
-        <v>572</v>
-      </c>
       <c r="C24" t="s">
-        <v>604</v>
+        <v>588</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B25" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="C25" t="s">
-        <v>605</v>
+        <v>589</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B26" t="s">
-        <v>574</v>
+        <v>558</v>
       </c>
       <c r="C26" t="s">
-        <v>606</v>
+        <v>590</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B27" t="s">
-        <v>575</v>
+        <v>559</v>
       </c>
       <c r="C27" t="s">
-        <v>607</v>
+        <v>591</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B28" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="C28" t="s">
-        <v>608</v>
+        <v>592</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B29" t="s">
-        <v>577</v>
+        <v>561</v>
       </c>
       <c r="C29" t="s">
-        <v>609</v>
+        <v>593</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B30" t="s">
-        <v>578</v>
+        <v>562</v>
       </c>
       <c r="C30" t="s">
-        <v>610</v>
+        <v>594</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B31" t="s">
-        <v>579</v>
+        <v>563</v>
       </c>
       <c r="C31" t="s">
-        <v>611</v>
+        <v>595</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B32" t="s">
-        <v>580</v>
+        <v>564</v>
       </c>
       <c r="C32" t="s">
-        <v>612</v>
+        <v>596</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B33" t="s">
-        <v>581</v>
+        <v>565</v>
       </c>
       <c r="C33" t="s">
-        <v>613</v>
+        <v>597</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B34" t="s">
-        <v>582</v>
+        <v>566</v>
       </c>
       <c r="C34" t="s">
-        <v>614</v>
+        <v>598</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B35" t="s">
-        <v>583</v>
+        <v>567</v>
       </c>
       <c r="C35" t="s">
-        <v>615</v>
+        <v>599</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B36" t="s">
-        <v>584</v>
+        <v>568</v>
       </c>
       <c r="C36" t="s">
-        <v>616</v>
+        <v>600</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B37" t="s">
-        <v>585</v>
+        <v>569</v>
       </c>
       <c r="C37" t="s">
-        <v>617</v>
+        <v>601</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B38" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="C38" t="s">
-        <v>618</v>
+        <v>602</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B39" t="s">
-        <v>587</v>
+        <v>571</v>
       </c>
       <c r="C39" t="s">
-        <v>619</v>
+        <v>603</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B40" t="s">
-        <v>588</v>
+        <v>572</v>
       </c>
       <c r="C40" t="s">
-        <v>620</v>
+        <v>604</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="B41" t="s">
-        <v>589</v>
+        <v>573</v>
       </c>
       <c r="C41" t="s">
-        <v>621</v>
+        <v>605</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B42" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C42" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D42" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B43" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C43" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D43" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B44" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
       <c r="C44" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="D44" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
+        <v>439</v>
+      </c>
+      <c r="B45" t="s">
         <v>443</v>
       </c>
-      <c r="B45" t="s">
-        <v>447</v>
-      </c>
       <c r="C45" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="D45" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="B46" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C46" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="D46" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
+        <v>446</v>
+      </c>
+      <c r="B47" t="s">
         <v>450</v>
       </c>
-      <c r="B47" t="s">
-        <v>454</v>
-      </c>
       <c r="C47" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="D47" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5867,10 +5855,10 @@
         <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="D48" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5878,13 +5866,13 @@
         <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C49" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="D49" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5892,13 +5880,13 @@
         <v>98</v>
       </c>
       <c r="B50" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C50" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="D50" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5906,195 +5894,195 @@
         <v>98</v>
       </c>
       <c r="B51" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C51" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="D51" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B52" t="s">
         <v>96</v>
       </c>
       <c r="C52" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D52" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B53" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C53" t="s">
-        <v>465</v>
+        <v>620</v>
       </c>
       <c r="D53" t="s">
-        <v>466</v>
+        <v>461</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="B54" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C54" t="s">
-        <v>467</v>
+        <v>621</v>
       </c>
       <c r="D54" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B55" t="s">
         <v>96</v>
       </c>
       <c r="C55" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D55" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B56" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C56" t="s">
-        <v>470</v>
+        <v>623</v>
       </c>
       <c r="D56" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="B57" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C57" t="s">
-        <v>472</v>
+        <v>622</v>
       </c>
       <c r="D57" t="s">
-        <v>473</v>
+        <v>465</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B58" t="s">
         <v>96</v>
       </c>
       <c r="C58" t="s">
-        <v>475</v>
+        <v>467</v>
       </c>
       <c r="D58" t="s">
-        <v>476</v>
+        <v>468</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>474</v>
+        <v>466</v>
       </c>
       <c r="B59" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="C59" t="s">
-        <v>477</v>
+        <v>469</v>
       </c>
       <c r="D59" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B60" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C60" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
       <c r="D60" t="s">
-        <v>480</v>
+        <v>472</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>479</v>
+        <v>471</v>
       </c>
       <c r="B61" t="s">
-        <v>481</v>
+        <v>473</v>
       </c>
       <c r="C61" t="s">
-        <v>482</v>
+        <v>474</v>
       </c>
       <c r="D61" t="s">
-        <v>483</v>
+        <v>475</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>484</v>
+        <v>476</v>
       </c>
       <c r="B62" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C62" t="s">
-        <v>485</v>
+        <v>477</v>
       </c>
       <c r="D62" t="s">
-        <v>486</v>
+        <v>478</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B63" t="s">
         <v>96</v>
       </c>
       <c r="C63" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="D63" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>487</v>
+        <v>479</v>
       </c>
       <c r="B64" t="s">
-        <v>488</v>
+        <v>480</v>
       </c>
       <c r="C64" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D64" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
   </sheetData>
@@ -6114,30 +6102,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>489</v>
+        <v>481</v>
       </c>
       <c r="B1" t="s">
-        <v>490</v>
+        <v>482</v>
       </c>
       <c r="C1" t="s">
-        <v>491</v>
+        <v>483</v>
       </c>
       <c r="D1" t="s">
-        <v>492</v>
+        <v>484</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>626</v>
+        <v>609</v>
       </c>
       <c r="B2" t="s">
-        <v>493</v>
+        <v>485</v>
       </c>
       <c r="C2" t="s">
-        <v>627</v>
+        <v>610</v>
       </c>
       <c r="D2" t="s">
-        <v>494</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -6146,11 +6134,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
   <Receiver>
@@ -6200,80 +6183,22 @@
 </spe:Receivers>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C69700093184405E3670241B7C6447099EBC6EC" ma:contentTypeVersion="22" ma:contentTypeDescription="" ma:contentTypeScope="" ma:versionID="9828ed9dccc8f308ec8ef9d8079bb49d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="b147f249-7416-4137-943c-c9568737db59" xmlns:ns5="http://schemas.microsoft.com/sharepoint/v4" xmlns:ns6="be3559c3-162a-46c1-b278-386731838041" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="788da77500539f78e7497a486befbf8f" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -6712,17 +6637,88 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
@@ -6730,37 +6726,15 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7E97AFA-DF02-4BAF-A424-8DC01B9A260B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6783,10 +6757,24 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixed child/woman number - changed position
Errors remain in selecting women and children from household listing
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="80" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{45697E2A-AC7E-4240-9A1D-F3E69973E7BF}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8411BE0A-8A53-42BF-9B97-4619DD2883E3}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="632">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="633">
   <si>
     <t>type</t>
   </si>
@@ -327,9 +327,6 @@
     <t>numchildren</t>
   </si>
   <si>
-    <t>count-selected(${children})</t>
-  </si>
-  <si>
     <t>child</t>
   </si>
   <si>
@@ -345,9 +342,6 @@
     <t>child_selected_position</t>
   </si>
   <si>
-    <t>position(..)-1</t>
-  </si>
-  <si>
     <t>child_hh_position</t>
   </si>
   <si>
@@ -415,9 +409,6 @@
   </si>
   <si>
     <t>. &lt;= today()</t>
-  </si>
-  <si>
-    <t>${dob_known} ='1'</t>
   </si>
   <si>
     <t>xmonths</t>
@@ -1724,9 +1715,6 @@
     <t>join(' ',${hh_roster}[is_woman = true()]/hh_position)</t>
   </si>
   <si>
-    <t>count-selected(${women})</t>
-  </si>
-  <si>
     <t>${numwomen}</t>
   </si>
   <si>
@@ -2048,9 +2036,6 @@
     <t>Now entering data for child: ${child_name} (${CHSEX}) with age in years: ${child_age_years}</t>
   </si>
   <si>
-    <t>${child_name} is ${MONTHS} months old.</t>
-  </si>
-  <si>
     <t>Woman's MUAC in MM of ${wom_name}</t>
   </si>
   <si>
@@ -2075,9 +2060,6 @@
     <t>Woman section</t>
   </si>
   <si>
-    <t>Selposit-${wom_selected_position} HHposit- ${wom_hh_position} Name-${wom_name} Sex-${sex} Age-${wom_age_years} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
-  </si>
-  <si>
     <t>${child_name}  has SEVERE ACUTE MALNUTRITION (SAM).</t>
   </si>
   <si>
@@ -2100,6 +2082,27 @@
   </si>
   <si>
     <t>if(${age_years} &gt;14 and ${age_years} &lt;50 and ${sex}= 'f',1,0)</t>
+  </si>
+  <si>
+    <t>${child_name} - is ${MONTHS} months old.</t>
+  </si>
+  <si>
+    <t>sum(${is_child})</t>
+  </si>
+  <si>
+    <t>sum(${is_woman})</t>
+  </si>
+  <si>
+    <t>position(..)-1</t>
+  </si>
+  <si>
+    <t>${dob_known} =1</t>
+  </si>
+  <si>
+    <t>Select_pos-${wom_selected_position} HH_pos- ${wom_hh_position} Name-${wom_name} Sex-${sex} Age-${wom_age_years} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select_pos-${child_selected_position} HH_pos- ${child_hh_position} Name-${child_name} Sex-${CHSEX} Age-${child_age_years} </t>
   </si>
 </sst>
 </file>
@@ -2514,11 +2517,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N194"/>
+  <dimension ref="A1:N196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2612,13 +2615,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="B6" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="C6" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2765,10 +2768,10 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="E17" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2858,7 +2861,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
@@ -2875,12 +2878,12 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="G24" s="8" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2948,7 +2951,7 @@
         <v>80</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2956,10 +2959,10 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3055,7 +3058,7 @@
         <v>100</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>101</v>
+        <v>627</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3063,10 +3066,10 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3074,10 +3077,10 @@
         <v>17</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>506</v>
+        <v>628</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3085,10 +3088,10 @@
         <v>48</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3097,16 +3100,16 @@
         <v>59</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>104</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3114,10 +3117,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G46" t="s">
-        <v>107</v>
+        <v>629</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3125,10 +3128,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G47" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3136,10 +3139,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G48" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3147,10 +3150,10 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G49" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3158,10 +3161,10 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G50" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3169,402 +3172,392 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" t="s">
+        <v>609</v>
+      </c>
+      <c r="E51" t="s">
+        <v>115</v>
+      </c>
+      <c r="M51" t="s">
         <v>116</v>
       </c>
-      <c r="C51" t="s">
-        <v>613</v>
-      </c>
-      <c r="E51" t="s">
-        <v>117</v>
-      </c>
-      <c r="M51" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A52" t="s">
-        <v>25</v>
-      </c>
-      <c r="B52" t="s">
-        <v>119</v>
-      </c>
-      <c r="M52" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A53" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" t="s">
-        <v>120</v>
-      </c>
-      <c r="C53" t="s">
-        <v>121</v>
-      </c>
-      <c r="D53" t="s">
-        <v>123</v>
-      </c>
-      <c r="E53" t="s">
-        <v>122</v>
-      </c>
-      <c r="F53" t="s">
-        <v>124</v>
-      </c>
-      <c r="H53" t="s">
-        <v>22</v>
-      </c>
-    </row>
+    </row>
+    <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="C52" s="7" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="54" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>125</v>
-      </c>
-      <c r="C54" t="s">
-        <v>126</v>
-      </c>
-      <c r="D54" t="s">
-        <v>128</v>
-      </c>
-      <c r="E54" t="s">
-        <v>127</v>
-      </c>
-      <c r="F54" t="s">
-        <v>129</v>
-      </c>
-      <c r="I54" t="s">
-        <v>29</v>
-      </c>
-      <c r="J54" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="M54" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C55" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E55" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="F55" t="s">
-        <v>136</v>
-      </c>
-      <c r="J55" t="s">
-        <v>137</v>
-      </c>
-      <c r="K55" t="s">
-        <v>138</v>
-      </c>
-      <c r="L55" t="s">
-        <v>139</v>
-      </c>
-      <c r="M55" t="s">
-        <v>140</v>
+        <v>122</v>
+      </c>
+      <c r="H55" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B56" t="s">
-        <v>141</v>
-      </c>
-      <c r="G56" t="s">
-        <v>142</v>
+        <v>123</v>
+      </c>
+      <c r="C56" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" t="s">
+        <v>126</v>
+      </c>
+      <c r="E56" t="s">
+        <v>125</v>
+      </c>
+      <c r="F56" t="s">
+        <v>127</v>
+      </c>
+      <c r="I56" t="s">
+        <v>29</v>
+      </c>
+      <c r="J56" t="s">
+        <v>128</v>
       </c>
       <c r="M56" t="s">
-        <v>140</v>
+        <v>630</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
-      </c>
-      <c r="G57" t="s">
-        <v>144</v>
+        <v>129</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+      <c r="D57" t="s">
+        <v>132</v>
+      </c>
+      <c r="E57" t="s">
+        <v>131</v>
+      </c>
+      <c r="F57" t="s">
+        <v>133</v>
+      </c>
+      <c r="J57" t="s">
+        <v>134</v>
+      </c>
+      <c r="K57" t="s">
+        <v>135</v>
+      </c>
+      <c r="L57" t="s">
+        <v>136</v>
+      </c>
+      <c r="M57" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B58" t="s">
-        <v>145</v>
-      </c>
-      <c r="C58" t="s">
-        <v>146</v>
-      </c>
-      <c r="E58" t="s">
-        <v>147</v>
+        <v>138</v>
+      </c>
+      <c r="G58" t="s">
+        <v>139</v>
       </c>
       <c r="M58" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
+        <v>17</v>
+      </c>
+      <c r="B59" t="s">
+        <v>140</v>
+      </c>
+      <c r="G59" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
         <v>48</v>
       </c>
-      <c r="B59" t="s">
-        <v>149</v>
-      </c>
-      <c r="C59" t="s">
-        <v>614</v>
-      </c>
-      <c r="E59" t="s">
-        <v>150</v>
-      </c>
-      <c r="M59" t="s">
-        <v>151</v>
+      <c r="B60" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" t="s">
+        <v>143</v>
+      </c>
+      <c r="E60" t="s">
+        <v>144</v>
+      </c>
+      <c r="M60" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A62" t="s">
-        <v>153</v>
-      </c>
-      <c r="B62" t="s">
-        <v>154</v>
-      </c>
-      <c r="C62" t="s">
-        <v>155</v>
-      </c>
-      <c r="D62" t="s">
-        <v>157</v>
-      </c>
-      <c r="E62" t="s">
-        <v>156</v>
-      </c>
-      <c r="F62" t="s">
-        <v>158</v>
-      </c>
-      <c r="J62" t="s">
-        <v>159</v>
-      </c>
-      <c r="K62" t="s">
-        <v>160</v>
-      </c>
-      <c r="L62" t="s">
-        <v>161</v>
+        <v>146</v>
+      </c>
+      <c r="C61" t="s">
+        <v>626</v>
+      </c>
+      <c r="E61" t="s">
+        <v>147</v>
+      </c>
+      <c r="M61" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>162</v>
+        <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>163</v>
-      </c>
-      <c r="C63" t="s">
-        <v>164</v>
-      </c>
-      <c r="E63" t="s">
-        <v>165</v>
-      </c>
-      <c r="M63" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" t="s">
+        <v>152</v>
+      </c>
+      <c r="D64" t="s">
+        <v>154</v>
+      </c>
+      <c r="E64" t="s">
         <v>153</v>
       </c>
-      <c r="B64" t="s">
-        <v>167</v>
-      </c>
-      <c r="C64" t="s">
-        <v>168</v>
-      </c>
-      <c r="D64" t="s">
-        <v>170</v>
-      </c>
-      <c r="E64" t="s">
-        <v>169</v>
-      </c>
       <c r="F64" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="J64" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="K64" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="L64" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B65" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="C65" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="E65" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="M65" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="B66" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="C66" t="s">
-        <v>181</v>
+        <v>165</v>
+      </c>
+      <c r="D66" t="s">
+        <v>167</v>
       </c>
       <c r="E66" t="s">
-        <v>182</v>
-      </c>
-      <c r="M66" t="s">
-        <v>183</v>
+        <v>166</v>
+      </c>
+      <c r="F66" t="s">
+        <v>168</v>
+      </c>
+      <c r="J66" t="s">
+        <v>169</v>
+      </c>
+      <c r="K66" t="s">
+        <v>170</v>
+      </c>
+      <c r="L66" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>48</v>
+        <v>172</v>
       </c>
       <c r="B67" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C67" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="E67" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="M67" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B68" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C68" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="E68" t="s">
-        <v>190</v>
-      </c>
-      <c r="J68" t="s">
-        <v>191</v>
-      </c>
-      <c r="K68" t="s">
-        <v>192</v>
-      </c>
-      <c r="L68" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="M68" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>162</v>
+        <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="C69" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="E69" t="s">
-        <v>197</v>
+        <v>183</v>
+      </c>
+      <c r="M69" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>78</v>
+        <v>30</v>
       </c>
       <c r="B70" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="C70" t="s">
-        <v>199</v>
+        <v>186</v>
       </c>
       <c r="E70" t="s">
-        <v>200</v>
-      </c>
-      <c r="H70" t="s">
-        <v>22</v>
+        <v>187</v>
+      </c>
+      <c r="J70" t="s">
+        <v>188</v>
+      </c>
+      <c r="K70" t="s">
+        <v>189</v>
+      </c>
+      <c r="L70" t="s">
+        <v>190</v>
       </c>
       <c r="M70" t="s">
-        <v>201</v>
+        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>43</v>
+        <v>159</v>
       </c>
       <c r="B71" t="s">
-        <v>152</v>
+        <v>192</v>
+      </c>
+      <c r="C71" t="s">
+        <v>193</v>
+      </c>
+      <c r="E71" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B72" t="s">
-        <v>119</v>
+        <v>195</v>
+      </c>
+      <c r="C72" t="s">
+        <v>196</v>
+      </c>
+      <c r="E72" t="s">
+        <v>197</v>
+      </c>
+      <c r="H72" t="s">
+        <v>22</v>
+      </c>
+      <c r="M72" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B73" t="s">
-        <v>202</v>
-      </c>
-      <c r="G73" t="s">
-        <v>203</v>
+        <v>149</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B74" t="s">
-        <v>204</v>
-      </c>
-      <c r="G74" t="s">
-        <v>205</v>
+        <v>117</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3572,10 +3565,10 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="G75" t="s">
-        <v>486</v>
+        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3583,10 +3576,10 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G76" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3594,13 +3587,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="G77" t="s">
-        <v>210</v>
-      </c>
-      <c r="M77" t="s">
-        <v>211</v>
+        <v>483</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3608,13 +3598,10 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G78" t="s">
-        <v>213</v>
-      </c>
-      <c r="M78" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3622,10 +3609,13 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="G79" t="s">
-        <v>215</v>
+        <v>207</v>
+      </c>
+      <c r="M79" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3633,13 +3623,13 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="G80" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="M80" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3647,13 +3637,10 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="G81" t="s">
-        <v>219</v>
-      </c>
-      <c r="M81" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3661,10 +3648,13 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="G82" t="s">
-        <v>221</v>
+        <v>214</v>
+      </c>
+      <c r="M82" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3672,13 +3662,13 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="G83" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="M83" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3686,13 +3676,10 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="G84" t="s">
-        <v>225</v>
-      </c>
-      <c r="M84" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3700,10 +3687,13 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="G85" t="s">
-        <v>227</v>
+        <v>220</v>
+      </c>
+      <c r="M85" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3711,10 +3701,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="G86" t="s">
-        <v>229</v>
+        <v>222</v>
+      </c>
+      <c r="M86" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3722,10 +3715,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="G87" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3733,10 +3726,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G88" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3744,10 +3737,10 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="G89" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3755,10 +3748,10 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="G90" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3766,10 +3759,10 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G91" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3777,10 +3770,10 @@
         <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="G92" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3788,350 +3781,335 @@
         <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G93" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+        <v>236</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" t="s">
+        <v>17</v>
+      </c>
+      <c r="B94" t="s">
+        <v>237</v>
+      </c>
+      <c r="G94" t="s">
+        <v>238</v>
+      </c>
+    </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B95" t="s">
-        <v>244</v>
-      </c>
-      <c r="M95" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A96" t="s">
-        <v>48</v>
-      </c>
-      <c r="B96" t="s">
-        <v>246</v>
-      </c>
-      <c r="C96" t="s">
-        <v>247</v>
-      </c>
-      <c r="E96" t="s">
-        <v>248</v>
-      </c>
-    </row>
+        <v>239</v>
+      </c>
+      <c r="G95" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B97" t="s">
-        <v>249</v>
-      </c>
-      <c r="C97" t="s">
-        <v>250</v>
-      </c>
-      <c r="D97" t="s">
-        <v>123</v>
-      </c>
-      <c r="E97" t="s">
-        <v>251</v>
-      </c>
-      <c r="F97" t="s">
-        <v>124</v>
+        <v>241</v>
+      </c>
+      <c r="M97" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B98" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C98" t="s">
-        <v>253</v>
-      </c>
-      <c r="D98" t="s">
-        <v>128</v>
+        <v>244</v>
       </c>
       <c r="E98" t="s">
-        <v>254</v>
-      </c>
-      <c r="F98" t="s">
-        <v>129</v>
-      </c>
-      <c r="I98" t="s">
-        <v>29</v>
-      </c>
-      <c r="J98" t="s">
-        <v>130</v>
-      </c>
-      <c r="M98" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B99" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C99" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D99" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E99" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="F99" t="s">
-        <v>136</v>
-      </c>
-      <c r="J99" t="s">
-        <v>259</v>
-      </c>
-      <c r="K99" t="s">
-        <v>138</v>
-      </c>
-      <c r="L99" t="s">
-        <v>139</v>
-      </c>
-      <c r="M99" t="s">
-        <v>260</v>
+        <v>122</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B100" t="s">
-        <v>261</v>
-      </c>
-      <c r="G100" t="s">
-        <v>262</v>
+        <v>249</v>
+      </c>
+      <c r="C100" t="s">
+        <v>250</v>
+      </c>
+      <c r="D100" t="s">
+        <v>126</v>
+      </c>
+      <c r="E100" t="s">
+        <v>251</v>
+      </c>
+      <c r="F100" t="s">
+        <v>127</v>
+      </c>
+      <c r="I100" t="s">
+        <v>29</v>
+      </c>
+      <c r="J100" t="s">
+        <v>128</v>
       </c>
       <c r="M100" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B101" t="s">
-        <v>263</v>
-      </c>
-      <c r="G101" t="s">
-        <v>264</v>
+        <v>253</v>
+      </c>
+      <c r="C101" t="s">
+        <v>254</v>
+      </c>
+      <c r="D101" t="s">
+        <v>132</v>
+      </c>
+      <c r="E101" t="s">
+        <v>255</v>
+      </c>
+      <c r="F101" t="s">
+        <v>133</v>
+      </c>
+      <c r="J101" t="s">
+        <v>256</v>
+      </c>
+      <c r="K101" t="s">
+        <v>135</v>
+      </c>
+      <c r="L101" t="s">
+        <v>136</v>
+      </c>
+      <c r="M101" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B102" t="s">
-        <v>265</v>
-      </c>
-      <c r="C102" t="s">
-        <v>266</v>
-      </c>
-      <c r="E102" t="s">
-        <v>267</v>
+        <v>258</v>
+      </c>
+      <c r="G102" t="s">
+        <v>259</v>
       </c>
       <c r="M102" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>269</v>
-      </c>
-      <c r="C103" t="s">
-        <v>270</v>
-      </c>
-      <c r="E103" t="s">
-        <v>271</v>
-      </c>
-      <c r="M103" t="s">
-        <v>272</v>
+        <v>260</v>
+      </c>
+      <c r="G103" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
       <c r="B104" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="C104" t="s">
-        <v>274</v>
-      </c>
-      <c r="D104" t="s">
-        <v>157</v>
+        <v>263</v>
       </c>
       <c r="E104" t="s">
-        <v>275</v>
-      </c>
-      <c r="F104" t="s">
-        <v>158</v>
-      </c>
-      <c r="J104" t="s">
-        <v>159</v>
-      </c>
-      <c r="K104" t="s">
-        <v>160</v>
-      </c>
-      <c r="L104" t="s">
-        <v>161</v>
+        <v>264</v>
+      </c>
+      <c r="M104" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>162</v>
+        <v>48</v>
       </c>
       <c r="B105" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C105" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="E105" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="M105" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B106" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C106" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D106" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E106" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="F106" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="J106" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="K106" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="L106" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B107" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="C107" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="E107" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="M107" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="B108" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C108" t="s">
-        <v>181</v>
+        <v>278</v>
+      </c>
+      <c r="D108" t="s">
+        <v>167</v>
       </c>
       <c r="E108" t="s">
-        <v>182</v>
-      </c>
-      <c r="M108" t="s">
-        <v>288</v>
+        <v>279</v>
+      </c>
+      <c r="F108" t="s">
+        <v>168</v>
+      </c>
+      <c r="J108" t="s">
+        <v>169</v>
+      </c>
+      <c r="K108" t="s">
+        <v>170</v>
+      </c>
+      <c r="L108" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>48</v>
+        <v>172</v>
       </c>
       <c r="B109" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="C109" t="s">
-        <v>185</v>
+        <v>281</v>
       </c>
       <c r="E109" t="s">
-        <v>186</v>
+        <v>282</v>
       </c>
       <c r="M109" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B110" t="s">
-        <v>291</v>
-      </c>
-      <c r="G110" t="s">
-        <v>292</v>
+        <v>284</v>
+      </c>
+      <c r="C110" t="s">
+        <v>178</v>
+      </c>
+      <c r="E110" t="s">
+        <v>179</v>
+      </c>
+      <c r="M110" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B111" t="s">
-        <v>293</v>
-      </c>
-      <c r="G111" t="s">
-        <v>294</v>
+        <v>286</v>
+      </c>
+      <c r="C111" t="s">
+        <v>182</v>
+      </c>
+      <c r="E111" t="s">
+        <v>183</v>
+      </c>
+      <c r="M111" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B112" t="s">
-        <v>295</v>
-      </c>
-      <c r="C112" t="s">
-        <v>296</v>
-      </c>
-      <c r="E112" t="s">
-        <v>297</v>
-      </c>
-      <c r="J112" t="s">
-        <v>191</v>
-      </c>
-      <c r="K112" t="s">
-        <v>192</v>
-      </c>
-      <c r="L112" t="s">
-        <v>193</v>
-      </c>
-      <c r="M112" t="s">
-        <v>298</v>
+        <v>288</v>
+      </c>
+      <c r="G112" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4139,21 +4117,36 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="G113" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B114" t="s">
-        <v>301</v>
-      </c>
-      <c r="G114" t="s">
-        <v>302</v>
+        <v>292</v>
+      </c>
+      <c r="C114" t="s">
+        <v>293</v>
+      </c>
+      <c r="E114" t="s">
+        <v>294</v>
+      </c>
+      <c r="J114" t="s">
+        <v>188</v>
+      </c>
+      <c r="K114" t="s">
+        <v>189</v>
+      </c>
+      <c r="L114" t="s">
+        <v>190</v>
+      </c>
+      <c r="M114" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4161,10 +4154,10 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="G115" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4172,10 +4165,10 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="G116" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4183,10 +4176,10 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="G117" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4194,357 +4187,342 @@
         <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="G118" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A119" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B119" t="s">
-        <v>244</v>
+        <v>304</v>
+      </c>
+      <c r="G119" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A120" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>311</v>
-      </c>
-      <c r="M120" t="s">
-        <v>312</v>
+        <v>306</v>
+      </c>
+      <c r="G120" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B121" t="s">
-        <v>313</v>
-      </c>
-      <c r="C121" t="s">
-        <v>247</v>
-      </c>
-      <c r="E121" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="B122" t="s">
-        <v>314</v>
-      </c>
-      <c r="C122" t="s">
-        <v>250</v>
-      </c>
-      <c r="D122" t="s">
-        <v>123</v>
-      </c>
-      <c r="E122" t="s">
-        <v>251</v>
-      </c>
-      <c r="F122" t="s">
-        <v>124</v>
+        <v>308</v>
+      </c>
+      <c r="M122" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B123" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C123" t="s">
-        <v>253</v>
-      </c>
-      <c r="D123" t="s">
-        <v>128</v>
+        <v>244</v>
       </c>
       <c r="E123" t="s">
-        <v>316</v>
-      </c>
-      <c r="F123" t="s">
-        <v>129</v>
-      </c>
-      <c r="I123" t="s">
-        <v>29</v>
-      </c>
-      <c r="J123" t="s">
-        <v>130</v>
-      </c>
-      <c r="M123" t="s">
-        <v>317</v>
+        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B124" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C124" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="D124" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="E124" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="F124" t="s">
-        <v>136</v>
-      </c>
-      <c r="J124" t="s">
-        <v>259</v>
-      </c>
-      <c r="K124" t="s">
-        <v>138</v>
-      </c>
-      <c r="L124" t="s">
-        <v>139</v>
-      </c>
-      <c r="M124" t="s">
-        <v>319</v>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B125" t="s">
-        <v>320</v>
-      </c>
-      <c r="G125" t="s">
-        <v>321</v>
+        <v>312</v>
+      </c>
+      <c r="C125" t="s">
+        <v>250</v>
+      </c>
+      <c r="D125" t="s">
+        <v>126</v>
+      </c>
+      <c r="E125" t="s">
+        <v>313</v>
+      </c>
+      <c r="F125" t="s">
+        <v>127</v>
+      </c>
+      <c r="I125" t="s">
+        <v>29</v>
+      </c>
+      <c r="J125" t="s">
+        <v>128</v>
       </c>
       <c r="M125" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B126" t="s">
-        <v>322</v>
-      </c>
-      <c r="G126" t="s">
-        <v>323</v>
+        <v>315</v>
+      </c>
+      <c r="C126" t="s">
+        <v>254</v>
+      </c>
+      <c r="D126" t="s">
+        <v>132</v>
+      </c>
+      <c r="E126" t="s">
+        <v>255</v>
+      </c>
+      <c r="F126" t="s">
+        <v>133</v>
+      </c>
+      <c r="J126" t="s">
+        <v>256</v>
+      </c>
+      <c r="K126" t="s">
+        <v>135</v>
+      </c>
+      <c r="L126" t="s">
+        <v>136</v>
+      </c>
+      <c r="M126" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B127" t="s">
-        <v>324</v>
-      </c>
-      <c r="C127" t="s">
-        <v>266</v>
-      </c>
-      <c r="E127" t="s">
-        <v>267</v>
+        <v>317</v>
+      </c>
+      <c r="G127" t="s">
+        <v>318</v>
       </c>
       <c r="M127" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A128" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B128" t="s">
-        <v>326</v>
-      </c>
-      <c r="C128" t="s">
-        <v>327</v>
-      </c>
-      <c r="E128" t="s">
-        <v>328</v>
-      </c>
-      <c r="M128" t="s">
-        <v>329</v>
+        <v>319</v>
+      </c>
+      <c r="G128" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>153</v>
+        <v>48</v>
       </c>
       <c r="B129" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C129" t="s">
-        <v>274</v>
-      </c>
-      <c r="D129" t="s">
-        <v>157</v>
+        <v>263</v>
       </c>
       <c r="E129" t="s">
-        <v>275</v>
-      </c>
-      <c r="F129" t="s">
-        <v>158</v>
-      </c>
-      <c r="J129" t="s">
-        <v>159</v>
-      </c>
-      <c r="K129" t="s">
-        <v>160</v>
-      </c>
-      <c r="L129" t="s">
-        <v>161</v>
+        <v>264</v>
+      </c>
+      <c r="M129" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>162</v>
+        <v>48</v>
       </c>
       <c r="B130" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C130" t="s">
-        <v>277</v>
+        <v>324</v>
       </c>
       <c r="E130" t="s">
-        <v>278</v>
+        <v>325</v>
       </c>
       <c r="M130" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B131" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="C131" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D131" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="E131" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="F131" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="J131" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="K131" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="L131" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="B132" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="C132" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="E132" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="M132" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>48</v>
+        <v>150</v>
       </c>
       <c r="B133" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="C133" t="s">
-        <v>181</v>
+        <v>278</v>
+      </c>
+      <c r="D133" t="s">
+        <v>167</v>
       </c>
       <c r="E133" t="s">
-        <v>182</v>
-      </c>
-      <c r="M133" t="s">
-        <v>337</v>
+        <v>279</v>
+      </c>
+      <c r="F133" t="s">
+        <v>168</v>
+      </c>
+      <c r="J133" t="s">
+        <v>169</v>
+      </c>
+      <c r="K133" t="s">
+        <v>170</v>
+      </c>
+      <c r="L133" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>48</v>
+        <v>172</v>
       </c>
       <c r="B134" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C134" t="s">
-        <v>185</v>
+        <v>281</v>
       </c>
       <c r="E134" t="s">
-        <v>186</v>
+        <v>282</v>
       </c>
       <c r="M134" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B135" t="s">
-        <v>340</v>
-      </c>
-      <c r="G135" t="s">
-        <v>341</v>
+        <v>333</v>
+      </c>
+      <c r="C135" t="s">
+        <v>178</v>
+      </c>
+      <c r="E135" t="s">
+        <v>179</v>
+      </c>
+      <c r="M135" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B136" t="s">
-        <v>342</v>
-      </c>
-      <c r="G136" t="s">
-        <v>343</v>
+        <v>335</v>
+      </c>
+      <c r="C136" t="s">
+        <v>182</v>
+      </c>
+      <c r="E136" t="s">
+        <v>183</v>
+      </c>
+      <c r="M136" t="s">
+        <v>336</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B137" t="s">
-        <v>344</v>
-      </c>
-      <c r="C137" t="s">
-        <v>296</v>
-      </c>
-      <c r="E137" t="s">
-        <v>297</v>
-      </c>
-      <c r="J137" t="s">
-        <v>191</v>
-      </c>
-      <c r="K137" t="s">
-        <v>192</v>
-      </c>
-      <c r="L137" t="s">
-        <v>193</v>
-      </c>
-      <c r="M137" t="s">
-        <v>345</v>
+        <v>337</v>
+      </c>
+      <c r="G137" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4552,21 +4530,36 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="G138" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B139" t="s">
-        <v>348</v>
-      </c>
-      <c r="G139" t="s">
-        <v>349</v>
+        <v>341</v>
+      </c>
+      <c r="C139" t="s">
+        <v>293</v>
+      </c>
+      <c r="E139" t="s">
+        <v>294</v>
+      </c>
+      <c r="J139" t="s">
+        <v>188</v>
+      </c>
+      <c r="K139" t="s">
+        <v>189</v>
+      </c>
+      <c r="L139" t="s">
+        <v>190</v>
+      </c>
+      <c r="M139" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4574,10 +4567,10 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="G140" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4585,10 +4578,10 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="G141" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4596,10 +4589,10 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="G142" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4607,49 +4600,40 @@
         <v>17</v>
       </c>
       <c r="B143" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="G143" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A144" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B144" t="s">
-        <v>311</v>
+        <v>351</v>
+      </c>
+      <c r="G144" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A145" t="s">
+        <v>17</v>
+      </c>
+      <c r="B145" t="s">
+        <v>353</v>
+      </c>
+      <c r="G145" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
-        <v>78</v>
+        <v>43</v>
       </c>
       <c r="B146" t="s">
-        <v>521</v>
-      </c>
-      <c r="C146" t="s">
-        <v>527</v>
-      </c>
-      <c r="M146" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A147" t="s">
-        <v>78</v>
-      </c>
-      <c r="B147" t="s">
-        <v>522</v>
-      </c>
-      <c r="C147" t="s">
-        <v>528</v>
-      </c>
-      <c r="D147" t="s">
-        <v>534</v>
-      </c>
-      <c r="M147" t="s">
-        <v>606</v>
+        <v>308</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4657,16 +4641,13 @@
         <v>78</v>
       </c>
       <c r="B148" t="s">
+        <v>517</v>
+      </c>
+      <c r="C148" t="s">
         <v>523</v>
       </c>
-      <c r="C148" t="s">
-        <v>529</v>
-      </c>
-      <c r="D148" t="s">
-        <v>533</v>
-      </c>
       <c r="M148" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4674,13 +4655,16 @@
         <v>78</v>
       </c>
       <c r="B149" t="s">
+        <v>518</v>
+      </c>
+      <c r="C149" t="s">
         <v>524</v>
       </c>
-      <c r="C149" t="s">
+      <c r="D149" t="s">
         <v>530</v>
       </c>
       <c r="M149" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4688,13 +4672,16 @@
         <v>78</v>
       </c>
       <c r="B150" t="s">
+        <v>519</v>
+      </c>
+      <c r="C150" t="s">
         <v>525</v>
       </c>
-      <c r="C150" t="s">
-        <v>531</v>
+      <c r="D150" t="s">
+        <v>529</v>
       </c>
       <c r="M150" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4702,81 +4689,69 @@
         <v>78</v>
       </c>
       <c r="B151" t="s">
+        <v>520</v>
+      </c>
+      <c r="C151" t="s">
         <v>526</v>
       </c>
-      <c r="C151" t="s">
-        <v>532</v>
-      </c>
       <c r="M151" t="s">
-        <v>604</v>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A152" t="s">
+        <v>78</v>
+      </c>
+      <c r="B152" t="s">
+        <v>521</v>
+      </c>
+      <c r="C152" t="s">
+        <v>527</v>
+      </c>
+      <c r="M152" t="s">
+        <v>600</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B153" t="s">
-        <v>358</v>
-      </c>
-      <c r="G153" t="s">
-        <v>95</v>
+        <v>522</v>
+      </c>
+      <c r="C153" t="s">
+        <v>528</v>
       </c>
       <c r="M153" t="s">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A154" t="s">
-        <v>17</v>
-      </c>
-      <c r="B154" t="s">
-        <v>360</v>
-      </c>
-      <c r="G154" t="s">
-        <v>95</v>
-      </c>
-      <c r="M154" t="s">
-        <v>361</v>
+        <v>600</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A155" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>362</v>
-      </c>
-      <c r="C155" t="s">
-        <v>624</v>
-      </c>
-      <c r="D155" t="s">
-        <v>364</v>
-      </c>
-      <c r="E155" t="s">
-        <v>363</v>
-      </c>
-      <c r="F155" t="s">
-        <v>365</v>
+        <v>355</v>
+      </c>
+      <c r="G155" t="s">
+        <v>95</v>
       </c>
       <c r="M155" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A156" t="s">
-        <v>367</v>
+        <v>17</v>
       </c>
       <c r="B156" t="s">
-        <v>368</v>
-      </c>
-      <c r="C156" t="s">
-        <v>626</v>
-      </c>
-      <c r="E156" t="s">
-        <v>369</v>
+        <v>357</v>
+      </c>
+      <c r="G156" t="s">
+        <v>95</v>
       </c>
       <c r="M156" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4784,67 +4759,79 @@
         <v>48</v>
       </c>
       <c r="B157" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="C157" t="s">
-        <v>625</v>
+        <v>618</v>
       </c>
       <c r="D157" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="E157" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="F157" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="M157" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="B158" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="C158" t="s">
-        <v>627</v>
+        <v>620</v>
       </c>
       <c r="E158" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
       <c r="M158" t="s">
-        <v>374</v>
+        <v>363</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A159" t="s">
+        <v>48</v>
+      </c>
+      <c r="B159" t="s">
+        <v>367</v>
+      </c>
+      <c r="C159" t="s">
+        <v>619</v>
+      </c>
+      <c r="D159" t="s">
+        <v>369</v>
+      </c>
+      <c r="E159" t="s">
+        <v>368</v>
+      </c>
+      <c r="F159" t="s">
+        <v>370</v>
+      </c>
+      <c r="M159" t="s">
+        <v>371</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
-        <v>17</v>
+        <v>372</v>
       </c>
       <c r="B160" t="s">
-        <v>378</v>
-      </c>
-      <c r="G160" t="s">
-        <v>95</v>
+        <v>373</v>
+      </c>
+      <c r="C160" t="s">
+        <v>621</v>
+      </c>
+      <c r="E160" t="s">
+        <v>374</v>
       </c>
       <c r="M160" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A161" t="s">
-        <v>17</v>
-      </c>
-      <c r="B161" t="s">
-        <v>380</v>
-      </c>
-      <c r="G161" t="s">
-        <v>95</v>
-      </c>
-      <c r="M161" t="s">
-        <v>609</v>
+        <v>371</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4852,13 +4839,13 @@
         <v>17</v>
       </c>
       <c r="B162" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="G162" t="s">
         <v>95</v>
       </c>
       <c r="M162" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4866,59 +4853,63 @@
         <v>17</v>
       </c>
       <c r="B163" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="G163" t="s">
         <v>95</v>
       </c>
       <c r="M163" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="164" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A164" s="2" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="164" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A164" t="s">
+        <v>17</v>
+      </c>
+      <c r="B164" t="s">
+        <v>378</v>
+      </c>
+      <c r="G164" t="s">
+        <v>95</v>
+      </c>
+      <c r="M164" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="165" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A165" t="s">
+        <v>17</v>
+      </c>
+      <c r="B165" t="s">
+        <v>380</v>
+      </c>
+      <c r="G165" t="s">
+        <v>95</v>
+      </c>
+      <c r="M165" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B164" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="166" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" s="1" t="s">
+      <c r="B166" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A168" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B166" s="1" t="s">
-        <v>489</v>
-      </c>
-      <c r="C166" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="N166" s="1" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="167" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A167" t="s">
-        <v>17</v>
-      </c>
-      <c r="B167" s="3" t="s">
-        <v>508</v>
-      </c>
-      <c r="C167" s="4"/>
-      <c r="G167" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="168" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" t="s">
-        <v>17</v>
-      </c>
-      <c r="B168" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="C168" s="4"/>
-      <c r="G168" s="3" t="s">
-        <v>517</v>
+      <c r="B168" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="N168" s="1" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="169" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4926,11 +4917,11 @@
         <v>17</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>510</v>
+        <v>504</v>
       </c>
       <c r="C169" s="4"/>
-      <c r="G169" s="3" t="s">
-        <v>514</v>
+      <c r="G169" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="170" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4938,116 +4929,100 @@
         <v>17</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>511</v>
+        <v>505</v>
       </c>
       <c r="C170" s="4"/>
       <c r="G170" s="3" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
     </row>
     <row r="171" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A171" t="s">
+        <v>17</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="C171" s="4"/>
+      <c r="G171" s="3" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A172" t="s">
+        <v>17</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="C172" s="4"/>
+      <c r="G172" s="3" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A173" t="s">
         <v>48</v>
       </c>
-      <c r="B171" t="s">
-        <v>512</v>
-      </c>
-      <c r="C171" s="5" t="s">
-        <v>513</v>
-      </c>
-      <c r="E171" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="M171" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="172" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A172" s="7" t="s">
+      <c r="B173" t="s">
+        <v>508</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>509</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="M173" s="3" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B172" s="7" t="s">
-        <v>501</v>
-      </c>
-      <c r="C172" s="7" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A173" t="s">
+      <c r="B174" s="7" t="s">
+        <v>498</v>
+      </c>
+      <c r="C174" s="7" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" t="s">
         <v>78</v>
       </c>
-      <c r="B173" t="s">
-        <v>487</v>
-      </c>
-      <c r="C173" t="s">
-        <v>518</v>
-      </c>
-      <c r="E173" t="s">
+      <c r="B175" t="s">
+        <v>484</v>
+      </c>
+      <c r="C175" t="s">
+        <v>514</v>
+      </c>
+      <c r="E175" t="s">
         <v>79</v>
       </c>
-      <c r="H173" t="s">
+      <c r="H175" t="s">
         <v>22</v>
-      </c>
-      <c r="M173" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A174" t="s">
-        <v>78</v>
-      </c>
-      <c r="B174" t="s">
-        <v>488</v>
-      </c>
-      <c r="C174" t="s">
-        <v>519</v>
-      </c>
-      <c r="E174" t="s">
-        <v>79</v>
-      </c>
-      <c r="H174" t="s">
-        <v>22</v>
-      </c>
-      <c r="M174" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A175" t="s">
-        <v>490</v>
-      </c>
-      <c r="B175" t="s">
-        <v>491</v>
-      </c>
-      <c r="C175" s="6" t="s">
-        <v>615</v>
-      </c>
-      <c r="J175" t="s">
-        <v>492</v>
-      </c>
-      <c r="K175" t="s">
-        <v>493</v>
       </c>
       <c r="M175" s="3" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="176" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
-        <v>490</v>
+        <v>78</v>
       </c>
       <c r="B176" t="s">
-        <v>494</v>
-      </c>
-      <c r="C176" s="6" t="s">
-        <v>616</v>
-      </c>
-      <c r="J176" t="s">
-        <v>496</v>
-      </c>
-      <c r="K176" t="s">
-        <v>497</v>
+        <v>485</v>
+      </c>
+      <c r="C176" t="s">
+        <v>515</v>
+      </c>
+      <c r="E176" t="s">
+        <v>79</v>
+      </c>
+      <c r="H176" t="s">
+        <v>22</v>
       </c>
       <c r="M176" s="3" t="s">
         <v>516</v>
@@ -5055,180 +5030,198 @@
     </row>
     <row r="177" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
+        <v>487</v>
+      </c>
+      <c r="B177" t="s">
+        <v>488</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>610</v>
+      </c>
+      <c r="J177" t="s">
+        <v>489</v>
+      </c>
+      <c r="K177" t="s">
         <v>490</v>
       </c>
-      <c r="B177" t="s">
+      <c r="M177" s="3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A178" t="s">
+        <v>487</v>
+      </c>
+      <c r="B178" t="s">
+        <v>491</v>
+      </c>
+      <c r="C178" s="6" t="s">
+        <v>611</v>
+      </c>
+      <c r="J178" t="s">
+        <v>493</v>
+      </c>
+      <c r="K178" t="s">
+        <v>494</v>
+      </c>
+      <c r="M178" s="3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A179" t="s">
+        <v>487</v>
+      </c>
+      <c r="B179" t="s">
+        <v>492</v>
+      </c>
+      <c r="C179" s="6" t="s">
+        <v>612</v>
+      </c>
+      <c r="J179" t="s">
+        <v>496</v>
+      </c>
+      <c r="K179" t="s">
         <v>495</v>
       </c>
-      <c r="C177" s="6" t="s">
-        <v>617</v>
-      </c>
-      <c r="J177" t="s">
-        <v>499</v>
-      </c>
-      <c r="K177" t="s">
-        <v>498</v>
-      </c>
-      <c r="M177" s="3" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="179" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A179" s="1" t="s">
+      <c r="M179" s="3" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A181" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B179" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" t="s">
-        <v>97</v>
-      </c>
-      <c r="B181" t="s">
-        <v>385</v>
-      </c>
-      <c r="C181" t="s">
-        <v>386</v>
-      </c>
-      <c r="D181" t="s">
-        <v>388</v>
-      </c>
-      <c r="E181" t="s">
-        <v>387</v>
-      </c>
-      <c r="F181" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="182" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A182" t="s">
-        <v>390</v>
-      </c>
-      <c r="B182" t="s">
-        <v>391</v>
-      </c>
-      <c r="C182" t="s">
-        <v>392</v>
-      </c>
-      <c r="D182" t="s">
-        <v>394</v>
-      </c>
-      <c r="E182" t="s">
-        <v>393</v>
-      </c>
-      <c r="F182" t="s">
-        <v>395</v>
-      </c>
-      <c r="H182" t="s">
-        <v>22</v>
-      </c>
-      <c r="M182" t="s">
-        <v>396</v>
+      <c r="B181" s="1" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A183" t="s">
-        <v>397</v>
+        <v>97</v>
       </c>
       <c r="B183" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C183" t="s">
-        <v>392</v>
+        <v>383</v>
       </c>
       <c r="D183" t="s">
-        <v>394</v>
+        <v>385</v>
       </c>
       <c r="E183" t="s">
-        <v>393</v>
+        <v>384</v>
       </c>
       <c r="F183" t="s">
-        <v>395</v>
-      </c>
-      <c r="M183" t="s">
-        <v>52</v>
+        <v>386</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
-        <v>399</v>
+        <v>387</v>
       </c>
       <c r="B184" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="C184" t="s">
+        <v>389</v>
+      </c>
+      <c r="D184" t="s">
+        <v>391</v>
+      </c>
+      <c r="E184" t="s">
+        <v>390</v>
+      </c>
+      <c r="F184" t="s">
         <v>392</v>
-      </c>
-      <c r="E184" t="s">
-        <v>393</v>
       </c>
       <c r="H184" t="s">
         <v>22</v>
       </c>
       <c r="M184" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
-        <v>48</v>
+        <v>394</v>
       </c>
       <c r="B185" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C185" t="s">
-        <v>403</v>
+        <v>389</v>
+      </c>
+      <c r="D185" t="s">
+        <v>391</v>
       </c>
       <c r="E185" t="s">
-        <v>404</v>
+        <v>390</v>
+      </c>
+      <c r="F185" t="s">
+        <v>392</v>
       </c>
       <c r="M185" t="s">
-        <v>405</v>
+        <v>52</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
-        <v>20</v>
+        <v>396</v>
       </c>
       <c r="B186" t="s">
-        <v>406</v>
+        <v>397</v>
       </c>
       <c r="C186" t="s">
-        <v>407</v>
+        <v>389</v>
       </c>
       <c r="E186" t="s">
-        <v>408</v>
+        <v>390</v>
+      </c>
+      <c r="H186" t="s">
+        <v>22</v>
+      </c>
+      <c r="M186" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B187" t="s">
-        <v>44</v>
+        <v>399</v>
+      </c>
+      <c r="C187" t="s">
+        <v>400</v>
+      </c>
+      <c r="E187" t="s">
+        <v>401</v>
+      </c>
+      <c r="M187" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A188" t="s">
+        <v>20</v>
+      </c>
+      <c r="B188" t="s">
+        <v>403</v>
+      </c>
+      <c r="C188" t="s">
+        <v>404</v>
+      </c>
+      <c r="E188" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B189" t="s">
-        <v>409</v>
-      </c>
-      <c r="G189" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="190" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A190" t="s">
-        <v>17</v>
-      </c>
-      <c r="B190" t="s">
-        <v>411</v>
-      </c>
-      <c r="G190" t="s">
-        <v>412</v>
+        <v>44</v>
       </c>
     </row>
     <row r="191" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5236,10 +5229,10 @@
         <v>17</v>
       </c>
       <c r="B191" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="G191" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5247,10 +5240,10 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="G192" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5258,10 +5251,10 @@
         <v>17</v>
       </c>
       <c r="B193" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="G193" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5269,10 +5262,32 @@
         <v>17</v>
       </c>
       <c r="B194" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="G194" t="s">
-        <v>420</v>
+        <v>413</v>
+      </c>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A195" t="s">
+        <v>17</v>
+      </c>
+      <c r="B195" t="s">
+        <v>414</v>
+      </c>
+      <c r="G195" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A196" t="s">
+        <v>17</v>
+      </c>
+      <c r="B196" t="s">
+        <v>416</v>
+      </c>
+      <c r="G196" t="s">
+        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -5296,7 +5311,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5316,10 +5331,10 @@
         <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="D2" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5327,24 +5342,24 @@
         <v>96</v>
       </c>
       <c r="B3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="B4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C4" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5355,10 +5370,10 @@
         <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D5" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5366,13 +5381,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5380,471 +5395,471 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C7" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D7" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B8" t="s">
         <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B9" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C9" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B10" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C10" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
+        <v>534</v>
+      </c>
+      <c r="B11" t="s">
+        <v>455</v>
+      </c>
+      <c r="C11" t="s">
         <v>538</v>
-      </c>
-      <c r="B11" t="s">
-        <v>458</v>
-      </c>
-      <c r="C11" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B12" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C12" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B13" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="C13" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B14" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="C14" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B15" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="C15" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B16" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C16" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B17" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C17" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B18" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C18" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B19" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="C19" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B20" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="C20" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B21" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="C21" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B22" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C22" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B23" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="C23" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B24" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="C24" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B25" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C25" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B26" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="C26" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B27" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C27" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B28" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="C28" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B29" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="C29" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B30" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="C30" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B31" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="C31" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B32" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="C32" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B33" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="C33" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B34" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="C34" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B35" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="C35" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B36" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="C36" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B37" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="C37" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B38" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="C38" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B39" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="C39" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B40" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="C40" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="B41" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="C41" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B42" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C42" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D42" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="B43" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C43" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D43" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
+        <v>435</v>
+      </c>
+      <c r="B44" t="s">
+        <v>436</v>
+      </c>
+      <c r="C44" t="s">
+        <v>437</v>
+      </c>
+      <c r="D44" t="s">
         <v>438</v>
-      </c>
-      <c r="B44" t="s">
-        <v>439</v>
-      </c>
-      <c r="C44" t="s">
-        <v>440</v>
-      </c>
-      <c r="D44" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="B45" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C45" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="D45" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>442</v>
+      </c>
+      <c r="B46" t="s">
+        <v>443</v>
+      </c>
+      <c r="C46" t="s">
+        <v>444</v>
+      </c>
+      <c r="D46" t="s">
         <v>445</v>
-      </c>
-      <c r="B46" t="s">
-        <v>446</v>
-      </c>
-      <c r="C46" t="s">
-        <v>447</v>
-      </c>
-      <c r="D46" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B47" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C47" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D47" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5855,10 +5870,10 @@
         <v>95</v>
       </c>
       <c r="C48" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="D48" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5866,13 +5881,13 @@
         <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C49" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D49" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5880,13 +5895,13 @@
         <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C50" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="D50" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5894,195 +5909,195 @@
         <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C51" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="D51" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B52" t="s">
         <v>95</v>
       </c>
       <c r="C52" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D52" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B53" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C53" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="D53" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="B54" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C54" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D54" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B55" t="s">
         <v>95</v>
       </c>
       <c r="C55" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D55" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B56" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C56" t="s">
-        <v>621</v>
+        <v>616</v>
       </c>
       <c r="D56" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="B57" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C57" t="s">
-        <v>620</v>
+        <v>615</v>
       </c>
       <c r="D57" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="B58" t="s">
         <v>95</v>
       </c>
       <c r="C58" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="D58" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
+        <v>462</v>
+      </c>
+      <c r="B59" t="s">
+        <v>421</v>
+      </c>
+      <c r="C59" t="s">
         <v>465</v>
       </c>
-      <c r="B59" t="s">
-        <v>424</v>
-      </c>
-      <c r="C59" t="s">
-        <v>468</v>
-      </c>
       <c r="D59" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="B60" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C60" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="D60" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
+        <v>467</v>
+      </c>
+      <c r="B61" t="s">
+        <v>469</v>
+      </c>
+      <c r="C61" t="s">
         <v>470</v>
       </c>
-      <c r="B61" t="s">
-        <v>472</v>
-      </c>
-      <c r="C61" t="s">
-        <v>473</v>
-      </c>
       <c r="D61" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="B62" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C62" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D62" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B63" t="s">
         <v>95</v>
       </c>
       <c r="C63" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="D63" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="B64" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C64" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="D64" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -6102,30 +6117,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>477</v>
+      </c>
+      <c r="B1" t="s">
+        <v>478</v>
+      </c>
+      <c r="C1" t="s">
+        <v>479</v>
+      </c>
+      <c r="D1" t="s">
         <v>480</v>
-      </c>
-      <c r="B1" t="s">
-        <v>481</v>
-      </c>
-      <c r="C1" t="s">
-        <v>482</v>
-      </c>
-      <c r="D1" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="B2" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="C2" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="D2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
   </sheetData>
@@ -6135,7 +6150,11 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6190,75 +6209,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6701,19 +6662,73 @@
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6727,23 +6742,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6772,9 +6781,15 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
selection of woman / child from HH working
removed true - added =1
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{8411BE0A-8A53-42BF-9B97-4619DD2883E3}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3C7EEF80-2F8D-4F8D-A455-9888AE0535A0}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -319,9 +319,6 @@
   </si>
   <si>
     <t>children</t>
-  </si>
-  <si>
-    <t>join(' ',${hh_roster}[is_child = true()]/hh_position)</t>
   </si>
   <si>
     <t>numchildren</t>
@@ -1712,9 +1709,6 @@
     <t>numwomen</t>
   </si>
   <si>
-    <t>join(' ',${hh_roster}[is_woman = true()]/hh_position)</t>
-  </si>
-  <si>
     <t>${numwomen}</t>
   </si>
   <si>
@@ -2103,6 +2097,12 @@
   </si>
   <si>
     <t xml:space="preserve">Select_pos-${child_selected_position} HH_pos- ${child_hh_position} Name-${child_name} Sex-${CHSEX} Age-${child_age_years} </t>
+  </si>
+  <si>
+    <t>join(' ',${hh_roster}[is_child = 1]/hh_position)</t>
+  </si>
+  <si>
+    <t>join(' ',${hh_roster}[is_woman = 1]/hh_position)</t>
   </si>
 </sst>
 </file>
@@ -2520,8 +2520,8 @@
   <dimension ref="A1:N196"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2615,13 +2615,13 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
+        <v>529</v>
+      </c>
+      <c r="B6" t="s">
+        <v>530</v>
+      </c>
+      <c r="C6" t="s">
         <v>531</v>
-      </c>
-      <c r="B6" t="s">
-        <v>532</v>
-      </c>
-      <c r="C6" t="s">
-        <v>533</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -2768,10 +2768,10 @@
         <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="E17" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="H17" t="s">
         <v>22</v>
@@ -2861,7 +2861,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
@@ -2878,12 +2878,12 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="G24" s="8" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2951,7 +2951,7 @@
         <v>80</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2959,10 +2959,10 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3047,7 +3047,7 @@
         <v>98</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>99</v>
+        <v>631</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3055,10 +3055,10 @@
         <v>17</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3066,10 +3066,10 @@
         <v>17</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>502</v>
+        <v>632</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3077,10 +3077,10 @@
         <v>17</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3088,10 +3088,10 @@
         <v>48</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3100,16 +3100,16 @@
         <v>59</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="E45" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="E45" s="2" t="s">
+      <c r="N45" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3117,10 +3117,10 @@
         <v>17</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3128,10 +3128,10 @@
         <v>17</v>
       </c>
       <c r="B47" t="s">
+        <v>105</v>
+      </c>
+      <c r="G47" t="s">
         <v>106</v>
-      </c>
-      <c r="G47" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3139,10 +3139,10 @@
         <v>17</v>
       </c>
       <c r="B48" t="s">
+        <v>107</v>
+      </c>
+      <c r="G48" t="s">
         <v>108</v>
-      </c>
-      <c r="G48" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3150,10 +3150,10 @@
         <v>17</v>
       </c>
       <c r="B49" t="s">
+        <v>109</v>
+      </c>
+      <c r="G49" t="s">
         <v>110</v>
-      </c>
-      <c r="G49" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3161,10 +3161,10 @@
         <v>17</v>
       </c>
       <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="G50" t="s">
         <v>112</v>
-      </c>
-      <c r="G50" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3172,16 +3172,16 @@
         <v>48</v>
       </c>
       <c r="B51" t="s">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
+        <v>607</v>
+      </c>
+      <c r="E51" t="s">
         <v>114</v>
       </c>
-      <c r="C51" t="s">
-        <v>609</v>
-      </c>
-      <c r="E51" t="s">
+      <c r="M51" t="s">
         <v>115</v>
-      </c>
-      <c r="M51" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3189,10 +3189,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3201,10 +3201,10 @@
         <v>25</v>
       </c>
       <c r="B54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M54" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3212,19 +3212,19 @@
         <v>78</v>
       </c>
       <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" t="s">
         <v>118</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" t="s">
         <v>119</v>
       </c>
-      <c r="D55" t="s">
+      <c r="F55" t="s">
         <v>121</v>
-      </c>
-      <c r="E55" t="s">
-        <v>120</v>
-      </c>
-      <c r="F55" t="s">
-        <v>122</v>
       </c>
       <c r="H55" t="s">
         <v>22</v>
@@ -3235,28 +3235,28 @@
         <v>28</v>
       </c>
       <c r="B56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" t="s">
         <v>123</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>125</v>
+      </c>
+      <c r="E56" t="s">
         <v>124</v>
       </c>
-      <c r="D56" t="s">
+      <c r="F56" t="s">
         <v>126</v>
-      </c>
-      <c r="E56" t="s">
-        <v>125</v>
-      </c>
-      <c r="F56" t="s">
-        <v>127</v>
       </c>
       <c r="I56" t="s">
         <v>29</v>
       </c>
       <c r="J56" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M56" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3264,31 +3264,31 @@
         <v>30</v>
       </c>
       <c r="B57" t="s">
+        <v>128</v>
+      </c>
+      <c r="C57" t="s">
         <v>129</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>131</v>
+      </c>
+      <c r="E57" t="s">
         <v>130</v>
       </c>
-      <c r="D57" t="s">
+      <c r="F57" t="s">
         <v>132</v>
       </c>
-      <c r="E57" t="s">
-        <v>131</v>
-      </c>
-      <c r="F57" t="s">
+      <c r="J57" t="s">
         <v>133</v>
       </c>
-      <c r="J57" t="s">
+      <c r="K57" t="s">
         <v>134</v>
       </c>
-      <c r="K57" t="s">
+      <c r="L57" t="s">
         <v>135</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>136</v>
-      </c>
-      <c r="M57" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3296,13 +3296,13 @@
         <v>17</v>
       </c>
       <c r="B58" t="s">
+        <v>137</v>
+      </c>
+      <c r="G58" t="s">
         <v>138</v>
       </c>
-      <c r="G58" t="s">
-        <v>139</v>
-      </c>
       <c r="M58" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3310,10 +3310,10 @@
         <v>17</v>
       </c>
       <c r="B59" t="s">
+        <v>139</v>
+      </c>
+      <c r="G59" t="s">
         <v>140</v>
-      </c>
-      <c r="G59" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3321,16 +3321,16 @@
         <v>48</v>
       </c>
       <c r="B60" t="s">
+        <v>141</v>
+      </c>
+      <c r="C60" t="s">
         <v>142</v>
       </c>
-      <c r="C60" t="s">
+      <c r="E60" t="s">
         <v>143</v>
       </c>
-      <c r="E60" t="s">
+      <c r="M60" t="s">
         <v>144</v>
-      </c>
-      <c r="M60" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3338,16 +3338,16 @@
         <v>48</v>
       </c>
       <c r="B61" t="s">
+        <v>145</v>
+      </c>
+      <c r="C61" t="s">
+        <v>624</v>
+      </c>
+      <c r="E61" t="s">
         <v>146</v>
       </c>
-      <c r="C61" t="s">
-        <v>626</v>
-      </c>
-      <c r="E61" t="s">
+      <c r="M61" t="s">
         <v>147</v>
-      </c>
-      <c r="M61" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3355,99 +3355,99 @@
         <v>25</v>
       </c>
       <c r="B63" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
+        <v>149</v>
+      </c>
+      <c r="B64" t="s">
         <v>150</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>151</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
+        <v>153</v>
+      </c>
+      <c r="E64" t="s">
         <v>152</v>
       </c>
-      <c r="D64" t="s">
+      <c r="F64" t="s">
         <v>154</v>
       </c>
-      <c r="E64" t="s">
-        <v>153</v>
-      </c>
-      <c r="F64" t="s">
+      <c r="J64" t="s">
         <v>155</v>
       </c>
-      <c r="J64" t="s">
+      <c r="K64" t="s">
         <v>156</v>
       </c>
-      <c r="K64" t="s">
+      <c r="L64" t="s">
         <v>157</v>
-      </c>
-      <c r="L64" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
+        <v>158</v>
+      </c>
+      <c r="B65" t="s">
         <v>159</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>160</v>
       </c>
-      <c r="C65" t="s">
+      <c r="E65" t="s">
         <v>161</v>
       </c>
-      <c r="E65" t="s">
+      <c r="M65" t="s">
         <v>162</v>
-      </c>
-      <c r="M65" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
         <v>164</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
+        <v>166</v>
+      </c>
+      <c r="E66" t="s">
         <v>165</v>
       </c>
-      <c r="D66" t="s">
+      <c r="F66" t="s">
         <v>167</v>
       </c>
-      <c r="E66" t="s">
-        <v>166</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="J66" t="s">
         <v>168</v>
       </c>
-      <c r="J66" t="s">
+      <c r="K66" t="s">
         <v>169</v>
       </c>
-      <c r="K66" t="s">
+      <c r="L66" t="s">
         <v>170</v>
-      </c>
-      <c r="L66" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
+        <v>171</v>
+      </c>
+      <c r="B67" t="s">
         <v>172</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>173</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
         <v>174</v>
       </c>
-      <c r="E67" t="s">
+      <c r="M67" t="s">
         <v>175</v>
-      </c>
-      <c r="M67" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3455,16 +3455,16 @@
         <v>48</v>
       </c>
       <c r="B68" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" t="s">
         <v>177</v>
       </c>
-      <c r="C68" t="s">
+      <c r="E68" t="s">
         <v>178</v>
       </c>
-      <c r="E68" t="s">
+      <c r="M68" t="s">
         <v>179</v>
-      </c>
-      <c r="M68" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3472,16 +3472,16 @@
         <v>48</v>
       </c>
       <c r="B69" t="s">
+        <v>180</v>
+      </c>
+      <c r="C69" t="s">
         <v>181</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E69" t="s">
         <v>182</v>
       </c>
-      <c r="E69" t="s">
+      <c r="M69" t="s">
         <v>183</v>
-      </c>
-      <c r="M69" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3489,39 +3489,39 @@
         <v>30</v>
       </c>
       <c r="B70" t="s">
+        <v>184</v>
+      </c>
+      <c r="C70" t="s">
         <v>185</v>
       </c>
-      <c r="C70" t="s">
+      <c r="E70" t="s">
         <v>186</v>
       </c>
-      <c r="E70" t="s">
+      <c r="J70" t="s">
         <v>187</v>
       </c>
-      <c r="J70" t="s">
+      <c r="K70" t="s">
         <v>188</v>
       </c>
-      <c r="K70" t="s">
+      <c r="L70" t="s">
         <v>189</v>
       </c>
-      <c r="L70" t="s">
+      <c r="M70" t="s">
         <v>190</v>
-      </c>
-      <c r="M70" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B71" t="s">
+        <v>191</v>
+      </c>
+      <c r="C71" t="s">
         <v>192</v>
       </c>
-      <c r="C71" t="s">
+      <c r="E71" t="s">
         <v>193</v>
-      </c>
-      <c r="E71" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3529,19 +3529,19 @@
         <v>78</v>
       </c>
       <c r="B72" t="s">
+        <v>194</v>
+      </c>
+      <c r="C72" t="s">
         <v>195</v>
       </c>
-      <c r="C72" t="s">
+      <c r="E72" t="s">
         <v>196</v>
-      </c>
-      <c r="E72" t="s">
-        <v>197</v>
       </c>
       <c r="H72" t="s">
         <v>22</v>
       </c>
       <c r="M72" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3549,7 +3549,7 @@
         <v>43</v>
       </c>
       <c r="B73" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3557,7 +3557,7 @@
         <v>43</v>
       </c>
       <c r="B74" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3565,10 +3565,10 @@
         <v>17</v>
       </c>
       <c r="B75" t="s">
+        <v>198</v>
+      </c>
+      <c r="G75" t="s">
         <v>199</v>
-      </c>
-      <c r="G75" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3576,10 +3576,10 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
+        <v>200</v>
+      </c>
+      <c r="G76" t="s">
         <v>201</v>
-      </c>
-      <c r="G76" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3587,10 +3587,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G77" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3598,10 +3598,10 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
+        <v>203</v>
+      </c>
+      <c r="G78" t="s">
         <v>204</v>
-      </c>
-      <c r="G78" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3609,13 +3609,13 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
+        <v>205</v>
+      </c>
+      <c r="G79" t="s">
         <v>206</v>
       </c>
-      <c r="G79" t="s">
+      <c r="M79" t="s">
         <v>207</v>
-      </c>
-      <c r="M79" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3623,13 +3623,13 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
+        <v>208</v>
+      </c>
+      <c r="G80" t="s">
         <v>209</v>
       </c>
-      <c r="G80" t="s">
-        <v>210</v>
-      </c>
       <c r="M80" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3637,10 +3637,10 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
+        <v>210</v>
+      </c>
+      <c r="G81" t="s">
         <v>211</v>
-      </c>
-      <c r="G81" t="s">
-        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3648,13 +3648,13 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
+        <v>212</v>
+      </c>
+      <c r="G82" t="s">
         <v>213</v>
       </c>
-      <c r="G82" t="s">
-        <v>214</v>
-      </c>
       <c r="M82" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3662,13 +3662,13 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
+        <v>214</v>
+      </c>
+      <c r="G83" t="s">
         <v>215</v>
       </c>
-      <c r="G83" t="s">
-        <v>216</v>
-      </c>
       <c r="M83" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3676,10 +3676,10 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
+        <v>216</v>
+      </c>
+      <c r="G84" t="s">
         <v>217</v>
-      </c>
-      <c r="G84" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3687,13 +3687,13 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
+        <v>218</v>
+      </c>
+      <c r="G85" t="s">
         <v>219</v>
       </c>
-      <c r="G85" t="s">
-        <v>220</v>
-      </c>
       <c r="M85" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3701,13 +3701,13 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
+        <v>220</v>
+      </c>
+      <c r="G86" t="s">
         <v>221</v>
       </c>
-      <c r="G86" t="s">
-        <v>222</v>
-      </c>
       <c r="M86" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3715,10 +3715,10 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
+        <v>222</v>
+      </c>
+      <c r="G87" t="s">
         <v>223</v>
-      </c>
-      <c r="G87" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3726,10 +3726,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
+        <v>224</v>
+      </c>
+      <c r="G88" t="s">
         <v>225</v>
-      </c>
-      <c r="G88" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3737,10 +3737,10 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
+        <v>226</v>
+      </c>
+      <c r="G89" t="s">
         <v>227</v>
-      </c>
-      <c r="G89" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3748,10 +3748,10 @@
         <v>17</v>
       </c>
       <c r="B90" t="s">
+        <v>228</v>
+      </c>
+      <c r="G90" t="s">
         <v>229</v>
-      </c>
-      <c r="G90" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3759,10 +3759,10 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
+        <v>230</v>
+      </c>
+      <c r="G91" t="s">
         <v>231</v>
-      </c>
-      <c r="G91" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3770,10 +3770,10 @@
         <v>17</v>
       </c>
       <c r="B92" t="s">
+        <v>232</v>
+      </c>
+      <c r="G92" t="s">
         <v>233</v>
-      </c>
-      <c r="G92" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3781,10 +3781,10 @@
         <v>17</v>
       </c>
       <c r="B93" t="s">
+        <v>234</v>
+      </c>
+      <c r="G93" t="s">
         <v>235</v>
-      </c>
-      <c r="G93" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3792,10 +3792,10 @@
         <v>17</v>
       </c>
       <c r="B94" t="s">
+        <v>236</v>
+      </c>
+      <c r="G94" t="s">
         <v>237</v>
-      </c>
-      <c r="G94" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3803,10 +3803,10 @@
         <v>17</v>
       </c>
       <c r="B95" t="s">
+        <v>238</v>
+      </c>
+      <c r="G95" t="s">
         <v>239</v>
-      </c>
-      <c r="G95" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="96" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3815,10 +3815,10 @@
         <v>25</v>
       </c>
       <c r="B97" t="s">
+        <v>240</v>
+      </c>
+      <c r="M97" t="s">
         <v>241</v>
-      </c>
-      <c r="M97" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3826,13 +3826,13 @@
         <v>48</v>
       </c>
       <c r="B98" t="s">
+        <v>242</v>
+      </c>
+      <c r="C98" t="s">
         <v>243</v>
       </c>
-      <c r="C98" t="s">
+      <c r="E98" t="s">
         <v>244</v>
-      </c>
-      <c r="E98" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3840,19 +3840,19 @@
         <v>78</v>
       </c>
       <c r="B99" t="s">
+        <v>245</v>
+      </c>
+      <c r="C99" t="s">
         <v>246</v>
       </c>
-      <c r="C99" t="s">
+      <c r="D99" t="s">
+        <v>120</v>
+      </c>
+      <c r="E99" t="s">
         <v>247</v>
       </c>
-      <c r="D99" t="s">
+      <c r="F99" t="s">
         <v>121</v>
-      </c>
-      <c r="E99" t="s">
-        <v>248</v>
-      </c>
-      <c r="F99" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3860,28 +3860,28 @@
         <v>28</v>
       </c>
       <c r="B100" t="s">
+        <v>248</v>
+      </c>
+      <c r="C100" t="s">
         <v>249</v>
       </c>
-      <c r="C100" t="s">
+      <c r="D100" t="s">
+        <v>125</v>
+      </c>
+      <c r="E100" t="s">
         <v>250</v>
       </c>
-      <c r="D100" t="s">
+      <c r="F100" t="s">
         <v>126</v>
-      </c>
-      <c r="E100" t="s">
-        <v>251</v>
-      </c>
-      <c r="F100" t="s">
-        <v>127</v>
       </c>
       <c r="I100" t="s">
         <v>29</v>
       </c>
       <c r="J100" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M100" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3889,31 +3889,31 @@
         <v>30</v>
       </c>
       <c r="B101" t="s">
+        <v>252</v>
+      </c>
+      <c r="C101" t="s">
         <v>253</v>
       </c>
-      <c r="C101" t="s">
+      <c r="D101" t="s">
+        <v>131</v>
+      </c>
+      <c r="E101" t="s">
         <v>254</v>
       </c>
-      <c r="D101" t="s">
+      <c r="F101" t="s">
         <v>132</v>
       </c>
-      <c r="E101" t="s">
+      <c r="J101" t="s">
         <v>255</v>
       </c>
-      <c r="F101" t="s">
-        <v>133</v>
-      </c>
-      <c r="J101" t="s">
+      <c r="K101" t="s">
+        <v>134</v>
+      </c>
+      <c r="L101" t="s">
+        <v>135</v>
+      </c>
+      <c r="M101" t="s">
         <v>256</v>
-      </c>
-      <c r="K101" t="s">
-        <v>135</v>
-      </c>
-      <c r="L101" t="s">
-        <v>136</v>
-      </c>
-      <c r="M101" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3921,13 +3921,13 @@
         <v>17</v>
       </c>
       <c r="B102" t="s">
+        <v>257</v>
+      </c>
+      <c r="G102" t="s">
         <v>258</v>
       </c>
-      <c r="G102" t="s">
-        <v>259</v>
-      </c>
       <c r="M102" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="103" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3935,10 +3935,10 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
+        <v>259</v>
+      </c>
+      <c r="G103" t="s">
         <v>260</v>
-      </c>
-      <c r="G103" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3946,16 +3946,16 @@
         <v>48</v>
       </c>
       <c r="B104" t="s">
+        <v>261</v>
+      </c>
+      <c r="C104" t="s">
         <v>262</v>
       </c>
-      <c r="C104" t="s">
+      <c r="E104" t="s">
         <v>263</v>
       </c>
-      <c r="E104" t="s">
+      <c r="M104" t="s">
         <v>264</v>
-      </c>
-      <c r="M104" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3963,108 +3963,108 @@
         <v>48</v>
       </c>
       <c r="B105" t="s">
+        <v>265</v>
+      </c>
+      <c r="C105" t="s">
         <v>266</v>
       </c>
-      <c r="C105" t="s">
+      <c r="E105" t="s">
         <v>267</v>
       </c>
-      <c r="E105" t="s">
+      <c r="M105" t="s">
         <v>268</v>
-      </c>
-      <c r="M105" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B106" t="s">
+        <v>269</v>
+      </c>
+      <c r="C106" t="s">
         <v>270</v>
       </c>
-      <c r="C106" t="s">
+      <c r="D106" t="s">
+        <v>153</v>
+      </c>
+      <c r="E106" t="s">
         <v>271</v>
       </c>
-      <c r="D106" t="s">
+      <c r="F106" t="s">
         <v>154</v>
       </c>
-      <c r="E106" t="s">
-        <v>272</v>
-      </c>
-      <c r="F106" t="s">
+      <c r="J106" t="s">
         <v>155</v>
       </c>
-      <c r="J106" t="s">
+      <c r="K106" t="s">
         <v>156</v>
       </c>
-      <c r="K106" t="s">
+      <c r="L106" t="s">
         <v>157</v>
-      </c>
-      <c r="L106" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B107" t="s">
+        <v>272</v>
+      </c>
+      <c r="C107" t="s">
         <v>273</v>
       </c>
-      <c r="C107" t="s">
+      <c r="E107" t="s">
         <v>274</v>
       </c>
-      <c r="E107" t="s">
+      <c r="M107" t="s">
         <v>275</v>
-      </c>
-      <c r="M107" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B108" t="s">
+        <v>276</v>
+      </c>
+      <c r="C108" t="s">
         <v>277</v>
       </c>
-      <c r="C108" t="s">
+      <c r="D108" t="s">
+        <v>166</v>
+      </c>
+      <c r="E108" t="s">
         <v>278</v>
       </c>
-      <c r="D108" t="s">
+      <c r="F108" t="s">
         <v>167</v>
       </c>
-      <c r="E108" t="s">
-        <v>279</v>
-      </c>
-      <c r="F108" t="s">
+      <c r="J108" t="s">
         <v>168</v>
       </c>
-      <c r="J108" t="s">
+      <c r="K108" t="s">
         <v>169</v>
       </c>
-      <c r="K108" t="s">
+      <c r="L108" t="s">
         <v>170</v>
-      </c>
-      <c r="L108" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B109" t="s">
+        <v>279</v>
+      </c>
+      <c r="C109" t="s">
         <v>280</v>
       </c>
-      <c r="C109" t="s">
+      <c r="E109" t="s">
         <v>281</v>
       </c>
-      <c r="E109" t="s">
+      <c r="M109" t="s">
         <v>282</v>
-      </c>
-      <c r="M109" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4072,16 +4072,16 @@
         <v>48</v>
       </c>
       <c r="B110" t="s">
+        <v>283</v>
+      </c>
+      <c r="C110" t="s">
+        <v>177</v>
+      </c>
+      <c r="E110" t="s">
+        <v>178</v>
+      </c>
+      <c r="M110" t="s">
         <v>284</v>
-      </c>
-      <c r="C110" t="s">
-        <v>178</v>
-      </c>
-      <c r="E110" t="s">
-        <v>179</v>
-      </c>
-      <c r="M110" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4089,16 +4089,16 @@
         <v>48</v>
       </c>
       <c r="B111" t="s">
+        <v>285</v>
+      </c>
+      <c r="C111" t="s">
+        <v>181</v>
+      </c>
+      <c r="E111" t="s">
+        <v>182</v>
+      </c>
+      <c r="M111" t="s">
         <v>286</v>
-      </c>
-      <c r="C111" t="s">
-        <v>182</v>
-      </c>
-      <c r="E111" t="s">
-        <v>183</v>
-      </c>
-      <c r="M111" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4106,10 +4106,10 @@
         <v>17</v>
       </c>
       <c r="B112" t="s">
+        <v>287</v>
+      </c>
+      <c r="G112" t="s">
         <v>288</v>
-      </c>
-      <c r="G112" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4117,10 +4117,10 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
+        <v>289</v>
+      </c>
+      <c r="G113" t="s">
         <v>290</v>
-      </c>
-      <c r="G113" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4128,25 +4128,25 @@
         <v>30</v>
       </c>
       <c r="B114" t="s">
+        <v>291</v>
+      </c>
+      <c r="C114" t="s">
         <v>292</v>
       </c>
-      <c r="C114" t="s">
+      <c r="E114" t="s">
         <v>293</v>
       </c>
-      <c r="E114" t="s">
+      <c r="J114" t="s">
+        <v>187</v>
+      </c>
+      <c r="K114" t="s">
+        <v>188</v>
+      </c>
+      <c r="L114" t="s">
+        <v>189</v>
+      </c>
+      <c r="M114" t="s">
         <v>294</v>
-      </c>
-      <c r="J114" t="s">
-        <v>188</v>
-      </c>
-      <c r="K114" t="s">
-        <v>189</v>
-      </c>
-      <c r="L114" t="s">
-        <v>190</v>
-      </c>
-      <c r="M114" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4154,10 +4154,10 @@
         <v>17</v>
       </c>
       <c r="B115" t="s">
+        <v>295</v>
+      </c>
+      <c r="G115" t="s">
         <v>296</v>
-      </c>
-      <c r="G115" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4165,10 +4165,10 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
+        <v>297</v>
+      </c>
+      <c r="G116" t="s">
         <v>298</v>
-      </c>
-      <c r="G116" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4176,10 +4176,10 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
+        <v>299</v>
+      </c>
+      <c r="G117" t="s">
         <v>300</v>
-      </c>
-      <c r="G117" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4187,10 +4187,10 @@
         <v>17</v>
       </c>
       <c r="B118" t="s">
+        <v>301</v>
+      </c>
+      <c r="G118" t="s">
         <v>302</v>
-      </c>
-      <c r="G118" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4198,10 +4198,10 @@
         <v>17</v>
       </c>
       <c r="B119" t="s">
+        <v>303</v>
+      </c>
+      <c r="G119" t="s">
         <v>304</v>
-      </c>
-      <c r="G119" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4209,10 +4209,10 @@
         <v>17</v>
       </c>
       <c r="B120" t="s">
+        <v>305</v>
+      </c>
+      <c r="G120" t="s">
         <v>306</v>
-      </c>
-      <c r="G120" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4220,7 +4220,7 @@
         <v>43</v>
       </c>
       <c r="B121" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4228,10 +4228,10 @@
         <v>25</v>
       </c>
       <c r="B122" t="s">
+        <v>307</v>
+      </c>
+      <c r="M122" t="s">
         <v>308</v>
-      </c>
-      <c r="M122" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4239,13 +4239,13 @@
         <v>48</v>
       </c>
       <c r="B123" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C123" t="s">
+        <v>243</v>
+      </c>
+      <c r="E123" t="s">
         <v>244</v>
-      </c>
-      <c r="E123" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4253,19 +4253,19 @@
         <v>78</v>
       </c>
       <c r="B124" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C124" t="s">
+        <v>246</v>
+      </c>
+      <c r="D124" t="s">
+        <v>120</v>
+      </c>
+      <c r="E124" t="s">
         <v>247</v>
       </c>
-      <c r="D124" t="s">
+      <c r="F124" t="s">
         <v>121</v>
-      </c>
-      <c r="E124" t="s">
-        <v>248</v>
-      </c>
-      <c r="F124" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4273,28 +4273,28 @@
         <v>28</v>
       </c>
       <c r="B125" t="s">
+        <v>311</v>
+      </c>
+      <c r="C125" t="s">
+        <v>249</v>
+      </c>
+      <c r="D125" t="s">
+        <v>125</v>
+      </c>
+      <c r="E125" t="s">
         <v>312</v>
       </c>
-      <c r="C125" t="s">
-        <v>250</v>
-      </c>
-      <c r="D125" t="s">
+      <c r="F125" t="s">
         <v>126</v>
-      </c>
-      <c r="E125" t="s">
-        <v>313</v>
-      </c>
-      <c r="F125" t="s">
-        <v>127</v>
       </c>
       <c r="I125" t="s">
         <v>29</v>
       </c>
       <c r="J125" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M125" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4302,31 +4302,31 @@
         <v>30</v>
       </c>
       <c r="B126" t="s">
+        <v>314</v>
+      </c>
+      <c r="C126" t="s">
+        <v>253</v>
+      </c>
+      <c r="D126" t="s">
+        <v>131</v>
+      </c>
+      <c r="E126" t="s">
+        <v>254</v>
+      </c>
+      <c r="F126" t="s">
+        <v>132</v>
+      </c>
+      <c r="J126" t="s">
+        <v>255</v>
+      </c>
+      <c r="K126" t="s">
+        <v>134</v>
+      </c>
+      <c r="L126" t="s">
+        <v>135</v>
+      </c>
+      <c r="M126" t="s">
         <v>315</v>
-      </c>
-      <c r="C126" t="s">
-        <v>254</v>
-      </c>
-      <c r="D126" t="s">
-        <v>132</v>
-      </c>
-      <c r="E126" t="s">
-        <v>255</v>
-      </c>
-      <c r="F126" t="s">
-        <v>133</v>
-      </c>
-      <c r="J126" t="s">
-        <v>256</v>
-      </c>
-      <c r="K126" t="s">
-        <v>135</v>
-      </c>
-      <c r="L126" t="s">
-        <v>136</v>
-      </c>
-      <c r="M126" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4334,13 +4334,13 @@
         <v>17</v>
       </c>
       <c r="B127" t="s">
+        <v>316</v>
+      </c>
+      <c r="G127" t="s">
         <v>317</v>
       </c>
-      <c r="G127" t="s">
-        <v>318</v>
-      </c>
       <c r="M127" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4348,10 +4348,10 @@
         <v>17</v>
       </c>
       <c r="B128" t="s">
+        <v>318</v>
+      </c>
+      <c r="G128" t="s">
         <v>319</v>
-      </c>
-      <c r="G128" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4359,16 +4359,16 @@
         <v>48</v>
       </c>
       <c r="B129" t="s">
+        <v>320</v>
+      </c>
+      <c r="C129" t="s">
+        <v>262</v>
+      </c>
+      <c r="E129" t="s">
+        <v>263</v>
+      </c>
+      <c r="M129" t="s">
         <v>321</v>
-      </c>
-      <c r="C129" t="s">
-        <v>263</v>
-      </c>
-      <c r="E129" t="s">
-        <v>264</v>
-      </c>
-      <c r="M129" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4376,108 +4376,108 @@
         <v>48</v>
       </c>
       <c r="B130" t="s">
+        <v>322</v>
+      </c>
+      <c r="C130" t="s">
         <v>323</v>
       </c>
-      <c r="C130" t="s">
+      <c r="E130" t="s">
         <v>324</v>
       </c>
-      <c r="E130" t="s">
+      <c r="M130" t="s">
         <v>325</v>
-      </c>
-      <c r="M130" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B131" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C131" t="s">
+        <v>270</v>
+      </c>
+      <c r="D131" t="s">
+        <v>153</v>
+      </c>
+      <c r="E131" t="s">
         <v>271</v>
       </c>
-      <c r="D131" t="s">
+      <c r="F131" t="s">
         <v>154</v>
       </c>
-      <c r="E131" t="s">
-        <v>272</v>
-      </c>
-      <c r="F131" t="s">
+      <c r="J131" t="s">
         <v>155</v>
       </c>
-      <c r="J131" t="s">
+      <c r="K131" t="s">
         <v>156</v>
       </c>
-      <c r="K131" t="s">
+      <c r="L131" t="s">
         <v>157</v>
-      </c>
-      <c r="L131" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B132" t="s">
+        <v>327</v>
+      </c>
+      <c r="C132" t="s">
+        <v>273</v>
+      </c>
+      <c r="E132" t="s">
+        <v>274</v>
+      </c>
+      <c r="M132" t="s">
         <v>328</v>
-      </c>
-      <c r="C132" t="s">
-        <v>274</v>
-      </c>
-      <c r="E132" t="s">
-        <v>275</v>
-      </c>
-      <c r="M132" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B133" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C133" t="s">
+        <v>277</v>
+      </c>
+      <c r="D133" t="s">
+        <v>166</v>
+      </c>
+      <c r="E133" t="s">
         <v>278</v>
       </c>
-      <c r="D133" t="s">
+      <c r="F133" t="s">
         <v>167</v>
       </c>
-      <c r="E133" t="s">
-        <v>279</v>
-      </c>
-      <c r="F133" t="s">
+      <c r="J133" t="s">
         <v>168</v>
       </c>
-      <c r="J133" t="s">
+      <c r="K133" t="s">
         <v>169</v>
       </c>
-      <c r="K133" t="s">
+      <c r="L133" t="s">
         <v>170</v>
-      </c>
-      <c r="L133" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B134" t="s">
+        <v>330</v>
+      </c>
+      <c r="C134" t="s">
+        <v>280</v>
+      </c>
+      <c r="E134" t="s">
+        <v>281</v>
+      </c>
+      <c r="M134" t="s">
         <v>331</v>
-      </c>
-      <c r="C134" t="s">
-        <v>281</v>
-      </c>
-      <c r="E134" t="s">
-        <v>282</v>
-      </c>
-      <c r="M134" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4485,16 +4485,16 @@
         <v>48</v>
       </c>
       <c r="B135" t="s">
+        <v>332</v>
+      </c>
+      <c r="C135" t="s">
+        <v>177</v>
+      </c>
+      <c r="E135" t="s">
+        <v>178</v>
+      </c>
+      <c r="M135" t="s">
         <v>333</v>
-      </c>
-      <c r="C135" t="s">
-        <v>178</v>
-      </c>
-      <c r="E135" t="s">
-        <v>179</v>
-      </c>
-      <c r="M135" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4502,16 +4502,16 @@
         <v>48</v>
       </c>
       <c r="B136" t="s">
+        <v>334</v>
+      </c>
+      <c r="C136" t="s">
+        <v>181</v>
+      </c>
+      <c r="E136" t="s">
+        <v>182</v>
+      </c>
+      <c r="M136" t="s">
         <v>335</v>
-      </c>
-      <c r="C136" t="s">
-        <v>182</v>
-      </c>
-      <c r="E136" t="s">
-        <v>183</v>
-      </c>
-      <c r="M136" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4519,10 +4519,10 @@
         <v>17</v>
       </c>
       <c r="B137" t="s">
+        <v>336</v>
+      </c>
+      <c r="G137" t="s">
         <v>337</v>
-      </c>
-      <c r="G137" t="s">
-        <v>338</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4530,10 +4530,10 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
+        <v>338</v>
+      </c>
+      <c r="G138" t="s">
         <v>339</v>
-      </c>
-      <c r="G138" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4541,25 +4541,25 @@
         <v>30</v>
       </c>
       <c r="B139" t="s">
+        <v>340</v>
+      </c>
+      <c r="C139" t="s">
+        <v>292</v>
+      </c>
+      <c r="E139" t="s">
+        <v>293</v>
+      </c>
+      <c r="J139" t="s">
+        <v>187</v>
+      </c>
+      <c r="K139" t="s">
+        <v>188</v>
+      </c>
+      <c r="L139" t="s">
+        <v>189</v>
+      </c>
+      <c r="M139" t="s">
         <v>341</v>
-      </c>
-      <c r="C139" t="s">
-        <v>293</v>
-      </c>
-      <c r="E139" t="s">
-        <v>294</v>
-      </c>
-      <c r="J139" t="s">
-        <v>188</v>
-      </c>
-      <c r="K139" t="s">
-        <v>189</v>
-      </c>
-      <c r="L139" t="s">
-        <v>190</v>
-      </c>
-      <c r="M139" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4567,10 +4567,10 @@
         <v>17</v>
       </c>
       <c r="B140" t="s">
+        <v>342</v>
+      </c>
+      <c r="G140" t="s">
         <v>343</v>
-      </c>
-      <c r="G140" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4578,10 +4578,10 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
+        <v>344</v>
+      </c>
+      <c r="G141" t="s">
         <v>345</v>
-      </c>
-      <c r="G141" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4589,10 +4589,10 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
+        <v>346</v>
+      </c>
+      <c r="G142" t="s">
         <v>347</v>
-      </c>
-      <c r="G142" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4600,10 +4600,10 @@
         <v>17</v>
       </c>
       <c r="B143" t="s">
+        <v>348</v>
+      </c>
+      <c r="G143" t="s">
         <v>349</v>
-      </c>
-      <c r="G143" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4611,10 +4611,10 @@
         <v>17</v>
       </c>
       <c r="B144" t="s">
+        <v>350</v>
+      </c>
+      <c r="G144" t="s">
         <v>351</v>
-      </c>
-      <c r="G144" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4622,10 +4622,10 @@
         <v>17</v>
       </c>
       <c r="B145" t="s">
+        <v>352</v>
+      </c>
+      <c r="G145" t="s">
         <v>353</v>
-      </c>
-      <c r="G145" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4633,7 +4633,7 @@
         <v>43</v>
       </c>
       <c r="B146" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4641,13 +4641,13 @@
         <v>78</v>
       </c>
       <c r="B148" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C148" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="M148" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4655,16 +4655,16 @@
         <v>78</v>
       </c>
       <c r="B149" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="C149" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="D149" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="M149" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4672,16 +4672,16 @@
         <v>78</v>
       </c>
       <c r="B150" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="C150" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="D150" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="M150" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4689,13 +4689,13 @@
         <v>78</v>
       </c>
       <c r="B151" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C151" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="M151" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4703,13 +4703,13 @@
         <v>78</v>
       </c>
       <c r="B152" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="C152" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="M152" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="153" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4717,13 +4717,13 @@
         <v>78</v>
       </c>
       <c r="B153" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="C153" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="M153" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4731,13 +4731,13 @@
         <v>17</v>
       </c>
       <c r="B155" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G155" t="s">
         <v>95</v>
       </c>
       <c r="M155" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4745,13 +4745,13 @@
         <v>17</v>
       </c>
       <c r="B156" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G156" t="s">
         <v>95</v>
       </c>
       <c r="M156" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4759,39 +4759,39 @@
         <v>48</v>
       </c>
       <c r="B157" t="s">
+        <v>358</v>
+      </c>
+      <c r="C157" t="s">
+        <v>616</v>
+      </c>
+      <c r="D157" t="s">
+        <v>360</v>
+      </c>
+      <c r="E157" t="s">
         <v>359</v>
       </c>
-      <c r="C157" t="s">
-        <v>618</v>
-      </c>
-      <c r="D157" t="s">
+      <c r="F157" t="s">
         <v>361</v>
       </c>
-      <c r="E157" t="s">
-        <v>360</v>
-      </c>
-      <c r="F157" t="s">
+      <c r="M157" t="s">
         <v>362</v>
-      </c>
-      <c r="M157" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
+        <v>363</v>
+      </c>
+      <c r="B158" t="s">
         <v>364</v>
       </c>
-      <c r="B158" t="s">
+      <c r="C158" t="s">
+        <v>618</v>
+      </c>
+      <c r="E158" t="s">
         <v>365</v>
       </c>
-      <c r="C158" t="s">
-        <v>620</v>
-      </c>
-      <c r="E158" t="s">
-        <v>366</v>
-      </c>
       <c r="M158" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4799,39 +4799,39 @@
         <v>48</v>
       </c>
       <c r="B159" t="s">
+        <v>366</v>
+      </c>
+      <c r="C159" t="s">
+        <v>617</v>
+      </c>
+      <c r="D159" t="s">
+        <v>368</v>
+      </c>
+      <c r="E159" t="s">
         <v>367</v>
       </c>
-      <c r="C159" t="s">
-        <v>619</v>
-      </c>
-      <c r="D159" t="s">
+      <c r="F159" t="s">
         <v>369</v>
       </c>
-      <c r="E159" t="s">
-        <v>368</v>
-      </c>
-      <c r="F159" t="s">
+      <c r="M159" t="s">
         <v>370</v>
-      </c>
-      <c r="M159" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
+        <v>371</v>
+      </c>
+      <c r="B160" t="s">
         <v>372</v>
       </c>
-      <c r="B160" t="s">
+      <c r="C160" t="s">
+        <v>619</v>
+      </c>
+      <c r="E160" t="s">
         <v>373</v>
       </c>
-      <c r="C160" t="s">
-        <v>621</v>
-      </c>
-      <c r="E160" t="s">
-        <v>374</v>
-      </c>
       <c r="M160" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="162" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4839,13 +4839,13 @@
         <v>17</v>
       </c>
       <c r="B162" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G162" t="s">
         <v>95</v>
       </c>
       <c r="M162" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4853,13 +4853,13 @@
         <v>17</v>
       </c>
       <c r="B163" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G163" t="s">
         <v>95</v>
       </c>
       <c r="M163" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4867,13 +4867,13 @@
         <v>17</v>
       </c>
       <c r="B164" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G164" t="s">
         <v>95</v>
       </c>
       <c r="M164" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4881,13 +4881,13 @@
         <v>17</v>
       </c>
       <c r="B165" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="G165" t="s">
         <v>95</v>
       </c>
       <c r="M165" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="166" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4895,7 +4895,7 @@
         <v>83</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="168" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4903,13 +4903,13 @@
         <v>59</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="N168" s="1" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
     </row>
     <row r="169" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4917,11 +4917,11 @@
         <v>17</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="C169" s="4"/>
       <c r="G169" t="s">
-        <v>82</v>
+        <v>627</v>
       </c>
     </row>
     <row r="170" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4929,11 +4929,11 @@
         <v>17</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="C170" s="4"/>
       <c r="G170" s="3" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="171" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4941,11 +4941,11 @@
         <v>17</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="C171" s="4"/>
       <c r="G171" s="3" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
     </row>
     <row r="172" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4953,11 +4953,11 @@
         <v>17</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C172" s="4"/>
       <c r="G172" s="3" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
     </row>
     <row r="173" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4965,16 +4965,16 @@
         <v>48</v>
       </c>
       <c r="B173" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="C173" s="5" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="E173" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="M173" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="174" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4982,10 +4982,10 @@
         <v>48</v>
       </c>
       <c r="B174" s="7" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4993,10 +4993,10 @@
         <v>78</v>
       </c>
       <c r="B175" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C175" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="E175" t="s">
         <v>79</v>
@@ -5005,7 +5005,7 @@
         <v>22</v>
       </c>
       <c r="M175" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5013,10 +5013,10 @@
         <v>78</v>
       </c>
       <c r="B176" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C176" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="E176" t="s">
         <v>79</v>
@@ -5025,67 +5025,67 @@
         <v>22</v>
       </c>
       <c r="M176" s="3" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="177" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
+        <v>486</v>
+      </c>
+      <c r="B177" t="s">
         <v>487</v>
       </c>
-      <c r="B177" t="s">
+      <c r="C177" s="6" t="s">
+        <v>608</v>
+      </c>
+      <c r="J177" t="s">
         <v>488</v>
       </c>
-      <c r="C177" s="6" t="s">
-        <v>610</v>
-      </c>
-      <c r="J177" t="s">
+      <c r="K177" t="s">
         <v>489</v>
       </c>
-      <c r="K177" t="s">
-        <v>490</v>
-      </c>
       <c r="M177" s="3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="178" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B178" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="J178" t="s">
+        <v>492</v>
+      </c>
+      <c r="K178" t="s">
         <v>493</v>
       </c>
-      <c r="K178" t="s">
-        <v>494</v>
-      </c>
       <c r="M178" s="3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="179" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B179" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="J179" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="K179" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="M179" s="3" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
     </row>
     <row r="181" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5093,7 +5093,7 @@
         <v>83</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5101,65 +5101,65 @@
         <v>97</v>
       </c>
       <c r="B183" t="s">
+        <v>381</v>
+      </c>
+      <c r="C183" t="s">
         <v>382</v>
       </c>
-      <c r="C183" t="s">
+      <c r="D183" t="s">
+        <v>384</v>
+      </c>
+      <c r="E183" t="s">
         <v>383</v>
       </c>
-      <c r="D183" t="s">
+      <c r="F183" t="s">
         <v>385</v>
-      </c>
-      <c r="E183" t="s">
-        <v>384</v>
-      </c>
-      <c r="F183" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
+        <v>386</v>
+      </c>
+      <c r="B184" t="s">
         <v>387</v>
       </c>
-      <c r="B184" t="s">
+      <c r="C184" t="s">
         <v>388</v>
       </c>
-      <c r="C184" t="s">
+      <c r="D184" t="s">
+        <v>390</v>
+      </c>
+      <c r="E184" t="s">
         <v>389</v>
       </c>
-      <c r="D184" t="s">
+      <c r="F184" t="s">
         <v>391</v>
-      </c>
-      <c r="E184" t="s">
-        <v>390</v>
-      </c>
-      <c r="F184" t="s">
-        <v>392</v>
       </c>
       <c r="H184" t="s">
         <v>22</v>
       </c>
       <c r="M184" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
+        <v>393</v>
+      </c>
+      <c r="B185" t="s">
         <v>394</v>
       </c>
-      <c r="B185" t="s">
-        <v>395</v>
-      </c>
       <c r="C185" t="s">
+        <v>388</v>
+      </c>
+      <c r="D185" t="s">
+        <v>390</v>
+      </c>
+      <c r="E185" t="s">
         <v>389</v>
       </c>
-      <c r="D185" t="s">
+      <c r="F185" t="s">
         <v>391</v>
-      </c>
-      <c r="E185" t="s">
-        <v>390</v>
-      </c>
-      <c r="F185" t="s">
-        <v>392</v>
       </c>
       <c r="M185" t="s">
         <v>52</v>
@@ -5167,22 +5167,22 @@
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
+        <v>395</v>
+      </c>
+      <c r="B186" t="s">
         <v>396</v>
       </c>
-      <c r="B186" t="s">
-        <v>397</v>
-      </c>
       <c r="C186" t="s">
+        <v>388</v>
+      </c>
+      <c r="E186" t="s">
         <v>389</v>
-      </c>
-      <c r="E186" t="s">
-        <v>390</v>
       </c>
       <c r="H186" t="s">
         <v>22</v>
       </c>
       <c r="M186" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5190,16 +5190,16 @@
         <v>48</v>
       </c>
       <c r="B187" t="s">
+        <v>398</v>
+      </c>
+      <c r="C187" t="s">
         <v>399</v>
       </c>
-      <c r="C187" t="s">
+      <c r="E187" t="s">
         <v>400</v>
       </c>
-      <c r="E187" t="s">
+      <c r="M187" t="s">
         <v>401</v>
-      </c>
-      <c r="M187" t="s">
-        <v>402</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5207,13 +5207,13 @@
         <v>20</v>
       </c>
       <c r="B188" t="s">
+        <v>402</v>
+      </c>
+      <c r="C188" t="s">
         <v>403</v>
       </c>
-      <c r="C188" t="s">
+      <c r="E188" t="s">
         <v>404</v>
-      </c>
-      <c r="E188" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5229,10 +5229,10 @@
         <v>17</v>
       </c>
       <c r="B191" t="s">
+        <v>405</v>
+      </c>
+      <c r="G191" t="s">
         <v>406</v>
-      </c>
-      <c r="G191" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5240,10 +5240,10 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
+        <v>407</v>
+      </c>
+      <c r="G192" t="s">
         <v>408</v>
-      </c>
-      <c r="G192" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5251,10 +5251,10 @@
         <v>17</v>
       </c>
       <c r="B193" t="s">
+        <v>409</v>
+      </c>
+      <c r="G193" t="s">
         <v>410</v>
-      </c>
-      <c r="G193" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5262,10 +5262,10 @@
         <v>17</v>
       </c>
       <c r="B194" t="s">
+        <v>411</v>
+      </c>
+      <c r="G194" t="s">
         <v>412</v>
-      </c>
-      <c r="G194" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5273,10 +5273,10 @@
         <v>17</v>
       </c>
       <c r="B195" t="s">
+        <v>413</v>
+      </c>
+      <c r="G195" t="s">
         <v>414</v>
-      </c>
-      <c r="G195" t="s">
-        <v>415</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5284,10 +5284,10 @@
         <v>17</v>
       </c>
       <c r="B196" t="s">
+        <v>415</v>
+      </c>
+      <c r="G196" t="s">
         <v>416</v>
-      </c>
-      <c r="G196" t="s">
-        <v>417</v>
       </c>
     </row>
   </sheetData>
@@ -5311,7 +5311,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -5331,10 +5331,10 @@
         <v>95</v>
       </c>
       <c r="C2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D2" t="s">
         <v>419</v>
-      </c>
-      <c r="D2" t="s">
-        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5342,24 +5342,24 @@
         <v>96</v>
       </c>
       <c r="B3" t="s">
+        <v>420</v>
+      </c>
+      <c r="C3" t="s">
         <v>421</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>422</v>
-      </c>
-      <c r="D3" t="s">
-        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C4" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5370,10 +5370,10 @@
         <v>95</v>
       </c>
       <c r="C5" t="s">
+        <v>424</v>
+      </c>
+      <c r="D5" t="s">
         <v>425</v>
-      </c>
-      <c r="D5" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5381,13 +5381,13 @@
         <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C6" t="s">
+        <v>426</v>
+      </c>
+      <c r="D6" t="s">
         <v>427</v>
-      </c>
-      <c r="D6" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5395,471 +5395,471 @@
         <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C7" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D7" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B8" t="s">
         <v>95</v>
       </c>
       <c r="C8" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
+        <v>532</v>
+      </c>
+      <c r="B9" t="s">
+        <v>420</v>
+      </c>
+      <c r="C9" t="s">
         <v>534</v>
-      </c>
-      <c r="B9" t="s">
-        <v>421</v>
-      </c>
-      <c r="C9" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B10" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C10" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B11" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C11" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B12" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C12" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B13" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C13" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="C14" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B15" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C15" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B16" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="C16" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B17" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C17" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B18" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="C18" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B19" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C19" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B20" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="C20" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B21" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C21" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B22" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C22" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B23" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C23" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B24" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C24" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B25" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C25" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B26" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C26" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B27" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C27" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B28" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="C28" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B29" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C29" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B30" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C30" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B31" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C31" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B32" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="C32" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B33" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C33" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B34" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C34" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B35" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C35" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B36" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C36" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B37" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C37" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B38" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C38" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B39" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="C39" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B40" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C40" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="B41" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C41" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
+        <v>431</v>
+      </c>
+      <c r="B42" t="s">
         <v>432</v>
       </c>
-      <c r="B42" t="s">
-        <v>433</v>
-      </c>
       <c r="C42" t="s">
+        <v>424</v>
+      </c>
+      <c r="D42" t="s">
         <v>425</v>
-      </c>
-      <c r="D42" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B43" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C43" t="s">
+        <v>426</v>
+      </c>
+      <c r="D43" t="s">
         <v>427</v>
-      </c>
-      <c r="D43" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
+        <v>434</v>
+      </c>
+      <c r="B44" t="s">
         <v>435</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>436</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>437</v>
-      </c>
-      <c r="D44" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B45" t="s">
+        <v>438</v>
+      </c>
+      <c r="C45" t="s">
         <v>439</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>440</v>
-      </c>
-      <c r="D45" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
+        <v>441</v>
+      </c>
+      <c r="B46" t="s">
         <v>442</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>443</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>444</v>
-      </c>
-      <c r="D46" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B47" t="s">
+        <v>445</v>
+      </c>
+      <c r="C47" t="s">
         <v>446</v>
       </c>
-      <c r="C47" t="s">
+      <c r="D47" t="s">
         <v>447</v>
-      </c>
-      <c r="D47" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5870,10 +5870,10 @@
         <v>95</v>
       </c>
       <c r="C48" t="s">
+        <v>448</v>
+      </c>
+      <c r="D48" t="s">
         <v>449</v>
-      </c>
-      <c r="D48" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5881,13 +5881,13 @@
         <v>97</v>
       </c>
       <c r="B49" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C49" t="s">
+        <v>450</v>
+      </c>
+      <c r="D49" t="s">
         <v>451</v>
-      </c>
-      <c r="D49" t="s">
-        <v>452</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5895,13 +5895,13 @@
         <v>97</v>
       </c>
       <c r="B50" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C50" t="s">
+        <v>452</v>
+      </c>
+      <c r="D50" t="s">
         <v>453</v>
-      </c>
-      <c r="D50" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -5909,195 +5909,195 @@
         <v>97</v>
       </c>
       <c r="B51" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C51" t="s">
+        <v>429</v>
+      </c>
+      <c r="D51" t="s">
         <v>430</v>
-      </c>
-      <c r="D51" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B52" t="s">
         <v>95</v>
       </c>
       <c r="C52" t="s">
+        <v>424</v>
+      </c>
+      <c r="D52" t="s">
         <v>425</v>
-      </c>
-      <c r="D52" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
+        <v>455</v>
+      </c>
+      <c r="B53" t="s">
+        <v>420</v>
+      </c>
+      <c r="C53" t="s">
+        <v>611</v>
+      </c>
+      <c r="D53" t="s">
         <v>456</v>
-      </c>
-      <c r="B53" t="s">
-        <v>421</v>
-      </c>
-      <c r="C53" t="s">
-        <v>613</v>
-      </c>
-      <c r="D53" t="s">
-        <v>457</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B54" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C54" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="D54" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B55" t="s">
         <v>95</v>
       </c>
       <c r="C55" t="s">
+        <v>424</v>
+      </c>
+      <c r="D55" t="s">
         <v>425</v>
-      </c>
-      <c r="D55" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
+        <v>458</v>
+      </c>
+      <c r="B56" t="s">
+        <v>420</v>
+      </c>
+      <c r="C56" t="s">
+        <v>614</v>
+      </c>
+      <c r="D56" t="s">
         <v>459</v>
-      </c>
-      <c r="B56" t="s">
-        <v>421</v>
-      </c>
-      <c r="C56" t="s">
-        <v>616</v>
-      </c>
-      <c r="D56" t="s">
-        <v>460</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B57" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C57" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D57" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B58" t="s">
         <v>95</v>
       </c>
       <c r="C58" t="s">
+        <v>462</v>
+      </c>
+      <c r="D58" t="s">
         <v>463</v>
-      </c>
-      <c r="D58" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B59" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C59" t="s">
+        <v>464</v>
+      </c>
+      <c r="D59" t="s">
         <v>465</v>
-      </c>
-      <c r="D59" t="s">
-        <v>466</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
+        <v>466</v>
+      </c>
+      <c r="B60" t="s">
+        <v>454</v>
+      </c>
+      <c r="C60" t="s">
         <v>467</v>
       </c>
-      <c r="B60" t="s">
-        <v>455</v>
-      </c>
-      <c r="C60" t="s">
-        <v>468</v>
-      </c>
       <c r="D60" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B61" t="s">
+        <v>468</v>
+      </c>
+      <c r="C61" t="s">
         <v>469</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>470</v>
-      </c>
-      <c r="D61" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
+        <v>471</v>
+      </c>
+      <c r="B62" t="s">
+        <v>428</v>
+      </c>
+      <c r="C62" t="s">
         <v>472</v>
       </c>
-      <c r="B62" t="s">
-        <v>429</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>473</v>
-      </c>
-      <c r="D62" t="s">
-        <v>474</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B63" t="s">
         <v>95</v>
       </c>
       <c r="C63" t="s">
+        <v>424</v>
+      </c>
+      <c r="D63" t="s">
         <v>425</v>
-      </c>
-      <c r="D63" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
+        <v>474</v>
+      </c>
+      <c r="B64" t="s">
         <v>475</v>
       </c>
-      <c r="B64" t="s">
-        <v>476</v>
-      </c>
       <c r="C64" t="s">
+        <v>426</v>
+      </c>
+      <c r="D64" t="s">
         <v>427</v>
-      </c>
-      <c r="D64" t="s">
-        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -6117,30 +6117,30 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B1" t="s">
         <v>477</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>478</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>479</v>
-      </c>
-      <c r="D1" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="B2" t="s">
+        <v>480</v>
+      </c>
+      <c r="C2" t="s">
+        <v>602</v>
+      </c>
+      <c r="D2" t="s">
         <v>481</v>
-      </c>
-      <c r="C2" t="s">
-        <v>604</v>
-      </c>
-      <c r="D2" t="s">
-        <v>482</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
correction for anthro for U5 children only
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3C7EEF80-2F8D-4F8D-A455-9888AE0535A0}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F5D6E8BA-4AD6-4664-A183-4F4A45F075AD}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="637">
   <si>
     <t>type</t>
   </si>
@@ -2078,9 +2078,6 @@
     <t>if(${age_years} &gt;14 and ${age_years} &lt;50 and ${sex}= 'f',1,0)</t>
   </si>
   <si>
-    <t>${child_name} - is ${MONTHS} months old.</t>
-  </si>
-  <si>
     <t>sum(${is_child})</t>
   </si>
   <si>
@@ -2093,16 +2090,31 @@
     <t>${dob_known} =1</t>
   </si>
   <si>
-    <t>Select_pos-${wom_selected_position} HH_pos- ${wom_hh_position} Name-${wom_name} Sex-${sex} Age-${wom_age_years} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select_pos-${child_selected_position} HH_pos- ${child_hh_position} Name-${child_name} Sex-${CHSEX} Age-${child_age_years} </t>
-  </si>
-  <si>
     <t>join(' ',${hh_roster}[is_child = 1]/hh_position)</t>
   </si>
   <si>
     <t>join(' ',${hh_roster}[is_woman = 1]/hh_position)</t>
+  </si>
+  <si>
+    <t>${child_name}- is ${MONTHS} months old.</t>
+  </si>
+  <si>
+    <t>show child_info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select-pos-${child_selected_position} HH-pos- ${child_hh_position} Name-${child_name} </t>
+  </si>
+  <si>
+    <t>Select-pos-${wom_selected_position} HH-pos- ${wom_hh_position} Name-${wom_name} Sex-${sex} Age-${wom_age_years} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
+  </si>
+  <si>
+    <t>child_u5</t>
+  </si>
+  <si>
+    <t>(${MONTHS} &lt;60 ) or ( ${MONTHS} =98 )</t>
+  </si>
+  <si>
+    <t>${child_u5}=1</t>
   </si>
 </sst>
 </file>
@@ -2519,9 +2531,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N196"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3047,7 +3059,7 @@
         <v>98</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3058,7 +3070,7 @@
         <v>99</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3069,7 +3081,7 @@
         <v>499</v>
       </c>
       <c r="G41" s="7" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3080,7 +3092,7 @@
         <v>500</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3120,7 +3132,7 @@
         <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3189,10 +3201,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>497</v>
+        <v>631</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>630</v>
+        <v>632</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3256,7 +3268,7 @@
         <v>127</v>
       </c>
       <c r="M56" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3341,13 +3353,27 @@
         <v>145</v>
       </c>
       <c r="C61" t="s">
-        <v>624</v>
+        <v>630</v>
       </c>
       <c r="E61" t="s">
         <v>146</v>
       </c>
       <c r="M61" t="s">
         <v>147</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" t="s">
+        <v>634</v>
+      </c>
+      <c r="G62">
+        <v>1</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3357,6 +3383,9 @@
       <c r="B63" t="s">
         <v>148</v>
       </c>
+      <c r="M63" s="8" t="s">
+        <v>636</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
@@ -3632,7 +3661,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>17</v>
       </c>
@@ -3643,7 +3672,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" t="s">
         <v>17</v>
       </c>
@@ -3657,7 +3686,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>17</v>
       </c>
@@ -3671,7 +3700,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" t="s">
         <v>17</v>
       </c>
@@ -3682,7 +3711,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" t="s">
         <v>17</v>
       </c>
@@ -3696,7 +3725,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" t="s">
         <v>17</v>
       </c>
@@ -3710,7 +3739,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" t="s">
         <v>17</v>
       </c>
@@ -3721,7 +3750,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" t="s">
         <v>17</v>
       </c>
@@ -3732,7 +3761,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" t="s">
         <v>17</v>
       </c>
@@ -3742,8 +3771,12 @@
       <c r="G89" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M89" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="N89" s="7"/>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>17</v>
       </c>
@@ -3753,8 +3786,12 @@
       <c r="G90" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M90" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="N90" s="7"/>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" t="s">
         <v>17</v>
       </c>
@@ -3764,8 +3801,10 @@
       <c r="G91" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M91" s="7"/>
+      <c r="N91" s="7"/>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" t="s">
         <v>17</v>
       </c>
@@ -3775,8 +3814,10 @@
       <c r="G92" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M92" s="7"/>
+      <c r="N92" s="7"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" t="s">
         <v>17</v>
       </c>
@@ -3786,8 +3827,12 @@
       <c r="G93" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M93" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="N93" s="7"/>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" t="s">
         <v>17</v>
       </c>
@@ -3797,8 +3842,12 @@
       <c r="G94" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="M94" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="N94" s="7"/>
+    </row>
+    <row r="95" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" t="s">
         <v>17</v>
       </c>
@@ -3808,8 +3857,12 @@
       <c r="G95" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="96" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
+      <c r="M95" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="N95" s="7"/>
+    </row>
+    <row r="96" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" t="s">
         <v>25</v>
@@ -4921,7 +4974,7 @@
       </c>
       <c r="C169" s="4"/>
       <c r="G169" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4985,7 +5038,7 @@
         <v>497</v>
       </c>
       <c r="C174" s="7" t="s">
-        <v>629</v>
+        <v>633</v>
       </c>
     </row>
     <row r="175" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -6150,11 +6203,7 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6209,17 +6258,75 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6662,73 +6769,19 @@
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6742,17 +6795,23 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6781,15 +6840,9 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
age ranges for VitA and measles questions
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F5D6E8BA-4AD6-4664-A183-4F4A45F075AD}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{19706F7B-2325-4CFF-BBD8-A2DD014C83A9}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1034" uniqueCount="637">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="642">
   <si>
     <t>type</t>
   </si>
@@ -2006,9 +2006,6 @@
     <t xml:space="preserve">${MONTHS}&lt;24  or (${MONTHS}=98 and ${HEIGHT}&lt;=87) </t>
   </si>
   <si>
-    <t xml:space="preserve">${MONTHS}&gt;5 or (${MONTHS}=98 and ${HEIGHT}&gt;67) </t>
-  </si>
-  <si>
     <t>ACO_SMART_Survey_2021</t>
   </si>
   <si>
@@ -2102,26 +2099,67 @@
     <t>show child_info</t>
   </si>
   <si>
-    <t xml:space="preserve">Select-pos-${child_selected_position} HH-pos- ${child_hh_position} Name-${child_name} </t>
-  </si>
-  <si>
     <t>Select-pos-${wom_selected_position} HH-pos- ${wom_hh_position} Name-${wom_name} Sex-${sex} Age-${wom_age_years} Pregnant- ${curr_pregnant} Breastfeed- ${curr_breastfeed}</t>
   </si>
   <si>
     <t>child_u5</t>
   </si>
   <si>
-    <t>(${MONTHS} &lt;60 ) or ( ${MONTHS} =98 )</t>
-  </si>
-  <si>
     <t>${child_u5}=1</t>
+  </si>
+  <si>
+    <t>REMEASURE:: ${child_name}'s date of birth:</t>
+  </si>
+  <si>
+    <t>${child_u5}='1'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">note </t>
+  </si>
+  <si>
+    <t>show child_U5</t>
+  </si>
+  <si>
+    <t>Select-pos-${child_selected_position} HH-pos- ${child_hh_position} Name-${child_name}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Child is U5- ${child_u5}</t>
+  </si>
+  <si>
+    <t>if (${MONTHS} &lt;60 or ${MONTHS} =98, '1','0')</t>
+  </si>
+  <si>
+    <r>
+      <t>(${MONTHS}&gt;5 and ${MONTHS} &lt;60</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or (${MONTHS}=98 and ${HEIGHT}&gt;67) </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2131,6 +2169,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2529,11 +2575,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N196"/>
+  <dimension ref="A1:N197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M60" sqref="M60"/>
+      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R155" sqref="R155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2873,7 +2919,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
@@ -2890,12 +2936,12 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="G24" s="8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2963,7 +3009,7 @@
         <v>80</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2974,7 +3020,7 @@
         <v>498</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3058,8 +3104,8 @@
       <c r="B39" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G39" s="7" t="s">
-        <v>628</v>
+      <c r="G39" s="2" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3070,7 +3116,7 @@
         <v>99</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3080,8 +3126,8 @@
       <c r="B41" s="1" t="s">
         <v>499</v>
       </c>
-      <c r="G41" s="7" t="s">
-        <v>629</v>
+      <c r="G41" s="1" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3092,7 +3138,7 @@
         <v>500</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3100,10 +3146,10 @@
         <v>48</v>
       </c>
       <c r="B43" s="7" t="s">
+        <v>619</v>
+      </c>
+      <c r="C43" s="7" t="s">
         <v>620</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3132,7 +3178,7 @@
         <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3187,7 +3233,7 @@
         <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E51" t="s">
         <v>114</v>
@@ -3201,10 +3247,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3268,7 +3314,7 @@
         <v>127</v>
       </c>
       <c r="M56" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3353,7 +3399,7 @@
         <v>145</v>
       </c>
       <c r="C61" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E61" t="s">
         <v>146</v>
@@ -3367,133 +3413,124 @@
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>634</v>
-      </c>
-      <c r="G62">
-        <v>1</v>
-      </c>
-      <c r="M62" s="3" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A63" t="s">
-        <v>25</v>
-      </c>
-      <c r="B63" t="s">
-        <v>148</v>
-      </c>
-      <c r="M63" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" s="7" t="s">
         <v>636</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="C63" s="7" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>149</v>
+        <v>25</v>
       </c>
       <c r="B64" t="s">
-        <v>150</v>
-      </c>
-      <c r="C64" t="s">
-        <v>151</v>
-      </c>
-      <c r="D64" t="s">
-        <v>153</v>
-      </c>
-      <c r="E64" t="s">
-        <v>152</v>
-      </c>
-      <c r="F64" t="s">
-        <v>154</v>
-      </c>
-      <c r="J64" t="s">
-        <v>155</v>
-      </c>
-      <c r="K64" t="s">
-        <v>156</v>
-      </c>
-      <c r="L64" t="s">
-        <v>157</v>
+        <v>148</v>
+      </c>
+      <c r="M64" s="8" t="s">
+        <v>635</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C65" t="s">
-        <v>160</v>
+        <v>151</v>
+      </c>
+      <c r="D65" t="s">
+        <v>153</v>
       </c>
       <c r="E65" t="s">
-        <v>161</v>
-      </c>
-      <c r="M65" t="s">
-        <v>162</v>
+        <v>152</v>
+      </c>
+      <c r="F65" t="s">
+        <v>154</v>
+      </c>
+      <c r="J65" t="s">
+        <v>155</v>
+      </c>
+      <c r="K65" t="s">
+        <v>156</v>
+      </c>
+      <c r="L65" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B66" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C66" t="s">
-        <v>164</v>
-      </c>
-      <c r="D66" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="E66" t="s">
-        <v>165</v>
-      </c>
-      <c r="F66" t="s">
-        <v>167</v>
-      </c>
-      <c r="J66" t="s">
-        <v>168</v>
-      </c>
-      <c r="K66" t="s">
-        <v>169</v>
-      </c>
-      <c r="L66" t="s">
-        <v>170</v>
+        <v>161</v>
+      </c>
+      <c r="M66" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="B67" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C67" t="s">
-        <v>173</v>
+        <v>164</v>
+      </c>
+      <c r="D67" t="s">
+        <v>166</v>
       </c>
       <c r="E67" t="s">
-        <v>174</v>
-      </c>
-      <c r="M67" t="s">
-        <v>175</v>
+        <v>165</v>
+      </c>
+      <c r="F67" t="s">
+        <v>167</v>
+      </c>
+      <c r="J67" t="s">
+        <v>168</v>
+      </c>
+      <c r="K67" t="s">
+        <v>169</v>
+      </c>
+      <c r="L67" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="B68" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C68" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E68" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="M68" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3501,84 +3538,93 @@
         <v>48</v>
       </c>
       <c r="B69" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E69" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M69" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="B70" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C70" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="E70" t="s">
-        <v>186</v>
-      </c>
-      <c r="J70" t="s">
-        <v>187</v>
-      </c>
-      <c r="K70" t="s">
-        <v>188</v>
-      </c>
-      <c r="L70" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="M70" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>158</v>
+        <v>30</v>
       </c>
       <c r="B71" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="C71" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="E71" t="s">
-        <v>193</v>
+        <v>186</v>
+      </c>
+      <c r="J71" t="s">
+        <v>187</v>
+      </c>
+      <c r="K71" t="s">
+        <v>188</v>
+      </c>
+      <c r="L71" t="s">
+        <v>189</v>
+      </c>
+      <c r="M71" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>78</v>
+        <v>158</v>
       </c>
       <c r="B72" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C72" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="E72" t="s">
-        <v>196</v>
-      </c>
-      <c r="H72" t="s">
-        <v>22</v>
-      </c>
-      <c r="M72" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>148</v>
+        <v>194</v>
+      </c>
+      <c r="C73" t="s">
+        <v>195</v>
+      </c>
+      <c r="E73" t="s">
+        <v>196</v>
+      </c>
+      <c r="H73" t="s">
+        <v>22</v>
+      </c>
+      <c r="M73" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3586,18 +3632,15 @@
         <v>43</v>
       </c>
       <c r="B74" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B75" t="s">
-        <v>198</v>
-      </c>
-      <c r="G75" t="s">
-        <v>199</v>
+        <v>116</v>
       </c>
     </row>
     <row r="76" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3605,10 +3648,10 @@
         <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G76" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3616,10 +3659,10 @@
         <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G77" t="s">
-        <v>482</v>
+        <v>201</v>
       </c>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3627,10 +3670,10 @@
         <v>17</v>
       </c>
       <c r="B78" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G78" t="s">
-        <v>204</v>
+        <v>482</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3638,13 +3681,10 @@
         <v>17</v>
       </c>
       <c r="B79" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G79" t="s">
-        <v>206</v>
-      </c>
-      <c r="M79" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3652,10 +3692,10 @@
         <v>17</v>
       </c>
       <c r="B80" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G80" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="M80" t="s">
         <v>207</v>
@@ -3666,10 +3706,13 @@
         <v>17</v>
       </c>
       <c r="B81" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="G81" t="s">
-        <v>211</v>
+        <v>209</v>
+      </c>
+      <c r="M81" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3677,13 +3720,10 @@
         <v>17</v>
       </c>
       <c r="B82" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="G82" t="s">
-        <v>213</v>
-      </c>
-      <c r="M82" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3691,10 +3731,10 @@
         <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G83" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="M83" t="s">
         <v>207</v>
@@ -3705,10 +3745,13 @@
         <v>17</v>
       </c>
       <c r="B84" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="G84" t="s">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="M84" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3716,13 +3759,10 @@
         <v>17</v>
       </c>
       <c r="B85" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G85" t="s">
-        <v>219</v>
-      </c>
-      <c r="M85" t="s">
-        <v>207</v>
+        <v>217</v>
       </c>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3730,10 +3770,10 @@
         <v>17</v>
       </c>
       <c r="B86" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G86" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M86" t="s">
         <v>207</v>
@@ -3744,10 +3784,13 @@
         <v>17</v>
       </c>
       <c r="B87" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="G87" t="s">
-        <v>223</v>
+        <v>221</v>
+      </c>
+      <c r="M87" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3755,10 +3798,10 @@
         <v>17</v>
       </c>
       <c r="B88" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="G88" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3766,28 +3809,24 @@
         <v>17</v>
       </c>
       <c r="B89" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G89" t="s">
-        <v>227</v>
-      </c>
-      <c r="M89" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="N89" s="7"/>
+        <v>225</v>
+      </c>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" t="s">
         <v>17</v>
       </c>
       <c r="B90" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G90" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M90" s="7" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="N90" s="7"/>
     </row>
@@ -3796,12 +3835,14 @@
         <v>17</v>
       </c>
       <c r="B91" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="G91" t="s">
-        <v>231</v>
-      </c>
-      <c r="M91" s="7"/>
+        <v>229</v>
+      </c>
+      <c r="M91" s="7" t="s">
+        <v>633</v>
+      </c>
       <c r="N91" s="7"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3809,10 +3850,10 @@
         <v>17</v>
       </c>
       <c r="B92" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G92" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M92" s="7"/>
       <c r="N92" s="7"/>
@@ -3822,14 +3863,12 @@
         <v>17</v>
       </c>
       <c r="B93" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="G93" t="s">
-        <v>235</v>
-      </c>
-      <c r="M93" s="7" t="s">
-        <v>636</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="M93" s="7"/>
       <c r="N93" s="7"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3837,13 +3876,13 @@
         <v>17</v>
       </c>
       <c r="B94" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="G94" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="M94" s="7" t="s">
-        <v>636</v>
+        <v>633</v>
       </c>
       <c r="N94" s="7"/>
     </row>
@@ -3852,132 +3891,133 @@
         <v>17</v>
       </c>
       <c r="B95" t="s">
+        <v>236</v>
+      </c>
+      <c r="G95" t="s">
+        <v>237</v>
+      </c>
+      <c r="M95" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="N95" s="7"/>
+    </row>
+    <row r="96" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" t="s">
+        <v>17</v>
+      </c>
+      <c r="B96" t="s">
         <v>238</v>
       </c>
-      <c r="G95" t="s">
+      <c r="G96" t="s">
         <v>239</v>
       </c>
-      <c r="M95" s="7" t="s">
-        <v>636</v>
-      </c>
-      <c r="N95" s="7"/>
-    </row>
-    <row r="96" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A97" t="s">
-        <v>25</v>
-      </c>
-      <c r="B97" t="s">
-        <v>240</v>
-      </c>
-      <c r="M97" t="s">
-        <v>241</v>
-      </c>
-    </row>
+      <c r="M96" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="N96" s="7"/>
+    </row>
+    <row r="97" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
     <row r="98" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>242</v>
-      </c>
-      <c r="C98" t="s">
-        <v>243</v>
-      </c>
-      <c r="E98" t="s">
-        <v>244</v>
+        <v>240</v>
+      </c>
+      <c r="M98" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B99" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C99" t="s">
-        <v>246</v>
-      </c>
-      <c r="D99" t="s">
-        <v>120</v>
+        <v>243</v>
       </c>
       <c r="E99" t="s">
-        <v>247</v>
-      </c>
-      <c r="F99" t="s">
-        <v>121</v>
+        <v>244</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B100" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C100" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D100" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E100" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F100" t="s">
-        <v>126</v>
-      </c>
-      <c r="I100" t="s">
-        <v>29</v>
-      </c>
-      <c r="J100" t="s">
-        <v>127</v>
-      </c>
-      <c r="M100" t="s">
-        <v>251</v>
+        <v>121</v>
       </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B101" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C101" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D101" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E101" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F101" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="I101" t="s">
+        <v>29</v>
       </c>
       <c r="J101" t="s">
-        <v>255</v>
-      </c>
-      <c r="K101" t="s">
-        <v>134</v>
-      </c>
-      <c r="L101" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="M101" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B102" t="s">
-        <v>257</v>
-      </c>
-      <c r="G102" t="s">
-        <v>258</v>
+        <v>252</v>
+      </c>
+      <c r="C102" t="s">
+        <v>253</v>
+      </c>
+      <c r="D102" t="s">
+        <v>131</v>
+      </c>
+      <c r="E102" t="s">
+        <v>254</v>
+      </c>
+      <c r="F102" t="s">
+        <v>132</v>
+      </c>
+      <c r="J102" t="s">
+        <v>255</v>
+      </c>
+      <c r="K102" t="s">
+        <v>134</v>
+      </c>
+      <c r="L102" t="s">
+        <v>135</v>
       </c>
       <c r="M102" t="s">
         <v>256</v>
@@ -3988,27 +4028,24 @@
         <v>17</v>
       </c>
       <c r="B103" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="G103" t="s">
-        <v>260</v>
+        <v>258</v>
+      </c>
+      <c r="M103" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B104" t="s">
-        <v>261</v>
-      </c>
-      <c r="C104" t="s">
-        <v>262</v>
-      </c>
-      <c r="E104" t="s">
-        <v>263</v>
-      </c>
-      <c r="M104" t="s">
-        <v>264</v>
+        <v>259</v>
+      </c>
+      <c r="G104" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4016,125 +4053,125 @@
         <v>48</v>
       </c>
       <c r="B105" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C105" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="E105" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="M105" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>48</v>
       </c>
       <c r="B106" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C106" t="s">
-        <v>270</v>
-      </c>
-      <c r="D106" t="s">
-        <v>153</v>
+        <v>266</v>
       </c>
       <c r="E106" t="s">
-        <v>271</v>
-      </c>
-      <c r="F106" t="s">
-        <v>154</v>
-      </c>
-      <c r="J106" t="s">
-        <v>155</v>
-      </c>
-      <c r="K106" t="s">
-        <v>156</v>
-      </c>
-      <c r="L106" t="s">
-        <v>157</v>
+        <v>267</v>
+      </c>
+      <c r="M106" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="107" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B107" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C107" t="s">
-        <v>273</v>
+        <v>270</v>
+      </c>
+      <c r="D107" t="s">
+        <v>153</v>
       </c>
       <c r="E107" t="s">
-        <v>274</v>
-      </c>
-      <c r="M107" t="s">
-        <v>275</v>
+        <v>271</v>
+      </c>
+      <c r="F107" t="s">
+        <v>154</v>
+      </c>
+      <c r="J107" t="s">
+        <v>155</v>
+      </c>
+      <c r="K107" t="s">
+        <v>156</v>
+      </c>
+      <c r="L107" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="108" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B108" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C108" t="s">
-        <v>277</v>
-      </c>
-      <c r="D108" t="s">
-        <v>166</v>
+        <v>273</v>
       </c>
       <c r="E108" t="s">
-        <v>278</v>
-      </c>
-      <c r="F108" t="s">
-        <v>167</v>
-      </c>
-      <c r="J108" t="s">
-        <v>168</v>
-      </c>
-      <c r="K108" t="s">
-        <v>169</v>
-      </c>
-      <c r="L108" t="s">
-        <v>170</v>
+        <v>274</v>
+      </c>
+      <c r="M108" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="109" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="B109" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C109" t="s">
-        <v>280</v>
+        <v>277</v>
+      </c>
+      <c r="D109" t="s">
+        <v>166</v>
       </c>
       <c r="E109" t="s">
-        <v>281</v>
-      </c>
-      <c r="M109" t="s">
-        <v>282</v>
+        <v>278</v>
+      </c>
+      <c r="F109" t="s">
+        <v>167</v>
+      </c>
+      <c r="J109" t="s">
+        <v>168</v>
+      </c>
+      <c r="K109" t="s">
+        <v>169</v>
+      </c>
+      <c r="L109" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="110" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="B110" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C110" t="s">
-        <v>177</v>
+        <v>280</v>
       </c>
       <c r="E110" t="s">
-        <v>178</v>
+        <v>281</v>
       </c>
       <c r="M110" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4142,27 +4179,33 @@
         <v>48</v>
       </c>
       <c r="B111" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C111" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E111" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M111" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="112" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B112" t="s">
-        <v>287</v>
-      </c>
-      <c r="G112" t="s">
-        <v>288</v>
+        <v>285</v>
+      </c>
+      <c r="C112" t="s">
+        <v>181</v>
+      </c>
+      <c r="E112" t="s">
+        <v>182</v>
+      </c>
+      <c r="M112" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4170,47 +4213,47 @@
         <v>17</v>
       </c>
       <c r="B113" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="G113" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B114" t="s">
-        <v>291</v>
-      </c>
-      <c r="C114" t="s">
-        <v>292</v>
-      </c>
-      <c r="E114" t="s">
-        <v>293</v>
-      </c>
-      <c r="J114" t="s">
-        <v>187</v>
-      </c>
-      <c r="K114" t="s">
-        <v>188</v>
-      </c>
-      <c r="L114" t="s">
-        <v>189</v>
-      </c>
-      <c r="M114" t="s">
-        <v>294</v>
+        <v>289</v>
+      </c>
+      <c r="G114" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A115" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B115" t="s">
-        <v>295</v>
-      </c>
-      <c r="G115" t="s">
-        <v>296</v>
+        <v>291</v>
+      </c>
+      <c r="C115" t="s">
+        <v>292</v>
+      </c>
+      <c r="E115" t="s">
+        <v>293</v>
+      </c>
+      <c r="J115" t="s">
+        <v>187</v>
+      </c>
+      <c r="K115" t="s">
+        <v>188</v>
+      </c>
+      <c r="L115" t="s">
+        <v>189</v>
+      </c>
+      <c r="M115" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4218,10 +4261,10 @@
         <v>17</v>
       </c>
       <c r="B116" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="G116" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4229,10 +4272,10 @@
         <v>17</v>
       </c>
       <c r="B117" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="G117" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4240,10 +4283,10 @@
         <v>17</v>
       </c>
       <c r="B118" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G118" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="119" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4251,10 +4294,10 @@
         <v>17</v>
       </c>
       <c r="B119" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G119" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="120" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4262,135 +4305,132 @@
         <v>17</v>
       </c>
       <c r="B120" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="G120" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A121" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="B121" t="s">
-        <v>240</v>
+        <v>305</v>
+      </c>
+      <c r="G121" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A122" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B122" t="s">
-        <v>307</v>
-      </c>
-      <c r="M122" t="s">
-        <v>308</v>
+        <v>240</v>
       </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A123" t="s">
-        <v>48</v>
+        <v>25</v>
       </c>
       <c r="B123" t="s">
-        <v>309</v>
-      </c>
-      <c r="C123" t="s">
-        <v>243</v>
-      </c>
-      <c r="E123" t="s">
-        <v>244</v>
+        <v>307</v>
+      </c>
+      <c r="M123" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="B124" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C124" t="s">
-        <v>246</v>
-      </c>
-      <c r="D124" t="s">
-        <v>120</v>
+        <v>243</v>
       </c>
       <c r="E124" t="s">
-        <v>247</v>
-      </c>
-      <c r="F124" t="s">
-        <v>121</v>
+        <v>244</v>
       </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>28</v>
+        <v>78</v>
       </c>
       <c r="B125" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C125" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D125" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="E125" t="s">
-        <v>312</v>
+        <v>247</v>
       </c>
       <c r="F125" t="s">
-        <v>126</v>
-      </c>
-      <c r="I125" t="s">
-        <v>29</v>
-      </c>
-      <c r="J125" t="s">
-        <v>127</v>
-      </c>
-      <c r="M125" t="s">
-        <v>313</v>
+        <v>121</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B126" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C126" t="s">
-        <v>253</v>
+        <v>634</v>
       </c>
       <c r="D126" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E126" t="s">
-        <v>254</v>
+        <v>312</v>
       </c>
       <c r="F126" t="s">
-        <v>132</v>
+        <v>126</v>
+      </c>
+      <c r="I126" t="s">
+        <v>29</v>
       </c>
       <c r="J126" t="s">
-        <v>255</v>
-      </c>
-      <c r="K126" t="s">
-        <v>134</v>
-      </c>
-      <c r="L126" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="M126" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A127" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B127" t="s">
-        <v>316</v>
-      </c>
-      <c r="G127" t="s">
-        <v>317</v>
+        <v>314</v>
+      </c>
+      <c r="C127" t="s">
+        <v>253</v>
+      </c>
+      <c r="D127" t="s">
+        <v>131</v>
+      </c>
+      <c r="E127" t="s">
+        <v>254</v>
+      </c>
+      <c r="F127" t="s">
+        <v>132</v>
+      </c>
+      <c r="J127" t="s">
+        <v>255</v>
+      </c>
+      <c r="K127" t="s">
+        <v>134</v>
+      </c>
+      <c r="L127" t="s">
+        <v>135</v>
       </c>
       <c r="M127" t="s">
         <v>315</v>
@@ -4401,27 +4441,24 @@
         <v>17</v>
       </c>
       <c r="B128" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="G128" t="s">
-        <v>319</v>
+        <v>317</v>
+      </c>
+      <c r="M128" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="129" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A129" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B129" t="s">
-        <v>320</v>
-      </c>
-      <c r="C129" t="s">
-        <v>262</v>
-      </c>
-      <c r="E129" t="s">
-        <v>263</v>
-      </c>
-      <c r="M129" t="s">
-        <v>321</v>
+        <v>318</v>
+      </c>
+      <c r="G129" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4429,125 +4466,125 @@
         <v>48</v>
       </c>
       <c r="B130" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C130" t="s">
-        <v>323</v>
+        <v>262</v>
       </c>
       <c r="E130" t="s">
-        <v>324</v>
+        <v>263</v>
       </c>
       <c r="M130" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>149</v>
+        <v>48</v>
       </c>
       <c r="B131" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C131" t="s">
-        <v>270</v>
-      </c>
-      <c r="D131" t="s">
-        <v>153</v>
+        <v>323</v>
       </c>
       <c r="E131" t="s">
-        <v>271</v>
-      </c>
-      <c r="F131" t="s">
-        <v>154</v>
-      </c>
-      <c r="J131" t="s">
-        <v>155</v>
-      </c>
-      <c r="K131" t="s">
-        <v>156</v>
-      </c>
-      <c r="L131" t="s">
-        <v>157</v>
+        <v>324</v>
+      </c>
+      <c r="M131" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B132" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C132" t="s">
-        <v>273</v>
+        <v>270</v>
+      </c>
+      <c r="D132" t="s">
+        <v>153</v>
       </c>
       <c r="E132" t="s">
-        <v>274</v>
-      </c>
-      <c r="M132" t="s">
-        <v>328</v>
+        <v>271</v>
+      </c>
+      <c r="F132" t="s">
+        <v>154</v>
+      </c>
+      <c r="J132" t="s">
+        <v>155</v>
+      </c>
+      <c r="K132" t="s">
+        <v>156</v>
+      </c>
+      <c r="L132" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="B133" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C133" t="s">
-        <v>277</v>
-      </c>
-      <c r="D133" t="s">
-        <v>166</v>
+        <v>273</v>
       </c>
       <c r="E133" t="s">
-        <v>278</v>
-      </c>
-      <c r="F133" t="s">
-        <v>167</v>
-      </c>
-      <c r="J133" t="s">
-        <v>168</v>
-      </c>
-      <c r="K133" t="s">
-        <v>169</v>
-      </c>
-      <c r="L133" t="s">
-        <v>170</v>
+        <v>274</v>
+      </c>
+      <c r="M133" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>171</v>
+        <v>149</v>
       </c>
       <c r="B134" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C134" t="s">
-        <v>280</v>
+        <v>277</v>
+      </c>
+      <c r="D134" t="s">
+        <v>166</v>
       </c>
       <c r="E134" t="s">
-        <v>281</v>
-      </c>
-      <c r="M134" t="s">
-        <v>331</v>
+        <v>278</v>
+      </c>
+      <c r="F134" t="s">
+        <v>167</v>
+      </c>
+      <c r="J134" t="s">
+        <v>168</v>
+      </c>
+      <c r="K134" t="s">
+        <v>169</v>
+      </c>
+      <c r="L134" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>48</v>
+        <v>171</v>
       </c>
       <c r="B135" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C135" t="s">
-        <v>177</v>
+        <v>280</v>
       </c>
       <c r="E135" t="s">
-        <v>178</v>
+        <v>281</v>
       </c>
       <c r="M135" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4555,27 +4592,33 @@
         <v>48</v>
       </c>
       <c r="B136" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C136" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="E136" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="M136" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="B137" t="s">
-        <v>336</v>
-      </c>
-      <c r="G137" t="s">
-        <v>337</v>
+        <v>334</v>
+      </c>
+      <c r="C137" t="s">
+        <v>181</v>
+      </c>
+      <c r="E137" t="s">
+        <v>182</v>
+      </c>
+      <c r="M137" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4583,47 +4626,47 @@
         <v>17</v>
       </c>
       <c r="B138" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G138" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="139" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A139" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B139" t="s">
-        <v>340</v>
-      </c>
-      <c r="C139" t="s">
-        <v>292</v>
-      </c>
-      <c r="E139" t="s">
-        <v>293</v>
-      </c>
-      <c r="J139" t="s">
-        <v>187</v>
-      </c>
-      <c r="K139" t="s">
-        <v>188</v>
-      </c>
-      <c r="L139" t="s">
-        <v>189</v>
-      </c>
-      <c r="M139" t="s">
-        <v>341</v>
+        <v>338</v>
+      </c>
+      <c r="G139" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="140" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A140" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B140" t="s">
-        <v>342</v>
-      </c>
-      <c r="G140" t="s">
-        <v>343</v>
+        <v>340</v>
+      </c>
+      <c r="C140" t="s">
+        <v>292</v>
+      </c>
+      <c r="E140" t="s">
+        <v>293</v>
+      </c>
+      <c r="J140" t="s">
+        <v>187</v>
+      </c>
+      <c r="K140" t="s">
+        <v>188</v>
+      </c>
+      <c r="L140" t="s">
+        <v>189</v>
+      </c>
+      <c r="M140" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="141" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4631,10 +4674,10 @@
         <v>17</v>
       </c>
       <c r="B141" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G141" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="142" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4642,10 +4685,10 @@
         <v>17</v>
       </c>
       <c r="B142" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G142" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="143" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4653,10 +4696,10 @@
         <v>17</v>
       </c>
       <c r="B143" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G143" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="144" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4664,10 +4707,10 @@
         <v>17</v>
       </c>
       <c r="B144" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G144" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="145" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4675,32 +4718,29 @@
         <v>17</v>
       </c>
       <c r="B145" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="G145" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="146" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A146" t="s">
+        <v>17</v>
+      </c>
+      <c r="B146" t="s">
+        <v>352</v>
+      </c>
+      <c r="G146" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A147" t="s">
         <v>43</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B147" t="s">
         <v>307</v>
-      </c>
-    </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A148" t="s">
-        <v>78</v>
-      </c>
-      <c r="B148" t="s">
-        <v>515</v>
-      </c>
-      <c r="C148" t="s">
-        <v>521</v>
-      </c>
-      <c r="M148" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4708,16 +4748,13 @@
         <v>78</v>
       </c>
       <c r="B149" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C149" t="s">
-        <v>522</v>
-      </c>
-      <c r="D149" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
       <c r="M149" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4725,16 +4762,16 @@
         <v>78</v>
       </c>
       <c r="B150" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C150" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D150" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="M150" t="s">
-        <v>600</v>
+        <v>641</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4742,13 +4779,16 @@
         <v>78</v>
       </c>
       <c r="B151" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C151" t="s">
-        <v>524</v>
-      </c>
-      <c r="M151" t="s">
-        <v>598</v>
+        <v>523</v>
+      </c>
+      <c r="D151" t="s">
+        <v>527</v>
+      </c>
+      <c r="M151" s="8" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4756,10 +4796,10 @@
         <v>78</v>
       </c>
       <c r="B152" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C152" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="M152" t="s">
         <v>598</v>
@@ -4770,27 +4810,27 @@
         <v>78</v>
       </c>
       <c r="B153" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C153" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="M153" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="155" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A155" t="s">
-        <v>17</v>
-      </c>
-      <c r="B155" t="s">
-        <v>354</v>
-      </c>
-      <c r="G155" t="s">
-        <v>95</v>
-      </c>
-      <c r="M155" t="s">
-        <v>355</v>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A154" t="s">
+        <v>78</v>
+      </c>
+      <c r="B154" t="s">
+        <v>520</v>
+      </c>
+      <c r="C154" t="s">
+        <v>526</v>
+      </c>
+      <c r="M154" t="s">
+        <v>598</v>
       </c>
     </row>
     <row r="156" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4798,50 +4838,47 @@
         <v>17</v>
       </c>
       <c r="B156" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G156" t="s">
         <v>95</v>
       </c>
       <c r="M156" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="157" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A157" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="B157" t="s">
-        <v>358</v>
-      </c>
-      <c r="C157" t="s">
-        <v>616</v>
-      </c>
-      <c r="D157" t="s">
-        <v>360</v>
-      </c>
-      <c r="E157" t="s">
-        <v>359</v>
-      </c>
-      <c r="F157" t="s">
-        <v>361</v>
+        <v>356</v>
+      </c>
+      <c r="G157" t="s">
+        <v>95</v>
       </c>
       <c r="M157" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="158" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
-        <v>363</v>
+        <v>48</v>
       </c>
       <c r="B158" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="C158" t="s">
-        <v>618</v>
+        <v>615</v>
+      </c>
+      <c r="D158" t="s">
+        <v>360</v>
       </c>
       <c r="E158" t="s">
-        <v>365</v>
+        <v>359</v>
+      </c>
+      <c r="F158" t="s">
+        <v>361</v>
       </c>
       <c r="M158" t="s">
         <v>362</v>
@@ -4849,56 +4886,59 @@
     </row>
     <row r="159" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
-        <v>48</v>
+        <v>363</v>
       </c>
       <c r="B159" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C159" t="s">
         <v>617</v>
       </c>
-      <c r="D159" t="s">
-        <v>368</v>
-      </c>
       <c r="E159" t="s">
-        <v>367</v>
-      </c>
-      <c r="F159" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="M159" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
     </row>
     <row r="160" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
-        <v>371</v>
+        <v>48</v>
       </c>
       <c r="B160" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C160" t="s">
-        <v>619</v>
+        <v>616</v>
+      </c>
+      <c r="D160" t="s">
+        <v>368</v>
       </c>
       <c r="E160" t="s">
-        <v>373</v>
+        <v>367</v>
+      </c>
+      <c r="F160" t="s">
+        <v>369</v>
       </c>
       <c r="M160" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A162" t="s">
-        <v>17</v>
-      </c>
-      <c r="B162" t="s">
-        <v>374</v>
-      </c>
-      <c r="G162" t="s">
-        <v>95</v>
-      </c>
-      <c r="M162" t="s">
-        <v>375</v>
+    <row r="161" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A161" t="s">
+        <v>371</v>
+      </c>
+      <c r="B161" t="s">
+        <v>372</v>
+      </c>
+      <c r="C161" t="s">
+        <v>618</v>
+      </c>
+      <c r="E161" t="s">
+        <v>373</v>
+      </c>
+      <c r="M161" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4906,13 +4946,13 @@
         <v>17</v>
       </c>
       <c r="B163" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G163" t="s">
         <v>95</v>
       </c>
       <c r="M163" t="s">
-        <v>603</v>
+        <v>375</v>
       </c>
     </row>
     <row r="164" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4920,13 +4960,13 @@
         <v>17</v>
       </c>
       <c r="B164" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G164" t="s">
         <v>95</v>
       </c>
       <c r="M164" t="s">
-        <v>378</v>
+        <v>602</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -4934,47 +4974,49 @@
         <v>17</v>
       </c>
       <c r="B165" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="G165" t="s">
         <v>95</v>
       </c>
       <c r="M165" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A166" t="s">
+        <v>17</v>
+      </c>
+      <c r="B166" t="s">
+        <v>379</v>
+      </c>
+      <c r="G166" t="s">
+        <v>95</v>
+      </c>
+      <c r="M166" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="166" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A166" s="2" t="s">
+    <row r="167" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A167" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B166" s="2" t="s">
+      <c r="B167" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="168" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A168" s="1" t="s">
+    <row r="169" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A169" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B168" s="1" t="s">
+      <c r="B169" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="C168" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="N168" s="1" t="s">
+      <c r="C169" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="N169" s="1" t="s">
         <v>501</v>
-      </c>
-    </row>
-    <row r="169" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A169" t="s">
-        <v>17</v>
-      </c>
-      <c r="B169" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="C169" s="4"/>
-      <c r="G169" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="170" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4982,11 +5024,11 @@
         <v>17</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="C170" s="4"/>
-      <c r="G170" s="3" t="s">
-        <v>511</v>
+      <c r="G170" t="s">
+        <v>625</v>
       </c>
     </row>
     <row r="171" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -4994,11 +5036,11 @@
         <v>17</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="C171" s="4"/>
       <c r="G171" s="3" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
     </row>
     <row r="172" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5006,59 +5048,51 @@
         <v>17</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C172" s="4"/>
       <c r="G172" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="173" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A173" t="s">
+        <v>17</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>505</v>
+      </c>
+      <c r="C173" s="4"/>
+      <c r="G173" s="3" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A174" t="s">
         <v>48</v>
       </c>
-      <c r="B173" t="s">
+      <c r="B174" t="s">
         <v>506</v>
       </c>
-      <c r="C173" s="5" t="s">
+      <c r="C174" s="5" t="s">
         <v>507</v>
       </c>
-      <c r="E173" s="3" t="s">
+      <c r="E174" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="M173" s="3" t="s">
+      <c r="M174" s="3" t="s">
         <v>514</v>
       </c>
     </row>
-    <row r="174" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A174" s="7" t="s">
+    <row r="175" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A175" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B174" s="7" t="s">
+      <c r="B175" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="C174" s="7" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.55000000000000004">
-      <c r="A175" t="s">
-        <v>78</v>
-      </c>
-      <c r="B175" t="s">
-        <v>483</v>
-      </c>
-      <c r="C175" t="s">
-        <v>512</v>
-      </c>
-      <c r="E175" t="s">
-        <v>79</v>
-      </c>
-      <c r="H175" t="s">
-        <v>22</v>
-      </c>
-      <c r="M175" s="3" t="s">
-        <v>514</v>
+      <c r="C175" s="7" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5066,10 +5100,10 @@
         <v>78</v>
       </c>
       <c r="B176" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C176" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="E176" t="s">
         <v>79</v>
@@ -5081,24 +5115,24 @@
         <v>514</v>
       </c>
     </row>
-    <row r="177" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
-        <v>486</v>
+        <v>78</v>
       </c>
       <c r="B177" t="s">
-        <v>487</v>
-      </c>
-      <c r="C177" s="6" t="s">
-        <v>608</v>
-      </c>
-      <c r="J177" t="s">
-        <v>488</v>
-      </c>
-      <c r="K177" t="s">
-        <v>489</v>
+        <v>484</v>
+      </c>
+      <c r="C177" t="s">
+        <v>513</v>
+      </c>
+      <c r="E177" t="s">
+        <v>79</v>
+      </c>
+      <c r="H177" t="s">
+        <v>22</v>
       </c>
       <c r="M177" s="3" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
     </row>
     <row r="178" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5106,16 +5140,16 @@
         <v>486</v>
       </c>
       <c r="B178" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="J178" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="K178" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="M178" s="3" t="s">
         <v>510</v>
@@ -5126,81 +5160,75 @@
         <v>486</v>
       </c>
       <c r="B179" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="J179" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="K179" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="M179" s="3" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="181" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A181" s="1" t="s">
+    <row r="180" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A180" t="s">
+        <v>486</v>
+      </c>
+      <c r="B180" t="s">
+        <v>491</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>609</v>
+      </c>
+      <c r="J180" t="s">
+        <v>495</v>
+      </c>
+      <c r="K180" t="s">
+        <v>494</v>
+      </c>
+      <c r="M180" s="3" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A182" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B181" s="1" t="s">
+      <c r="B182" s="1" t="s">
         <v>485</v>
-      </c>
-    </row>
-    <row r="183" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A183" t="s">
-        <v>97</v>
-      </c>
-      <c r="B183" t="s">
-        <v>381</v>
-      </c>
-      <c r="C183" t="s">
-        <v>382</v>
-      </c>
-      <c r="D183" t="s">
-        <v>384</v>
-      </c>
-      <c r="E183" t="s">
-        <v>383</v>
-      </c>
-      <c r="F183" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A184" t="s">
-        <v>386</v>
+        <v>97</v>
       </c>
       <c r="B184" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C184" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D184" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="E184" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="F184" t="s">
-        <v>391</v>
-      </c>
-      <c r="H184" t="s">
-        <v>22</v>
-      </c>
-      <c r="M184" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
     </row>
     <row r="185" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="B185" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C185" t="s">
         <v>388</v>
@@ -5214,78 +5242,93 @@
       <c r="F185" t="s">
         <v>391</v>
       </c>
+      <c r="H185" t="s">
+        <v>22</v>
+      </c>
       <c r="M185" t="s">
-        <v>52</v>
+        <v>392</v>
       </c>
     </row>
     <row r="186" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B186" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C186" t="s">
         <v>388</v>
       </c>
+      <c r="D186" t="s">
+        <v>390</v>
+      </c>
       <c r="E186" t="s">
         <v>389</v>
       </c>
-      <c r="H186" t="s">
-        <v>22</v>
+      <c r="F186" t="s">
+        <v>391</v>
       </c>
       <c r="M186" t="s">
-        <v>397</v>
+        <v>52</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
-        <v>48</v>
+        <v>395</v>
       </c>
       <c r="B187" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C187" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="E187" t="s">
-        <v>400</v>
+        <v>389</v>
+      </c>
+      <c r="H187" t="s">
+        <v>22</v>
       </c>
       <c r="M187" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="B188" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C188" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E188" t="s">
-        <v>404</v>
+        <v>400</v>
+      </c>
+      <c r="M188" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A189" t="s">
+        <v>20</v>
+      </c>
+      <c r="B189" t="s">
+        <v>402</v>
+      </c>
+      <c r="C189" t="s">
+        <v>403</v>
+      </c>
+      <c r="E189" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A190" t="s">
         <v>43</v>
       </c>
-      <c r="B189" t="s">
+      <c r="B190" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="191" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A191" t="s">
-        <v>17</v>
-      </c>
-      <c r="B191" t="s">
-        <v>405</v>
-      </c>
-      <c r="G191" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5293,10 +5336,10 @@
         <v>17</v>
       </c>
       <c r="B192" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="G192" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5304,10 +5347,10 @@
         <v>17</v>
       </c>
       <c r="B193" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="G193" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5315,10 +5358,10 @@
         <v>17</v>
       </c>
       <c r="B194" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="G194" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5326,10 +5369,10 @@
         <v>17</v>
       </c>
       <c r="B195" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="G195" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5337,15 +5380,27 @@
         <v>17</v>
       </c>
       <c r="B196" t="s">
+        <v>413</v>
+      </c>
+      <c r="G196" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A197" t="s">
+        <v>17</v>
+      </c>
+      <c r="B197" t="s">
         <v>415</v>
       </c>
-      <c r="G196" t="s">
+      <c r="G197" t="s">
         <v>416</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5993,7 +6048,7 @@
         <v>420</v>
       </c>
       <c r="C53" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D53" t="s">
         <v>456</v>
@@ -6007,7 +6062,7 @@
         <v>428</v>
       </c>
       <c r="C54" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D54" t="s">
         <v>457</v>
@@ -6035,7 +6090,7 @@
         <v>420</v>
       </c>
       <c r="C56" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D56" t="s">
         <v>459</v>
@@ -6049,7 +6104,7 @@
         <v>428</v>
       </c>
       <c r="C57" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D57" t="s">
         <v>460</v>
@@ -6184,13 +6239,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B2" t="s">
         <v>480</v>
       </c>
       <c r="C2" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D2" t="s">
         <v>481</v>
@@ -6203,7 +6258,11 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6258,75 +6317,17 @@
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="73f51738-d318-4883-9d64-4f0bd0ccc55e" ContentTypeId="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970" PreviousValue="false"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
-      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
-    </_dlc_DocIdUrl>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>5</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6769,19 +6770,73 @@
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <_dlc_DocId xmlns="b147f249-7416-4137-943c-c9568737db59">F5P3HXZH6X3Y-362526909-19140</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="be3559c3-162a-46c1-b278-386731838041" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="b147f249-7416-4137-943c-c9568737db59" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <TaxKeywordTaxHTField xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <_dlc_DocIdUrl xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <Url>https://unicef.sharepoint.com/teams/IND-Nutrition/_layouts/15/DocIdRedir.aspx?ID=F5P3HXZH6X3Y-362526909-19140</Url>
+      <Description>F5P3HXZH6X3Y-362526909-19140</Description>
+    </_dlc_DocIdUrl>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SharedWithUsers xmlns="b147f249-7416-4137-943c-c9568737db59">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>5</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6795,23 +6850,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC306C06-1920-4B93-A068-89E2CCFE2C3A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
-    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6840,9 +6889,15 @@
 </file>
 
 <file path=customXml/itemProps6.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="b147f249-7416-4137-943c-c9568737db59"/>
+    <ds:schemaRef ds:uri="be3559c3-162a-46c1-b278-386731838041"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
corrected draft name(date/time) Removed EXCESS constraints
In previous version of questionnaire with ACF Canada - excess constraints impeding data collection with constraint = true
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{19706F7B-2325-4CFF-BBD8-A2DD014C83A9}"/>
+  <xr:revisionPtr revIDLastSave="182" documentId="8_{8E94355A-06AA-4C33-A936-AFAC2A996A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FB89AB17-5449-496B-A19E-1422322FE6ED}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1037" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="648">
   <si>
     <t>type</t>
   </si>
@@ -2006,12 +2006,6 @@
     <t xml:space="preserve">${MONTHS}&lt;24  or (${MONTHS}=98 and ${HEIGHT}&lt;=87) </t>
   </si>
   <si>
-    <t>ACO_SMART_Survey_2021</t>
-  </si>
-  <si>
-    <t>concat('ACO_SMART_Survey_2021','_HH',${HH})</t>
-  </si>
-  <si>
     <t>(${WEIGHT}&gt;0 or ${HEIGHT}&gt;0 or ${MUAC}&gt;0 or ${EDEMA} = 'y' or ${EDEMA} = 'n')</t>
   </si>
   <si>
@@ -2153,6 +2147,30 @@
       </rPr>
       <t xml:space="preserve"> or (${MONTHS}=98 and ${HEIGHT}&gt;67) </t>
     </r>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>disp time</t>
+  </si>
+  <si>
+    <t>concat('ACO_HH',${HH},'_',${time})</t>
+  </si>
+  <si>
+    <t>start - ${start} time-${time}</t>
+  </si>
+  <si>
+    <t>substr(${start},2,16)</t>
+  </si>
+  <si>
+    <t>ACO_SMART_Survey_2022</t>
+  </si>
+  <si>
+    <t>${consent} = 2</t>
+  </si>
+  <si>
+    <t>Please measure MUAC on the left arm of the child. Position yourself on the right of the child/caregiver.</t>
   </si>
 </sst>
 </file>
@@ -2575,11 +2593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N197"/>
+  <dimension ref="A1:N199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A145" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R155" sqref="R155"/>
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F85" sqref="F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2919,7 +2937,7 @@
         <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="C23" t="s">
         <v>64</v>
@@ -2936,12 +2954,12 @@
         <v>17</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="G24" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -2957,9 +2975,6 @@
       <c r="E25" t="s">
         <v>69</v>
       </c>
-      <c r="H25" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
@@ -2980,9 +2995,6 @@
       <c r="F26" t="s">
         <v>74</v>
       </c>
-      <c r="H26" t="s">
-        <v>22</v>
-      </c>
       <c r="J26" t="s">
         <v>75</v>
       </c>
@@ -3009,7 +3021,7 @@
         <v>80</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="32" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3020,7 +3032,7 @@
         <v>498</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3067,9 +3079,6 @@
       <c r="E36" t="s">
         <v>88</v>
       </c>
-      <c r="H36" t="s">
-        <v>22</v>
-      </c>
       <c r="M36" t="s">
         <v>53</v>
       </c>
@@ -3105,7 +3114,7 @@
         <v>98</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="40" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3116,7 +3125,7 @@
         <v>99</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
     </row>
     <row r="41" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3127,7 +3136,7 @@
         <v>499</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
     </row>
     <row r="42" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3138,7 +3147,7 @@
         <v>500</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
     </row>
     <row r="43" spans="1:14" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3146,10 +3155,10 @@
         <v>48</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="44" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3178,7 +3187,7 @@
         <v>104</v>
       </c>
       <c r="G46" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -3233,7 +3242,7 @@
         <v>113</v>
       </c>
       <c r="C51" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="E51" t="s">
         <v>114</v>
@@ -3247,10 +3256,10 @@
         <v>48</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="53" spans="1:13" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004"/>
@@ -3284,9 +3293,6 @@
       <c r="F55" t="s">
         <v>121</v>
       </c>
-      <c r="H55" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
@@ -3314,7 +3320,7 @@
         <v>127</v>
       </c>
       <c r="M56" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3399,7 +3405,7 @@
         <v>145</v>
       </c>
       <c r="C61" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="E61" t="s">
         <v>146</v>
@@ -3413,21 +3419,21 @@
         <v>17</v>
       </c>
       <c r="B62" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
     </row>
     <row r="63" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="7" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="C63" s="7" t="s">
         <v>637</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3438,7 +3444,7 @@
         <v>148</v>
       </c>
       <c r="M64" s="8" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3577,6 +3583,9 @@
       <c r="C71" t="s">
         <v>185</v>
       </c>
+      <c r="D71" t="s">
+        <v>647</v>
+      </c>
       <c r="E71" t="s">
         <v>186</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>227</v>
       </c>
       <c r="M90" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="N90" s="7"/>
     </row>
@@ -3841,7 +3850,7 @@
         <v>229</v>
       </c>
       <c r="M91" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="N91" s="7"/>
     </row>
@@ -3882,7 +3891,7 @@
         <v>235</v>
       </c>
       <c r="M94" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="N94" s="7"/>
     </row>
@@ -3897,7 +3906,7 @@
         <v>237</v>
       </c>
       <c r="M95" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="N95" s="7"/>
     </row>
@@ -3912,7 +3921,7 @@
         <v>239</v>
       </c>
       <c r="M96" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="N96" s="7"/>
     </row>
@@ -4383,7 +4392,7 @@
         <v>311</v>
       </c>
       <c r="C126" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="D126" t="s">
         <v>125</v>
@@ -4771,7 +4780,7 @@
         <v>528</v>
       </c>
       <c r="M150" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="151" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4788,7 +4797,7 @@
         <v>527</v>
       </c>
       <c r="M151" s="8" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
     </row>
     <row r="152" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -4869,7 +4878,7 @@
         <v>358</v>
       </c>
       <c r="C158" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D158" t="s">
         <v>360</v>
@@ -4892,7 +4901,7 @@
         <v>364</v>
       </c>
       <c r="C159" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="E159" t="s">
         <v>365</v>
@@ -4909,7 +4918,7 @@
         <v>366</v>
       </c>
       <c r="C160" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D160" t="s">
         <v>368</v>
@@ -4932,7 +4941,7 @@
         <v>372</v>
       </c>
       <c r="C161" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E161" t="s">
         <v>373</v>
@@ -4966,7 +4975,7 @@
         <v>95</v>
       </c>
       <c r="M164" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="165" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5013,7 +5022,7 @@
         <v>485</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="N169" s="1" t="s">
         <v>501</v>
@@ -5028,7 +5037,7 @@
       </c>
       <c r="C170" s="4"/>
       <c r="G170" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
     </row>
     <row r="171" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -5092,7 +5101,7 @@
         <v>497</v>
       </c>
       <c r="C175" s="7" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
     </row>
     <row r="176" spans="1:14" x14ac:dyDescent="0.55000000000000004">
@@ -5108,9 +5117,6 @@
       <c r="E176" t="s">
         <v>79</v>
       </c>
-      <c r="H176" t="s">
-        <v>22</v>
-      </c>
       <c r="M176" s="3" t="s">
         <v>514</v>
       </c>
@@ -5128,9 +5134,6 @@
       <c r="E177" t="s">
         <v>79</v>
       </c>
-      <c r="H177" t="s">
-        <v>22</v>
-      </c>
       <c r="M177" s="3" t="s">
         <v>514</v>
       </c>
@@ -5143,7 +5146,7 @@
         <v>487</v>
       </c>
       <c r="C178" s="6" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="J178" t="s">
         <v>488</v>
@@ -5163,7 +5166,7 @@
         <v>490</v>
       </c>
       <c r="C179" s="6" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="J179" t="s">
         <v>492</v>
@@ -5183,7 +5186,7 @@
         <v>491</v>
       </c>
       <c r="C180" s="6" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="J180" t="s">
         <v>495</v>
@@ -5269,7 +5272,7 @@
         <v>391</v>
       </c>
       <c r="M186" t="s">
-        <v>52</v>
+        <v>646</v>
       </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -5331,37 +5334,38 @@
         <v>44</v>
       </c>
     </row>
-    <row r="192" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="A192" t="s">
-        <v>17</v>
-      </c>
-      <c r="B192" t="s">
-        <v>405</v>
-      </c>
-      <c r="G192" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="A193" t="s">
-        <v>17</v>
-      </c>
-      <c r="B193" t="s">
-        <v>407</v>
-      </c>
-      <c r="G193" t="s">
-        <v>408</v>
-      </c>
+    <row r="192" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A192" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="193" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A193" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B193" s="7" t="s">
+        <v>641</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>643</v>
+      </c>
+      <c r="G193" s="8"/>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A194" t="s">
         <v>17</v>
       </c>
       <c r="B194" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="G194" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5369,10 +5373,10 @@
         <v>17</v>
       </c>
       <c r="B195" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G195" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5380,10 +5384,10 @@
         <v>17</v>
       </c>
       <c r="B196" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="G196" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.55000000000000004">
@@ -5391,9 +5395,31 @@
         <v>17</v>
       </c>
       <c r="B197" t="s">
+        <v>411</v>
+      </c>
+      <c r="G197" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A198" t="s">
+        <v>17</v>
+      </c>
+      <c r="B198" t="s">
+        <v>413</v>
+      </c>
+      <c r="G198" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A199" t="s">
+        <v>17</v>
+      </c>
+      <c r="B199" t="s">
         <v>415</v>
       </c>
-      <c r="G197" t="s">
+      <c r="G199" t="s">
         <v>416</v>
       </c>
     </row>
@@ -6048,7 +6074,7 @@
         <v>420</v>
       </c>
       <c r="C53" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="D53" t="s">
         <v>456</v>
@@ -6062,7 +6088,7 @@
         <v>428</v>
       </c>
       <c r="C54" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D54" t="s">
         <v>457</v>
@@ -6090,7 +6116,7 @@
         <v>420</v>
       </c>
       <c r="C56" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D56" t="s">
         <v>459</v>
@@ -6104,7 +6130,7 @@
         <v>428</v>
       </c>
       <c r="C57" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D57" t="s">
         <v>460</v>
@@ -6218,7 +6244,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6239,13 +6265,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>600</v>
+        <v>645</v>
       </c>
       <c r="B2" t="s">
         <v>480</v>
       </c>
       <c r="C2" t="s">
-        <v>601</v>
+        <v>642</v>
       </c>
       <c r="D2" t="s">
         <v>481</v>

</xml_diff>

<commit_message>
REmove 2 $ from consent message - Dari / Pash
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="198" documentId="8_{0FB4861F-8ECE-44A2-A28F-46469FB9792C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3E8281E5-2099-4377-B364-28D6851A2E34}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="109_{F04355A7-C390-4C96-801B-3151D1B62B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F4FD3A49-386F-46B0-97E3-4483312B9189}"/>
   <bookViews>
-    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -786,9 +786,6 @@
   </si>
   <si>
     <t>select_one consent</t>
-  </si>
-  <si>
-    <t>سلام زما نوم دی ________. زه د ________ [سازمان/حکومتي ادارې] سره یم. مهرباني وکړئ اجازه راکړئ تاسو د ټیم نورو غړو ته معرفي کړم: _________ او _______. موږ نن ورځ دلته یو ترڅو د تغذیې او ________ په اړه د کورنۍ معلومات راټول کړو. که چیرې په کورنۍ کې د 5 کلونو څخه کم ماشومان شتون ولري موږ غواړو یو څه اندازه (وزن، قد، MUAC، اذیما / تشریح) په پام کې ونیسو ترڅو د ${ولایت}، د ${ولسوالۍ}کې د 5 کلونو څخه کم عمره تغذیه حالت معلومولو کې مرسته وکړي. . مهرباني وکړئ په یاد ولرئ چې اوس مهال معلومه نه ده چې د سروې د پایلو له پای ته رسیدو وروسته به کوم اقدامات (که کوم وي) ترسره شي. ټول معلومات به په بشپړه توګه محرم وساتل شي. ایا تاسو کومه پوښتنه لرئ؟ ایا زه پیل کولی شم؟</t>
   </si>
   <si>
     <t>note</t>
@@ -2403,9 +2400,6 @@
     <t>Age in years (0 - 120)</t>
   </si>
   <si>
-    <t>سلام اسم من است ________. من با ________ [سازمان/سازمان دولتی] هستم. لطفا اجازه دهید شما را به سایر اعضای تیم معرفی کنم: _________ و _______. ما امروز اینجا هستیم تا اطلاعات خانوار مربوط به تغذیه و ________ را جمع آوری کنیم. اگر کودک زیر 5 سال در خانواده وجود دارد، مایلیم اندازه گیری هایی (وزن، قد، MUAC، oedema / توضیح دهید) برای کمک به تعیین وضعیت کلی تغذیه زیر 5 سال در ${وانجام دهیم. . لطفاً توجه داشته باشید که در حال حاضر مشخص نیست که پس از نهایی شدن نتایج نظرسنجی چه اقداماتی (در صورت وجود) انجام خواهد شد. تمامی اطلاعات کاملاً محرمانه خواهد بود. آیا سوالی دارید؟ می توانم شروع کنم؟</t>
-  </si>
-  <si>
     <t>"+" را فشار دهید - برای افزودن یکی دیگر از اعضای خانواده تا زمانی که همه اعضا فهرست شوند. پس از تکمیل فهرست، برای ادامه پرسشنامه،"" را فشار دهید.</t>
   </si>
   <si>
@@ -2677,6 +2671,12 @@
   </si>
   <si>
     <t>د ښځې وزن {wom_name}$ کیلوګرام کې</t>
+  </si>
+  <si>
+    <t>سلام اسم من است ________. من با ________ [سازمان/سازمان دولتی] هستم. لطفا اجازه دهید شما را به سایر اعضای تیم معرفی کنم: _________ و _______. ما امروز اینجا هستیم تا اطلاعات خانوار مربوط به تغذیه و ________ را جمع آوری کنیم. اگر کودک زیر 5 سال در خانواده وجود دارد، مایلیم اندازه گیری هایی (وزن، قد، MUAC، oedema / توضیح دهید) برای کمک به تعیین وضعیت کلی تغذیه زیر 5 سال در . . لطفاً توجه داشته باشید که در حال حاضر مشخص نیست که پس از نهایی شدن نتایج نظرسنجی چه اقداماتی (در صورت وجود) انجام خواهد شد. تمامی اطلاعات کاملاً محرمانه خواهد بود. آیا سوالی دارید؟ می توانم شروع کنم؟</t>
+  </si>
+  <si>
+    <t>سلام زما نوم دی ________. زه د ________ [سازمان/حکومتي ادارې] سره یم. مهرباني وکړئ اجازه راکړئ تاسو د ټیم نورو غړو ته معرفي کړم: _________ او _______. موږ نن ورځ دلته یو ترڅو د تغذیې او ________ په اړه د کورنۍ معلومات راټول کړو. که چیرې په کورنۍ کې د 5 کلونو څخه کم ماشومان شتون ولري موږ غواړو یو څه اندازه (وزن، قد، MUAC، اذیما / تشریح) په پام کې ونیسو ترڅو د ، د  کلونو څخه کم عمره تغذیه حالت معلومولو کې مرسته وکړي. . مهرباني وکړئ په یاد ولرئ چې اوس مهال معلومه نه ده چې د سروې د پایلو له پای ته رسیدو وروسته به کوم اقدامات (که کوم وي) ترسره شي. ټول معلومات به په بشپړه توګه محرم وساتل شي. ایا تاسو کومه پوښتنه لرئ؟ ایا زه پیل کولی شم؟</t>
   </si>
 </sst>
 </file>
@@ -3234,9 +3234,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q199"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43:XFD43"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3292,10 +3292,10 @@
         <v>212</v>
       </c>
       <c r="N1" t="s">
+        <v>716</v>
+      </c>
+      <c r="O1" t="s">
         <v>717</v>
-      </c>
-      <c r="O1" t="s">
-        <v>718</v>
       </c>
       <c r="P1" t="s">
         <v>213</v>
@@ -3414,7 +3414,7 @@
         <v>226</v>
       </c>
       <c r="L10" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3437,7 +3437,7 @@
         <v>226</v>
       </c>
       <c r="L11" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3460,7 +3460,7 @@
         <v>226</v>
       </c>
       <c r="L12" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -3487,7 +3487,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="348" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:16" ht="330.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>250</v>
       </c>
@@ -3495,15 +3495,15 @@
         <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="22" t="s">
-        <v>721</v>
+        <v>811</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="23" t="s">
-        <v>251</v>
+        <v>812</v>
       </c>
       <c r="H17" s="11"/>
       <c r="J17" t="s">
@@ -3512,24 +3512,24 @@
     </row>
     <row r="18" spans="1:16" ht="87" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
+        <v>251</v>
+      </c>
+      <c r="B18" t="s">
         <v>252</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="E18" s="10" t="s">
         <v>254</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>255</v>
       </c>
       <c r="F18" s="11"/>
       <c r="G18" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H18" s="11"/>
       <c r="P18" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3544,58 +3544,58 @@
       <c r="G19" s="11"/>
       <c r="H19" s="11"/>
       <c r="P19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="104.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B20" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="9" t="s">
+        <v>721</v>
+      </c>
+      <c r="E20" s="25" t="s">
         <v>260</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>723</v>
-      </c>
-      <c r="E20" s="25" t="s">
+      <c r="F20" s="22" t="s">
+        <v>720</v>
+      </c>
+      <c r="G20" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="F20" s="22" t="s">
-        <v>722</v>
-      </c>
-      <c r="G20" s="26" t="s">
+      <c r="H20" s="23" t="s">
         <v>262</v>
       </c>
-      <c r="H20" s="23" t="s">
-        <v>263</v>
-      </c>
       <c r="P20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="21" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
+        <v>263</v>
+      </c>
+      <c r="B21" t="s">
         <v>264</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" s="3" t="s">
         <v>265</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="E21" s="13" t="s">
         <v>266</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>267</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H21" s="11"/>
       <c r="P21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3603,7 +3603,7 @@
         <v>231</v>
       </c>
       <c r="B22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E22" s="11"/>
       <c r="F22" s="11"/>
@@ -3618,17 +3618,17 @@
         <v>227</v>
       </c>
       <c r="B23" t="s">
+        <v>269</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="E23" s="15" t="s">
         <v>271</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>272</v>
       </c>
       <c r="F23" s="11"/>
       <c r="G23" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="H23" s="11"/>
       <c r="J23" t="s">
@@ -3640,32 +3640,32 @@
         <v>218</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
+        <v>275</v>
+      </c>
+      <c r="B25" t="s">
         <v>276</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="E25" s="15" t="s">
         <v>278</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>279</v>
       </c>
       <c r="F25" s="11"/>
       <c r="G25" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H25" s="11"/>
     </row>
@@ -3674,37 +3674,37 @@
         <v>234</v>
       </c>
       <c r="B26" t="s">
+        <v>279</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>280</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="E26" s="22" t="s">
+        <v>722</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="E26" s="22" t="s">
-        <v>724</v>
-      </c>
-      <c r="F26" s="10" t="s">
+      <c r="G26" s="23" t="s">
+        <v>723</v>
+      </c>
+      <c r="H26" s="12" t="s">
         <v>283</v>
       </c>
-      <c r="G26" s="23" t="s">
-        <v>725</v>
-      </c>
-      <c r="H26" s="12" t="s">
+      <c r="L26" t="s">
         <v>284</v>
       </c>
-      <c r="L26" t="s">
-        <v>285</v>
-      </c>
       <c r="M26" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="N26" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="O26" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3730,7 +3730,7 @@
         <v>247</v>
       </c>
       <c r="B30" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="11"/>
@@ -3742,24 +3742,24 @@
         <v>218</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="H31" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="I31" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="F31" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="G31" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="32" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3767,24 +3767,24 @@
         <v>218</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
       <c r="E32" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H32" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -3792,22 +3792,22 @@
         <v>218</v>
       </c>
       <c r="B33" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E33" s="11"/>
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
       <c r="H33" s="11"/>
       <c r="I33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B34" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E34" s="11"/>
       <c r="F34" s="11"/>
@@ -3819,36 +3819,36 @@
         <v>218</v>
       </c>
       <c r="B35" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="11"/>
       <c r="G35" s="11"/>
       <c r="H35" s="11"/>
       <c r="I35" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="52.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
+        <v>295</v>
+      </c>
+      <c r="B36" t="s">
         <v>296</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="E36" s="22" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="23" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="H36" s="11"/>
       <c r="P36" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:17" ht="174" x14ac:dyDescent="0.55000000000000004">
@@ -3856,28 +3856,28 @@
         <v>234</v>
       </c>
       <c r="B37" t="s">
+        <v>298</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="D37" s="9" t="s">
+        <v>727</v>
+      </c>
+      <c r="E37" s="13" t="s">
         <v>300</v>
       </c>
-      <c r="D37" s="9" t="s">
-        <v>729</v>
-      </c>
-      <c r="E37" s="13" t="s">
+      <c r="F37" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="G37" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="G37" s="14" t="s">
+      <c r="H37" s="23" t="s">
         <v>303</v>
       </c>
-      <c r="H37" s="23" t="s">
+      <c r="P37" t="s">
         <v>304</v>
-      </c>
-      <c r="P37" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -3891,24 +3891,24 @@
         <v>218</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
       <c r="E39" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G39" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H39" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="40" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3916,24 +3916,24 @@
         <v>218</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
       <c r="E40" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G40" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H40" s="16" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="41" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3941,24 +3941,24 @@
         <v>218</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
       <c r="E41" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F41" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="42" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -3966,48 +3966,48 @@
         <v>218</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
       <c r="E42" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F42" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="43" spans="1:17" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B43" s="33" t="s">
+        <v>313</v>
+      </c>
+      <c r="C43" s="34" t="s">
         <v>314</v>
-      </c>
-      <c r="C43" s="34" t="s">
-        <v>315</v>
       </c>
       <c r="D43" s="34"/>
       <c r="E43" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F43" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -4018,29 +4018,29 @@
     </row>
     <row r="45" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>316</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>317</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="18" t="s">
+        <v>317</v>
+      </c>
+      <c r="F45" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="G45" s="18" t="s">
         <v>318</v>
       </c>
-      <c r="F45" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="G45" s="18" t="s">
+      <c r="H45" s="16" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q45" s="2" t="s">
         <v>319</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q45" s="2" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -4048,14 +4048,14 @@
         <v>218</v>
       </c>
       <c r="B46" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E46" s="11"/>
       <c r="F46" s="11"/>
       <c r="G46" s="11"/>
       <c r="H46" s="11"/>
       <c r="I46" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -4063,14 +4063,14 @@
         <v>218</v>
       </c>
       <c r="B47" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E47" s="11"/>
       <c r="F47" s="11"/>
       <c r="G47" s="11"/>
       <c r="H47" s="11"/>
       <c r="I47" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -4078,14 +4078,14 @@
         <v>218</v>
       </c>
       <c r="B48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E48" s="11"/>
       <c r="F48" s="11"/>
       <c r="G48" s="11"/>
       <c r="H48" s="11"/>
       <c r="I48" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4093,14 +4093,14 @@
         <v>218</v>
       </c>
       <c r="B49" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
       <c r="G49" s="11"/>
       <c r="H49" s="11"/>
       <c r="I49" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4108,60 +4108,60 @@
         <v>218</v>
       </c>
       <c r="B50" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
       <c r="H50" s="11"/>
       <c r="I50" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="52.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B51" t="s">
+        <v>330</v>
+      </c>
+      <c r="C51" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>332</v>
-      </c>
       <c r="E51" s="22" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="23" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H51" s="11"/>
       <c r="P51" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="52" spans="1:16" s="33" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B52" s="33" t="s">
+        <v>333</v>
+      </c>
+      <c r="C52" s="34" t="s">
         <v>334</v>
-      </c>
-      <c r="C52" s="34" t="s">
-        <v>335</v>
       </c>
       <c r="D52" s="34"/>
       <c r="E52" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="F52" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G52" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H52" s="35" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4175,75 +4175,75 @@
         <v>231</v>
       </c>
       <c r="B54" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
       <c r="G54" s="11"/>
       <c r="H54" s="11"/>
       <c r="P54" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="69.599999999999994" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B55" t="s">
+        <v>336</v>
+      </c>
+      <c r="C55" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="C55" s="3" t="s">
+      <c r="D55" s="3" t="s">
         <v>338</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="27" t="s">
+        <v>729</v>
+      </c>
+      <c r="F55" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="E55" s="27" t="s">
-        <v>731</v>
-      </c>
-      <c r="F55" s="10" t="s">
+      <c r="G55" s="23" t="s">
+        <v>730</v>
+      </c>
+      <c r="H55" s="12" t="s">
         <v>340</v>
-      </c>
-      <c r="G55" s="23" t="s">
-        <v>732</v>
-      </c>
-      <c r="H55" s="12" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
+        <v>341</v>
+      </c>
+      <c r="B56" t="s">
         <v>342</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="D56" s="3" t="s">
         <v>344</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="27" t="s">
+        <v>731</v>
+      </c>
+      <c r="F56" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="E56" s="27" t="s">
-        <v>733</v>
-      </c>
-      <c r="F56" s="10" t="s">
+      <c r="G56" s="23" t="s">
+        <v>732</v>
+      </c>
+      <c r="H56" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="G56" s="23" t="s">
-        <v>734</v>
-      </c>
-      <c r="H56" s="12" t="s">
+      <c r="K56" t="s">
         <v>347</v>
       </c>
-      <c r="K56" t="s">
+      <c r="L56" t="s">
         <v>348</v>
       </c>
-      <c r="L56" t="s">
+      <c r="P56" t="s">
         <v>349</v>
-      </c>
-      <c r="P56" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="69.599999999999994" x14ac:dyDescent="0.55000000000000004">
@@ -4251,40 +4251,40 @@
         <v>234</v>
       </c>
       <c r="B57" t="s">
+        <v>350</v>
+      </c>
+      <c r="C57" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="C57" s="3" t="s">
+      <c r="D57" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="E57" s="27" t="s">
+        <v>734</v>
+      </c>
+      <c r="F57" s="10" t="s">
         <v>353</v>
       </c>
-      <c r="E57" s="27" t="s">
-        <v>736</v>
-      </c>
-      <c r="F57" s="10" t="s">
+      <c r="G57" s="23" t="s">
+        <v>735</v>
+      </c>
+      <c r="H57" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="G57" s="23" t="s">
-        <v>737</v>
-      </c>
-      <c r="H57" s="12" t="s">
+      <c r="L57" t="s">
         <v>355</v>
       </c>
-      <c r="L57" t="s">
+      <c r="M57" t="s">
         <v>356</v>
       </c>
-      <c r="M57" t="s">
+      <c r="N57" t="s">
+        <v>356</v>
+      </c>
+      <c r="O57" t="s">
+        <v>356</v>
+      </c>
+      <c r="P57" t="s">
         <v>357</v>
-      </c>
-      <c r="N57" t="s">
-        <v>357</v>
-      </c>
-      <c r="O57" t="s">
-        <v>357</v>
-      </c>
-      <c r="P57" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4292,17 +4292,17 @@
         <v>218</v>
       </c>
       <c r="B58" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E58" s="11"/>
       <c r="F58" s="11"/>
       <c r="G58" s="11"/>
       <c r="H58" s="11"/>
       <c r="I58" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="P58" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4310,58 +4310,58 @@
         <v>218</v>
       </c>
       <c r="B59" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E59" s="11"/>
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
       <c r="H59" s="11"/>
       <c r="I59" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="60" spans="1:16" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B60" t="s">
+        <v>362</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>363</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>364</v>
-      </c>
       <c r="E60" s="27" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="28" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="H60" s="11"/>
       <c r="P60" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="34.799999999999997" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B61" t="s">
+        <v>365</v>
+      </c>
+      <c r="C61" s="3" t="s">
         <v>366</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="E61" s="19" t="s">
         <v>367</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>368</v>
       </c>
       <c r="F61" s="11"/>
       <c r="G61" s="20" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H61" s="11"/>
       <c r="P61" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4369,21 +4369,21 @@
         <v>218</v>
       </c>
       <c r="B62" t="s">
+        <v>370</v>
+      </c>
+      <c r="I62" t="s">
         <v>371</v>
-      </c>
-      <c r="I62" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="63" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="33" t="s">
+        <v>372</v>
+      </c>
+      <c r="B63" s="33" t="s">
         <v>373</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="C63" s="34" t="s">
         <v>374</v>
-      </c>
-      <c r="C63" s="34" t="s">
-        <v>375</v>
       </c>
       <c r="D63" s="34"/>
       <c r="E63" s="34"/>
@@ -4396,160 +4396,160 @@
         <v>231</v>
       </c>
       <c r="B64" t="s">
+        <v>375</v>
+      </c>
+      <c r="P64" s="6" t="s">
         <v>376</v>
-      </c>
-      <c r="P64" s="6" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
+        <v>377</v>
+      </c>
+      <c r="B65" t="s">
         <v>378</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="D65" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="E65" s="9" t="s">
+        <v>738</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E65" s="9" t="s">
-        <v>740</v>
-      </c>
-      <c r="F65" s="3" t="s">
+      <c r="G65" s="9" t="s">
+        <v>739</v>
+      </c>
+      <c r="H65" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G65" s="9" t="s">
-        <v>741</v>
-      </c>
-      <c r="H65" s="3" t="s">
+      <c r="L65" t="s">
         <v>383</v>
       </c>
-      <c r="L65" t="s">
+      <c r="M65" t="s">
         <v>384</v>
       </c>
-      <c r="M65" t="s">
-        <v>385</v>
-      </c>
       <c r="N65" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O65" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
+        <v>385</v>
+      </c>
+      <c r="B66" t="s">
         <v>386</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="3" t="s">
         <v>387</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>388</v>
-      </c>
       <c r="E66" s="9" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B67" t="s">
+        <v>388</v>
+      </c>
+      <c r="C67" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="D67" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="E67" s="9" t="s">
+        <v>742</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="E67" s="9" t="s">
-        <v>744</v>
-      </c>
-      <c r="F67" s="3" t="s">
+      <c r="G67" s="9" t="s">
+        <v>743</v>
+      </c>
+      <c r="H67" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="G67" s="9" t="s">
-        <v>745</v>
-      </c>
-      <c r="H67" s="3" t="s">
+      <c r="L67" t="s">
         <v>393</v>
       </c>
-      <c r="L67" t="s">
+      <c r="M67" t="s">
         <v>394</v>
       </c>
-      <c r="M67" t="s">
-        <v>395</v>
-      </c>
       <c r="N67" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O67" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
+        <v>395</v>
+      </c>
+      <c r="B68" t="s">
         <v>396</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="E68" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="E68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>399</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B69" t="s">
+        <v>400</v>
+      </c>
+      <c r="C69" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="G69" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="G69" s="3" t="s">
+      <c r="P69" t="s">
         <v>404</v>
-      </c>
-      <c r="P69" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B70" t="s">
+        <v>405</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="E70" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="P70" t="s">
         <v>409</v>
-      </c>
-      <c r="P70" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -4557,80 +4557,80 @@
         <v>234</v>
       </c>
       <c r="B71" t="s">
+        <v>410</v>
+      </c>
+      <c r="C71" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="D71" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="E71" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="F71" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="G71" s="9" t="s">
+        <v>744</v>
+      </c>
+      <c r="H71" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="G71" s="9" t="s">
-        <v>746</v>
-      </c>
-      <c r="H71" s="3" t="s">
+      <c r="L71" t="s">
         <v>416</v>
       </c>
-      <c r="L71" t="s">
+      <c r="M71" t="s">
         <v>417</v>
       </c>
-      <c r="M71" t="s">
+      <c r="N71" t="s">
+        <v>417</v>
+      </c>
+      <c r="O71" t="s">
+        <v>417</v>
+      </c>
+      <c r="P71" t="s">
         <v>418</v>
-      </c>
-      <c r="N71" t="s">
-        <v>418</v>
-      </c>
-      <c r="O71" t="s">
-        <v>418</v>
-      </c>
-      <c r="P71" t="s">
-        <v>419</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B72" t="s">
+        <v>419</v>
+      </c>
+      <c r="C72" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="C72" s="3" t="s">
-        <v>421</v>
-      </c>
       <c r="E72" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B73" t="s">
+        <v>421</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="C73" s="3" t="s">
-        <v>423</v>
-      </c>
       <c r="E73" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="J73" t="s">
         <v>226</v>
       </c>
       <c r="P73" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4638,7 +4638,7 @@
         <v>247</v>
       </c>
       <c r="B74" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4646,7 +4646,7 @@
         <v>247</v>
       </c>
       <c r="B75" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4654,10 +4654,10 @@
         <v>218</v>
       </c>
       <c r="B76" t="s">
+        <v>424</v>
+      </c>
+      <c r="I76" t="s">
         <v>425</v>
-      </c>
-      <c r="I76" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4665,10 +4665,10 @@
         <v>218</v>
       </c>
       <c r="B77" t="s">
+        <v>426</v>
+      </c>
+      <c r="I77" t="s">
         <v>427</v>
-      </c>
-      <c r="I77" t="s">
-        <v>428</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4676,10 +4676,10 @@
         <v>218</v>
       </c>
       <c r="B78" t="s">
+        <v>428</v>
+      </c>
+      <c r="I78" t="s">
         <v>429</v>
-      </c>
-      <c r="I78" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4687,10 +4687,10 @@
         <v>218</v>
       </c>
       <c r="B79" t="s">
+        <v>430</v>
+      </c>
+      <c r="I79" t="s">
         <v>431</v>
-      </c>
-      <c r="I79" t="s">
-        <v>432</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4698,13 +4698,13 @@
         <v>218</v>
       </c>
       <c r="B80" t="s">
+        <v>432</v>
+      </c>
+      <c r="I80" t="s">
         <v>433</v>
       </c>
-      <c r="I80" t="s">
+      <c r="P80" t="s">
         <v>434</v>
-      </c>
-      <c r="P80" t="s">
-        <v>435</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4712,13 +4712,13 @@
         <v>218</v>
       </c>
       <c r="B81" t="s">
+        <v>435</v>
+      </c>
+      <c r="I81" t="s">
         <v>436</v>
       </c>
-      <c r="I81" t="s">
-        <v>437</v>
-      </c>
       <c r="P81" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4726,10 +4726,10 @@
         <v>218</v>
       </c>
       <c r="B82" t="s">
+        <v>437</v>
+      </c>
+      <c r="I82" t="s">
         <v>438</v>
-      </c>
-      <c r="I82" t="s">
-        <v>439</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4737,13 +4737,13 @@
         <v>218</v>
       </c>
       <c r="B83" t="s">
+        <v>439</v>
+      </c>
+      <c r="I83" t="s">
         <v>440</v>
       </c>
-      <c r="I83" t="s">
-        <v>441</v>
-      </c>
       <c r="P83" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4751,13 +4751,13 @@
         <v>218</v>
       </c>
       <c r="B84" t="s">
+        <v>441</v>
+      </c>
+      <c r="I84" t="s">
         <v>442</v>
       </c>
-      <c r="I84" t="s">
-        <v>443</v>
-      </c>
       <c r="P84" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4765,10 +4765,10 @@
         <v>218</v>
       </c>
       <c r="B85" t="s">
+        <v>443</v>
+      </c>
+      <c r="I85" t="s">
         <v>444</v>
-      </c>
-      <c r="I85" t="s">
-        <v>445</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4776,13 +4776,13 @@
         <v>218</v>
       </c>
       <c r="B86" t="s">
+        <v>445</v>
+      </c>
+      <c r="I86" t="s">
         <v>446</v>
       </c>
-      <c r="I86" t="s">
-        <v>447</v>
-      </c>
       <c r="P86" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4790,13 +4790,13 @@
         <v>218</v>
       </c>
       <c r="B87" t="s">
+        <v>447</v>
+      </c>
+      <c r="I87" t="s">
         <v>448</v>
       </c>
-      <c r="I87" t="s">
-        <v>449</v>
-      </c>
       <c r="P87" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4804,10 +4804,10 @@
         <v>218</v>
       </c>
       <c r="B88" t="s">
+        <v>449</v>
+      </c>
+      <c r="I88" t="s">
         <v>450</v>
-      </c>
-      <c r="I88" t="s">
-        <v>451</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4815,10 +4815,10 @@
         <v>218</v>
       </c>
       <c r="B89" t="s">
+        <v>451</v>
+      </c>
+      <c r="I89" t="s">
         <v>452</v>
-      </c>
-      <c r="I89" t="s">
-        <v>453</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4826,13 +4826,13 @@
         <v>218</v>
       </c>
       <c r="B90" t="s">
+        <v>453</v>
+      </c>
+      <c r="I90" t="s">
         <v>454</v>
       </c>
-      <c r="I90" t="s">
+      <c r="P90" s="6" t="s">
         <v>455</v>
-      </c>
-      <c r="P90" s="6" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4840,13 +4840,13 @@
         <v>218</v>
       </c>
       <c r="B91" t="s">
+        <v>456</v>
+      </c>
+      <c r="I91" t="s">
         <v>457</v>
       </c>
-      <c r="I91" t="s">
-        <v>458</v>
-      </c>
       <c r="P91" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4854,10 +4854,10 @@
         <v>218</v>
       </c>
       <c r="B92" t="s">
+        <v>458</v>
+      </c>
+      <c r="I92" t="s">
         <v>459</v>
-      </c>
-      <c r="I92" t="s">
-        <v>460</v>
       </c>
       <c r="P92" s="6"/>
     </row>
@@ -4866,10 +4866,10 @@
         <v>218</v>
       </c>
       <c r="B93" t="s">
+        <v>460</v>
+      </c>
+      <c r="I93" t="s">
         <v>461</v>
-      </c>
-      <c r="I93" t="s">
-        <v>462</v>
       </c>
       <c r="P93" s="6"/>
     </row>
@@ -4878,13 +4878,13 @@
         <v>218</v>
       </c>
       <c r="B94" t="s">
+        <v>462</v>
+      </c>
+      <c r="I94" t="s">
         <v>463</v>
       </c>
-      <c r="I94" t="s">
-        <v>464</v>
-      </c>
       <c r="P94" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4892,13 +4892,13 @@
         <v>218</v>
       </c>
       <c r="B95" t="s">
+        <v>464</v>
+      </c>
+      <c r="I95" t="s">
         <v>465</v>
       </c>
-      <c r="I95" t="s">
-        <v>466</v>
-      </c>
       <c r="P95" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4906,13 +4906,13 @@
         <v>218</v>
       </c>
       <c r="B96" t="s">
+        <v>466</v>
+      </c>
+      <c r="I96" t="s">
         <v>467</v>
       </c>
-      <c r="I96" t="s">
-        <v>468</v>
-      </c>
       <c r="P96" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4920,88 +4920,88 @@
         <v>231</v>
       </c>
       <c r="B98" t="s">
+        <v>468</v>
+      </c>
+      <c r="P98" t="s">
         <v>469</v>
-      </c>
-      <c r="P98" t="s">
-        <v>470</v>
       </c>
     </row>
     <row r="99" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B99" t="s">
+        <v>470</v>
+      </c>
+      <c r="C99" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="C99" s="3" t="s">
-        <v>472</v>
-      </c>
       <c r="E99" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B100" t="s">
+        <v>472</v>
+      </c>
+      <c r="C100" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="C100" s="3" t="s">
+      <c r="D100" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>751</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="G100" s="9" t="s">
+        <v>752</v>
+      </c>
+      <c r="H100" s="3" t="s">
         <v>474</v>
-      </c>
-      <c r="D100" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="E100" s="9" t="s">
-        <v>753</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="G100" s="9" t="s">
-        <v>754</v>
-      </c>
-      <c r="H100" s="3" t="s">
-        <v>475</v>
       </c>
     </row>
     <row r="101" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B101" t="s">
+        <v>475</v>
+      </c>
+      <c r="C101" s="3" t="s">
         <v>476</v>
       </c>
-      <c r="C101" s="3" t="s">
+      <c r="D101" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>753</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G101" s="9" t="s">
+        <v>754</v>
+      </c>
+      <c r="H101" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="K101" t="s">
+        <v>347</v>
+      </c>
+      <c r="L101" t="s">
+        <v>348</v>
+      </c>
+      <c r="P101" t="s">
         <v>477</v>
-      </c>
-      <c r="D101" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>755</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G101" s="9" t="s">
-        <v>756</v>
-      </c>
-      <c r="H101" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="K101" t="s">
-        <v>348</v>
-      </c>
-      <c r="L101" t="s">
-        <v>349</v>
-      </c>
-      <c r="P101" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="102" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -5009,40 +5009,40 @@
         <v>234</v>
       </c>
       <c r="B102" t="s">
+        <v>478</v>
+      </c>
+      <c r="C102" s="3" t="s">
         <v>479</v>
       </c>
-      <c r="C102" s="3" t="s">
+      <c r="D102" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>755</v>
+      </c>
+      <c r="F102" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="D102" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E102" s="9" t="s">
-        <v>757</v>
-      </c>
-      <c r="F102" s="3" t="s">
+      <c r="G102" s="9" t="s">
+        <v>756</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="L102" t="s">
         <v>481</v>
       </c>
-      <c r="G102" s="9" t="s">
-        <v>758</v>
-      </c>
-      <c r="H102" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="L102" t="s">
+      <c r="M102" t="s">
+        <v>356</v>
+      </c>
+      <c r="N102" t="s">
+        <v>356</v>
+      </c>
+      <c r="O102" t="s">
+        <v>356</v>
+      </c>
+      <c r="P102" t="s">
         <v>482</v>
-      </c>
-      <c r="M102" t="s">
-        <v>357</v>
-      </c>
-      <c r="N102" t="s">
-        <v>357</v>
-      </c>
-      <c r="O102" t="s">
-        <v>357</v>
-      </c>
-      <c r="P102" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5050,13 +5050,13 @@
         <v>218</v>
       </c>
       <c r="B103" t="s">
+        <v>483</v>
+      </c>
+      <c r="I103" t="s">
         <v>484</v>
       </c>
-      <c r="I103" t="s">
-        <v>485</v>
-      </c>
       <c r="P103" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5064,206 +5064,206 @@
         <v>218</v>
       </c>
       <c r="B104" t="s">
+        <v>485</v>
+      </c>
+      <c r="I104" t="s">
         <v>486</v>
-      </c>
-      <c r="I104" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B105" t="s">
+        <v>487</v>
+      </c>
+      <c r="C105" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="C105" s="3" t="s">
+      <c r="E105" s="9" t="s">
+        <v>757</v>
+      </c>
+      <c r="G105" s="9" t="s">
+        <v>758</v>
+      </c>
+      <c r="P105" t="s">
         <v>489</v>
-      </c>
-      <c r="E105" s="9" t="s">
-        <v>759</v>
-      </c>
-      <c r="G105" s="9" t="s">
-        <v>760</v>
-      </c>
-      <c r="P105" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="106" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B106" t="s">
+        <v>490</v>
+      </c>
+      <c r="C106" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="C106" s="3" t="s">
+      <c r="E106" s="9" t="s">
+        <v>760</v>
+      </c>
+      <c r="G106" s="9" t="s">
+        <v>759</v>
+      </c>
+      <c r="P106" t="s">
         <v>492</v>
-      </c>
-      <c r="E106" s="9" t="s">
-        <v>762</v>
-      </c>
-      <c r="G106" s="9" t="s">
-        <v>761</v>
-      </c>
-      <c r="P106" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="107" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B107" t="s">
+        <v>493</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>494</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>495</v>
-      </c>
       <c r="D107" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>761</v>
+      </c>
+      <c r="F107" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E107" s="9" t="s">
-        <v>763</v>
-      </c>
-      <c r="F107" s="3" t="s">
+      <c r="G107" s="9" t="s">
+        <v>762</v>
+      </c>
+      <c r="H107" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G107" s="9" t="s">
-        <v>764</v>
-      </c>
-      <c r="H107" s="3" t="s">
+      <c r="L107" t="s">
         <v>383</v>
       </c>
-      <c r="L107" t="s">
+      <c r="M107" t="s">
         <v>384</v>
       </c>
-      <c r="M107" t="s">
-        <v>385</v>
-      </c>
       <c r="N107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O107" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="108" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B108" t="s">
+        <v>495</v>
+      </c>
+      <c r="C108" s="3" t="s">
         <v>496</v>
       </c>
-      <c r="C108" s="3" t="s">
+      <c r="E108" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="G108" s="3" t="s">
         <v>497</v>
       </c>
-      <c r="E108" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="G108" s="3" t="s">
+      <c r="P108" t="s">
         <v>498</v>
-      </c>
-      <c r="P108" t="s">
-        <v>499</v>
       </c>
     </row>
     <row r="109" spans="1:16" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B109" t="s">
+        <v>499</v>
+      </c>
+      <c r="C109" s="3" t="s">
         <v>500</v>
       </c>
-      <c r="C109" s="3" t="s">
+      <c r="D109" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E109" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="D109" s="3" t="s">
+      <c r="F109" s="3" t="s">
         <v>391</v>
       </c>
-      <c r="E109" s="9" t="s">
-        <v>502</v>
-      </c>
-      <c r="F109" s="3" t="s">
+      <c r="G109" s="9" t="s">
+        <v>764</v>
+      </c>
+      <c r="H109" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="G109" s="9" t="s">
-        <v>766</v>
-      </c>
-      <c r="H109" s="3" t="s">
+      <c r="L109" t="s">
         <v>393</v>
       </c>
-      <c r="L109" t="s">
+      <c r="M109" t="s">
         <v>394</v>
       </c>
-      <c r="M109" t="s">
-        <v>395</v>
-      </c>
       <c r="N109" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O109" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="110" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B110" t="s">
+        <v>502</v>
+      </c>
+      <c r="C110" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="E110" s="3" t="s">
         <v>504</v>
       </c>
-      <c r="E110" s="3" t="s">
+      <c r="G110" s="3" t="s">
         <v>505</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="P110" t="s">
         <v>506</v>
-      </c>
-      <c r="P110" t="s">
-        <v>507</v>
       </c>
     </row>
     <row r="111" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B111" t="s">
+        <v>507</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="G111" s="3" t="s">
         <v>508</v>
       </c>
-      <c r="C111" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="E111" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="G111" s="3" t="s">
+      <c r="P111" t="s">
         <v>509</v>
-      </c>
-      <c r="P111" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="112" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B112" t="s">
+        <v>510</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="E112" s="3" t="s">
         <v>511</v>
       </c>
-      <c r="C112" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E112" s="3" t="s">
+      <c r="G112" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="P112" t="s">
         <v>512</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="P112" t="s">
-        <v>513</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5271,10 +5271,10 @@
         <v>218</v>
       </c>
       <c r="B113" t="s">
+        <v>513</v>
+      </c>
+      <c r="I113" t="s">
         <v>514</v>
-      </c>
-      <c r="I113" t="s">
-        <v>515</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5282,10 +5282,10 @@
         <v>218</v>
       </c>
       <c r="B114" t="s">
+        <v>515</v>
+      </c>
+      <c r="I114" t="s">
         <v>516</v>
-      </c>
-      <c r="I114" t="s">
-        <v>517</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5293,31 +5293,31 @@
         <v>234</v>
       </c>
       <c r="B115" t="s">
+        <v>517</v>
+      </c>
+      <c r="C115" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="E115" s="9" t="s">
+        <v>765</v>
+      </c>
+      <c r="G115" s="9" t="s">
+        <v>766</v>
+      </c>
+      <c r="L115" t="s">
+        <v>416</v>
+      </c>
+      <c r="M115" t="s">
+        <v>417</v>
+      </c>
+      <c r="N115" t="s">
+        <v>417</v>
+      </c>
+      <c r="O115" t="s">
+        <v>417</v>
+      </c>
+      <c r="P115" t="s">
         <v>519</v>
-      </c>
-      <c r="E115" s="9" t="s">
-        <v>767</v>
-      </c>
-      <c r="G115" s="9" t="s">
-        <v>768</v>
-      </c>
-      <c r="L115" t="s">
-        <v>417</v>
-      </c>
-      <c r="M115" t="s">
-        <v>418</v>
-      </c>
-      <c r="N115" t="s">
-        <v>418</v>
-      </c>
-      <c r="O115" t="s">
-        <v>418</v>
-      </c>
-      <c r="P115" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5325,10 +5325,10 @@
         <v>218</v>
       </c>
       <c r="B116" t="s">
+        <v>520</v>
+      </c>
+      <c r="I116" t="s">
         <v>521</v>
-      </c>
-      <c r="I116" t="s">
-        <v>522</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5336,10 +5336,10 @@
         <v>218</v>
       </c>
       <c r="B117" t="s">
+        <v>522</v>
+      </c>
+      <c r="I117" t="s">
         <v>523</v>
-      </c>
-      <c r="I117" t="s">
-        <v>524</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5347,10 +5347,10 @@
         <v>218</v>
       </c>
       <c r="B118" t="s">
+        <v>524</v>
+      </c>
+      <c r="I118" t="s">
         <v>525</v>
-      </c>
-      <c r="I118" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5358,10 +5358,10 @@
         <v>218</v>
       </c>
       <c r="B119" t="s">
+        <v>526</v>
+      </c>
+      <c r="I119" t="s">
         <v>527</v>
-      </c>
-      <c r="I119" t="s">
-        <v>528</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5369,10 +5369,10 @@
         <v>218</v>
       </c>
       <c r="B120" t="s">
+        <v>528</v>
+      </c>
+      <c r="I120" t="s">
         <v>529</v>
-      </c>
-      <c r="I120" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5380,10 +5380,10 @@
         <v>218</v>
       </c>
       <c r="B121" t="s">
+        <v>530</v>
+      </c>
+      <c r="I121" t="s">
         <v>531</v>
-      </c>
-      <c r="I121" t="s">
-        <v>532</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5391,7 +5391,7 @@
         <v>247</v>
       </c>
       <c r="B122" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5399,88 +5399,88 @@
         <v>231</v>
       </c>
       <c r="B123" t="s">
+        <v>532</v>
+      </c>
+      <c r="P123" t="s">
         <v>533</v>
-      </c>
-      <c r="P123" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="124" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A124" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B124" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
     </row>
     <row r="125" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A125" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B125" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D125" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="E125" s="29" t="s">
+        <v>769</v>
+      </c>
+      <c r="F125" s="3" t="s">
         <v>339</v>
       </c>
-      <c r="E125" s="29" t="s">
-        <v>771</v>
-      </c>
-      <c r="F125" s="3" t="s">
+      <c r="G125" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="H125" s="3" t="s">
         <v>340</v>
-      </c>
-      <c r="G125" s="9" t="s">
-        <v>772</v>
-      </c>
-      <c r="H125" s="3" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="126" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A126" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B126" t="s">
+        <v>536</v>
+      </c>
+      <c r="C126" s="3" t="s">
         <v>537</v>
       </c>
-      <c r="C126" s="3" t="s">
+      <c r="D126" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="E126" s="29" t="s">
+        <v>771</v>
+      </c>
+      <c r="F126" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G126" s="29" t="s">
+        <v>772</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="K126" t="s">
+        <v>347</v>
+      </c>
+      <c r="L126" t="s">
+        <v>348</v>
+      </c>
+      <c r="P126" t="s">
         <v>538</v>
-      </c>
-      <c r="D126" s="3" t="s">
-        <v>345</v>
-      </c>
-      <c r="E126" s="29" t="s">
-        <v>773</v>
-      </c>
-      <c r="F126" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G126" s="29" t="s">
-        <v>774</v>
-      </c>
-      <c r="H126" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="K126" t="s">
-        <v>348</v>
-      </c>
-      <c r="L126" t="s">
-        <v>349</v>
-      </c>
-      <c r="P126" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="127" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -5488,40 +5488,40 @@
         <v>234</v>
       </c>
       <c r="B127" t="s">
+        <v>539</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E127" s="29" t="s">
+        <v>773</v>
+      </c>
+      <c r="F127" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="G127" s="29" t="s">
+        <v>756</v>
+      </c>
+      <c r="H127" s="3" t="s">
         <v>540</v>
       </c>
-      <c r="C127" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="D127" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E127" s="29" t="s">
-        <v>775</v>
-      </c>
-      <c r="F127" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="G127" s="29" t="s">
-        <v>758</v>
-      </c>
-      <c r="H127" s="3" t="s">
+      <c r="L127" t="s">
+        <v>481</v>
+      </c>
+      <c r="M127" t="s">
+        <v>356</v>
+      </c>
+      <c r="N127" t="s">
+        <v>356</v>
+      </c>
+      <c r="O127" t="s">
+        <v>356</v>
+      </c>
+      <c r="P127" t="s">
         <v>541</v>
-      </c>
-      <c r="L127" t="s">
-        <v>482</v>
-      </c>
-      <c r="M127" t="s">
-        <v>357</v>
-      </c>
-      <c r="N127" t="s">
-        <v>357</v>
-      </c>
-      <c r="O127" t="s">
-        <v>357</v>
-      </c>
-      <c r="P127" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5529,13 +5529,13 @@
         <v>218</v>
       </c>
       <c r="B128" t="s">
+        <v>542</v>
+      </c>
+      <c r="I128" t="s">
         <v>543</v>
       </c>
-      <c r="I128" t="s">
-        <v>544</v>
-      </c>
       <c r="P128" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5543,206 +5543,206 @@
         <v>218</v>
       </c>
       <c r="B129" t="s">
+        <v>544</v>
+      </c>
+      <c r="I129" t="s">
         <v>545</v>
-      </c>
-      <c r="I129" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A130" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B130" t="s">
+        <v>546</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>488</v>
+      </c>
+      <c r="E130" s="29" t="s">
+        <v>774</v>
+      </c>
+      <c r="G130" s="29" t="s">
+        <v>775</v>
+      </c>
+      <c r="P130" t="s">
         <v>547</v>
-      </c>
-      <c r="C130" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="E130" s="29" t="s">
-        <v>776</v>
-      </c>
-      <c r="G130" s="29" t="s">
-        <v>777</v>
-      </c>
-      <c r="P130" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="131" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A131" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B131" t="s">
+        <v>548</v>
+      </c>
+      <c r="C131" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="C131" s="3" t="s">
+      <c r="E131" s="30" t="s">
+        <v>776</v>
+      </c>
+      <c r="G131" s="30" t="s">
+        <v>777</v>
+      </c>
+      <c r="P131" t="s">
         <v>550</v>
-      </c>
-      <c r="E131" s="30" t="s">
-        <v>778</v>
-      </c>
-      <c r="G131" s="30" t="s">
-        <v>779</v>
-      </c>
-      <c r="P131" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="132" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B132" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D132" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="E132" s="31" t="s">
+        <v>761</v>
+      </c>
+      <c r="F132" s="3" t="s">
         <v>381</v>
       </c>
-      <c r="E132" s="31" t="s">
-        <v>763</v>
-      </c>
-      <c r="F132" s="3" t="s">
+      <c r="G132" s="32" t="s">
+        <v>778</v>
+      </c>
+      <c r="H132" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="G132" s="32" t="s">
-        <v>780</v>
-      </c>
-      <c r="H132" s="3" t="s">
+      <c r="L132" t="s">
         <v>383</v>
       </c>
-      <c r="L132" t="s">
+      <c r="M132" t="s">
         <v>384</v>
       </c>
-      <c r="M132" t="s">
-        <v>385</v>
-      </c>
       <c r="N132" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="O132" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="133" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B133" t="s">
+        <v>552</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="E133" s="32" t="s">
+        <v>763</v>
+      </c>
+      <c r="G133" s="32" t="s">
+        <v>779</v>
+      </c>
+      <c r="P133" t="s">
         <v>553</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="E133" s="32" t="s">
-        <v>765</v>
-      </c>
-      <c r="G133" s="32" t="s">
-        <v>781</v>
-      </c>
-      <c r="P133" t="s">
-        <v>554</v>
       </c>
     </row>
     <row r="134" spans="1:16" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B134" t="s">
+        <v>554</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="E134" s="32" t="s">
+        <v>780</v>
+      </c>
+      <c r="F134" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="G134" s="32" t="s">
+        <v>764</v>
+      </c>
+      <c r="H134" s="3" t="s">
         <v>555</v>
       </c>
-      <c r="C134" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="D134" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="E134" s="32" t="s">
-        <v>782</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="G134" s="32" t="s">
-        <v>766</v>
-      </c>
-      <c r="H134" s="3" t="s">
-        <v>556</v>
-      </c>
       <c r="L134" t="s">
+        <v>393</v>
+      </c>
+      <c r="M134" t="s">
         <v>394</v>
       </c>
-      <c r="M134" t="s">
-        <v>395</v>
-      </c>
       <c r="N134" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="O134" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="135" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B135" t="s">
+        <v>556</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="E135" s="21" t="s">
+        <v>504</v>
+      </c>
+      <c r="G135" s="21" t="s">
         <v>557</v>
       </c>
-      <c r="C135" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="E135" s="21" t="s">
-        <v>505</v>
-      </c>
-      <c r="G135" s="21" t="s">
+      <c r="P135" t="s">
         <v>558</v>
-      </c>
-      <c r="P135" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="136" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A136" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B136" t="s">
+        <v>559</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="E136" s="3" t="s">
         <v>560</v>
       </c>
-      <c r="C136" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="E136" s="3" t="s">
+      <c r="G136" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="P136" t="s">
         <v>561</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>404</v>
-      </c>
-      <c r="P136" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="137" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A137" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B137" t="s">
+        <v>562</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="E137" s="3" t="s">
         <v>563</v>
       </c>
-      <c r="C137" s="3" t="s">
-        <v>407</v>
-      </c>
-      <c r="E137" s="3" t="s">
+      <c r="G137" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="P137" t="s">
         <v>564</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="P137" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5750,10 +5750,10 @@
         <v>218</v>
       </c>
       <c r="B138" t="s">
+        <v>565</v>
+      </c>
+      <c r="I138" t="s">
         <v>566</v>
-      </c>
-      <c r="I138" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5761,10 +5761,10 @@
         <v>218</v>
       </c>
       <c r="B139" t="s">
+        <v>567</v>
+      </c>
+      <c r="I139" t="s">
         <v>568</v>
-      </c>
-      <c r="I139" t="s">
-        <v>569</v>
       </c>
     </row>
     <row r="140" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5772,31 +5772,31 @@
         <v>234</v>
       </c>
       <c r="B140" t="s">
+        <v>569</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="E140" s="32" t="s">
+        <v>781</v>
+      </c>
+      <c r="G140" s="32" t="s">
+        <v>782</v>
+      </c>
+      <c r="L140" t="s">
+        <v>416</v>
+      </c>
+      <c r="M140" t="s">
+        <v>417</v>
+      </c>
+      <c r="N140" t="s">
+        <v>417</v>
+      </c>
+      <c r="O140" t="s">
+        <v>417</v>
+      </c>
+      <c r="P140" t="s">
         <v>570</v>
-      </c>
-      <c r="C140" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="E140" s="32" t="s">
-        <v>783</v>
-      </c>
-      <c r="G140" s="32" t="s">
-        <v>784</v>
-      </c>
-      <c r="L140" t="s">
-        <v>417</v>
-      </c>
-      <c r="M140" t="s">
-        <v>418</v>
-      </c>
-      <c r="N140" t="s">
-        <v>418</v>
-      </c>
-      <c r="O140" t="s">
-        <v>418</v>
-      </c>
-      <c r="P140" t="s">
-        <v>571</v>
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5804,10 +5804,10 @@
         <v>218</v>
       </c>
       <c r="B141" t="s">
+        <v>571</v>
+      </c>
+      <c r="I141" t="s">
         <v>572</v>
-      </c>
-      <c r="I141" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5815,10 +5815,10 @@
         <v>218</v>
       </c>
       <c r="B142" t="s">
+        <v>573</v>
+      </c>
+      <c r="I142" t="s">
         <v>574</v>
-      </c>
-      <c r="I142" t="s">
-        <v>575</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5826,10 +5826,10 @@
         <v>218</v>
       </c>
       <c r="B143" t="s">
+        <v>575</v>
+      </c>
+      <c r="I143" t="s">
         <v>576</v>
-      </c>
-      <c r="I143" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5837,10 +5837,10 @@
         <v>218</v>
       </c>
       <c r="B144" t="s">
+        <v>577</v>
+      </c>
+      <c r="I144" t="s">
         <v>578</v>
-      </c>
-      <c r="I144" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5848,10 +5848,10 @@
         <v>218</v>
       </c>
       <c r="B145" t="s">
+        <v>579</v>
+      </c>
+      <c r="I145" t="s">
         <v>580</v>
-      </c>
-      <c r="I145" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5859,10 +5859,10 @@
         <v>218</v>
       </c>
       <c r="B146" t="s">
+        <v>581</v>
+      </c>
+      <c r="I146" t="s">
         <v>582</v>
-      </c>
-      <c r="I146" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5870,146 +5870,146 @@
         <v>247</v>
       </c>
       <c r="B147" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="149" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A149" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B149" t="s">
+        <v>583</v>
+      </c>
+      <c r="C149" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="C149" s="3" t="s">
-        <v>585</v>
-      </c>
       <c r="E149" s="9" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F149" s="9"/>
       <c r="G149" s="9" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="P149" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="150" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A150" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B150" t="s">
+        <v>586</v>
+      </c>
+      <c r="C150" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="D150" s="3" t="s">
         <v>588</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="E150" s="9" t="s">
+        <v>785</v>
+      </c>
+      <c r="F150" s="3" t="s">
         <v>589</v>
       </c>
-      <c r="E150" s="9" t="s">
-        <v>787</v>
-      </c>
-      <c r="F150" s="3" t="s">
+      <c r="G150" s="9" t="s">
+        <v>786</v>
+      </c>
+      <c r="H150" s="3" t="s">
         <v>590</v>
       </c>
-      <c r="G150" s="9" t="s">
-        <v>788</v>
-      </c>
-      <c r="H150" s="3" t="s">
+      <c r="P150" t="s">
         <v>591</v>
-      </c>
-      <c r="P150" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="151" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A151" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B151" t="s">
+        <v>592</v>
+      </c>
+      <c r="C151" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="D151" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="D151" s="3" t="s">
+      <c r="E151" s="9" t="s">
+        <v>787</v>
+      </c>
+      <c r="F151" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="E151" s="9" t="s">
-        <v>789</v>
-      </c>
-      <c r="F151" s="3" t="s">
+      <c r="G151" s="9" t="s">
+        <v>788</v>
+      </c>
+      <c r="H151" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="G151" s="9" t="s">
-        <v>790</v>
-      </c>
-      <c r="H151" s="3" t="s">
-        <v>597</v>
-      </c>
       <c r="P151" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="152" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A152" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B152" t="s">
+        <v>597</v>
+      </c>
+      <c r="C152" s="3" t="s">
         <v>598</v>
       </c>
-      <c r="C152" s="3" t="s">
+      <c r="E152" s="9" t="s">
+        <v>789</v>
+      </c>
+      <c r="G152" s="9" t="s">
+        <v>790</v>
+      </c>
+      <c r="P152" t="s">
         <v>599</v>
-      </c>
-      <c r="E152" s="9" t="s">
-        <v>791</v>
-      </c>
-      <c r="G152" s="9" t="s">
-        <v>792</v>
-      </c>
-      <c r="P152" t="s">
-        <v>600</v>
       </c>
     </row>
     <row r="153" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A153" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B153" t="s">
+        <v>600</v>
+      </c>
+      <c r="C153" s="3" t="s">
         <v>601</v>
       </c>
-      <c r="C153" s="3" t="s">
-        <v>602</v>
-      </c>
       <c r="E153" s="9" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="G153" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="P153" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="154" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A154" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B154" t="s">
+        <v>602</v>
+      </c>
+      <c r="C154" s="3" t="s">
         <v>603</v>
       </c>
-      <c r="C154" s="3" t="s">
-        <v>604</v>
-      </c>
       <c r="E154" s="9" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="G154" s="9" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="P154" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6017,13 +6017,13 @@
         <v>218</v>
       </c>
       <c r="B156" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I156" t="s">
         <v>6</v>
       </c>
       <c r="P156" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6031,111 +6031,111 @@
         <v>218</v>
       </c>
       <c r="B157" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I157" t="s">
         <v>6</v>
       </c>
       <c r="P157" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="158" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A158" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B158" t="s">
+        <v>608</v>
+      </c>
+      <c r="C158" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="D158" s="3" t="s">
         <v>610</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="E158" s="31" t="s">
         <v>611</v>
       </c>
-      <c r="E158" s="31" t="s">
+      <c r="F158" s="3" t="s">
         <v>612</v>
       </c>
-      <c r="F158" s="3" t="s">
+      <c r="G158" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="H158" s="3" t="s">
         <v>613</v>
       </c>
-      <c r="G158" s="9" t="s">
-        <v>797</v>
-      </c>
-      <c r="H158" s="3" t="s">
+      <c r="P158" t="s">
         <v>614</v>
-      </c>
-      <c r="P158" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="159" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A159" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B159" t="s">
+        <v>615</v>
+      </c>
+      <c r="C159" s="3" t="s">
         <v>616</v>
       </c>
-      <c r="C159" s="3" t="s">
-        <v>617</v>
-      </c>
       <c r="E159" s="9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="G159" s="9" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="P159" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="160" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A160" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B160" t="s">
+        <v>617</v>
+      </c>
+      <c r="C160" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="D160" s="3" t="s">
         <v>619</v>
       </c>
-      <c r="D160" s="3" t="s">
+      <c r="E160" s="9" t="s">
         <v>620</v>
       </c>
-      <c r="E160" s="9" t="s">
+      <c r="F160" s="3" t="s">
         <v>621</v>
       </c>
-      <c r="F160" s="3" t="s">
+      <c r="G160" s="9" t="s">
         <v>622</v>
       </c>
-      <c r="G160" s="9" t="s">
+      <c r="H160" s="3" t="s">
         <v>623</v>
       </c>
-      <c r="H160" s="3" t="s">
+      <c r="P160" t="s">
         <v>624</v>
-      </c>
-      <c r="P160" t="s">
-        <v>625</v>
       </c>
     </row>
     <row r="161" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A161" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B161" t="s">
+        <v>625</v>
+      </c>
+      <c r="C161" s="3" t="s">
         <v>626</v>
       </c>
-      <c r="C161" s="3" t="s">
-        <v>627</v>
-      </c>
       <c r="E161" s="9" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="G161" s="9" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="P161" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6143,13 +6143,13 @@
         <v>218</v>
       </c>
       <c r="B163" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I163" t="s">
         <v>6</v>
       </c>
       <c r="P163" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6157,13 +6157,13 @@
         <v>218</v>
       </c>
       <c r="B164" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I164" t="s">
         <v>6</v>
       </c>
       <c r="P164" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6171,13 +6171,13 @@
         <v>218</v>
       </c>
       <c r="B165" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I165" t="s">
         <v>6</v>
       </c>
       <c r="P165" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6185,21 +6185,21 @@
         <v>218</v>
       </c>
       <c r="B166" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I166" t="s">
         <v>6</v>
       </c>
       <c r="P166" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="167" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A167" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
@@ -6210,13 +6210,13 @@
     </row>
     <row r="169" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A169" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B169" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="C169" s="8" t="s">
         <v>636</v>
-      </c>
-      <c r="C169" s="8" t="s">
-        <v>637</v>
       </c>
       <c r="D169" s="8"/>
       <c r="E169" s="8"/>
@@ -6224,7 +6224,7 @@
       <c r="G169" s="8"/>
       <c r="H169" s="8"/>
       <c r="Q169" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6232,10 +6232,10 @@
         <v>218</v>
       </c>
       <c r="B170" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I170" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6243,10 +6243,10 @@
         <v>218</v>
       </c>
       <c r="B171" t="s">
+        <v>639</v>
+      </c>
+      <c r="I171" t="s">
         <v>640</v>
-      </c>
-      <c r="I171" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6254,10 +6254,10 @@
         <v>218</v>
       </c>
       <c r="B172" t="s">
+        <v>641</v>
+      </c>
+      <c r="I172" t="s">
         <v>642</v>
-      </c>
-      <c r="I172" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6265,41 +6265,41 @@
         <v>218</v>
       </c>
       <c r="B173" t="s">
+        <v>643</v>
+      </c>
+      <c r="I173" t="s">
         <v>644</v>
-      </c>
-      <c r="I173" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="174" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A174" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B174" t="s">
+        <v>645</v>
+      </c>
+      <c r="C174" s="3" t="s">
         <v>646</v>
       </c>
-      <c r="C174" s="3" t="s">
+      <c r="E174" s="9" t="s">
+        <v>800</v>
+      </c>
+      <c r="G174" s="9" t="s">
+        <v>801</v>
+      </c>
+      <c r="P174" t="s">
         <v>647</v>
-      </c>
-      <c r="E174" s="9" t="s">
-        <v>802</v>
-      </c>
-      <c r="G174" s="9" t="s">
-        <v>803</v>
-      </c>
-      <c r="P174" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="175" spans="1:17" s="33" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A175" s="33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B175" s="33" t="s">
+        <v>648</v>
+      </c>
+      <c r="C175" s="34" t="s">
         <v>649</v>
-      </c>
-      <c r="C175" s="34" t="s">
-        <v>650</v>
       </c>
       <c r="D175" s="34"/>
       <c r="E175" s="34"/>
@@ -6309,146 +6309,146 @@
     </row>
     <row r="176" spans="1:17" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A176" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B176" t="s">
+        <v>650</v>
+      </c>
+      <c r="C176" s="3" t="s">
         <v>651</v>
       </c>
-      <c r="C176" s="3" t="s">
-        <v>652</v>
-      </c>
       <c r="E176" s="9" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G176" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="P176" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="177" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A177" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B177" t="s">
+        <v>652</v>
+      </c>
+      <c r="C177" s="3" t="s">
         <v>653</v>
       </c>
-      <c r="C177" s="3" t="s">
-        <v>654</v>
-      </c>
       <c r="E177" s="3" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="G177" s="9" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="P177" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
+        <v>654</v>
+      </c>
+      <c r="B178" t="s">
         <v>655</v>
       </c>
-      <c r="B178" t="s">
+      <c r="C178" s="3" t="s">
         <v>656</v>
       </c>
-      <c r="C178" s="3" t="s">
+      <c r="E178" s="3" t="s">
         <v>657</v>
       </c>
-      <c r="E178" s="3" t="s">
+      <c r="G178" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="L178" t="s">
         <v>658</v>
       </c>
-      <c r="G178" s="9" t="s">
-        <v>808</v>
-      </c>
-      <c r="L178" t="s">
+      <c r="M178" t="s">
         <v>659</v>
       </c>
-      <c r="M178" t="s">
+      <c r="N178" t="s">
+        <v>659</v>
+      </c>
+      <c r="O178" t="s">
+        <v>659</v>
+      </c>
+      <c r="P178" t="s">
         <v>660</v>
-      </c>
-      <c r="N178" t="s">
-        <v>660</v>
-      </c>
-      <c r="O178" t="s">
-        <v>660</v>
-      </c>
-      <c r="P178" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B179" t="s">
+        <v>661</v>
+      </c>
+      <c r="C179" s="3" t="s">
         <v>662</v>
       </c>
-      <c r="C179" s="3" t="s">
+      <c r="E179" s="3" t="s">
+        <v>807</v>
+      </c>
+      <c r="G179" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="L179" t="s">
         <v>663</v>
       </c>
-      <c r="E179" s="3" t="s">
-        <v>809</v>
-      </c>
-      <c r="G179" s="9" t="s">
-        <v>810</v>
-      </c>
-      <c r="L179" t="s">
+      <c r="M179" t="s">
         <v>664</v>
       </c>
-      <c r="M179" t="s">
-        <v>665</v>
-      </c>
       <c r="N179" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="O179" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="P179" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B180" t="s">
+        <v>665</v>
+      </c>
+      <c r="C180" s="3" t="s">
         <v>666</v>
       </c>
-      <c r="C180" s="3" t="s">
+      <c r="E180" s="9" t="s">
+        <v>809</v>
+      </c>
+      <c r="G180" s="9" t="s">
+        <v>810</v>
+      </c>
+      <c r="L180" t="s">
         <v>667</v>
       </c>
-      <c r="E180" s="9" t="s">
-        <v>811</v>
-      </c>
-      <c r="G180" s="9" t="s">
-        <v>812</v>
-      </c>
-      <c r="L180" t="s">
+      <c r="M180" t="s">
         <v>668</v>
       </c>
-      <c r="M180" t="s">
-        <v>669</v>
-      </c>
       <c r="N180" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="O180" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="P180" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="182" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A182" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="8"/>
@@ -6462,135 +6462,135 @@
         <v>148</v>
       </c>
       <c r="B184" t="s">
+        <v>669</v>
+      </c>
+      <c r="C184" s="3" t="s">
         <v>670</v>
       </c>
-      <c r="C184" s="3" t="s">
+      <c r="D184" s="3" t="s">
         <v>671</v>
       </c>
-      <c r="D184" s="3" t="s">
+      <c r="E184" s="3" t="s">
         <v>672</v>
       </c>
-      <c r="E184" s="3" t="s">
+      <c r="F184" s="3" t="s">
         <v>673</v>
       </c>
-      <c r="F184" s="3" t="s">
+      <c r="G184" s="3" t="s">
         <v>674</v>
       </c>
-      <c r="G184" s="3" t="s">
+      <c r="H184" s="3" t="s">
         <v>675</v>
-      </c>
-      <c r="H184" s="3" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="185" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
+        <v>676</v>
+      </c>
+      <c r="B185" t="s">
         <v>677</v>
       </c>
-      <c r="B185" t="s">
+      <c r="C185" s="3" t="s">
         <v>678</v>
       </c>
-      <c r="C185" s="3" t="s">
+      <c r="D185" s="3" t="s">
         <v>679</v>
       </c>
-      <c r="D185" s="3" t="s">
+      <c r="E185" s="3" t="s">
         <v>680</v>
       </c>
-      <c r="E185" s="3" t="s">
+      <c r="F185" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="F185" s="3" t="s">
+      <c r="G185" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="G185" s="3" t="s">
+      <c r="H185" s="3" t="s">
         <v>683</v>
-      </c>
-      <c r="H185" s="3" t="s">
-        <v>684</v>
       </c>
       <c r="J185" t="s">
         <v>226</v>
       </c>
       <c r="P185" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="186" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
+        <v>685</v>
+      </c>
+      <c r="B186" t="s">
         <v>686</v>
       </c>
-      <c r="B186" t="s">
+      <c r="C186" s="3" t="s">
+        <v>678</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>679</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>681</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>682</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>683</v>
+      </c>
+      <c r="P186" t="s">
         <v>687</v>
-      </c>
-      <c r="C186" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="D186" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="E186" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="F186" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="G186" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="H186" s="3" t="s">
-        <v>684</v>
-      </c>
-      <c r="P186" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="187" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
+        <v>688</v>
+      </c>
+      <c r="B187" t="s">
         <v>689</v>
       </c>
-      <c r="B187" t="s">
-        <v>690</v>
-      </c>
       <c r="C187" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E187" s="3" t="s">
+        <v>680</v>
+      </c>
+      <c r="F187" s="3" t="s">
         <v>681</v>
       </c>
-      <c r="F187" s="3" t="s">
+      <c r="G187" s="3" t="s">
         <v>682</v>
       </c>
-      <c r="G187" s="3" t="s">
+      <c r="H187" s="3" t="s">
         <v>683</v>
-      </c>
-      <c r="H187" s="3" t="s">
-        <v>684</v>
       </c>
       <c r="J187" t="s">
         <v>226</v>
       </c>
       <c r="P187" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="188" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A188" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B188" t="s">
+        <v>691</v>
+      </c>
+      <c r="C188" s="3" t="s">
         <v>692</v>
       </c>
-      <c r="C188" s="3" t="s">
+      <c r="E188" s="3" t="s">
         <v>693</v>
       </c>
-      <c r="E188" s="3" t="s">
+      <c r="G188" s="3" t="s">
         <v>694</v>
       </c>
-      <c r="G188" s="3" t="s">
+      <c r="P188" t="s">
         <v>695</v>
-      </c>
-      <c r="P188" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="189" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -6598,16 +6598,16 @@
         <v>227</v>
       </c>
       <c r="B189" t="s">
+        <v>696</v>
+      </c>
+      <c r="C189" s="3" t="s">
         <v>697</v>
       </c>
-      <c r="C189" s="3" t="s">
+      <c r="E189" s="3" t="s">
         <v>698</v>
       </c>
-      <c r="E189" s="3" t="s">
+      <c r="G189" s="3" t="s">
         <v>699</v>
-      </c>
-      <c r="G189" s="3" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6623,21 +6623,21 @@
         <v>218</v>
       </c>
       <c r="B192" t="s">
+        <v>700</v>
+      </c>
+      <c r="I192" t="s">
         <v>701</v>
-      </c>
-      <c r="I192" t="s">
-        <v>702</v>
       </c>
     </row>
     <row r="193" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="33" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B193" s="33" t="s">
+        <v>702</v>
+      </c>
+      <c r="C193" s="34" t="s">
         <v>703</v>
-      </c>
-      <c r="C193" s="34" t="s">
-        <v>704</v>
       </c>
       <c r="D193" s="34"/>
       <c r="E193" s="34"/>
@@ -6650,10 +6650,10 @@
         <v>218</v>
       </c>
       <c r="B194" t="s">
+        <v>704</v>
+      </c>
+      <c r="I194" t="s">
         <v>705</v>
-      </c>
-      <c r="I194" t="s">
-        <v>706</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6661,10 +6661,10 @@
         <v>218</v>
       </c>
       <c r="B195" t="s">
+        <v>706</v>
+      </c>
+      <c r="I195" t="s">
         <v>707</v>
-      </c>
-      <c r="I195" t="s">
-        <v>708</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6672,10 +6672,10 @@
         <v>218</v>
       </c>
       <c r="B196" t="s">
+        <v>708</v>
+      </c>
+      <c r="I196" t="s">
         <v>709</v>
-      </c>
-      <c r="I196" t="s">
-        <v>710</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6683,10 +6683,10 @@
         <v>218</v>
       </c>
       <c r="B197" t="s">
+        <v>710</v>
+      </c>
+      <c r="I197" t="s">
         <v>711</v>
-      </c>
-      <c r="I197" t="s">
-        <v>712</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6694,10 +6694,10 @@
         <v>218</v>
       </c>
       <c r="B198" t="s">
+        <v>712</v>
+      </c>
+      <c r="I198" t="s">
         <v>713</v>
-      </c>
-      <c r="I198" t="s">
-        <v>714</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6705,10 +6705,10 @@
         <v>218</v>
       </c>
       <c r="B199" t="s">
+        <v>714</v>
+      </c>
+      <c r="I199" t="s">
         <v>715</v>
-      </c>
-      <c r="I199" t="s">
-        <v>716</v>
       </c>
     </row>
   </sheetData>
@@ -6722,7 +6722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
@@ -7893,143 +7893,15 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>22</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-    <_dlc_DocId xmlns="359fe316-fab8-49f4-87fa-a9923030124f">Z6MCZFE5NNQT-1373495628-1432</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="359fe316-fab8-49f4-87fa-a9923030124f" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <_dlc_DocIdUrl xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <Url>https://unicef.sharepoint.com/teams/AFG-Nutrition/_layouts/15/DocIdRedir.aspx?ID=Z6MCZFE5NNQT-1373495628-1432</Url>
-      <Description>Z6MCZFE5NNQT-1373495628-1432</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <UserInfo>
-        <DisplayName>Shaista Mehraban</DisplayName>
-        <AccountId>295</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Said M Yaqoob Azimi</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ahmad Nawid Qarizada</DisplayName>
-        <AccountId>206</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Melanie Galvin</DisplayName>
-        <AccountId>304</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970001ED9D7A792C89C46A2A86B92A3D9E4B0" ma:contentTypeVersion="43" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6635fd09095faeb866f46079413f6d37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="359fe316-fab8-49f4-87fa-a9923030124f" xmlns:ns5="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xmlns:ns6="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb5c23aaefc81f3be1817883f8b886f9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8468,14 +8340,142 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>22</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+    <_dlc_DocId xmlns="359fe316-fab8-49f4-87fa-a9923030124f">Z6MCZFE5NNQT-1373495628-1432</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="359fe316-fab8-49f4-87fa-a9923030124f" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <_dlc_DocIdUrl xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <Url>https://unicef.sharepoint.com/teams/AFG-Nutrition/_layouts/15/DocIdRedir.aspx?ID=Z6MCZFE5NNQT-1373495628-1432</Url>
+      <Description>Z6MCZFE5NNQT-1373495628-1432</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <UserInfo>
+        <DisplayName>Shaista Mehraban</DisplayName>
+        <AccountId>295</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Said M Yaqoob Azimi</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ahmad Nawid Qarizada</DisplayName>
+        <AccountId>206</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Melanie Galvin</DisplayName>
+        <AccountId>304</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8484,36 +8484,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="359fe316-fab8-49f4-87fa-a9923030124f"/>
-    <ds:schemaRef ds:uri="117936e8-0f80-4b9a-8a4d-392a13d0dc4e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381EF04D-88DF-4FBB-A10E-8C4034F401AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8536,10 +8514,32 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="359fe316-fab8-49f4-87fa-a9923030124f"/>
+    <ds:schemaRef ds:uri="117936e8-0f80-4b9a-8a4d-392a13d0dc4e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Test with ${name} in Dari
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="109_{F04355A7-C390-4C96-801B-3151D1B62B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F4FD3A49-386F-46B0-97E3-4483312B9189}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="109_{F04355A7-C390-4C96-801B-3151D1B62B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{402F3F4E-E1CD-4FDA-B2E7-FFB6D2D8E11D}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2406,12 +2406,6 @@
     <t>Press "+ "  to add another household member until all members are listed. When listing is complete, continue with the questionnaire.</t>
   </si>
   <si>
-    <t>سن عضو خانواده  {name}$  چقدر است (به اساس سال تکمیل شده)؟</t>
-  </si>
-  <si>
-    <t>د کورنۍ غړي {name}$  (په بشپړو کلونو کې) عمر څومره دی؟</t>
-  </si>
-  <si>
     <t>فقط برای تأیید، شما به {numfamily}$ نفر(ها)/افراد در خانواده را امروز  متذکر شده اید؟</t>
   </si>
   <si>
@@ -2677,6 +2671,12 @@
   </si>
   <si>
     <t>سلام زما نوم دی ________. زه د ________ [سازمان/حکومتي ادارې] سره یم. مهرباني وکړئ اجازه راکړئ تاسو د ټیم نورو غړو ته معرفي کړم: _________ او _______. موږ نن ورځ دلته یو ترڅو د تغذیې او ________ په اړه د کورنۍ معلومات راټول کړو. که چیرې په کورنۍ کې د 5 کلونو څخه کم ماشومان شتون ولري موږ غواړو یو څه اندازه (وزن، قد، MUAC، اذیما / تشریح) په پام کې ونیسو ترڅو د ، د  کلونو څخه کم عمره تغذیه حالت معلومولو کې مرسته وکړي. . مهرباني وکړئ په یاد ولرئ چې اوس مهال معلومه نه ده چې د سروې د پایلو له پای ته رسیدو وروسته به کوم اقدامات (که کوم وي) ترسره شي. ټول معلومات به په بشپړه توګه محرم وساتل شي. ایا تاسو کومه پوښتنه لرئ؟ ایا زه پیل کولی شم؟</t>
+  </si>
+  <si>
+    <t>سن عضو خانواده  ${name}  چقدر است (به اساس سال تکمیل شده)؟</t>
+  </si>
+  <si>
+    <t>د کورنۍ غړي ${name}  (په بشپړو کلونو کې) عمر څومره دی؟</t>
   </si>
 </sst>
 </file>
@@ -3235,8 +3235,8 @@
   <dimension ref="A1:Q199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3495,15 +3495,15 @@
         <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="22" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="23" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="H17" s="11"/>
       <c r="J17" t="s">
@@ -3683,13 +3683,13 @@
         <v>281</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>722</v>
+        <v>811</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>282</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>723</v>
+        <v>812</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>283</v>
@@ -3840,11 +3840,11 @@
         <v>297</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="23" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="H36" s="11"/>
       <c r="P36" t="s">
@@ -3862,7 +3862,7 @@
         <v>299</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>300</v>
@@ -4129,11 +4129,11 @@
         <v>331</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="23" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="H51" s="11"/>
       <c r="P51" t="s">
@@ -4199,13 +4199,13 @@
         <v>338</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>339</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>340</v>
@@ -4225,13 +4225,13 @@
         <v>344</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>345</v>
       </c>
       <c r="G56" s="23" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>346</v>
@@ -4260,13 +4260,13 @@
         <v>352</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>353</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>354</v>
@@ -4331,11 +4331,11 @@
         <v>363</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="28" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="H60" s="11"/>
       <c r="P60" t="s">
@@ -4416,13 +4416,13 @@
         <v>380</v>
       </c>
       <c r="E65" s="9" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>381</v>
       </c>
       <c r="G65" s="9" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="H65" s="3" t="s">
         <v>382</v>
@@ -4451,10 +4451,10 @@
         <v>387</v>
       </c>
       <c r="E66" s="9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="201.6" x14ac:dyDescent="0.55000000000000004">
@@ -4471,13 +4471,13 @@
         <v>390</v>
       </c>
       <c r="E67" s="9" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>391</v>
       </c>
       <c r="G67" s="9" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="H67" s="3" t="s">
         <v>392</v>
@@ -4572,7 +4572,7 @@
         <v>414</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="H71" s="3" t="s">
         <v>415</v>
@@ -4604,10 +4604,10 @@
         <v>420</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -4621,10 +4621,10 @@
         <v>422</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="J73" t="s">
         <v>226</v>
@@ -4937,10 +4937,10 @@
         <v>471</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -4957,13 +4957,13 @@
         <v>338</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>339</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="H100" s="3" t="s">
         <v>474</v>
@@ -4983,13 +4983,13 @@
         <v>344</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>345</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>346</v>
@@ -5018,13 +5018,13 @@
         <v>352</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>480</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>354</v>
@@ -5081,10 +5081,10 @@
         <v>488</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="P105" t="s">
         <v>489</v>
@@ -5101,10 +5101,10 @@
         <v>491</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="P106" t="s">
         <v>492</v>
@@ -5124,13 +5124,13 @@
         <v>380</v>
       </c>
       <c r="E107" s="9" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>381</v>
       </c>
       <c r="G107" s="9" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="H107" s="3" t="s">
         <v>382</v>
@@ -5159,7 +5159,7 @@
         <v>496</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>497</v>
@@ -5188,7 +5188,7 @@
         <v>391</v>
       </c>
       <c r="G109" s="9" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="H109" s="3" t="s">
         <v>392</v>
@@ -5299,10 +5299,10 @@
         <v>518</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="L115" t="s">
         <v>416</v>
@@ -5416,10 +5416,10 @@
         <v>471</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="125" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -5436,13 +5436,13 @@
         <v>338</v>
       </c>
       <c r="E125" s="29" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="F125" s="3" t="s">
         <v>339</v>
       </c>
       <c r="G125" s="9" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>340</v>
@@ -5462,13 +5462,13 @@
         <v>344</v>
       </c>
       <c r="E126" s="29" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="F126" s="3" t="s">
         <v>345</v>
       </c>
       <c r="G126" s="29" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>346</v>
@@ -5497,13 +5497,13 @@
         <v>352</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F127" s="3" t="s">
         <v>353</v>
       </c>
       <c r="G127" s="29" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="H127" s="3" t="s">
         <v>540</v>
@@ -5560,10 +5560,10 @@
         <v>488</v>
       </c>
       <c r="E130" s="29" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="G130" s="29" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="P130" t="s">
         <v>547</v>
@@ -5580,10 +5580,10 @@
         <v>549</v>
       </c>
       <c r="E131" s="30" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G131" s="30" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="P131" t="s">
         <v>550</v>
@@ -5603,13 +5603,13 @@
         <v>380</v>
       </c>
       <c r="E132" s="31" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="F132" s="3" t="s">
         <v>381</v>
       </c>
       <c r="G132" s="32" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="H132" s="3" t="s">
         <v>382</v>
@@ -5638,10 +5638,10 @@
         <v>496</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="P133" t="s">
         <v>553</v>
@@ -5661,13 +5661,13 @@
         <v>390</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="F134" s="3" t="s">
         <v>391</v>
       </c>
       <c r="G134" s="32" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="H134" s="3" t="s">
         <v>555</v>
@@ -5778,10 +5778,10 @@
         <v>518</v>
       </c>
       <c r="E140" s="32" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="L140" t="s">
         <v>416</v>
@@ -5884,11 +5884,11 @@
         <v>584</v>
       </c>
       <c r="E149" s="9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="F149" s="9"/>
       <c r="G149" s="9" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="P149" t="s">
         <v>585</v>
@@ -5908,13 +5908,13 @@
         <v>588</v>
       </c>
       <c r="E150" s="9" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="F150" s="3" t="s">
         <v>589</v>
       </c>
       <c r="G150" s="9" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="H150" s="3" t="s">
         <v>590</v>
@@ -5937,13 +5937,13 @@
         <v>594</v>
       </c>
       <c r="E151" s="9" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="F151" s="3" t="s">
         <v>595</v>
       </c>
       <c r="G151" s="9" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="H151" s="3" t="s">
         <v>596</v>
@@ -5963,10 +5963,10 @@
         <v>598</v>
       </c>
       <c r="E152" s="9" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="G152" s="9" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="P152" t="s">
         <v>599</v>
@@ -5983,10 +5983,10 @@
         <v>601</v>
       </c>
       <c r="E153" s="9" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="G153" s="9" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="P153" t="s">
         <v>599</v>
@@ -6003,10 +6003,10 @@
         <v>603</v>
       </c>
       <c r="E154" s="9" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="G154" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="P154" t="s">
         <v>599</v>
@@ -6060,7 +6060,7 @@
         <v>612</v>
       </c>
       <c r="G158" s="9" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="H158" s="3" t="s">
         <v>613</v>
@@ -6080,10 +6080,10 @@
         <v>616</v>
       </c>
       <c r="E159" s="9" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="G159" s="9" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="P159" t="s">
         <v>614</v>
@@ -6129,10 +6129,10 @@
         <v>626</v>
       </c>
       <c r="E161" s="9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="G161" s="9" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="P161" t="s">
         <v>624</v>
@@ -6282,10 +6282,10 @@
         <v>646</v>
       </c>
       <c r="E174" s="9" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="G174" s="9" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="P174" t="s">
         <v>647</v>
@@ -6318,10 +6318,10 @@
         <v>651</v>
       </c>
       <c r="E176" s="9" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="G176" s="9" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="P176" t="s">
         <v>647</v>
@@ -6338,10 +6338,10 @@
         <v>653</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G177" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="P177" t="s">
         <v>647</v>
@@ -6361,7 +6361,7 @@
         <v>657</v>
       </c>
       <c r="G178" s="9" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="L178" t="s">
         <v>658</v>
@@ -6390,10 +6390,10 @@
         <v>662</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="G179" s="9" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="L179" t="s">
         <v>663</v>
@@ -6422,10 +6422,10 @@
         <v>666</v>
       </c>
       <c r="E180" s="9" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="G180" s="9" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="L180" t="s">
         <v>667</v>
@@ -7893,15 +7893,143 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>22</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+    <_dlc_DocId xmlns="359fe316-fab8-49f4-87fa-a9923030124f">Z6MCZFE5NNQT-1373495628-1432</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="359fe316-fab8-49f4-87fa-a9923030124f" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <_dlc_DocIdUrl xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <Url>https://unicef.sharepoint.com/teams/AFG-Nutrition/_layouts/15/DocIdRedir.aspx?ID=Z6MCZFE5NNQT-1373495628-1432</Url>
+      <Description>Z6MCZFE5NNQT-1373495628-1432</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <UserInfo>
+        <DisplayName>Shaista Mehraban</DisplayName>
+        <AccountId>295</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Said M Yaqoob Azimi</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ahmad Nawid Qarizada</DisplayName>
+        <AccountId>206</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Melanie Galvin</DisplayName>
+        <AccountId>304</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970001ED9D7A792C89C46A2A86B92A3D9E4B0" ma:contentTypeVersion="43" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6635fd09095faeb866f46079413f6d37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="359fe316-fab8-49f4-87fa-a9923030124f" xmlns:ns5="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xmlns:ns6="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb5c23aaefc81f3be1817883f8b886f9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8340,142 +8468,14 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>22</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-    <_dlc_DocId xmlns="359fe316-fab8-49f4-87fa-a9923030124f">Z6MCZFE5NNQT-1373495628-1432</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="359fe316-fab8-49f4-87fa-a9923030124f" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <_dlc_DocIdUrl xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <Url>https://unicef.sharepoint.com/teams/AFG-Nutrition/_layouts/15/DocIdRedir.aspx?ID=Z6MCZFE5NNQT-1373495628-1432</Url>
-      <Description>Z6MCZFE5NNQT-1373495628-1432</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <UserInfo>
-        <DisplayName>Shaista Mehraban</DisplayName>
-        <AccountId>295</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Said M Yaqoob Azimi</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ahmad Nawid Qarizada</DisplayName>
-        <AccountId>206</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Melanie Galvin</DisplayName>
-        <AccountId>304</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8484,14 +8484,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="359fe316-fab8-49f4-87fa-a9923030124f"/>
+    <ds:schemaRef ds:uri="117936e8-0f80-4b9a-8a4d-392a13d0dc4e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381EF04D-88DF-4FBB-A10E-8C4034F401AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8514,32 +8536,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="359fe316-fab8-49f4-87fa-a9923030124f"/>
-    <ds:schemaRef ds:uri="117936e8-0f80-4b9a-8a4d-392a13d0dc4e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
corrected {name}$ to arabic style
</commit_message>
<xml_diff>
--- a/ACO_SMART_Survey_2021.xlsx
+++ b/ACO_SMART_Survey_2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unicef-my.sharepoint.com/personal/rojohnston_unicef_org1/Documents/1 UNICEF Work/1 Afghanistan/Surveys/UrbanSMART/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="109_{F04355A7-C390-4C96-801B-3151D1B62B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{402F3F4E-E1CD-4FDA-B2E7-FFB6D2D8E11D}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="109_{F04355A7-C390-4C96-801B-3151D1B62B2A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{25FD0BA1-F859-41F5-8C75-1FD431F5AAF5}"/>
   <bookViews>
     <workbookView xWindow="12180" yWindow="-11640" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="811">
   <si>
     <t>list_name</t>
   </si>
@@ -1136,12 +1136,6 @@
     <t>${child_name}- is ${MONTHS} months old.</t>
   </si>
   <si>
-    <t>${child_name}- ${MONTHS} ماه عمر دار..</t>
-  </si>
-  <si>
-    <t>${child_name}- د ${MONTHS} میاشتې عمر لري.</t>
-  </si>
-  <si>
     <t>${MONTHS} &lt; 98</t>
   </si>
   <si>
@@ -1272,9 +1266,6 @@
   </si>
   <si>
     <t xml:space="preserve">Please measure MUAC on the left arm of the child. Position yourself on the right of the child/caregiver. Take measure at the mid-point between the tips of the shoulder and elbow.  Please record measure in MM. </t>
-  </si>
-  <si>
-    <t>MUAC در میلی متر از ${child_name}</t>
   </si>
   <si>
     <t>لطفا MUAC را در بازوی چپ کودک اندازه گیری کنید. خود را در سمت راست کودک/مراقب قرار دهید. اندازه را در نقطه وسط بین نوک شانه و آرنج بگیرید. لطفا اندازه گیری را در میلی متر ثبت کنید.</t>
@@ -2073,9 +2064,6 @@
     <t>COMPLETE REFERRAL FORM to the SAM TREATMENT PROGRAM</t>
   </si>
   <si>
-    <t>${child_name}- دارای سوء تغذیه حاد شدید (SAM).</t>
-  </si>
-  <si>
     <t>فرم ارجاع به برنامه SAM TREATMENT را تکمیل کنید</t>
   </si>
   <si>
@@ -2100,15 +2088,9 @@
     <t>COMPLETE REFERRAL FORM to the MAM TREATMENT PROGRAM</t>
   </si>
   <si>
-    <t>${child_name}- دارای سوء تغذیه حاد متوسط ​​(MAM) است.</t>
-  </si>
-  <si>
     <t>فرم ارجاع  به برنامه MAM TREATMENT را تکمیل کنید</t>
   </si>
   <si>
-    <t>${child_name}- متوسط حاد خوارځواکي (MAM) لري.</t>
-  </si>
-  <si>
     <t>د MAM درملنې پروګرام ته د راجع کولو فورمه ډکه کړئ</t>
   </si>
   <si>
@@ -2211,9 +2193,6 @@
     <t>Woman's MUAC in MM of ${wom_name}</t>
   </si>
   <si>
-    <t>MUAC زن در میلی متر از ${wom_name}</t>
-  </si>
-  <si>
     <t xml:space="preserve">(. &gt;= 90 and . &lt;650) </t>
   </si>
   <si>
@@ -2406,267 +2385,12 @@
     <t>Press "+ "  to add another household member until all members are listed. When listing is complete, continue with the questionnaire.</t>
   </si>
   <si>
-    <t>فقط برای تأیید، شما به {numfamily}$ نفر(ها)/افراد در خانواده را امروز  متذکر شده اید؟</t>
-  </si>
-  <si>
-    <t>یوازې د تایید لپاره، تاسو نن ورځ په کورنۍ کې {numfamily}$ کس/خلک ذکر کړي دي؟</t>
-  </si>
-  <si>
     <t>Hello my name is ________.   I am with ________ [organization/governmental agency]. Please let me introduce you to the other team members: _________ .   We are here today to gather information about nutrition.  If there are any children under 5 or pregnant/lactating women in the household we would like to take some measurements (weight, height, MUAC, oedema / explain) to  determine nutrition conditions in the province.  Please note that it is not currently known what actions will be taken when the survey is complete. All information will be kept completely confidential.  Do you have any questions? May I begin?</t>
   </si>
   <si>
     <t>If the reported number does not match the total, please return to the household listing and correct the household member information. To delete one person, press "-" in the box with the person's details , then select "CONFIRM" to delete the person from the household.</t>
   </si>
   <si>
-    <t>اکنون معلومات فرزند را وارد کنید: {child_name} : ${CHSEX}$ با سن به سال: {child_age_years}$</t>
-  </si>
-  <si>
-    <t>آیا سند رسمی سن برای {child_name}$ دارید؟</t>
-  </si>
-  <si>
-    <t>ایا تاسو د {child_name}$ لپاره د عمر رسمي اسناد لرئ؟</t>
-  </si>
-  <si>
-    <t>تاریخ تولد {child_name}$:</t>
-  </si>
-  <si>
-    <t>د {child_name}$ د زیږون نیټه:</t>
-  </si>
-  <si>
-    <t>اوس د ماشوم معلومات داخل کړئ    {child_name} - ${CHSEX}$ عمر: {child_age_years}$</t>
-  </si>
-  <si>
-    <t>سن {child_name}$ در ماه های تکمیل شده:</t>
-  </si>
-  <si>
-    <t>په بشپړو میاشتو کې د {child_name}$ عمر:</t>
-  </si>
-  <si>
-    <t>سن {child_name}$ نامشخص است.</t>
-  </si>
-  <si>
-    <t>د {child_name}$ عمر معلوم نه دی.</t>
-  </si>
-  <si>
-    <t>وزن به کیلوگرم {child_name}$:</t>
-  </si>
-  <si>
-    <t>وزن په کیلوګرام کې {child_name}$:</t>
-  </si>
-  <si>
-    <t>آیا {child_name}$ برای اندازه گیری وزن لباس پوشیده بود؟</t>
-  </si>
-  <si>
-    <t>آیا {child_name}$ د وزن اندازه کولو لپاره جامې اغوستې وې؟</t>
-  </si>
-  <si>
-    <t>قد در سانتی متر {child_name}$:</t>
-  </si>
-  <si>
-    <t>لوړوالی په سانتي مترو کې {child_name}$:</t>
-  </si>
-  <si>
-    <t>MUAC په ملی مترو کې له ${child_name} څخه</t>
-  </si>
-  <si>
-    <t>آیا {child_name}$ اذیما دو طرفه دارد، یعنی تورم همراه با اذیماحفره‌ای در هر دو پا؟</t>
-  </si>
-  <si>
-    <t>ایا {child_name}$ دوه اړخیزه اذیما لري، چې په دواړو پښو کې پړسوب لري؟</t>
-  </si>
-  <si>
-    <t>لطفا با سرپرست تیم تایید کنید. آیا {child_name}$ اذیما دوطرفه دارد؟</t>
-  </si>
-  <si>
-    <t>مهرباني وکړئ د ټیم مشر سره تایید کړئ. ایا {child_name}$ دوه اړخیزه اذیما لري؟</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: وارد کردن معلومات برای کودک: {child_name} - ${CHSEX}$ با سن به سال: {child_age_years}$ باید دوباره اندازه‌گیری شود</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: د ماشوم لپاره د معلوماتو داخلول: {child_name} - ${CHSEX}$  په کلونو کې د عمر سره: {child_age_years}$ باید بیا اندازه شي</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد:آیا مدارک رسمی سن برای {child_name}$ دارید؟</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول:  ایا تاسو د {child_name}$ لپاره د عمر رسمي اسناد لرئ؟</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: تاریخ تولد {child_name}$:</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: {child_name}$ د زیږون نیټه</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: سن {child_name}$ در ماه های تکمیل شده:</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: په بشپړو میاشتو کې د {child_name}$ عمر:</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد:سن {child_name}$ نامشخص است.</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول:  د {child_name}$ عمر معلوم نه دی.</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: {child_name}$ د {MONTHS_2}$  میاشتې زوړ دی.</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: {child_name}$ د {MONTHS_2}$ ماهه است.</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: وزن به کیلوگرم {child_name}$ :</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: د کیلو ګرامه وزن کې {child_name}$ :</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: آیا {child_name}$ برای اندازه گیری وزن لباس پوشیده بود؟</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: د {child_name}$ په سانتی متر کې لوړوالی:</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: MUAC به میلی متر از {child name}$</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: MUAC په میلی متر کې {child name}$</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: وارد کردن داده ها برای فرزند  {child_name} : ${CHSEX}$  با سن به سال: {child_age_years}$ باید دوباره اندازه گیری شود</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: د ماشوم لپاره د معلوماتو داخلول : {child_name} : ${CHSEX}$ په کلونو کې د عمر سره: {child_age_years}$ باید بیا اندازه شي</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد:  آیا سند رسمی سن برای {child_name}$ دارید؟</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: ایا تاسو د {child_name}$ لپاره د عمر رسمي اسناد لرئ؟</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد:  تاریخ تولد {child_name}$:</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: {child_name}$ د زیږون نیټه:</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد:  سن {child_name}$  در ماه های تکمیل شده:</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: سن {child_name}$ نامشخص است.</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: د {child_name}$ عمر معلوم نه دی.</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد:  {child_name} : ${MONTHS_3}$  ماهه است.</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: د  {child_name}  :  ${MONTHS_3}$  میاشتې عمر لري.</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول:  وزن  په  کیلو ګرامه کې {child_name}$ :</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول:  آیا {child_name}$ د وزن اندازه کولو لپاره جامې اغوستې وې؟</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: قد {child_name}$ بر حسب سانتی متر:</t>
-  </si>
-  <si>
-    <t>اندازه گیری مجدد: MUAC در میلی متر از {child_name}$</t>
-  </si>
-  <si>
-    <t>بیا اندازه کول: MUAC د  {child_name}$ په میلی متر کې</t>
-  </si>
-  <si>
-    <t>آیا کودک {child name}$ در حال حاضر با شیر مادر تغذیه میشود ؟</t>
-  </si>
-  <si>
-    <t>ایا  {child name}$ اوس مهال د مور شیدې ورکوي؟</t>
-  </si>
-  <si>
-    <t>آیا کودک {child_name}$ ویتامین A در 6 ماه گذشته دریافت کرده است؟</t>
-  </si>
-  <si>
-    <t>آیا ماشوم {child_name}$ په تیرو شپږو میاشتو کې ویټامین A ترلاسه کړی؟</t>
-  </si>
-  <si>
-    <t>آیا کودک {child_name}$ واکسن سرخکان دریافت کرده است؟</t>
-  </si>
-  <si>
-    <t>آیا ماشوم {child_name}$ د شری واکسین اخیستی دی؟</t>
-  </si>
-  <si>
-    <t>آیا کودک {child_name}$ در ۲ هفته گذشته اسهال داشته است؟</t>
-  </si>
-  <si>
-    <t>آیا ماشوم {child_name}$ په تیرو 2 اونیو کې اسهال درلود؟</t>
-  </si>
-  <si>
-    <t>آیا کودک {child_name}$  در ۲ هفته گذشته سرفه همراه با تنفس سریع داشته است؟</t>
-  </si>
-  <si>
-    <t>آیا ماشوم  {child_name}$ په تیرو 2 اونیو کې د چټک تنفس سره ټوخی درلوده؟</t>
-  </si>
-  <si>
-    <t>آیا کودک  {child_name}$ در ۲ هفته گذشته تب داشته است؟</t>
-  </si>
-  <si>
-    <t>آیا ماشوم {child_name}$ په تیرو 2 اونیو کې تبه درلوده؟</t>
-  </si>
-  <si>
-    <t>${child_name} - سخت خوارځواکۍ (SAM) لري.</t>
-  </si>
-  <si>
-    <t>آیا  {child_name}$ را برای مدیریت خدمات سوء تغذیه حاد شدید معرفی کرده اید؟</t>
-  </si>
-  <si>
-    <t>ایا تاسو د شدید خوارځواکۍ خدماتو مدیریت لپاره  {child_name}$ راجع کړی ده؟</t>
-  </si>
-  <si>
-    <t>آیا شما {child_name}$ را برای مدیریت خدمات سوء تغذیه حاد متوسط ​​معرفی کرده اید؟</t>
-  </si>
-  <si>
-    <t>آیا تاسو د متوسط ​​حاد خوارځواکۍ خدماتو مدیریت لپاره  {child_name}$ راجع کړی؟</t>
-  </si>
-  <si>
-    <t>اکنون اطلاعات مربوط به زنان را وارد کنید: :  {wom_name}$ با سن  {wom_age_years}$ سال</t>
-  </si>
-  <si>
-    <t>اوس د میرمنو لپاره معلومات داخلول:  {wom_name}$ د  {wom_age_years}$ کلونو په عمر</t>
-  </si>
-  <si>
-    <t>آیا عضو خانواده  {wom_name}$ در حال حاضر باردار است؟</t>
-  </si>
-  <si>
-    <t>ایا د کورنۍ غړې  {wom_name}$ اوس مهال حامله ده؟</t>
-  </si>
-  <si>
-    <t>آیا عضو خانواده  {wom_name}$ در حال حاضر شیر می دهد؟</t>
-  </si>
-  <si>
-    <t>ایا د کورنۍ غړی  {wom_name}$ اوس مهال شیدې ورکوي؟</t>
-  </si>
-  <si>
-    <t>د ښځې MUAC د  {wom_name}$ په میلی متر کې</t>
-  </si>
-  <si>
-    <t>قد زن در سانتی متر  {wom_name}$</t>
-  </si>
-  <si>
-    <t>د ښځې لوړوالی د   {wom_name}$ په سانتی متر کې</t>
-  </si>
-  <si>
-    <t>وزن زن به کیلوگرم  {wom_name}$</t>
-  </si>
-  <si>
-    <t>د ښځې وزن {wom_name}$ کیلوګرام کې</t>
-  </si>
-  <si>
     <t>سلام اسم من است ________. من با ________ [سازمان/سازمان دولتی] هستم. لطفا اجازه دهید شما را به سایر اعضای تیم معرفی کنم: _________ و _______. ما امروز اینجا هستیم تا اطلاعات خانوار مربوط به تغذیه و ________ را جمع آوری کنیم. اگر کودک زیر 5 سال در خانواده وجود دارد، مایلیم اندازه گیری هایی (وزن، قد، MUAC، oedema / توضیح دهید) برای کمک به تعیین وضعیت کلی تغذیه زیر 5 سال در . . لطفاً توجه داشته باشید که در حال حاضر مشخص نیست که پس از نهایی شدن نتایج نظرسنجی چه اقداماتی (در صورت وجود) انجام خواهد شد. تمامی اطلاعات کاملاً محرمانه خواهد بود. آیا سوالی دارید؟ می توانم شروع کنم؟</t>
   </si>
   <si>
@@ -2677,6 +2401,276 @@
   </si>
   <si>
     <t>د کورنۍ غړي ${name}  (په بشپړو کلونو کې) عمر څومره دی؟</t>
+  </si>
+  <si>
+    <t>اوس د ماشوم معلومات داخل کړئ: $ {child_name} ($ {CHSEX}) عمر: $ {child_age_years}</t>
+  </si>
+  <si>
+    <t>آیا سند رسمی سن برای ${child_name} دارید؟</t>
+  </si>
+  <si>
+    <t>ایا تاسو د ${child_name} لپاره د عمر رسمي اسناد لرئ؟</t>
+  </si>
+  <si>
+    <t>تاریخ تولد ${child_name}:</t>
+  </si>
+  <si>
+    <t>د ${child_name} د زیږون نیټه:</t>
+  </si>
+  <si>
+    <t>سن ${child_name} در ماه های تکمیل شده:</t>
+  </si>
+  <si>
+    <t>په بشپړو میاشتو کې د ${child_name} عمر:</t>
+  </si>
+  <si>
+    <t>سن ${child_name} نامشخص است.</t>
+  </si>
+  <si>
+    <t>د ${child_name} عمر معلوم نه دی.</t>
+  </si>
+  <si>
+    <t>وزن به کیلوگرم ${child_name}:</t>
+  </si>
+  <si>
+    <t>وزن په کیلوګرام کې ${child_name}:</t>
+  </si>
+  <si>
+    <t>آیا ${child_name} برای اندازه گیری وزن لباس پوشیده بود؟</t>
+  </si>
+  <si>
+    <t>آیا ${child_name} د وزن اندازه کولو لپاره جامې اغوستې وې؟</t>
+  </si>
+  <si>
+    <t>قد در سانتی متر ${child_name}:</t>
+  </si>
+  <si>
+    <t>لوړوالی په سانتي مترو کې $ {child_name}:</t>
+  </si>
+  <si>
+    <t>آیا ${child_name} اذیما دو طرفه دارد، یعنی تورم همراه با اذیماحفره‌ای در هر دو پا؟</t>
+  </si>
+  <si>
+    <t>ایا ${child_name} دوه اړخیزه اذیما لري، چې په دواړو پښو کې پړسوب لري؟</t>
+  </si>
+  <si>
+    <t>لطفا با سرپرست تیم تایید کنید. آیا ${child_name} اذیما دوطرفه دارد؟</t>
+  </si>
+  <si>
+    <t>مهرباني وکړئ د ټیم مشر سره تایید کړئ. ایا ${child_name} دوه اړخیزه اذیما لري؟</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول:  ایا تاسو د ${child_name} لپاره د عمر رسمي اسناد لرئ؟</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: تاریخ تولد ${child_name}:</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: ${child_name} د زیږون نیټه</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: سن ${child_name} در ماه های تکمیل شده:</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: په بشپړو میاشتو کې د ${child_name} عمر:</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد:سن ${child_name} نامشخص است.</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول:  د ${child_name} عمر معلوم نه دی.</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: ${child_name} د ${MONTHS_2} میاشتې زوړ دی.</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: وزن به کیلوگرم ${child_name}:</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: د کیلو ګرامه وزن کې ${child_name}:</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: آیا ${child_name} برای اندازه گیری وزن لباس پوشیده بود؟</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: د ${child_name} په سانتی متر کې لوړوالی:</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: MUAC به میلی متر از ${child name}</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: MUAC په میلی متر کې ${child name}</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد:  آیا سند رسمی سن برای ${child_name} دارید؟</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: ایا تاسو د ${child_name} لپاره د عمر رسمي اسناد لرئ؟</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد:  تاریخ تولد ${child_name}:</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: ${child_name} د زیږون نیټه:</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد:  سن ${child_name} در ماه های تکمیل شده:</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: سن ${child_name} نامشخص است.</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: د ${child_name} عمر معلوم نه دی.</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول:  وزن  په  کیلو ګرامه کې ${child_name}:</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول:  آیا ${child_name} د وزن اندازه کولو لپاره جامې اغوستې وې؟</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: MUAC در میلی متر از ${child_name}</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: MUAC د ${child_name} په میلی متر کې</t>
+  </si>
+  <si>
+    <t>آیا کودک ${child name} در حال حاضر با شیر مادر تغذیه میشود ؟</t>
+  </si>
+  <si>
+    <t>آیا کودک ${child_name} ویتامین A در 6 ماه گذشته دریافت کرده است؟</t>
+  </si>
+  <si>
+    <t>آیا ماشوم ${child_name} په تیرو شپږو میاشتو کې ویټامین A ترلاسه کړی؟</t>
+  </si>
+  <si>
+    <t>آیا کودک ${child_name} واکسن سرخکان دریافت کرده است؟</t>
+  </si>
+  <si>
+    <t>آیا ماشوم ${child_name} د شری واکسین اخیستی دی؟</t>
+  </si>
+  <si>
+    <t>آیا کودک ${child_name} در ۲ هفته گذشته اسهال داشته است؟</t>
+  </si>
+  <si>
+    <t>آیا ماشوم ${child_name} په تیرو 2 اونیو کې اسهال درلود؟</t>
+  </si>
+  <si>
+    <t>آیا کودک ${child_name} در ۲ هفته گذشته سرفه همراه با تنفس سریع داشته است؟</t>
+  </si>
+  <si>
+    <t>آیا ماشوم ${child_name} په تیرو 2 اونیو کې د چټک تنفس سره ټوخی درلوده؟</t>
+  </si>
+  <si>
+    <t>آیا کودک ${child_name} در ۲ هفته گذشته تب داشته است؟</t>
+  </si>
+  <si>
+    <t>آیا ماشوم ${child_name} په تیرو 2 اونیو کې تبه درلوده؟</t>
+  </si>
+  <si>
+    <t>آیا ${child_name} را برای مدیریت خدمات سوء تغذیه حاد شدید معرفی کرده اید؟</t>
+  </si>
+  <si>
+    <t>ایا تاسو د شدید خوارځواکۍ خدماتو مدیریت لپاره ${child_name} راجع کړی ده؟</t>
+  </si>
+  <si>
+    <t>آیا شما ${child_name} را برای مدیریت خدمات سوء تغذیه حاد متوسط ​​معرفی کرده اید؟</t>
+  </si>
+  <si>
+    <t>آیا تاسو د متوسط ​​حاد خوارځواکۍ خدماتو مدیریت لپاره ${child_name} راجع کړی؟</t>
+  </si>
+  <si>
+    <t>اکنون اطلاعات مربوط به زنان را وارد کنید: : ${wom_name} با سن ${wom_age_years} سال</t>
+  </si>
+  <si>
+    <t>اوس د میرمنو لپاره معلومات داخلول: ${wom_name} د ${wom_age_years} کلونو په عمر</t>
+  </si>
+  <si>
+    <t>آیا عضو خانواده ${wom_name} در حال حاضر باردار است؟</t>
+  </si>
+  <si>
+    <t>ایا د کورنۍ غړې ${wom_name} اوس مهال حامله ده؟</t>
+  </si>
+  <si>
+    <t>آیا عضو خانواده ${wom_name} در حال حاضر شیر می دهد؟</t>
+  </si>
+  <si>
+    <t>ایا د کورنۍ غړی ${wom_name} اوس مهال شیدې ورکوي؟</t>
+  </si>
+  <si>
+    <t>د ښځې MUAC د ${wom_name} په میلی متر کې</t>
+  </si>
+  <si>
+    <t>قد زن در سانتی متر ${wom_name}</t>
+  </si>
+  <si>
+    <t>د ښځې لوړوالی د ${wom_name} په سانتی متر کې</t>
+  </si>
+  <si>
+    <t>وزن زن به کیلوگرم ${wom_name}</t>
+  </si>
+  <si>
+    <t>فقط برای تأیید، شما به ${numfamily} نفر(ها)/افراد در خانواده را امروز  متذکر شده اید؟</t>
+  </si>
+  <si>
+    <t>یوازې د تایید لپاره، تاسو نن ورځ په کورنۍ کې ${numfamily} کس/خلک ذکر کړي دي؟</t>
+  </si>
+  <si>
+    <t>اکنون معلومات فرزند را وارد کنید: ${child_name}$ : {CHSEX}  با سن به سال: ${child_age_years}</t>
+  </si>
+  <si>
+    <t>{child_name}$ : {MONTHS}$ ماه عمر دار..</t>
+  </si>
+  <si>
+    <t>{child_name}$ : د {MONTHS}$ میاشتې عمر لري.</t>
+  </si>
+  <si>
+    <t>MUAC در میلی متر از {child_name}$</t>
+  </si>
+  <si>
+    <t>MUAC په ملی مترو کې له  {child_name}$ څخه</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: وارد کردن معلومات برای کودک: ${child_name}$ : {CHSEX} با سن به سال:  ${child_age_years} باید دوباره اندازه‌گیری شود</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: د ماشوم لپاره د معلوماتو داخلول: ${child_name}$ : {CHSEX} په کلونو کې د عمر سره: ${child_age_years} باید بیا اندازه شي</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد:آیا مدارک رسمی سن برای ${child_name} دارید؟</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: ${child_name}$ {MONTHS_2} ماهه است.</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: وارد کردن داده ها برای فرزند: ${child_name}$ :  {CHSEX}  با سن به سال: ${child_age_years} باید دوباره اندازه گیری شود</t>
+  </si>
+  <si>
+    <t>بیا اندازه کول: د ${child_name}$ : {MONTHS_3} میاشتې عمر لري.</t>
+  </si>
+  <si>
+    <t>اندازه گیری مجدد: ${child_name}$ : {MONTHS_3} ماهه است.</t>
+  </si>
+  <si>
+    <t>ایا ${child name} اوس مهال د مور شیدې ورکوي؟</t>
+  </si>
+  <si>
+    <t>{child_name}$ - سخت خوارځواکۍ (SAM) لري.</t>
+  </si>
+  <si>
+    <t>{child_name}$ - متوسط حاد خوارځواکي (MAM) لري.</t>
+  </si>
+  <si>
+    <t>{child_name}$ - دارای سوء تغذیه حاد شدید (SAM).</t>
+  </si>
+  <si>
+    <t>{child_name}$ - دارای سوء تغذیه حاد متوسط ​​(MAM) است.</t>
+  </si>
+  <si>
+    <t>MUAC زن در میلی متر از {wom_name}$</t>
+  </si>
+  <si>
+    <t>د ښځې وزن ${wom_name}  کیلوګرام کې</t>
   </si>
 </sst>
 </file>
@@ -3235,8 +3229,8 @@
   <dimension ref="A1:Q199"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G204" sqref="G204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3292,10 +3286,10 @@
         <v>212</v>
       </c>
       <c r="N1" t="s">
-        <v>716</v>
+        <v>709</v>
       </c>
       <c r="O1" t="s">
-        <v>717</v>
+        <v>710</v>
       </c>
       <c r="P1" t="s">
         <v>213</v>
@@ -3414,7 +3408,7 @@
         <v>226</v>
       </c>
       <c r="L10" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3437,7 +3431,7 @@
         <v>226</v>
       </c>
       <c r="L11" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.55000000000000004">
@@ -3460,7 +3454,7 @@
         <v>226</v>
       </c>
       <c r="L12" t="s">
-        <v>718</v>
+        <v>711</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -3495,15 +3489,15 @@
         <v>16</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>724</v>
+        <v>715</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="22" t="s">
-        <v>809</v>
+        <v>717</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17" s="23" t="s">
-        <v>810</v>
+        <v>718</v>
       </c>
       <c r="H17" s="11"/>
       <c r="J17" t="s">
@@ -3558,13 +3552,13 @@
         <v>259</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>721</v>
+        <v>714</v>
       </c>
       <c r="E20" s="25" t="s">
         <v>260</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>720</v>
+        <v>713</v>
       </c>
       <c r="G20" s="26" t="s">
         <v>261</v>
@@ -3683,13 +3677,13 @@
         <v>281</v>
       </c>
       <c r="E26" s="22" t="s">
-        <v>811</v>
+        <v>719</v>
       </c>
       <c r="F26" s="10" t="s">
         <v>282</v>
       </c>
       <c r="G26" s="23" t="s">
-        <v>812</v>
+        <v>720</v>
       </c>
       <c r="H26" s="12" t="s">
         <v>283</v>
@@ -3698,13 +3692,13 @@
         <v>284</v>
       </c>
       <c r="M26" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="N26" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
       <c r="O26" t="s">
-        <v>719</v>
+        <v>712</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -3840,11 +3834,11 @@
         <v>297</v>
       </c>
       <c r="E36" s="22" t="s">
-        <v>722</v>
+        <v>790</v>
       </c>
       <c r="F36" s="11"/>
       <c r="G36" s="23" t="s">
-        <v>723</v>
+        <v>791</v>
       </c>
       <c r="H36" s="11"/>
       <c r="P36" t="s">
@@ -3862,7 +3856,7 @@
         <v>299</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>725</v>
+        <v>716</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>300</v>
@@ -4129,11 +4123,11 @@
         <v>331</v>
       </c>
       <c r="E51" s="22" t="s">
-        <v>726</v>
+        <v>792</v>
       </c>
       <c r="F51" s="11"/>
       <c r="G51" s="23" t="s">
-        <v>731</v>
+        <v>721</v>
       </c>
       <c r="H51" s="11"/>
       <c r="P51" t="s">
@@ -4199,13 +4193,13 @@
         <v>338</v>
       </c>
       <c r="E55" s="27" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="F55" s="10" t="s">
         <v>339</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="H55" s="12" t="s">
         <v>340</v>
@@ -4225,13 +4219,13 @@
         <v>344</v>
       </c>
       <c r="E56" s="27" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="F56" s="10" t="s">
         <v>345</v>
       </c>
       <c r="G56" s="23" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>346</v>
@@ -4260,13 +4254,13 @@
         <v>352</v>
       </c>
       <c r="E57" s="27" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="F57" s="10" t="s">
         <v>353</v>
       </c>
       <c r="G57" s="23" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>354</v>
@@ -4331,11 +4325,11 @@
         <v>363</v>
       </c>
       <c r="E60" s="27" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="F60" s="11"/>
       <c r="G60" s="28" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="H60" s="11"/>
       <c r="P60" t="s">
@@ -4353,15 +4347,15 @@
         <v>366</v>
       </c>
       <c r="E61" s="19" t="s">
-        <v>367</v>
+        <v>793</v>
       </c>
       <c r="F61" s="11"/>
       <c r="G61" s="20" t="s">
-        <v>368</v>
+        <v>794</v>
       </c>
       <c r="H61" s="11"/>
       <c r="P61" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4369,21 +4363,21 @@
         <v>218</v>
       </c>
       <c r="B62" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="I62" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="63" spans="1:16" s="33" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="33" t="s">
+        <v>370</v>
+      </c>
+      <c r="B63" s="33" t="s">
+        <v>371</v>
+      </c>
+      <c r="C63" s="34" t="s">
         <v>372</v>
-      </c>
-      <c r="B63" s="33" t="s">
-        <v>373</v>
-      </c>
-      <c r="C63" s="34" t="s">
-        <v>374</v>
       </c>
       <c r="D63" s="34"/>
       <c r="E63" s="34"/>
@@ -4396,120 +4390,120 @@
         <v>231</v>
       </c>
       <c r="B64" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="P64" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="65" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
+        <v>375</v>
+      </c>
+      <c r="B65" t="s">
+        <v>376</v>
+      </c>
+      <c r="C65" s="3" t="s">
         <v>377</v>
       </c>
-      <c r="B65" t="s">
+      <c r="D65" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="C65" s="3" t="s">
+      <c r="E65" s="9" t="s">
+        <v>730</v>
+      </c>
+      <c r="F65" s="3" t="s">
         <v>379</v>
       </c>
-      <c r="D65" s="3" t="s">
+      <c r="G65" s="9" t="s">
+        <v>731</v>
+      </c>
+      <c r="H65" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="E65" s="9" t="s">
-        <v>736</v>
-      </c>
-      <c r="F65" s="3" t="s">
+      <c r="L65" t="s">
         <v>381</v>
       </c>
-      <c r="G65" s="9" t="s">
-        <v>737</v>
-      </c>
-      <c r="H65" s="3" t="s">
+      <c r="M65" t="s">
         <v>382</v>
       </c>
-      <c r="L65" t="s">
-        <v>383</v>
-      </c>
-      <c r="M65" t="s">
-        <v>384</v>
-      </c>
       <c r="N65" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O65" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="66" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
+        <v>383</v>
+      </c>
+      <c r="B66" t="s">
+        <v>384</v>
+      </c>
+      <c r="C66" s="3" t="s">
         <v>385</v>
       </c>
-      <c r="B66" t="s">
-        <v>386</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>387</v>
-      </c>
       <c r="E66" s="9" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="G66" s="9" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
     </row>
     <row r="67" spans="1:16" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B67" t="s">
+        <v>386</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D67" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="C67" s="3" t="s">
+      <c r="E67" s="9" t="s">
+        <v>734</v>
+      </c>
+      <c r="F67" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="G67" s="9" t="s">
+        <v>735</v>
+      </c>
+      <c r="H67" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="E67" s="9" t="s">
-        <v>740</v>
-      </c>
-      <c r="F67" s="3" t="s">
+      <c r="L67" t="s">
         <v>391</v>
       </c>
-      <c r="G67" s="9" t="s">
-        <v>741</v>
-      </c>
-      <c r="H67" s="3" t="s">
+      <c r="M67" t="s">
         <v>392</v>
       </c>
-      <c r="L67" t="s">
-        <v>393</v>
-      </c>
-      <c r="M67" t="s">
-        <v>394</v>
-      </c>
       <c r="N67" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="O67" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
+        <v>393</v>
+      </c>
+      <c r="B68" t="s">
+        <v>394</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="B68" t="s">
+      <c r="E68" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>397</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>399</v>
       </c>
     </row>
     <row r="69" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -4517,19 +4511,19 @@
         <v>251</v>
       </c>
       <c r="B69" t="s">
+        <v>398</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="E69" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="C69" s="3" t="s">
+      <c r="G69" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="P69" t="s">
         <v>402</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="P69" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="70" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -4537,19 +4531,19 @@
         <v>251</v>
       </c>
       <c r="B70" t="s">
+        <v>403</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="E70" s="3" t="s">
         <v>405</v>
       </c>
-      <c r="C70" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="P70" t="s">
         <v>407</v>
-      </c>
-      <c r="G70" s="3" t="s">
-        <v>408</v>
-      </c>
-      <c r="P70" t="s">
-        <v>409</v>
       </c>
     </row>
     <row r="71" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -4557,57 +4551,57 @@
         <v>234</v>
       </c>
       <c r="B71" t="s">
+        <v>408</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="D71" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="C71" s="3" t="s">
+      <c r="E71" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="F71" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="D71" s="3" t="s">
+      <c r="G71" s="9" t="s">
+        <v>796</v>
+      </c>
+      <c r="H71" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="E71" s="9" t="s">
+      <c r="L71" t="s">
         <v>413</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="M71" t="s">
         <v>414</v>
       </c>
-      <c r="G71" s="9" t="s">
-        <v>742</v>
-      </c>
-      <c r="H71" s="3" t="s">
+      <c r="N71" t="s">
+        <v>414</v>
+      </c>
+      <c r="O71" t="s">
+        <v>414</v>
+      </c>
+      <c r="P71" t="s">
         <v>415</v>
-      </c>
-      <c r="L71" t="s">
-        <v>416</v>
-      </c>
-      <c r="M71" t="s">
-        <v>417</v>
-      </c>
-      <c r="N71" t="s">
-        <v>417</v>
-      </c>
-      <c r="O71" t="s">
-        <v>417</v>
-      </c>
-      <c r="P71" t="s">
-        <v>418</v>
       </c>
     </row>
     <row r="72" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B72" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="E72" s="9" t="s">
-        <v>743</v>
+        <v>736</v>
       </c>
       <c r="G72" s="9" t="s">
-        <v>744</v>
+        <v>737</v>
       </c>
     </row>
     <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -4615,22 +4609,22 @@
         <v>295</v>
       </c>
       <c r="B73" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="E73" s="9" t="s">
-        <v>745</v>
+        <v>738</v>
       </c>
       <c r="G73" s="9" t="s">
-        <v>746</v>
+        <v>739</v>
       </c>
       <c r="J73" t="s">
         <v>226</v>
       </c>
       <c r="P73" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4638,7 +4632,7 @@
         <v>247</v>
       </c>
       <c r="B74" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4654,10 +4648,10 @@
         <v>218</v>
       </c>
       <c r="B76" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I76" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4665,10 +4659,10 @@
         <v>218</v>
       </c>
       <c r="B77" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="I77" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4676,10 +4670,10 @@
         <v>218</v>
       </c>
       <c r="B78" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="I78" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4687,10 +4681,10 @@
         <v>218</v>
       </c>
       <c r="B79" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="I79" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4698,13 +4692,13 @@
         <v>218</v>
       </c>
       <c r="B80" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="I80" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="P80" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4712,13 +4706,13 @@
         <v>218</v>
       </c>
       <c r="B81" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="I81" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="P81" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4726,10 +4720,10 @@
         <v>218</v>
       </c>
       <c r="B82" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="I82" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4737,13 +4731,13 @@
         <v>218</v>
       </c>
       <c r="B83" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="I83" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="P83" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4751,13 +4745,13 @@
         <v>218</v>
       </c>
       <c r="B84" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="I84" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="P84" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4765,10 +4759,10 @@
         <v>218</v>
       </c>
       <c r="B85" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="I85" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4776,13 +4770,13 @@
         <v>218</v>
       </c>
       <c r="B86" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="I86" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="P86" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4790,13 +4784,13 @@
         <v>218</v>
       </c>
       <c r="B87" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="I87" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="P87" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4804,10 +4798,10 @@
         <v>218</v>
       </c>
       <c r="B88" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="I88" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4815,10 +4809,10 @@
         <v>218</v>
       </c>
       <c r="B89" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I89" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4826,13 +4820,13 @@
         <v>218</v>
       </c>
       <c r="B90" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="I90" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="P90" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4840,13 +4834,13 @@
         <v>218</v>
       </c>
       <c r="B91" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="I91" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="P91" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4854,10 +4848,10 @@
         <v>218</v>
       </c>
       <c r="B92" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="I92" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="P92" s="6"/>
     </row>
@@ -4866,10 +4860,10 @@
         <v>218</v>
       </c>
       <c r="B93" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="I93" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="P93" s="6"/>
     </row>
@@ -4878,13 +4872,13 @@
         <v>218</v>
       </c>
       <c r="B94" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="I94" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="P94" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4892,13 +4886,13 @@
         <v>218</v>
       </c>
       <c r="B95" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="I95" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="P95" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4906,13 +4900,13 @@
         <v>218</v>
       </c>
       <c r="B96" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="I96" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="P96" s="6" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -4920,10 +4914,10 @@
         <v>231</v>
       </c>
       <c r="B98" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="P98" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
     </row>
     <row r="99" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -4931,16 +4925,16 @@
         <v>251</v>
       </c>
       <c r="B99" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E99" s="9" t="s">
-        <v>747</v>
+        <v>797</v>
       </c>
       <c r="G99" s="9" t="s">
-        <v>748</v>
+        <v>798</v>
       </c>
     </row>
     <row r="100" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -4948,25 +4942,25 @@
         <v>295</v>
       </c>
       <c r="B100" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D100" s="3" t="s">
         <v>338</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>749</v>
+        <v>799</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>339</v>
       </c>
       <c r="G100" s="9" t="s">
-        <v>750</v>
+        <v>740</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
     </row>
     <row r="101" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -4974,22 +4968,22 @@
         <v>341</v>
       </c>
       <c r="B101" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="D101" s="3" t="s">
         <v>344</v>
       </c>
       <c r="E101" s="9" t="s">
-        <v>751</v>
+        <v>741</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>345</v>
       </c>
       <c r="G101" s="9" t="s">
-        <v>752</v>
+        <v>742</v>
       </c>
       <c r="H101" s="3" t="s">
         <v>346</v>
@@ -5001,7 +4995,7 @@
         <v>348</v>
       </c>
       <c r="P101" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
     </row>
     <row r="102" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -5009,28 +5003,28 @@
         <v>234</v>
       </c>
       <c r="B102" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>352</v>
       </c>
       <c r="E102" s="9" t="s">
-        <v>753</v>
+        <v>743</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G102" s="9" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
       <c r="H102" s="3" t="s">
         <v>354</v>
       </c>
       <c r="L102" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="M102" t="s">
         <v>356</v>
@@ -5042,7 +5036,7 @@
         <v>356</v>
       </c>
       <c r="P102" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5050,13 +5044,13 @@
         <v>218</v>
       </c>
       <c r="B103" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I103" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="P103" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5064,10 +5058,10 @@
         <v>218</v>
       </c>
       <c r="B104" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I104" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5075,19 +5069,19 @@
         <v>251</v>
       </c>
       <c r="B105" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>755</v>
+        <v>745</v>
       </c>
       <c r="G105" s="9" t="s">
-        <v>756</v>
+        <v>746</v>
       </c>
       <c r="P105" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
     <row r="106" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5095,135 +5089,135 @@
         <v>251</v>
       </c>
       <c r="B106" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>758</v>
+        <v>800</v>
       </c>
       <c r="G106" s="9" t="s">
-        <v>757</v>
+        <v>747</v>
       </c>
       <c r="P106" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="107" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B107" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D107" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>748</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G107" s="9" t="s">
+        <v>749</v>
+      </c>
+      <c r="H107" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="E107" s="9" t="s">
-        <v>759</v>
-      </c>
-      <c r="F107" s="3" t="s">
+      <c r="L107" t="s">
         <v>381</v>
       </c>
-      <c r="G107" s="9" t="s">
-        <v>760</v>
-      </c>
-      <c r="H107" s="3" t="s">
+      <c r="M107" t="s">
         <v>382</v>
       </c>
-      <c r="L107" t="s">
-        <v>383</v>
-      </c>
-      <c r="M107" t="s">
-        <v>384</v>
-      </c>
       <c r="N107" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O107" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="108" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B108" t="s">
+        <v>492</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>750</v>
+      </c>
+      <c r="G108" s="9" t="s">
+        <v>494</v>
+      </c>
+      <c r="P108" t="s">
         <v>495</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="E108" s="3" t="s">
-        <v>761</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="P108" t="s">
-        <v>498</v>
       </c>
     </row>
     <row r="109" spans="1:16" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B109" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D109" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="G109" s="9" t="s">
+        <v>751</v>
+      </c>
+      <c r="H109" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="E109" s="9" t="s">
-        <v>501</v>
-      </c>
-      <c r="F109" s="3" t="s">
+      <c r="L109" t="s">
         <v>391</v>
       </c>
-      <c r="G109" s="9" t="s">
-        <v>762</v>
-      </c>
-      <c r="H109" s="3" t="s">
+      <c r="M109" t="s">
         <v>392</v>
       </c>
-      <c r="L109" t="s">
-        <v>393</v>
-      </c>
-      <c r="M109" t="s">
-        <v>394</v>
-      </c>
       <c r="N109" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="O109" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="110" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B110" t="s">
+        <v>499</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>500</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="G110" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="C110" s="3" t="s">
+      <c r="P110" t="s">
         <v>503</v>
-      </c>
-      <c r="E110" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="P110" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="111" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -5231,19 +5225,19 @@
         <v>251</v>
       </c>
       <c r="B111" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="P111" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
     </row>
     <row r="112" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -5251,19 +5245,19 @@
         <v>251</v>
       </c>
       <c r="B112" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="C112" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="G112" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="E112" s="3" t="s">
-        <v>511</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>408</v>
-      </c>
       <c r="P112" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5271,10 +5265,10 @@
         <v>218</v>
       </c>
       <c r="B113" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I113" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5282,10 +5276,10 @@
         <v>218</v>
       </c>
       <c r="B114" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I114" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5293,31 +5287,31 @@
         <v>234</v>
       </c>
       <c r="B115" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E115" s="9" t="s">
-        <v>763</v>
+        <v>752</v>
       </c>
       <c r="G115" s="9" t="s">
-        <v>764</v>
+        <v>753</v>
       </c>
       <c r="L115" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="M115" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="N115" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O115" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="P115" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5325,10 +5319,10 @@
         <v>218</v>
       </c>
       <c r="B116" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I116" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5336,10 +5330,10 @@
         <v>218</v>
       </c>
       <c r="B117" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="I117" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5347,10 +5341,10 @@
         <v>218</v>
       </c>
       <c r="B118" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="I118" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5358,10 +5352,10 @@
         <v>218</v>
       </c>
       <c r="B119" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="I119" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5369,10 +5363,10 @@
         <v>218</v>
       </c>
       <c r="B120" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="I120" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5380,10 +5374,10 @@
         <v>218</v>
       </c>
       <c r="B121" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I121" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5391,7 +5385,7 @@
         <v>247</v>
       </c>
       <c r="B122" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5399,10 +5393,10 @@
         <v>231</v>
       </c>
       <c r="B123" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="P123" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
     </row>
     <row r="124" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -5410,16 +5404,16 @@
         <v>251</v>
       </c>
       <c r="B124" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="E124" s="9" t="s">
-        <v>765</v>
+        <v>801</v>
       </c>
       <c r="G124" s="9" t="s">
-        <v>766</v>
+        <v>798</v>
       </c>
     </row>
     <row r="125" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -5427,22 +5421,22 @@
         <v>295</v>
       </c>
       <c r="B125" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="D125" s="3" t="s">
         <v>338</v>
       </c>
       <c r="E125" s="29" t="s">
-        <v>767</v>
+        <v>754</v>
       </c>
       <c r="F125" s="3" t="s">
         <v>339</v>
       </c>
       <c r="G125" s="9" t="s">
-        <v>768</v>
+        <v>755</v>
       </c>
       <c r="H125" s="3" t="s">
         <v>340</v>
@@ -5453,22 +5447,22 @@
         <v>341</v>
       </c>
       <c r="B126" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="D126" s="3" t="s">
         <v>344</v>
       </c>
       <c r="E126" s="29" t="s">
-        <v>769</v>
+        <v>756</v>
       </c>
       <c r="F126" s="3" t="s">
         <v>345</v>
       </c>
       <c r="G126" s="29" t="s">
-        <v>770</v>
+        <v>757</v>
       </c>
       <c r="H126" s="3" t="s">
         <v>346</v>
@@ -5480,7 +5474,7 @@
         <v>348</v>
       </c>
       <c r="P126" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
     </row>
     <row r="127" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -5488,28 +5482,28 @@
         <v>234</v>
       </c>
       <c r="B127" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="D127" s="3" t="s">
         <v>352</v>
       </c>
       <c r="E127" s="29" t="s">
-        <v>771</v>
+        <v>758</v>
       </c>
       <c r="F127" s="3" t="s">
         <v>353</v>
       </c>
       <c r="G127" s="29" t="s">
-        <v>754</v>
+        <v>744</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="L127" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="M127" t="s">
         <v>356</v>
@@ -5521,7 +5515,7 @@
         <v>356</v>
       </c>
       <c r="P127" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5529,13 +5523,13 @@
         <v>218</v>
       </c>
       <c r="B128" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I128" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="P128" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5543,10 +5537,10 @@
         <v>218</v>
       </c>
       <c r="B129" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I129" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5554,19 +5548,19 @@
         <v>251</v>
       </c>
       <c r="B130" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="E130" s="29" t="s">
-        <v>772</v>
+        <v>759</v>
       </c>
       <c r="G130" s="29" t="s">
-        <v>773</v>
+        <v>760</v>
       </c>
       <c r="P130" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
     </row>
     <row r="131" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5574,135 +5568,135 @@
         <v>251</v>
       </c>
       <c r="B131" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="E131" s="30" t="s">
-        <v>774</v>
+        <v>803</v>
       </c>
       <c r="G131" s="30" t="s">
-        <v>775</v>
+        <v>802</v>
       </c>
       <c r="P131" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
     </row>
     <row r="132" spans="1:16" ht="100.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A132" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B132" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D132" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="E132" s="31" t="s">
+        <v>748</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G132" s="32" t="s">
+        <v>761</v>
+      </c>
+      <c r="H132" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="E132" s="31" t="s">
-        <v>759</v>
-      </c>
-      <c r="F132" s="3" t="s">
+      <c r="L132" t="s">
         <v>381</v>
       </c>
-      <c r="G132" s="32" t="s">
-        <v>776</v>
-      </c>
-      <c r="H132" s="3" t="s">
+      <c r="M132" t="s">
         <v>382</v>
       </c>
-      <c r="L132" t="s">
-        <v>383</v>
-      </c>
-      <c r="M132" t="s">
-        <v>384</v>
-      </c>
       <c r="N132" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="O132" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="133" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A133" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="B133" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>761</v>
+        <v>750</v>
       </c>
       <c r="G133" s="32" t="s">
-        <v>777</v>
+        <v>762</v>
       </c>
       <c r="P133" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
     </row>
     <row r="134" spans="1:16" ht="201.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A134" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B134" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>778</v>
+        <v>498</v>
       </c>
       <c r="F134" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="G134" s="32" t="s">
+        <v>751</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>552</v>
+      </c>
+      <c r="L134" t="s">
         <v>391</v>
       </c>
-      <c r="G134" s="32" t="s">
-        <v>762</v>
-      </c>
-      <c r="H134" s="3" t="s">
-        <v>555</v>
-      </c>
-      <c r="L134" t="s">
-        <v>393</v>
-      </c>
       <c r="M134" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="N134" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="O134" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="135" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A135" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B135" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="E135" s="21" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="G135" s="21" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="P135" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
     <row r="136" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -5710,19 +5704,19 @@
         <v>251</v>
       </c>
       <c r="B136" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C136" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>557</v>
+      </c>
+      <c r="G136" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="E136" s="3" t="s">
-        <v>560</v>
-      </c>
-      <c r="G136" s="3" t="s">
-        <v>403</v>
-      </c>
       <c r="P136" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
     </row>
     <row r="137" spans="1:16" ht="86.4" x14ac:dyDescent="0.55000000000000004">
@@ -5730,19 +5724,19 @@
         <v>251</v>
       </c>
       <c r="B137" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="C137" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="E137" s="3" t="s">
+        <v>560</v>
+      </c>
+      <c r="G137" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="E137" s="3" t="s">
-        <v>563</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>408</v>
-      </c>
       <c r="P137" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5750,10 +5744,10 @@
         <v>218</v>
       </c>
       <c r="B138" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="I138" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5761,10 +5755,10 @@
         <v>218</v>
       </c>
       <c r="B139" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="I139" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="140" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5772,31 +5766,31 @@
         <v>234</v>
       </c>
       <c r="B140" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E140" s="32" t="s">
-        <v>779</v>
+        <v>763</v>
       </c>
       <c r="G140" s="32" t="s">
-        <v>780</v>
+        <v>764</v>
       </c>
       <c r="L140" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="M140" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="N140" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="O140" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="P140" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5804,10 +5798,10 @@
         <v>218</v>
       </c>
       <c r="B141" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="I141" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5815,10 +5809,10 @@
         <v>218</v>
       </c>
       <c r="B142" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="I142" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5826,10 +5820,10 @@
         <v>218</v>
       </c>
       <c r="B143" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="I143" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5837,10 +5831,10 @@
         <v>218</v>
       </c>
       <c r="B144" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="I144" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5848,10 +5842,10 @@
         <v>218</v>
       </c>
       <c r="B145" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="I145" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5859,10 +5853,10 @@
         <v>218</v>
       </c>
       <c r="B146" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="I146" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -5870,7 +5864,7 @@
         <v>247</v>
       </c>
       <c r="B147" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
     </row>
     <row r="149" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5878,20 +5872,20 @@
         <v>295</v>
       </c>
       <c r="B149" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="E149" s="9" t="s">
-        <v>781</v>
+        <v>765</v>
       </c>
       <c r="F149" s="9"/>
       <c r="G149" s="9" t="s">
-        <v>782</v>
+        <v>804</v>
       </c>
       <c r="P149" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="150" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -5899,28 +5893,28 @@
         <v>295</v>
       </c>
       <c r="B150" t="s">
+        <v>583</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="D150" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="E150" s="9" t="s">
+        <v>766</v>
+      </c>
+      <c r="F150" s="3" t="s">
         <v>586</v>
       </c>
-      <c r="C150" s="3" t="s">
+      <c r="G150" s="9" t="s">
+        <v>767</v>
+      </c>
+      <c r="H150" s="3" t="s">
         <v>587</v>
       </c>
-      <c r="D150" s="3" t="s">
+      <c r="P150" t="s">
         <v>588</v>
-      </c>
-      <c r="E150" s="9" t="s">
-        <v>783</v>
-      </c>
-      <c r="F150" s="3" t="s">
-        <v>589</v>
-      </c>
-      <c r="G150" s="9" t="s">
-        <v>784</v>
-      </c>
-      <c r="H150" s="3" t="s">
-        <v>590</v>
-      </c>
-      <c r="P150" t="s">
-        <v>591</v>
       </c>
     </row>
     <row r="151" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -5928,28 +5922,28 @@
         <v>295</v>
       </c>
       <c r="B151" t="s">
+        <v>589</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="E151" s="9" t="s">
+        <v>768</v>
+      </c>
+      <c r="F151" s="3" t="s">
         <v>592</v>
       </c>
-      <c r="C151" s="3" t="s">
+      <c r="G151" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="H151" s="3" t="s">
         <v>593</v>
       </c>
-      <c r="D151" s="3" t="s">
-        <v>594</v>
-      </c>
-      <c r="E151" s="9" t="s">
-        <v>785</v>
-      </c>
-      <c r="F151" s="3" t="s">
-        <v>595</v>
-      </c>
-      <c r="G151" s="9" t="s">
-        <v>786</v>
-      </c>
-      <c r="H151" s="3" t="s">
-        <v>596</v>
-      </c>
       <c r="P151" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="152" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5957,19 +5951,19 @@
         <v>295</v>
       </c>
       <c r="B152" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="E152" s="9" t="s">
-        <v>787</v>
+        <v>770</v>
       </c>
       <c r="G152" s="9" t="s">
-        <v>788</v>
+        <v>771</v>
       </c>
       <c r="P152" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="153" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5977,19 +5971,19 @@
         <v>295</v>
       </c>
       <c r="B153" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="E153" s="9" t="s">
-        <v>789</v>
+        <v>772</v>
       </c>
       <c r="G153" s="9" t="s">
-        <v>790</v>
+        <v>773</v>
       </c>
       <c r="P153" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="154" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -5997,19 +5991,19 @@
         <v>295</v>
       </c>
       <c r="B154" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="E154" s="9" t="s">
-        <v>791</v>
+        <v>774</v>
       </c>
       <c r="G154" s="9" t="s">
-        <v>792</v>
+        <v>775</v>
       </c>
       <c r="P154" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6017,13 +6011,13 @@
         <v>218</v>
       </c>
       <c r="B156" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="I156" t="s">
         <v>6</v>
       </c>
       <c r="P156" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6031,13 +6025,13 @@
         <v>218</v>
       </c>
       <c r="B157" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="I157" t="s">
         <v>6</v>
       </c>
       <c r="P157" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
     </row>
     <row r="158" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -6045,28 +6039,28 @@
         <v>251</v>
       </c>
       <c r="B158" t="s">
+        <v>605</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>606</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>607</v>
+      </c>
+      <c r="E158" s="31" t="s">
+        <v>807</v>
+      </c>
+      <c r="F158" s="3" t="s">
         <v>608</v>
       </c>
-      <c r="C158" s="3" t="s">
+      <c r="G158" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="H158" s="3" t="s">
         <v>609</v>
       </c>
-      <c r="D158" s="3" t="s">
+      <c r="P158" t="s">
         <v>610</v>
-      </c>
-      <c r="E158" s="31" t="s">
-        <v>611</v>
-      </c>
-      <c r="F158" s="3" t="s">
-        <v>612</v>
-      </c>
-      <c r="G158" s="9" t="s">
-        <v>793</v>
-      </c>
-      <c r="H158" s="3" t="s">
-        <v>613</v>
-      </c>
-      <c r="P158" t="s">
-        <v>614</v>
       </c>
     </row>
     <row r="159" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -6074,19 +6068,19 @@
         <v>295</v>
       </c>
       <c r="B159" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="E159" s="9" t="s">
-        <v>794</v>
+        <v>776</v>
       </c>
       <c r="G159" s="9" t="s">
-        <v>795</v>
+        <v>777</v>
       </c>
       <c r="P159" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
     </row>
     <row r="160" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -6094,28 +6088,28 @@
         <v>251</v>
       </c>
       <c r="B160" t="s">
+        <v>613</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>615</v>
+      </c>
+      <c r="E160" s="9" t="s">
+        <v>808</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>616</v>
+      </c>
+      <c r="G160" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="H160" s="3" t="s">
         <v>617</v>
       </c>
-      <c r="C160" s="3" t="s">
+      <c r="P160" t="s">
         <v>618</v>
-      </c>
-      <c r="D160" s="3" t="s">
-        <v>619</v>
-      </c>
-      <c r="E160" s="9" t="s">
-        <v>620</v>
-      </c>
-      <c r="F160" s="3" t="s">
-        <v>621</v>
-      </c>
-      <c r="G160" s="9" t="s">
-        <v>622</v>
-      </c>
-      <c r="H160" s="3" t="s">
-        <v>623</v>
-      </c>
-      <c r="P160" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="161" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -6123,19 +6117,19 @@
         <v>295</v>
       </c>
       <c r="B161" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="E161" s="9" t="s">
-        <v>796</v>
+        <v>778</v>
       </c>
       <c r="G161" s="9" t="s">
-        <v>797</v>
+        <v>779</v>
       </c>
       <c r="P161" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="163" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6143,13 +6137,13 @@
         <v>218</v>
       </c>
       <c r="B163" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="I163" t="s">
         <v>6</v>
       </c>
       <c r="P163" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
     </row>
     <row r="164" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6157,13 +6151,13 @@
         <v>218</v>
       </c>
       <c r="B164" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="I164" t="s">
         <v>6</v>
       </c>
       <c r="P164" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6171,13 +6165,13 @@
         <v>218</v>
       </c>
       <c r="B165" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="I165" t="s">
         <v>6</v>
       </c>
       <c r="P165" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
     </row>
     <row r="166" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6185,13 +6179,13 @@
         <v>218</v>
       </c>
       <c r="B166" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="I166" t="s">
         <v>6</v>
       </c>
       <c r="P166" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
     </row>
     <row r="167" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6213,10 +6207,10 @@
         <v>263</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="C169" s="8" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="D169" s="8"/>
       <c r="E169" s="8"/>
@@ -6224,7 +6218,7 @@
       <c r="G169" s="8"/>
       <c r="H169" s="8"/>
       <c r="Q169" s="1" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6232,7 +6226,7 @@
         <v>218</v>
       </c>
       <c r="B170" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="I170" t="s">
         <v>321</v>
@@ -6243,10 +6237,10 @@
         <v>218</v>
       </c>
       <c r="B171" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="I171" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6254,10 +6248,10 @@
         <v>218</v>
       </c>
       <c r="B172" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="I172" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
     </row>
     <row r="173" spans="1:17" x14ac:dyDescent="0.55000000000000004">
@@ -6265,10 +6259,10 @@
         <v>218</v>
       </c>
       <c r="B173" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="I173" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
     </row>
     <row r="174" spans="1:17" ht="43.2" x14ac:dyDescent="0.55000000000000004">
@@ -6276,19 +6270,19 @@
         <v>251</v>
       </c>
       <c r="B174" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="C174" s="3" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="E174" s="9" t="s">
-        <v>798</v>
+        <v>780</v>
       </c>
       <c r="G174" s="9" t="s">
-        <v>799</v>
+        <v>781</v>
       </c>
       <c r="P174" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
     </row>
     <row r="175" spans="1:17" s="33" customFormat="1" ht="72" x14ac:dyDescent="0.55000000000000004">
@@ -6296,10 +6290,10 @@
         <v>251</v>
       </c>
       <c r="B175" s="33" t="s">
-        <v>648</v>
+        <v>642</v>
       </c>
       <c r="C175" s="34" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
       <c r="D175" s="34"/>
       <c r="E175" s="34"/>
@@ -6312,19 +6306,19 @@
         <v>295</v>
       </c>
       <c r="B176" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
       <c r="E176" s="9" t="s">
-        <v>800</v>
+        <v>782</v>
       </c>
       <c r="G176" s="9" t="s">
-        <v>801</v>
+        <v>783</v>
       </c>
       <c r="P176" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
     </row>
     <row r="177" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -6332,115 +6326,115 @@
         <v>295</v>
       </c>
       <c r="B177" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="E177" s="3" t="s">
-        <v>802</v>
+        <v>784</v>
       </c>
       <c r="G177" s="9" t="s">
-        <v>803</v>
+        <v>785</v>
       </c>
       <c r="P177" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A178" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="B178" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>656</v>
+        <v>650</v>
       </c>
       <c r="E178" s="3" t="s">
-        <v>657</v>
+        <v>809</v>
       </c>
       <c r="G178" s="9" t="s">
-        <v>804</v>
+        <v>786</v>
       </c>
       <c r="L178" t="s">
-        <v>658</v>
+        <v>651</v>
       </c>
       <c r="M178" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="N178" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="O178" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="P178" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A179" t="s">
+        <v>648</v>
+      </c>
+      <c r="B179" t="s">
         <v>654</v>
       </c>
-      <c r="B179" t="s">
-        <v>661</v>
-      </c>
       <c r="C179" s="3" t="s">
-        <v>662</v>
+        <v>655</v>
       </c>
       <c r="E179" s="3" t="s">
-        <v>805</v>
+        <v>787</v>
       </c>
       <c r="G179" s="9" t="s">
-        <v>806</v>
+        <v>788</v>
       </c>
       <c r="L179" t="s">
-        <v>663</v>
+        <v>656</v>
       </c>
       <c r="M179" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="N179" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="O179" t="s">
-        <v>664</v>
+        <v>657</v>
       </c>
       <c r="P179" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A180" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="B180" t="s">
-        <v>665</v>
+        <v>658</v>
       </c>
       <c r="C180" s="3" t="s">
-        <v>666</v>
+        <v>659</v>
       </c>
       <c r="E180" s="9" t="s">
-        <v>807</v>
+        <v>789</v>
       </c>
       <c r="G180" s="9" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="L180" t="s">
-        <v>667</v>
+        <v>660</v>
       </c>
       <c r="M180" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="N180" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="O180" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="P180" t="s">
-        <v>660</v>
+        <v>653</v>
       </c>
     </row>
     <row r="182" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -6448,7 +6442,7 @@
         <v>292</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="C182" s="8"/>
       <c r="D182" s="8"/>
@@ -6462,115 +6456,115 @@
         <v>148</v>
       </c>
       <c r="B184" t="s">
-        <v>669</v>
+        <v>662</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>670</v>
+        <v>663</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>671</v>
+        <v>664</v>
       </c>
       <c r="E184" s="3" t="s">
-        <v>672</v>
+        <v>665</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>673</v>
+        <v>666</v>
       </c>
       <c r="G184" s="3" t="s">
-        <v>674</v>
+        <v>667</v>
       </c>
       <c r="H184" s="3" t="s">
-        <v>675</v>
+        <v>668</v>
       </c>
     </row>
     <row r="185" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A185" t="s">
+        <v>669</v>
+      </c>
+      <c r="B185" t="s">
+        <v>670</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>671</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>672</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="H185" s="3" t="s">
         <v>676</v>
-      </c>
-      <c r="B185" t="s">
-        <v>677</v>
-      </c>
-      <c r="C185" s="3" t="s">
-        <v>678</v>
-      </c>
-      <c r="D185" s="3" t="s">
-        <v>679</v>
-      </c>
-      <c r="E185" s="3" t="s">
-        <v>680</v>
-      </c>
-      <c r="F185" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="G185" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="H185" s="3" t="s">
-        <v>683</v>
       </c>
       <c r="J185" t="s">
         <v>226</v>
       </c>
       <c r="P185" t="s">
-        <v>684</v>
+        <v>677</v>
       </c>
     </row>
     <row r="186" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A186" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
       <c r="B186" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>679</v>
+        <v>672</v>
       </c>
       <c r="E186" s="3" t="s">
+        <v>673</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>674</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>675</v>
+      </c>
+      <c r="H186" s="3" t="s">
+        <v>676</v>
+      </c>
+      <c r="P186" t="s">
         <v>680</v>
-      </c>
-      <c r="F186" s="3" t="s">
-        <v>681</v>
-      </c>
-      <c r="G186" s="3" t="s">
-        <v>682</v>
-      </c>
-      <c r="H186" s="3" t="s">
-        <v>683</v>
-      </c>
-      <c r="P186" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="187" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A187" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
       <c r="B187" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>678</v>
+        <v>671</v>
       </c>
       <c r="E187" s="3" t="s">
-        <v>680</v>
+        <v>673</v>
       </c>
       <c r="F187" s="3" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>682</v>
+        <v>675</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>683</v>
+        <v>676</v>
       </c>
       <c r="J187" t="s">
         <v>226</v>
       </c>
       <c r="P187" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="188" spans="1:16" ht="57.6" x14ac:dyDescent="0.55000000000000004">
@@ -6578,19 +6572,19 @@
         <v>251</v>
       </c>
       <c r="B188" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
       <c r="E188" s="3" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
       <c r="P188" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
     </row>
     <row r="189" spans="1:16" ht="28.8" x14ac:dyDescent="0.55000000000000004">
@@ -6598,16 +6592,16 @@
         <v>227</v>
       </c>
       <c r="B189" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
       <c r="E189" s="3" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.55000000000000004">
@@ -6623,21 +6617,21 @@
         <v>218</v>
       </c>
       <c r="B192" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
       <c r="I192" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="193" spans="1:9" s="33" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A193" s="33" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B193" s="33" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
       <c r="C193" s="34" t="s">
-        <v>703</v>
+        <v>696</v>
       </c>
       <c r="D193" s="34"/>
       <c r="E193" s="34"/>
@@ -6650,10 +6644,10 @@
         <v>218</v>
       </c>
       <c r="B194" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="I194" t="s">
-        <v>705</v>
+        <v>698</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6661,10 +6655,10 @@
         <v>218</v>
       </c>
       <c r="B195" t="s">
-        <v>706</v>
+        <v>699</v>
       </c>
       <c r="I195" t="s">
-        <v>707</v>
+        <v>700</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6672,10 +6666,10 @@
         <v>218</v>
       </c>
       <c r="B196" t="s">
-        <v>708</v>
+        <v>701</v>
       </c>
       <c r="I196" t="s">
-        <v>709</v>
+        <v>702</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6683,10 +6677,10 @@
         <v>218</v>
       </c>
       <c r="B197" t="s">
-        <v>710</v>
+        <v>703</v>
       </c>
       <c r="I197" t="s">
-        <v>711</v>
+        <v>704</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6694,10 +6688,10 @@
         <v>218</v>
       </c>
       <c r="B198" t="s">
-        <v>712</v>
+        <v>705</v>
       </c>
       <c r="I198" t="s">
-        <v>713</v>
+        <v>706</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.55000000000000004">
@@ -6705,10 +6699,10 @@
         <v>218</v>
       </c>
       <c r="B199" t="s">
-        <v>714</v>
+        <v>707</v>
       </c>
       <c r="I199" t="s">
-        <v>715</v>
+        <v>708</v>
       </c>
     </row>
   </sheetData>
@@ -7893,143 +7887,15 @@
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </mda26ace941f4791a7314a339fee829c>
-    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </h6a71f3e574e4344bc34f3fc9dd20054>
-    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
-    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
-    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
-    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j048a4f9aaad4a8990a1d5e5f53cb451>
-    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
-    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
-          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
-        </TermInfo>
-      </Terms>
-    </ga975397408f43e4b84ec8e5a598e523>
-    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <UserInfo>
-        <DisplayName/>
-        <AccountId xsi:nil="true"/>
-        <AccountType/>
-      </UserInfo>
-    </WrittenBy>
-    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Value>22</Value>
-    </TaxCatchAll>
-    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </j169e817e0ee4eb8974e6fc4a2762909>
-    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </k8c968e8c72a4eda96b7e8fdbe192be2>
-    <_dlc_DocId xmlns="359fe316-fab8-49f4-87fa-a9923030124f">Z6MCZFE5NNQT-1373495628-1432</_dlc_DocId>
-    <MediaLengthInSeconds xmlns="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xsi:nil="true"/>
-    <SemaphoreItemMetadata xmlns="359fe316-fab8-49f4-87fa-a9923030124f" xsi:nil="true"/>
-    <TaxKeywordTaxHTField xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-    <_dlc_DocIdUrl xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <Url>https://unicef.sharepoint.com/teams/AFG-Nutrition/_layouts/15/DocIdRedir.aspx?ID=Z6MCZFE5NNQT-1373495628-1432</Url>
-      <Description>Z6MCZFE5NNQT-1373495628-1432</Description>
-    </_dlc_DocIdUrl>
-    <SharedWithUsers xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
-      <UserInfo>
-        <DisplayName>Shaista Mehraban</DisplayName>
-        <AccountId>295</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Said M Yaqoob Azimi</DisplayName>
-        <AccountId>80</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Ahmad Nawid Qarizada</DisplayName>
-        <AccountId>206</AccountId>
-        <AccountType/>
-      </UserInfo>
-      <UserInfo>
-        <DisplayName>Melanie Galvin</DisplayName>
-        <AccountId>304</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="UNICEF Document" ma:contentTypeID="0x0101009BA85F8052A6DA4FA3E31FF9F74C6970001ED9D7A792C89C46A2A86B92A3D9E4B0" ma:contentTypeVersion="43" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6635fd09095faeb866f46079413f6d37">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="ca283e0b-db31-4043-a2ef-b80661bf084a" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="359fe316-fab8-49f4-87fa-a9923030124f" xmlns:ns5="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xmlns:ns6="http://schemas.microsoft.com/sharepoint/v4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="cb5c23aaefc81f3be1817883f8b886f9" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -8468,14 +8334,142 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <mda26ace941f4791a7314a339fee829c xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </mda26ace941f4791a7314a339fee829c>
+    <h6a71f3e574e4344bc34f3fc9dd20054 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </h6a71f3e574e4344bc34f3fc9dd20054>
+    <CategoryDescription xmlns="http://schemas.microsoft.com/sharepoint.v3" xsi:nil="true"/>
+    <ContentLanguage xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">English</ContentLanguage>
+    <DateTransmittedEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <IconOverlay xmlns="http://schemas.microsoft.com/sharepoint/v4" xsi:nil="true"/>
+    <j048a4f9aaad4a8990a1d5e5f53cb451 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j048a4f9aaad4a8990a1d5e5f53cb451>
+    <ContentStatus xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <SenderEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <RecipientsEmail xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a" xsi:nil="true"/>
+    <ga975397408f43e4b84ec8e5a598e523 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+        <TermInfo xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+          <TermName xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">India-2040</TermName>
+          <TermId xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">6135ebe8-487a-4055-a9b4-1bbc7248f4ec</TermId>
+        </TermInfo>
+      </Terms>
+    </ga975397408f43e4b84ec8e5a598e523>
+    <WrittenBy xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <UserInfo>
+        <DisplayName/>
+        <AccountId xsi:nil="true"/>
+        <AccountType/>
+      </UserInfo>
+    </WrittenBy>
+    <TaxCatchAll xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Value>22</Value>
+    </TaxCatchAll>
+    <j169e817e0ee4eb8974e6fc4a2762909 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </j169e817e0ee4eb8974e6fc4a2762909>
+    <k8c968e8c72a4eda96b7e8fdbe192be2 xmlns="ca283e0b-db31-4043-a2ef-b80661bf084a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </k8c968e8c72a4eda96b7e8fdbe192be2>
+    <_dlc_DocId xmlns="359fe316-fab8-49f4-87fa-a9923030124f">Z6MCZFE5NNQT-1373495628-1432</_dlc_DocId>
+    <MediaLengthInSeconds xmlns="117936e8-0f80-4b9a-8a4d-392a13d0dc4e" xsi:nil="true"/>
+    <SemaphoreItemMetadata xmlns="359fe316-fab8-49f4-87fa-a9923030124f" xsi:nil="true"/>
+    <TaxKeywordTaxHTField xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+    <_dlc_DocIdUrl xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <Url>https://unicef.sharepoint.com/teams/AFG-Nutrition/_layouts/15/DocIdRedir.aspx?ID=Z6MCZFE5NNQT-1373495628-1432</Url>
+      <Description>Z6MCZFE5NNQT-1373495628-1432</Description>
+    </_dlc_DocIdUrl>
+    <SharedWithUsers xmlns="359fe316-fab8-49f4-87fa-a9923030124f">
+      <UserInfo>
+        <DisplayName>Shaista Mehraban</DisplayName>
+        <AccountId>295</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Said M Yaqoob Azimi</DisplayName>
+        <AccountId>80</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Ahmad Nawid Qarizada</DisplayName>
+        <AccountId>206</AccountId>
+        <AccountType/>
+      </UserInfo>
+      <UserInfo>
+        <DisplayName>Melanie Galvin</DisplayName>
+        <AccountId>304</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
 <file path=customXml/item6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8484,36 +8478,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
-    <ds:schemaRef ds:uri="359fe316-fab8-49f4-87fa-a9923030124f"/>
-    <ds:schemaRef ds:uri="117936e8-0f80-4b9a-8a4d-392a13d0dc4e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381EF04D-88DF-4FBB-A10E-8C4034F401AA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8536,10 +8508,32 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E79A499-C8C2-4C1D-81D3-8E30D1773AC4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="ca283e0b-db31-4043-a2ef-b80661bf084a"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint.v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v4"/>
+    <ds:schemaRef ds:uri="359fe316-fab8-49f4-87fa-a9923030124f"/>
+    <ds:schemaRef ds:uri="117936e8-0f80-4b9a-8a4d-392a13d0dc4e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2C70C4BB-1EE6-4AB7-A889-61CDC4FF18D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F08C764-A25F-492B-9203-3CD2DDED2468}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07AB0993-6E0F-4C7C-A737-78841007CC31}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>